<commit_message>
peopleview fight can choose map now
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassic\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="284">
   <si>
     <t>老鼠</t>
   </si>
@@ -958,6 +958,33 @@
   </si>
   <si>
     <t>51000281;51000270</t>
+  </si>
+  <si>
+    <t>Rule</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>快速对战地图</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BattleMap</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>blank</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>doublec</t>
+  </si>
+  <si>
+    <t>oneline</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1159,7 +1186,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1348,6 +1375,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor theme="4"/>
       </patternFill>
     </fill>
@@ -1627,7 +1666,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1656,6 +1695,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1703,7 +1763,63 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="38">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="9" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF4F81BD"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF4F81BD"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF4F81BD"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF4F81BD"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2110,19 +2226,30 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF4F81BD"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF4F81BD"/>
-        </right>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
         <top style="thin">
-          <color rgb="FF4F81BD"/>
+          <color theme="4"/>
         </top>
-        <bottom style="thin">
-          <color rgb="FF4F81BD"/>
-        </bottom>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2137,33 +2264,20 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
+        <color theme="1"/>
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2640,54 +2754,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:O73" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
-  <autoFilter ref="A3:O73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:P73" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" tableBorderDxfId="35">
+  <autoFilter ref="A3:P73"/>
   <sortState ref="A4:O83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Id" dataDxfId="32"/>
-    <tableColumn id="2" name="Name" dataDxfId="31"/>
-    <tableColumn id="3" name="Type" dataDxfId="30"/>
-    <tableColumn id="6" name="World" dataDxfId="29"/>
-    <tableColumn id="7" name="Deck" dataDxfId="28"/>
-    <tableColumn id="8" name="Cards" dataDxfId="27"/>
-    <tableColumn id="10" name="Job" dataDxfId="26"/>
-    <tableColumn id="4" name="KingCard" dataDxfId="25"/>
-    <tableColumn id="5" name="Rule" dataDxfId="24"/>
-    <tableColumn id="11" name="Level" dataDxfId="23"/>
-    <tableColumn id="12" name="Reward" dataDxfId="22"/>
-    <tableColumn id="16" name="EnergyRate" dataDxfId="21"/>
-    <tableColumn id="13" name="Method" dataDxfId="20"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="19"/>
-    <tableColumn id="15" name="Figue" dataDxfId="18"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Id" dataDxfId="34"/>
+    <tableColumn id="2" name="Name" dataDxfId="33"/>
+    <tableColumn id="3" name="Type" dataDxfId="32"/>
+    <tableColumn id="6" name="World" dataDxfId="31"/>
+    <tableColumn id="7" name="Deck" dataDxfId="30"/>
+    <tableColumn id="8" name="Cards" dataDxfId="29"/>
+    <tableColumn id="10" name="Job" dataDxfId="28"/>
+    <tableColumn id="4" name="KingCard" dataDxfId="27"/>
+    <tableColumn id="5" name="Rule" dataDxfId="26"/>
+    <tableColumn id="11" name="Level" dataDxfId="25"/>
+    <tableColumn id="12" name="Reward" dataDxfId="24"/>
+    <tableColumn id="16" name="EnergyRate" dataDxfId="23"/>
+    <tableColumn id="13" name="Method" dataDxfId="22"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="21"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="4"/>
+    <tableColumn id="15" name="Figue" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:O14" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
-  <autoFilter ref="A3:O14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:P14" totalsRowShown="0" headerRowDxfId="0" dataDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A3:P14"/>
   <sortState ref="A4:O83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Id" dataDxfId="14"/>
-    <tableColumn id="2" name="Name" dataDxfId="13"/>
-    <tableColumn id="3" name="Type" dataDxfId="12"/>
-    <tableColumn id="6" name="World" dataDxfId="11"/>
-    <tableColumn id="7" name="Deck" dataDxfId="10"/>
-    <tableColumn id="8" name="Cards" dataDxfId="9"/>
-    <tableColumn id="10" name="Job" dataDxfId="8"/>
-    <tableColumn id="4" name="KingCard" dataDxfId="7"/>
-    <tableColumn id="5" name="Rule" dataDxfId="6"/>
-    <tableColumn id="11" name="Level" dataDxfId="5"/>
-    <tableColumn id="12" name="Reward" dataDxfId="4"/>
-    <tableColumn id="16" name="EnergyRate" dataDxfId="3"/>
-    <tableColumn id="13" name="Method" dataDxfId="2"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="1"/>
-    <tableColumn id="15" name="Figue" dataDxfId="0"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Id" dataDxfId="19"/>
+    <tableColumn id="2" name="Name" dataDxfId="18"/>
+    <tableColumn id="3" name="Type" dataDxfId="17"/>
+    <tableColumn id="6" name="World" dataDxfId="16"/>
+    <tableColumn id="7" name="Deck" dataDxfId="15"/>
+    <tableColumn id="8" name="Cards" dataDxfId="14"/>
+    <tableColumn id="10" name="Job" dataDxfId="13"/>
+    <tableColumn id="4" name="KingCard" dataDxfId="12"/>
+    <tableColumn id="5" name="Rule" dataDxfId="11"/>
+    <tableColumn id="11" name="Level" dataDxfId="10"/>
+    <tableColumn id="12" name="Reward" dataDxfId="9"/>
+    <tableColumn id="16" name="EnergyRate" dataDxfId="8"/>
+    <tableColumn id="13" name="Method" dataDxfId="7"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="6"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="3"/>
+    <tableColumn id="15" name="Figue" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2980,13 +3096,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
+      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2999,10 +3115,10 @@
     <col min="9" max="10" width="6.25" customWidth="1"/>
     <col min="11" max="12" width="11.875" customWidth="1"/>
     <col min="13" max="13" width="9.5" customWidth="1"/>
-    <col min="14" max="14" width="10.625" customWidth="1"/>
+    <col min="14" max="15" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>210</v>
       </c>
@@ -3045,11 +3161,14 @@
       <c r="N1" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>208</v>
       </c>
@@ -3092,11 +3211,14 @@
       <c r="N2" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>222</v>
       </c>
@@ -3122,7 +3244,7 @@
         <v>244</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>247</v>
+        <v>277</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>229</v>
@@ -3140,10 +3262,13 @@
         <v>232</v>
       </c>
       <c r="O3" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="P3" s="8" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43000001</v>
       </c>
@@ -3183,10 +3308,13 @@
         <v>4</v>
       </c>
       <c r="O4" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43000002</v>
       </c>
@@ -3226,10 +3354,13 @@
         <v>6</v>
       </c>
       <c r="O5" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P5" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43000003</v>
       </c>
@@ -3269,10 +3400,13 @@
         <v>8</v>
       </c>
       <c r="O6" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P6" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43000004</v>
       </c>
@@ -3312,10 +3446,13 @@
         <v>10</v>
       </c>
       <c r="O7" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P7" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43000005</v>
       </c>
@@ -3355,10 +3492,13 @@
         <v>12</v>
       </c>
       <c r="O8" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P8" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43000006</v>
       </c>
@@ -3398,10 +3538,13 @@
         <v>14</v>
       </c>
       <c r="O9" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P9" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43000007</v>
       </c>
@@ -3441,10 +3584,13 @@
         <v>16</v>
       </c>
       <c r="O10" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P10" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43000008</v>
       </c>
@@ -3484,10 +3630,13 @@
         <v>18</v>
       </c>
       <c r="O11" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P11" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43000009</v>
       </c>
@@ -3527,10 +3676,13 @@
         <v>20</v>
       </c>
       <c r="O12" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P12" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43000010</v>
       </c>
@@ -3570,10 +3722,13 @@
         <v>22</v>
       </c>
       <c r="O13" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P13" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43000011</v>
       </c>
@@ -3613,10 +3768,13 @@
         <v>24</v>
       </c>
       <c r="O14" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P14" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43000012</v>
       </c>
@@ -3656,10 +3814,13 @@
         <v>26</v>
       </c>
       <c r="O15" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P15" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43000013</v>
       </c>
@@ -3699,10 +3860,13 @@
         <v>28</v>
       </c>
       <c r="O16" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P16" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43000014</v>
       </c>
@@ -3742,10 +3906,13 @@
         <v>30</v>
       </c>
       <c r="O17" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P17" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43000015</v>
       </c>
@@ -3785,10 +3952,13 @@
         <v>32</v>
       </c>
       <c r="O18" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P18" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43000016</v>
       </c>
@@ -3828,10 +3998,13 @@
         <v>34</v>
       </c>
       <c r="O19" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P19" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43000017</v>
       </c>
@@ -3871,10 +4044,13 @@
         <v>36</v>
       </c>
       <c r="O20" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P20" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43000018</v>
       </c>
@@ -3914,10 +4090,13 @@
         <v>38</v>
       </c>
       <c r="O21" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P21" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43000019</v>
       </c>
@@ -3957,10 +4136,13 @@
         <v>40</v>
       </c>
       <c r="O22" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P22" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43000020</v>
       </c>
@@ -4000,10 +4182,13 @@
         <v>42</v>
       </c>
       <c r="O23" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P23" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43000021</v>
       </c>
@@ -4043,10 +4228,13 @@
         <v>44</v>
       </c>
       <c r="O24" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P24" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43000022</v>
       </c>
@@ -4086,10 +4274,13 @@
         <v>46</v>
       </c>
       <c r="O25" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P25" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43000023</v>
       </c>
@@ -4129,10 +4320,13 @@
         <v>48</v>
       </c>
       <c r="O26" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P26" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43000024</v>
       </c>
@@ -4172,10 +4366,13 @@
         <v>50</v>
       </c>
       <c r="O27" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P27" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43000025</v>
       </c>
@@ -4215,10 +4412,13 @@
         <v>52</v>
       </c>
       <c r="O28" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P28" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43000026</v>
       </c>
@@ -4258,10 +4458,13 @@
         <v>54</v>
       </c>
       <c r="O29" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P29" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43000027</v>
       </c>
@@ -4301,10 +4504,13 @@
         <v>56</v>
       </c>
       <c r="O30" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P30" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43000028</v>
       </c>
@@ -4344,10 +4550,13 @@
         <v>58</v>
       </c>
       <c r="O31" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P31" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43000029</v>
       </c>
@@ -4387,10 +4596,13 @@
         <v>60</v>
       </c>
       <c r="O32" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P32" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43000030</v>
       </c>
@@ -4430,10 +4642,13 @@
         <v>62</v>
       </c>
       <c r="O33" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P33" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43000031</v>
       </c>
@@ -4473,10 +4688,13 @@
         <v>64</v>
       </c>
       <c r="O34" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P34" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43000032</v>
       </c>
@@ -4516,10 +4734,13 @@
         <v>66</v>
       </c>
       <c r="O35" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P35" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43000033</v>
       </c>
@@ -4559,10 +4780,13 @@
         <v>68</v>
       </c>
       <c r="O36" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P36" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43000101</v>
       </c>
@@ -4604,10 +4828,13 @@
         <v>71</v>
       </c>
       <c r="O37" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P37" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43000102</v>
       </c>
@@ -4649,10 +4876,13 @@
         <v>74</v>
       </c>
       <c r="O38" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P38" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>43000103</v>
       </c>
@@ -4694,10 +4924,13 @@
         <v>78</v>
       </c>
       <c r="O39" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P39" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>43000104</v>
       </c>
@@ -4739,10 +4972,13 @@
         <v>82</v>
       </c>
       <c r="O40" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P40" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>43000105</v>
       </c>
@@ -4784,10 +5020,13 @@
         <v>86</v>
       </c>
       <c r="O41" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P41" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>43000106</v>
       </c>
@@ -4829,10 +5068,13 @@
         <v>90</v>
       </c>
       <c r="O42" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P42" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>43000107</v>
       </c>
@@ -4874,10 +5116,13 @@
         <v>93</v>
       </c>
       <c r="O43" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P43" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43000108</v>
       </c>
@@ -4919,10 +5164,13 @@
         <v>97</v>
       </c>
       <c r="O44" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P44" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>43000109</v>
       </c>
@@ -4964,10 +5212,13 @@
         <v>101</v>
       </c>
       <c r="O45" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P45" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>43000110</v>
       </c>
@@ -5009,10 +5260,13 @@
         <v>105</v>
       </c>
       <c r="O46" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P46" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>43000201</v>
       </c>
@@ -5054,10 +5308,13 @@
         <v>109</v>
       </c>
       <c r="O47" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P47" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>43000202</v>
       </c>
@@ -5099,10 +5356,13 @@
         <v>112</v>
       </c>
       <c r="O48" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P48" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>43000203</v>
       </c>
@@ -5144,10 +5404,13 @@
         <v>115</v>
       </c>
       <c r="O49" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P49" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>43000301</v>
       </c>
@@ -5189,10 +5452,13 @@
         <v>119</v>
       </c>
       <c r="O50" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P50" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>43000302</v>
       </c>
@@ -5234,10 +5500,13 @@
         <v>122</v>
       </c>
       <c r="O51" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P51" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>43000303</v>
       </c>
@@ -5279,10 +5548,13 @@
         <v>125</v>
       </c>
       <c r="O52" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P52" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>43000304</v>
       </c>
@@ -5324,10 +5596,13 @@
         <v>129</v>
       </c>
       <c r="O53" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P53" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>43000305</v>
       </c>
@@ -5369,10 +5644,13 @@
         <v>132</v>
       </c>
       <c r="O54" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P54" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>43000306</v>
       </c>
@@ -5414,10 +5692,13 @@
         <v>134</v>
       </c>
       <c r="O55" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P55" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>43000307</v>
       </c>
@@ -5459,10 +5740,13 @@
         <v>137</v>
       </c>
       <c r="O56" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P56" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>43000308</v>
       </c>
@@ -5504,10 +5788,13 @@
         <v>139</v>
       </c>
       <c r="O57" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P57" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>43000309</v>
       </c>
@@ -5549,10 +5836,13 @@
         <v>142</v>
       </c>
       <c r="O58" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P58" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>43000310</v>
       </c>
@@ -5594,10 +5884,13 @@
         <v>144</v>
       </c>
       <c r="O59" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P59" s="7" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>43000311</v>
       </c>
@@ -5639,10 +5932,13 @@
         <v>147</v>
       </c>
       <c r="O60" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P60" s="7" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>43000312</v>
       </c>
@@ -5684,10 +5980,13 @@
         <v>151</v>
       </c>
       <c r="O61" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P61" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>43000401</v>
       </c>
@@ -5729,10 +6028,13 @@
         <v>154</v>
       </c>
       <c r="O62" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P62" s="7" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>43000402</v>
       </c>
@@ -5774,10 +6076,13 @@
         <v>156</v>
       </c>
       <c r="O63" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P63" s="7" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>43000403</v>
       </c>
@@ -5819,10 +6124,13 @@
         <v>159</v>
       </c>
       <c r="O64" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P64" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>43000404</v>
       </c>
@@ -5864,10 +6172,13 @@
         <v>161</v>
       </c>
       <c r="O65" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P65" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>43000405</v>
       </c>
@@ -5909,10 +6220,13 @@
         <v>164</v>
       </c>
       <c r="O66" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P66" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>43000406</v>
       </c>
@@ -5954,10 +6268,13 @@
         <v>166</v>
       </c>
       <c r="O67" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P67" s="7" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>43000407</v>
       </c>
@@ -5999,10 +6316,13 @@
         <v>168</v>
       </c>
       <c r="O68" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P68" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>43000408</v>
       </c>
@@ -6044,10 +6364,13 @@
         <v>170</v>
       </c>
       <c r="O69" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P69" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>43000501</v>
       </c>
@@ -6089,10 +6412,13 @@
         <v>174</v>
       </c>
       <c r="O70" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P70" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>43000502</v>
       </c>
@@ -6134,10 +6460,13 @@
         <v>176</v>
       </c>
       <c r="O71" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P71" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>43000503</v>
       </c>
@@ -6179,10 +6508,13 @@
         <v>179</v>
       </c>
       <c r="O72" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P72" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>43000504</v>
       </c>
@@ -6224,6 +6556,9 @@
         <v>181</v>
       </c>
       <c r="O73" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P73" s="7" t="s">
         <v>181</v>
       </c>
     </row>
@@ -6240,13 +6575,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6259,152 +6594,161 @@
     <col min="9" max="10" width="6.125" customWidth="1"/>
     <col min="11" max="12" width="11.875" customWidth="1"/>
     <col min="13" max="13" width="9.5" customWidth="1"/>
-    <col min="14" max="14" width="10.625" customWidth="1"/>
-    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.625" customWidth="1"/>
+    <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="P1" s="12" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A2" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="P2" s="15" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A3" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="P3" s="16" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43010001</v>
       </c>
@@ -6444,10 +6788,13 @@
         <v>184</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+        <v>282</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43010002</v>
       </c>
@@ -6487,10 +6834,13 @@
         <v>3</v>
       </c>
       <c r="O5" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P5" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43010003</v>
       </c>
@@ -6530,10 +6880,13 @@
         <v>188</v>
       </c>
       <c r="O6" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="P6" s="7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43010004</v>
       </c>
@@ -6573,10 +6926,13 @@
         <v>190</v>
       </c>
       <c r="O7" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P7" s="7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43010005</v>
       </c>
@@ -6615,11 +6971,14 @@
       <c r="N8" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="O8" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P8" s="9" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43010006</v>
       </c>
@@ -6658,11 +7017,14 @@
       <c r="N9" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="O9" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P9" s="9" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43010101</v>
       </c>
@@ -6704,10 +7066,13 @@
         <v>194</v>
       </c>
       <c r="O10" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P10" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43010102</v>
       </c>
@@ -6749,10 +7114,13 @@
         <v>198</v>
       </c>
       <c r="O11" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P11" s="7" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43010103</v>
       </c>
@@ -6794,10 +7162,13 @@
         <v>201</v>
       </c>
       <c r="O12" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P12" s="7" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43010104</v>
       </c>
@@ -6839,10 +7210,13 @@
         <v>204</v>
       </c>
       <c r="O13" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P13" s="7" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43010105</v>
       </c>
@@ -6884,6 +7258,9 @@
         <v>207</v>
       </c>
       <c r="O14" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="P14" s="7" t="s">
         <v>207</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#8 deathskill and after skill winll be differenet
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="1" r:id="rId1"/>
@@ -2179,33 +2179,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <left style="thin">
           <color rgb="FF4F81BD"/>
@@ -2260,6 +2233,33 @@
           <bgColor theme="9" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2728,35 +2728,35 @@
     <tableColumn id="16" name="EnergyRate" dataDxfId="22"/>
     <tableColumn id="13" name="Method" dataDxfId="21"/>
     <tableColumn id="14" name="Emethod" dataDxfId="20"/>
-    <tableColumn id="17" name="Figue" dataDxfId="2"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="19"/>
+    <tableColumn id="17" name="Figue" dataDxfId="19"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:O14" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:O14" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A3:O14"/>
   <sortState ref="A4:O83">
     <sortCondition ref="A3:A83"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="Id" dataDxfId="15"/>
-    <tableColumn id="2" name="Name" dataDxfId="14"/>
-    <tableColumn id="3" name="Type" dataDxfId="13"/>
-    <tableColumn id="6" name="World" dataDxfId="12"/>
-    <tableColumn id="7" name="Deck" dataDxfId="11"/>
-    <tableColumn id="8" name="Cards" dataDxfId="10"/>
-    <tableColumn id="10" name="Job" dataDxfId="9"/>
-    <tableColumn id="4" name="KingCard" dataDxfId="8"/>
-    <tableColumn id="11" name="Level" dataDxfId="7"/>
-    <tableColumn id="12" name="Reward" dataDxfId="6"/>
-    <tableColumn id="16" name="EnergyRate" dataDxfId="5"/>
-    <tableColumn id="13" name="Method" dataDxfId="4"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="3"/>
-    <tableColumn id="9" name="Figue" dataDxfId="0"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="1"/>
+    <tableColumn id="1" name="Id" dataDxfId="14"/>
+    <tableColumn id="2" name="Name" dataDxfId="13"/>
+    <tableColumn id="3" name="Type" dataDxfId="12"/>
+    <tableColumn id="6" name="World" dataDxfId="11"/>
+    <tableColumn id="7" name="Deck" dataDxfId="10"/>
+    <tableColumn id="8" name="Cards" dataDxfId="9"/>
+    <tableColumn id="10" name="Job" dataDxfId="8"/>
+    <tableColumn id="4" name="KingCard" dataDxfId="7"/>
+    <tableColumn id="11" name="Level" dataDxfId="6"/>
+    <tableColumn id="12" name="Reward" dataDxfId="5"/>
+    <tableColumn id="16" name="EnergyRate" dataDxfId="4"/>
+    <tableColumn id="13" name="Method" dataDxfId="3"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="2"/>
+    <tableColumn id="9" name="Figue" dataDxfId="1"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3058,21 +3058,21 @@
       <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.25" customWidth="1"/>
-    <col min="3" max="3" width="5.25" customWidth="1"/>
-    <col min="6" max="6" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="10.125" customWidth="1"/>
-    <col min="8" max="8" width="8.625" customWidth="1"/>
-    <col min="9" max="9" width="6.25" customWidth="1"/>
-    <col min="10" max="11" width="11.875" customWidth="1"/>
-    <col min="12" max="12" width="9.5" customWidth="1"/>
-    <col min="13" max="13" width="10.625" customWidth="1"/>
-    <col min="15" max="15" width="10.625" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.21875" customWidth="1"/>
+    <col min="10" max="11" width="11.88671875" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>210</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>208</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>222</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>43000001</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>43000002</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>43000003</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>43000004</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>43000005</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>43000006</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>43000007</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>43000008</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>43000009</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>43000010</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>43000011</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>43000012</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>43000013</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>43000014</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>43000015</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>43000016</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>43000017</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>43000018</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>43000019</v>
       </c>
@@ -4030,7 +4030,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>43000020</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>43000021</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>43000022</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>43000023</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>43000024</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>43000025</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>43000026</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>43000027</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>43000028</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>43000029</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>43000030</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>43000031</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>43000032</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>43000033</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>43000101</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>43000102</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>43000103</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>43000104</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>43000105</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>43000106</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43000107</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43000108</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43000109</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43000110</v>
       </c>
@@ -5082,7 +5082,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>43000201</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>43000202</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>43000203</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>43000301</v>
       </c>
@@ -5262,7 +5262,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>43000302</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>43000303</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>43000304</v>
       </c>
@@ -5397,7 +5397,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>43000305</v>
       </c>
@@ -5442,7 +5442,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>43000306</v>
       </c>
@@ -5487,7 +5487,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>43000307</v>
       </c>
@@ -5532,7 +5532,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>43000308</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>43000309</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>43000310</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>43000311</v>
       </c>
@@ -5712,7 +5712,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>43000312</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>43000401</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>43000402</v>
       </c>
@@ -5847,7 +5847,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>43000403</v>
       </c>
@@ -5892,7 +5892,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>43000404</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>43000405</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>43000406</v>
       </c>
@@ -6027,7 +6027,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>43000407</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>43000408</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>43000501</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>43000502</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>43000503</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>43000504</v>
       </c>
@@ -6316,25 +6316,25 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1:I1048576"/>
+      <selection pane="bottomRight" activeCell="O4" sqref="O4:O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="3" max="3" width="5.125" customWidth="1"/>
-    <col min="6" max="6" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="6.125" customWidth="1"/>
-    <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="6.125" customWidth="1"/>
-    <col min="10" max="11" width="11.875" customWidth="1"/>
-    <col min="12" max="12" width="9.5" customWidth="1"/>
-    <col min="13" max="13" width="10.625" customWidth="1"/>
-    <col min="15" max="15" width="10.625" customWidth="1"/>
-    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" customWidth="1"/>
+    <col min="10" max="11" width="11.88671875" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>210</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>208</v>
       </c>
@@ -6428,7 +6428,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>222</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>43010001</v>
       </c>
@@ -6515,10 +6515,10 @@
         <v>277</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>43010002</v>
       </c>
@@ -6558,10 +6558,10 @@
         <v>186</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>43010003</v>
       </c>
@@ -6604,7 +6604,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>43010004</v>
       </c>
@@ -6644,10 +6644,10 @@
         <v>190</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>43010005</v>
       </c>
@@ -6687,10 +6687,10 @@
         <v>237</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>43010006</v>
       </c>
@@ -6730,10 +6730,10 @@
         <v>240</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>43010101</v>
       </c>
@@ -6775,10 +6775,10 @@
         <v>195</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>43010102</v>
       </c>
@@ -6820,10 +6820,10 @@
         <v>199</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>43010103</v>
       </c>
@@ -6865,10 +6865,10 @@
         <v>201</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>43010104</v>
       </c>
@@ -6910,10 +6910,10 @@
         <v>205</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>43010105</v>
       </c>
@@ -6955,7 +6955,7 @@
         <v>207</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
close #68 can config initial monster with Xlsx/People.xlsx
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="287">
   <si>
     <t>老鼠</t>
   </si>
@@ -877,6 +877,58 @@
   </si>
   <si>
     <t>atr6;atr4</t>
+  </si>
+  <si>
+    <t>左方Add</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>右方Add</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LeftMon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RightMon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>左方Add</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>右方Add</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51000229;-4;1;51000229;-4;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51019298;4;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51019299;4;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51019299;-4;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51019298;-4;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1652,7 +1704,115 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="38">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2535,52 +2695,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:N73" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
-  <autoFilter ref="A3:N73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:P73" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" tableBorderDxfId="35">
+  <autoFilter ref="A3:P73"/>
   <sortState ref="A4:O83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="30"/>
-    <tableColumn id="2" name="Name" dataDxfId="29"/>
-    <tableColumn id="3" name="Type" dataDxfId="28"/>
-    <tableColumn id="6" name="World" dataDxfId="27"/>
-    <tableColumn id="7" name="Deck" dataDxfId="26"/>
-    <tableColumn id="8" name="Cards" dataDxfId="25"/>
-    <tableColumn id="10" name="Job" dataDxfId="24"/>
-    <tableColumn id="4" name="KingCard" dataDxfId="23"/>
-    <tableColumn id="11" name="Level" dataDxfId="22"/>
-    <tableColumn id="12" name="Reward" dataDxfId="21"/>
-    <tableColumn id="13" name="Method" dataDxfId="20"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="19"/>
-    <tableColumn id="17" name="Figue" dataDxfId="18"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="17"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Id" dataDxfId="34"/>
+    <tableColumn id="2" name="Name" dataDxfId="33"/>
+    <tableColumn id="3" name="Type" dataDxfId="32"/>
+    <tableColumn id="6" name="World" dataDxfId="31"/>
+    <tableColumn id="7" name="Deck" dataDxfId="30"/>
+    <tableColumn id="8" name="Cards" dataDxfId="29"/>
+    <tableColumn id="10" name="Job" dataDxfId="28"/>
+    <tableColumn id="4" name="KingCard" dataDxfId="27"/>
+    <tableColumn id="11" name="Level" dataDxfId="26"/>
+    <tableColumn id="12" name="Reward" dataDxfId="25"/>
+    <tableColumn id="13" name="Method" dataDxfId="24"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="23"/>
+    <tableColumn id="5" name="LeftMon" dataDxfId="3"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="2"/>
+    <tableColumn id="17" name="Figue" dataDxfId="22"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:N14" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
-  <autoFilter ref="A3:N14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:P14" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+  <autoFilter ref="A3:P14"/>
   <sortState ref="A4:O83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="13"/>
-    <tableColumn id="2" name="Name" dataDxfId="12"/>
-    <tableColumn id="3" name="Type" dataDxfId="11"/>
-    <tableColumn id="6" name="World" dataDxfId="10"/>
-    <tableColumn id="7" name="Deck" dataDxfId="9"/>
-    <tableColumn id="8" name="Cards" dataDxfId="8"/>
-    <tableColumn id="10" name="Job" dataDxfId="7"/>
-    <tableColumn id="4" name="KingCard" dataDxfId="6"/>
-    <tableColumn id="11" name="Level" dataDxfId="5"/>
-    <tableColumn id="12" name="Reward" dataDxfId="4"/>
-    <tableColumn id="13" name="Method" dataDxfId="3"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="2"/>
-    <tableColumn id="9" name="Figue" dataDxfId="1"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="0"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Id" dataDxfId="17"/>
+    <tableColumn id="2" name="Name" dataDxfId="16"/>
+    <tableColumn id="3" name="Type" dataDxfId="15"/>
+    <tableColumn id="6" name="World" dataDxfId="14"/>
+    <tableColumn id="7" name="Deck" dataDxfId="13"/>
+    <tableColumn id="8" name="Cards" dataDxfId="12"/>
+    <tableColumn id="10" name="Job" dataDxfId="11"/>
+    <tableColumn id="4" name="KingCard" dataDxfId="10"/>
+    <tableColumn id="11" name="Level" dataDxfId="9"/>
+    <tableColumn id="12" name="Reward" dataDxfId="8"/>
+    <tableColumn id="13" name="Method" dataDxfId="7"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="6"/>
+    <tableColumn id="5" name="LeftMon" dataDxfId="1"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="0"/>
+    <tableColumn id="9" name="Figue" dataDxfId="5"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2873,13 +3037,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N73"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E43" sqref="E43"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2892,11 +3056,11 @@
     <col min="9" max="9" width="6.25" customWidth="1"/>
     <col min="10" max="10" width="11.875" customWidth="1"/>
     <col min="11" max="11" width="9.5" customWidth="1"/>
-    <col min="12" max="12" width="10.625" customWidth="1"/>
-    <col min="14" max="14" width="10.625" customWidth="1"/>
+    <col min="12" max="14" width="10.625" customWidth="1"/>
+    <col min="16" max="16" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>204</v>
       </c>
@@ -2933,14 +3097,20 @@
       <c r="L1" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="O1" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>202</v>
       </c>
@@ -2977,14 +3147,20 @@
       <c r="L2" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>216</v>
       </c>
@@ -3022,13 +3198,19 @@
         <v>226</v>
       </c>
       <c r="M3" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43000001</v>
       </c>
@@ -3061,14 +3243,16 @@
       <c r="L4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43000002</v>
       </c>
@@ -3101,14 +3285,16 @@
       <c r="L5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43000003</v>
       </c>
@@ -3141,14 +3327,16 @@
       <c r="L6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43000004</v>
       </c>
@@ -3181,14 +3369,16 @@
       <c r="L7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43000005</v>
       </c>
@@ -3221,14 +3411,16 @@
       <c r="L8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="P8" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43000006</v>
       </c>
@@ -3261,14 +3453,16 @@
       <c r="L9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="P9" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43000007</v>
       </c>
@@ -3301,14 +3495,16 @@
       <c r="L10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="P10" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43000008</v>
       </c>
@@ -3341,14 +3537,16 @@
       <c r="L11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="P11" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43000009</v>
       </c>
@@ -3381,14 +3579,16 @@
       <c r="L12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="P12" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43000010</v>
       </c>
@@ -3421,14 +3621,16 @@
       <c r="L13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="P13" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43000011</v>
       </c>
@@ -3461,14 +3663,16 @@
       <c r="L14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="P14" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43000012</v>
       </c>
@@ -3501,14 +3705,16 @@
       <c r="L15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="P15" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43000013</v>
       </c>
@@ -3541,14 +3747,16 @@
       <c r="L16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N16" s="4" t="s">
+      <c r="P16" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43000014</v>
       </c>
@@ -3581,14 +3789,16 @@
       <c r="L17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="P17" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43000015</v>
       </c>
@@ -3621,14 +3831,16 @@
       <c r="L18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N18" s="4" t="s">
+      <c r="P18" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43000016</v>
       </c>
@@ -3661,14 +3873,16 @@
       <c r="L19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N19" s="4" t="s">
+      <c r="P19" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43000017</v>
       </c>
@@ -3701,14 +3915,16 @@
       <c r="L20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M20" s="4" t="s">
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N20" s="4" t="s">
+      <c r="P20" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43000018</v>
       </c>
@@ -3741,14 +3957,16 @@
       <c r="L21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="M21" s="4" t="s">
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N21" s="4" t="s">
+      <c r="P21" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43000019</v>
       </c>
@@ -3781,14 +3999,16 @@
       <c r="L22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="N22" s="4" t="s">
+      <c r="P22" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43000020</v>
       </c>
@@ -3821,14 +4041,16 @@
       <c r="L23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="P23" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43000021</v>
       </c>
@@ -3861,14 +4083,16 @@
       <c r="L24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M24" s="4" t="s">
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="N24" s="4" t="s">
+      <c r="P24" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43000022</v>
       </c>
@@ -3901,14 +4125,16 @@
       <c r="L25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="M25" s="4" t="s">
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="N25" s="4" t="s">
+      <c r="P25" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43000023</v>
       </c>
@@ -3941,14 +4167,16 @@
       <c r="L26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="M26" s="4" t="s">
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="N26" s="4" t="s">
+      <c r="P26" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43000024</v>
       </c>
@@ -3981,14 +4209,16 @@
       <c r="L27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="M27" s="4" t="s">
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="N27" s="4" t="s">
+      <c r="P27" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43000025</v>
       </c>
@@ -4021,14 +4251,16 @@
       <c r="L28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M28" s="4" t="s">
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="N28" s="4" t="s">
+      <c r="P28" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43000026</v>
       </c>
@@ -4061,14 +4293,16 @@
       <c r="L29" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M29" s="4" t="s">
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="N29" s="4" t="s">
+      <c r="P29" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43000027</v>
       </c>
@@ -4101,14 +4335,16 @@
       <c r="L30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M30" s="4" t="s">
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="N30" s="4" t="s">
+      <c r="P30" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43000028</v>
       </c>
@@ -4141,14 +4377,16 @@
       <c r="L31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="M31" s="4" t="s">
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="N31" s="4" t="s">
+      <c r="P31" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43000029</v>
       </c>
@@ -4181,14 +4419,16 @@
       <c r="L32" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="M32" s="4" t="s">
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="N32" s="4" t="s">
+      <c r="P32" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43000030</v>
       </c>
@@ -4221,14 +4461,16 @@
       <c r="L33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="M33" s="4" t="s">
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="N33" s="4" t="s">
+      <c r="P33" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43000031</v>
       </c>
@@ -4261,14 +4503,16 @@
       <c r="L34" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="M34" s="4" t="s">
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N34" s="4" t="s">
+      <c r="P34" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43000032</v>
       </c>
@@ -4301,14 +4545,16 @@
       <c r="L35" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="M35" s="4" t="s">
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="N35" s="4" t="s">
+      <c r="P35" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43000033</v>
       </c>
@@ -4341,14 +4587,16 @@
       <c r="L36" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="M36" s="4" t="s">
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="N36" s="4" t="s">
+      <c r="P36" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43000101</v>
       </c>
@@ -4385,14 +4633,16 @@
       <c r="L37" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="M37" s="4" t="s">
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="N37" s="4" t="s">
+      <c r="P37" s="4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43000102</v>
       </c>
@@ -4429,14 +4679,16 @@
       <c r="L38" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="M38" s="4" t="s">
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N38" s="4" t="s">
+      <c r="P38" s="4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>43000103</v>
       </c>
@@ -4473,14 +4725,16 @@
       <c r="L39" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="M39" s="4" t="s">
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="N39" s="4" t="s">
+      <c r="P39" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>43000104</v>
       </c>
@@ -4517,14 +4771,16 @@
       <c r="L40" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="M40" s="4" t="s">
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="N40" s="4" t="s">
+      <c r="P40" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>43000105</v>
       </c>
@@ -4561,14 +4817,16 @@
       <c r="L41" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="M41" s="4" t="s">
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="N41" s="4" t="s">
+      <c r="P41" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>43000106</v>
       </c>
@@ -4605,14 +4863,16 @@
       <c r="L42" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="M42" s="4" t="s">
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="N42" s="4" t="s">
+      <c r="P42" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>43000107</v>
       </c>
@@ -4649,14 +4909,16 @@
       <c r="L43" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="M43" s="4" t="s">
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="N43" s="4" t="s">
+      <c r="P43" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43000108</v>
       </c>
@@ -4693,14 +4955,16 @@
       <c r="L44" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="M44" s="4" t="s">
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="N44" s="4" t="s">
+      <c r="P44" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>43000109</v>
       </c>
@@ -4737,14 +5001,16 @@
       <c r="L45" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="M45" s="4" t="s">
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="N45" s="4" t="s">
+      <c r="P45" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>43000110</v>
       </c>
@@ -4781,14 +5047,16 @@
       <c r="L46" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="M46" s="4" t="s">
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="N46" s="4" t="s">
+      <c r="P46" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>43000201</v>
       </c>
@@ -4825,14 +5093,16 @@
       <c r="L47" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="M47" s="4" t="s">
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="N47" s="4" t="s">
+      <c r="P47" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>43000202</v>
       </c>
@@ -4869,14 +5139,16 @@
       <c r="L48" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="M48" s="4" t="s">
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="N48" s="4" t="s">
+      <c r="P48" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>43000203</v>
       </c>
@@ -4913,14 +5185,16 @@
       <c r="L49" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="M49" s="4" t="s">
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="N49" s="4" t="s">
+      <c r="P49" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>43000301</v>
       </c>
@@ -4957,14 +5231,16 @@
       <c r="L50" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="M50" s="4" t="s">
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="N50" s="4" t="s">
+      <c r="P50" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>43000302</v>
       </c>
@@ -5001,14 +5277,16 @@
       <c r="L51" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="M51" s="4" t="s">
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="N51" s="4" t="s">
+      <c r="P51" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>43000303</v>
       </c>
@@ -5045,14 +5323,16 @@
       <c r="L52" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="M52" s="4" t="s">
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="N52" s="4" t="s">
+      <c r="P52" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>43000304</v>
       </c>
@@ -5089,14 +5369,16 @@
       <c r="L53" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="M53" s="4" t="s">
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="N53" s="4" t="s">
+      <c r="P53" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>43000305</v>
       </c>
@@ -5133,14 +5415,16 @@
       <c r="L54" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="M54" s="4" t="s">
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="N54" s="4" t="s">
+      <c r="P54" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>43000306</v>
       </c>
@@ -5177,14 +5461,16 @@
       <c r="L55" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="M55" s="4" t="s">
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="N55" s="4" t="s">
+      <c r="P55" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>43000307</v>
       </c>
@@ -5221,14 +5507,16 @@
       <c r="L56" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="M56" s="4" t="s">
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="N56" s="4" t="s">
+      <c r="P56" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>43000308</v>
       </c>
@@ -5265,14 +5553,16 @@
       <c r="L57" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="M57" s="4" t="s">
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="N57" s="4" t="s">
+      <c r="P57" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>43000309</v>
       </c>
@@ -5309,14 +5599,16 @@
       <c r="L58" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="M58" s="4" t="s">
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="N58" s="4" t="s">
+      <c r="P58" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>43000310</v>
       </c>
@@ -5353,14 +5645,16 @@
       <c r="L59" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="M59" s="4" t="s">
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="N59" s="4" t="s">
+      <c r="P59" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>43000311</v>
       </c>
@@ -5397,14 +5691,16 @@
       <c r="L60" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="M60" s="4" t="s">
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="N60" s="4" t="s">
+      <c r="P60" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>43000312</v>
       </c>
@@ -5441,14 +5737,16 @@
       <c r="L61" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="M61" s="4" t="s">
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="N61" s="4" t="s">
+      <c r="P61" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>43000401</v>
       </c>
@@ -5485,14 +5783,16 @@
       <c r="L62" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="M62" s="4" t="s">
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="N62" s="4" t="s">
+      <c r="P62" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>43000402</v>
       </c>
@@ -5529,14 +5829,16 @@
       <c r="L63" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="M63" s="4" t="s">
+      <c r="M63" s="4"/>
+      <c r="N63" s="4"/>
+      <c r="O63" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="N63" s="4" t="s">
+      <c r="P63" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>43000403</v>
       </c>
@@ -5573,14 +5875,16 @@
       <c r="L64" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="M64" s="4" t="s">
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="N64" s="4" t="s">
+      <c r="P64" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>43000404</v>
       </c>
@@ -5617,14 +5921,16 @@
       <c r="L65" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="M65" s="4" t="s">
+      <c r="M65" s="4"/>
+      <c r="N65" s="4"/>
+      <c r="O65" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="N65" s="4" t="s">
+      <c r="P65" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>43000405</v>
       </c>
@@ -5661,14 +5967,16 @@
       <c r="L66" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="M66" s="4" t="s">
+      <c r="M66" s="4"/>
+      <c r="N66" s="4"/>
+      <c r="O66" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="N66" s="4" t="s">
+      <c r="P66" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>43000406</v>
       </c>
@@ -5705,14 +6013,16 @@
       <c r="L67" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="M67" s="4" t="s">
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="N67" s="4" t="s">
+      <c r="P67" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>43000407</v>
       </c>
@@ -5749,14 +6059,16 @@
       <c r="L68" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="M68" s="4" t="s">
+      <c r="M68" s="4"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="N68" s="4" t="s">
+      <c r="P68" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>43000408</v>
       </c>
@@ -5793,14 +6105,16 @@
       <c r="L69" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="M69" s="4" t="s">
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="N69" s="4" t="s">
+      <c r="P69" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>43000501</v>
       </c>
@@ -5837,14 +6151,16 @@
       <c r="L70" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="M70" s="4" t="s">
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="N70" s="4" t="s">
+      <c r="P70" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>43000502</v>
       </c>
@@ -5881,14 +6197,16 @@
       <c r="L71" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="M71" s="4" t="s">
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="N71" s="4" t="s">
+      <c r="P71" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>43000503</v>
       </c>
@@ -5925,14 +6243,16 @@
       <c r="L72" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="M72" s="4" t="s">
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="N72" s="4" t="s">
+      <c r="P72" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>43000504</v>
       </c>
@@ -5969,10 +6289,12 @@
       <c r="L73" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="M73" s="4" t="s">
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="N73" s="4" t="s">
+      <c r="P73" s="4" t="s">
         <v>264</v>
       </c>
     </row>
@@ -5988,13 +6310,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1:K1048576"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6007,12 +6329,12 @@
     <col min="9" max="9" width="6.125" customWidth="1"/>
     <col min="10" max="10" width="11.875" customWidth="1"/>
     <col min="11" max="11" width="9.5" customWidth="1"/>
-    <col min="12" max="12" width="10.625" customWidth="1"/>
-    <col min="14" max="14" width="10.625" customWidth="1"/>
-    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="10.625" customWidth="1"/>
+    <col min="16" max="16" width="10.625" customWidth="1"/>
+    <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>204</v>
       </c>
@@ -6049,14 +6371,20 @@
       <c r="L1" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="O1" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>202</v>
       </c>
@@ -6093,14 +6421,20 @@
       <c r="L2" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="O2" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="P2" s="8" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>216</v>
       </c>
@@ -6138,13 +6472,19 @@
         <v>226</v>
       </c>
       <c r="M3" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43010001</v>
       </c>
@@ -6177,14 +6517,18 @@
       <c r="L4" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="4"/>
+      <c r="N4" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43010002</v>
       </c>
@@ -6217,14 +6561,16 @@
       <c r="L5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43010003</v>
       </c>
@@ -6257,14 +6603,16 @@
       <c r="L6" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43010004</v>
       </c>
@@ -6297,14 +6645,16 @@
       <c r="L7" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43010005</v>
       </c>
@@ -6334,17 +6684,23 @@
       <c r="K8" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L8" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="M8" s="6" t="s">
+      <c r="L8" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="O8" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="P8" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43010006</v>
       </c>
@@ -6375,16 +6731,22 @@
         <v>235</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="M9" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="O9" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="P9" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43010101</v>
       </c>
@@ -6419,14 +6781,16 @@
       <c r="L10" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="P10" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43010102</v>
       </c>
@@ -6461,14 +6825,16 @@
       <c r="L11" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="P11" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43010103</v>
       </c>
@@ -6503,14 +6869,16 @@
       <c r="L12" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="P12" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43010104</v>
       </c>
@@ -6545,14 +6913,16 @@
       <c r="L13" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="P13" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43010105</v>
       </c>
@@ -6587,10 +6957,12 @@
       <c r="L14" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="P14" s="4" t="s">
         <v>266</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish the battle difficulty balance
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="267">
   <si>
     <t>老鼠</t>
   </si>
@@ -739,18 +739,6 @@
   </si>
   <si>
     <t>test2e</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>王牌卡</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>KingCard</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -806,10 +794,6 @@
     <t>atr6;atr4</t>
   </si>
   <si>
-    <t>左方Add</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>右方Add</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -818,18 +802,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>LeftMon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>RightMon</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>左方Add</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>右方Add</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -838,26 +814,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51000229;-4;1;51000229;-4;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>51019298;4;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>51019299;4;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>51019299;-4;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>51019298;-4;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>掉落</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -879,6 +835,40 @@
   </si>
   <si>
     <t>int[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>特别怪物</t>
+  </si>
+  <si>
+    <t>特别怪物</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PetMon</t>
+  </si>
+  <si>
+    <t>PetMon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RightMon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51019299;4;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51019298;4;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51000229;4;-1;51000229;4;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1691,7 +1681,34 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1933,58 +1950,6 @@
         <bottom/>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2588,33 +2553,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="4"/>
@@ -2672,6 +2610,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2684,56 +2690,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:P73" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" tableBorderDxfId="35">
-  <autoFilter ref="A3:P73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:O73" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
+  <autoFilter ref="A3:O73"/>
   <sortState ref="A4:O83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="16">
-    <tableColumn id="1" name="Id" dataDxfId="34"/>
-    <tableColumn id="2" name="Name" dataDxfId="33"/>
-    <tableColumn id="3" name="Type" dataDxfId="32"/>
-    <tableColumn id="6" name="World" dataDxfId="31"/>
-    <tableColumn id="7" name="Deck" dataDxfId="30"/>
-    <tableColumn id="10" name="Job" dataDxfId="29"/>
-    <tableColumn id="4" name="KingCard" dataDxfId="28"/>
-    <tableColumn id="11" name="Level" dataDxfId="27"/>
-    <tableColumn id="12" name="Reward" dataDxfId="26"/>
-    <tableColumn id="13" name="Method" dataDxfId="25"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="24"/>
-    <tableColumn id="5" name="LeftMon" dataDxfId="23"/>
+  <tableColumns count="15">
+    <tableColumn id="1" name="Id" dataDxfId="32"/>
+    <tableColumn id="2" name="Name" dataDxfId="31"/>
+    <tableColumn id="3" name="Type" dataDxfId="30"/>
+    <tableColumn id="6" name="World" dataDxfId="29"/>
+    <tableColumn id="7" name="Deck" dataDxfId="28"/>
+    <tableColumn id="10" name="Job" dataDxfId="27"/>
+    <tableColumn id="11" name="Level" dataDxfId="26"/>
+    <tableColumn id="12" name="Reward" dataDxfId="25"/>
+    <tableColumn id="13" name="Method" dataDxfId="24"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="23"/>
     <tableColumn id="15" name="RightMon" dataDxfId="22"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="0"/>
     <tableColumn id="17" name="Figue" dataDxfId="21"/>
     <tableColumn id="9" name="BattleMap" dataDxfId="20"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="0"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:P14" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
-  <autoFilter ref="A3:P14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:O14" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A3:O14"/>
   <sortState ref="A4:O83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="16">
-    <tableColumn id="1" name="Id" dataDxfId="16"/>
-    <tableColumn id="2" name="Name" dataDxfId="15"/>
-    <tableColumn id="3" name="Type" dataDxfId="14"/>
-    <tableColumn id="6" name="World" dataDxfId="13"/>
-    <tableColumn id="7" name="Deck" dataDxfId="12"/>
-    <tableColumn id="10" name="Job" dataDxfId="11"/>
-    <tableColumn id="4" name="KingCard" dataDxfId="10"/>
+  <tableColumns count="15">
+    <tableColumn id="1" name="Id" dataDxfId="15"/>
+    <tableColumn id="2" name="Name" dataDxfId="14"/>
+    <tableColumn id="3" name="Type" dataDxfId="13"/>
+    <tableColumn id="6" name="World" dataDxfId="12"/>
+    <tableColumn id="7" name="Deck" dataDxfId="11"/>
+    <tableColumn id="10" name="Job" dataDxfId="10"/>
     <tableColumn id="11" name="Level" dataDxfId="9"/>
     <tableColumn id="12" name="Reward" dataDxfId="8"/>
     <tableColumn id="13" name="Method" dataDxfId="7"/>
     <tableColumn id="14" name="Emethod" dataDxfId="6"/>
-    <tableColumn id="5" name="LeftMon" dataDxfId="5"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="4"/>
-    <tableColumn id="9" name="Figue" dataDxfId="3"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="2"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="1"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="5"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="1"/>
+    <tableColumn id="9" name="Figue" dataDxfId="4"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="3"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2747,7 +2751,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CAEACD"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -3026,13 +3030,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P73"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P69" sqref="P69"/>
+      <selection pane="bottomRight" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3040,16 +3044,15 @@
     <col min="1" max="1" width="9.25" customWidth="1"/>
     <col min="3" max="3" width="5.25" customWidth="1"/>
     <col min="6" max="6" width="10.125" customWidth="1"/>
-    <col min="7" max="7" width="8.625" customWidth="1"/>
-    <col min="8" max="8" width="6.25" customWidth="1"/>
-    <col min="9" max="9" width="11.875" customWidth="1"/>
-    <col min="10" max="10" width="9.5" customWidth="1"/>
-    <col min="11" max="13" width="10.625" customWidth="1"/>
-    <col min="15" max="15" width="10.625" customWidth="1"/>
-    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.25" customWidth="1"/>
+    <col min="8" max="8" width="11.875" customWidth="1"/>
+    <col min="9" max="9" width="9.5" customWidth="1"/>
+    <col min="10" max="12" width="10.625" customWidth="1"/>
+    <col min="14" max="14" width="10.625" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>203</v>
       </c>
@@ -3069,37 +3072,34 @@
         <v>208</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>244</v>
+        <v>240</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>212</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="N1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>213</v>
       </c>
+      <c r="N1" s="14" t="s">
+        <v>242</v>
+      </c>
       <c r="O1" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>201</v>
       </c>
@@ -3119,37 +3119,34 @@
         <v>201</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>234</v>
+        <v>201</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>202</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>202</v>
+      <c r="N2" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>214</v>
       </c>
@@ -3169,37 +3166,34 @@
         <v>219</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>224</v>
-      </c>
       <c r="O3" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43000001</v>
       </c>
@@ -3219,29 +3213,26 @@
         <v>11001001</v>
       </c>
       <c r="G4" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H4" s="4">
         <v>1</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="M4" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="N4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P4" s="23"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O4" s="23"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43000002</v>
       </c>
@@ -3261,29 +3252,26 @@
         <v>11001001</v>
       </c>
       <c r="G5" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H5" s="4">
         <v>2</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="M5" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="N5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P5" s="23"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O5" s="23"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43000003</v>
       </c>
@@ -3303,29 +3291,26 @@
         <v>11001001</v>
       </c>
       <c r="G6" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H6" s="4">
         <v>4</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="M6" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="N6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P6" s="23"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O6" s="23"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43000004</v>
       </c>
@@ -3345,29 +3330,26 @@
         <v>11001001</v>
       </c>
       <c r="G7" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H7" s="4">
         <v>5</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="M7" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="N7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P7" s="23"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O7" s="23"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43000005</v>
       </c>
@@ -3387,29 +3369,26 @@
         <v>11001001</v>
       </c>
       <c r="G8" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H8" s="4">
         <v>7</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+      <c r="M8" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="N8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P8" s="23"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O8" s="23"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43000006</v>
       </c>
@@ -3429,29 +3408,26 @@
         <v>11001001</v>
       </c>
       <c r="G9" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H9" s="4">
         <v>11</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="M9" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="N9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P9" s="23"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O9" s="23"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43000007</v>
       </c>
@@ -3471,29 +3447,26 @@
         <v>11001001</v>
       </c>
       <c r="G10" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H10" s="4">
-        <v>3</v>
-      </c>
-      <c r="I10" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="N10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P10" s="23"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O10" s="23"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43000008</v>
       </c>
@@ -3513,29 +3486,26 @@
         <v>11001001</v>
       </c>
       <c r="G11" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H11" s="4">
         <v>13</v>
       </c>
-      <c r="I11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+      <c r="M11" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="N11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P11" s="23"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O11" s="23"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43000009</v>
       </c>
@@ -3555,29 +3525,26 @@
         <v>11001001</v>
       </c>
       <c r="G12" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H12" s="4">
         <v>13</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K12" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+      <c r="M12" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="N12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P12" s="23"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O12" s="23"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43000010</v>
       </c>
@@ -3597,29 +3564,26 @@
         <v>11001001</v>
       </c>
       <c r="G13" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H13" s="4">
         <v>6</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="M13" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="N13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P13" s="23"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O13" s="23"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43000011</v>
       </c>
@@ -3639,29 +3603,26 @@
         <v>11001001</v>
       </c>
       <c r="G14" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H14" s="4">
         <v>5</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K14" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="M14" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="N14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P14" s="23"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O14" s="23"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43000012</v>
       </c>
@@ -3681,29 +3642,26 @@
         <v>11001001</v>
       </c>
       <c r="G15" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H15" s="4">
         <v>12</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K15" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="M15" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="N15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P15" s="23"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O15" s="23"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43000013</v>
       </c>
@@ -3723,29 +3681,26 @@
         <v>11001001</v>
       </c>
       <c r="G16" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H16" s="4">
         <v>10</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="M16" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="N16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P16" s="23"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O16" s="23"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43000014</v>
       </c>
@@ -3765,29 +3720,26 @@
         <v>11001001</v>
       </c>
       <c r="G17" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H17" s="4">
         <v>12</v>
       </c>
-      <c r="I17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K17" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+      <c r="M17" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="N17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="O17" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P17" s="23"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O17" s="23"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43000015</v>
       </c>
@@ -3807,29 +3759,26 @@
         <v>11001001</v>
       </c>
       <c r="G18" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H18" s="4">
         <v>12</v>
       </c>
-      <c r="I18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K18" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
+      <c r="M18" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="N18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P18" s="23"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O18" s="23"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43000016</v>
       </c>
@@ -3849,29 +3798,26 @@
         <v>11001001</v>
       </c>
       <c r="G19" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H19" s="4">
         <v>1</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K19" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
+      <c r="M19" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="N19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O19" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P19" s="23"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O19" s="23"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43000017</v>
       </c>
@@ -3891,29 +3837,26 @@
         <v>11001001</v>
       </c>
       <c r="G20" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H20" s="4">
         <v>1</v>
       </c>
-      <c r="I20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K20" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="M20" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="N20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P20" s="23"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O20" s="23"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43000018</v>
       </c>
@@ -3933,29 +3876,26 @@
         <v>11001001</v>
       </c>
       <c r="G21" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H21" s="4">
         <v>9</v>
       </c>
-      <c r="I21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J21" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K21" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="K21" s="4"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
+      <c r="M21" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="N21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P21" s="23"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O21" s="23"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43000019</v>
       </c>
@@ -3975,29 +3915,26 @@
         <v>11001001</v>
       </c>
       <c r="G22" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H22" s="4">
         <v>15</v>
       </c>
-      <c r="I22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K22" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
+      <c r="M22" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="N22" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O22" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P22" s="23"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O22" s="23"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43000020</v>
       </c>
@@ -4017,29 +3954,26 @@
         <v>11001001</v>
       </c>
       <c r="G23" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H23" s="4">
         <v>4</v>
       </c>
-      <c r="I23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J23" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K23" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="K23" s="4"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
+      <c r="M23" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="N23" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="O23" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P23" s="23"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O23" s="23"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43000021</v>
       </c>
@@ -4059,29 +3993,26 @@
         <v>11001001</v>
       </c>
       <c r="G24" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H24" s="4">
         <v>15</v>
       </c>
-      <c r="I24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K24" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
+      <c r="M24" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="N24" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="O24" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P24" s="23"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O24" s="23"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43000022</v>
       </c>
@@ -4101,29 +4032,26 @@
         <v>11001001</v>
       </c>
       <c r="G25" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H25" s="4">
         <v>14</v>
       </c>
-      <c r="I25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K25" s="4" t="s">
         <v>46</v>
       </c>
+      <c r="K25" s="4"/>
       <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
+      <c r="M25" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="N25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="O25" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P25" s="23"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O25" s="23"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43000023</v>
       </c>
@@ -4143,29 +4071,26 @@
         <v>11001001</v>
       </c>
       <c r="G26" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H26" s="4">
         <v>17</v>
       </c>
-      <c r="I26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J26" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K26" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
+      <c r="M26" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="N26" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="O26" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P26" s="23"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O26" s="23"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43000024</v>
       </c>
@@ -4185,29 +4110,26 @@
         <v>11001001</v>
       </c>
       <c r="G27" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H27" s="4">
         <v>34</v>
       </c>
-      <c r="I27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K27" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="K27" s="4"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
+      <c r="M27" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="N27" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="O27" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P27" s="23"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O27" s="23"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43000025</v>
       </c>
@@ -4227,29 +4149,26 @@
         <v>11001001</v>
       </c>
       <c r="G28" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H28" s="4">
         <v>35</v>
       </c>
-      <c r="I28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K28" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="K28" s="4"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
+      <c r="M28" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="N28" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="O28" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P28" s="23"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O28" s="23"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43000026</v>
       </c>
@@ -4269,29 +4188,26 @@
         <v>11001001</v>
       </c>
       <c r="G29" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H29" s="4">
         <v>35</v>
       </c>
-      <c r="I29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K29" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
+      <c r="M29" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="N29" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="O29" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P29" s="23"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O29" s="23"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43000027</v>
       </c>
@@ -4311,29 +4227,26 @@
         <v>11001001</v>
       </c>
       <c r="G30" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H30" s="4">
         <v>5</v>
       </c>
-      <c r="I30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J30" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K30" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="M30" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="N30" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="O30" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P30" s="23"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O30" s="23"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43000028</v>
       </c>
@@ -4353,29 +4266,26 @@
         <v>11001001</v>
       </c>
       <c r="G31" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H31" s="4">
         <v>16</v>
       </c>
-      <c r="I31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J31" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K31" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
+      <c r="M31" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="N31" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="O31" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P31" s="23"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O31" s="23"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43000029</v>
       </c>
@@ -4395,29 +4305,26 @@
         <v>11001001</v>
       </c>
       <c r="G32" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H32" s="4">
         <v>19</v>
       </c>
-      <c r="I32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J32" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K32" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
+      <c r="M32" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="N32" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="O32" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P32" s="23"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O32" s="23"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43000030</v>
       </c>
@@ -4437,29 +4344,26 @@
         <v>11001001</v>
       </c>
       <c r="G33" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H33" s="4">
         <v>16</v>
       </c>
-      <c r="I33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K33" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
+      <c r="M33" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="N33" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O33" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P33" s="23"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O33" s="23"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43000031</v>
       </c>
@@ -4479,29 +4383,26 @@
         <v>11001001</v>
       </c>
       <c r="G34" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H34" s="4">
         <v>7</v>
       </c>
-      <c r="I34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J34" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K34" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
+      <c r="M34" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="N34" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="O34" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P34" s="23"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O34" s="23"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43000032</v>
       </c>
@@ -4521,29 +4422,26 @@
         <v>11001001</v>
       </c>
       <c r="G35" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H35" s="4">
         <v>18</v>
       </c>
-      <c r="I35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J35" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K35" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
+      <c r="M35" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="N35" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="O35" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P35" s="23"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O35" s="23"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43000033</v>
       </c>
@@ -4563,29 +4461,26 @@
         <v>11001001</v>
       </c>
       <c r="G36" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H36" s="4">
         <v>7</v>
       </c>
-      <c r="I36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J36" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K36" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="K36" s="4"/>
       <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
+      <c r="M36" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="N36" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="O36" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P36" s="23"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+      <c r="O36" s="23"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43000101</v>
       </c>
@@ -4605,33 +4500,30 @@
         <v>11000001</v>
       </c>
       <c r="G37" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H37" s="4">
         <v>2</v>
       </c>
-      <c r="I37" s="4">
-        <v>2</v>
+      <c r="I37" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K37" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="K37" s="4"/>
       <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
+      <c r="M37" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="N37" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="O37" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="P37" s="23">
+        <v>238</v>
+      </c>
+      <c r="O37" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43000102</v>
       </c>
@@ -4651,33 +4543,30 @@
         <v>11000003</v>
       </c>
       <c r="G38" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H38" s="4">
-        <v>4</v>
-      </c>
-      <c r="I38" s="4">
+        <v>3</v>
+      </c>
+      <c r="I38" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K38" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="K38" s="4"/>
       <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
+      <c r="M38" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="N38" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="O38" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="P38" s="23">
+        <v>238</v>
+      </c>
+      <c r="O38" s="23">
         <v>22031004</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>43000103</v>
       </c>
@@ -4697,33 +4586,30 @@
         <v>11000002</v>
       </c>
       <c r="G39" s="4">
-        <v>0</v>
-      </c>
-      <c r="H39" s="4">
         <v>7</v>
       </c>
+      <c r="H39" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="I39" s="4" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K39" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="K39" s="4"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
+      <c r="M39" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="N39" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O39" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P39" s="23">
+        <v>237</v>
+      </c>
+      <c r="O39" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>43000104</v>
       </c>
@@ -4737,39 +4623,36 @@
         <v>70</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F40">
         <v>11000008</v>
       </c>
       <c r="G40" s="4">
-        <v>0</v>
-      </c>
-      <c r="H40" s="4">
         <v>9</v>
       </c>
+      <c r="H40" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="I40" s="4" t="s">
-        <v>80</v>
+        <v>3</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K40" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
+      <c r="M40" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="N40" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="O40" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P40" s="23">
+        <v>237</v>
+      </c>
+      <c r="O40" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>43000105</v>
       </c>
@@ -4789,33 +4672,30 @@
         <v>11000007</v>
       </c>
       <c r="G41" s="4">
-        <v>0</v>
-      </c>
-      <c r="H41" s="4">
         <v>12</v>
       </c>
+      <c r="H41" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="I41" s="4" t="s">
-        <v>84</v>
+        <v>3</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K41" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="K41" s="4"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
+      <c r="M41" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="N41" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O41" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P41" s="23">
+        <v>237</v>
+      </c>
+      <c r="O41" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>43000106</v>
       </c>
@@ -4835,33 +4715,30 @@
         <v>11000005</v>
       </c>
       <c r="G42" s="4">
-        <v>0</v>
-      </c>
-      <c r="H42" s="4">
         <v>14</v>
       </c>
+      <c r="H42" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="I42" s="4" t="s">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K42" s="4" t="s">
         <v>89</v>
       </c>
+      <c r="K42" s="4"/>
       <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
+      <c r="M42" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="N42" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="O42" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P42" s="23">
+        <v>237</v>
+      </c>
+      <c r="O42" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>43000107</v>
       </c>
@@ -4881,33 +4758,30 @@
         <v>11000007</v>
       </c>
       <c r="G43" s="4">
-        <v>0</v>
-      </c>
-      <c r="H43" s="4">
         <v>15</v>
       </c>
+      <c r="H43" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="I43" s="4" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K43" s="4" t="s">
         <v>92</v>
       </c>
+      <c r="K43" s="4"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
+      <c r="M43" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="N43" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="O43" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P43" s="23">
+        <v>237</v>
+      </c>
+      <c r="O43" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43000108</v>
       </c>
@@ -4927,33 +4801,30 @@
         <v>11000005</v>
       </c>
       <c r="G44" s="4">
-        <v>0</v>
-      </c>
-      <c r="H44" s="4">
         <v>18</v>
       </c>
+      <c r="H44" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="I44" s="4" t="s">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K44" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
+      <c r="M44" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="N44" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="O44" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P44" s="23">
+        <v>237</v>
+      </c>
+      <c r="O44" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>43000109</v>
       </c>
@@ -4973,33 +4844,30 @@
         <v>11000006</v>
       </c>
       <c r="G45" s="4">
-        <v>0</v>
-      </c>
-      <c r="H45" s="4">
         <v>21</v>
       </c>
+      <c r="H45" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="I45" s="4" t="s">
-        <v>99</v>
+        <v>3</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K45" s="4" t="s">
         <v>100</v>
       </c>
+      <c r="K45" s="4"/>
       <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
+      <c r="M45" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="N45" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="O45" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P45" s="23">
+        <v>237</v>
+      </c>
+      <c r="O45" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>43000110</v>
       </c>
@@ -5019,33 +4887,30 @@
         <v>11000006</v>
       </c>
       <c r="G46" s="4">
-        <v>0</v>
-      </c>
-      <c r="H46" s="4">
         <v>24</v>
       </c>
+      <c r="H46" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="I46" s="4" t="s">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K46" s="4" t="s">
         <v>104</v>
       </c>
+      <c r="K46" s="4"/>
       <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
+      <c r="M46" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="N46" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="O46" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P46" s="23">
+        <v>237</v>
+      </c>
+      <c r="O46" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>43000201</v>
       </c>
@@ -5065,33 +4930,30 @@
         <v>11000007</v>
       </c>
       <c r="G47" s="4">
-        <v>0</v>
-      </c>
-      <c r="H47" s="4">
         <v>22</v>
       </c>
+      <c r="H47" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="I47" s="4" t="s">
-        <v>107</v>
+        <v>3</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K47" s="4" t="s">
         <v>108</v>
       </c>
+      <c r="K47" s="4"/>
       <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
+      <c r="M47" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="N47" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="O47" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P47" s="23">
+        <v>237</v>
+      </c>
+      <c r="O47" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>43000202</v>
       </c>
@@ -5111,33 +4973,30 @@
         <v>11000001</v>
       </c>
       <c r="G48" s="4">
-        <v>0</v>
-      </c>
-      <c r="H48" s="4">
         <v>17</v>
       </c>
+      <c r="H48" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="I48" s="4" t="s">
-        <v>110</v>
+        <v>3</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K48" s="4" t="s">
         <v>111</v>
       </c>
+      <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
+      <c r="M48" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="N48" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="O48" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P48" s="23">
+        <v>237</v>
+      </c>
+      <c r="O48" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>43000203</v>
       </c>
@@ -5157,33 +5016,30 @@
         <v>11000002</v>
       </c>
       <c r="G49" s="4">
-        <v>0</v>
-      </c>
-      <c r="H49" s="4">
         <v>22</v>
       </c>
+      <c r="H49" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="I49" s="4" t="s">
-        <v>113</v>
+        <v>3</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K49" s="4" t="s">
         <v>114</v>
       </c>
+      <c r="K49" s="4"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
+      <c r="M49" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="N49" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="O49" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P49" s="23">
+        <v>237</v>
+      </c>
+      <c r="O49" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>43000301</v>
       </c>
@@ -5203,33 +5059,30 @@
         <v>11000002</v>
       </c>
       <c r="G50" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H50" s="4">
-        <v>7</v>
-      </c>
-      <c r="I50" s="4">
         <v>2</v>
       </c>
+      <c r="I50" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J50" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K50" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="K50" s="4"/>
       <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
+      <c r="M50" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N50" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="O50" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P50" s="23">
+        <v>237</v>
+      </c>
+      <c r="O50" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>43000302</v>
       </c>
@@ -5249,33 +5102,30 @@
         <v>11000008</v>
       </c>
       <c r="G51" s="4">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H51" s="4">
-        <v>9</v>
-      </c>
-      <c r="I51" s="4">
+        <v>3</v>
+      </c>
+      <c r="I51" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K51" s="4" t="s">
         <v>121</v>
       </c>
+      <c r="K51" s="4"/>
       <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
+      <c r="M51" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="N51" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="O51" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P51" s="23">
+        <v>237</v>
+      </c>
+      <c r="O51" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>43000303</v>
       </c>
@@ -5295,33 +5145,30 @@
         <v>11000004</v>
       </c>
       <c r="G52" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H52" s="4">
-        <v>5</v>
-      </c>
-      <c r="I52" s="4">
         <v>2</v>
       </c>
+      <c r="I52" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J52" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K52" s="4" t="s">
         <v>124</v>
       </c>
+      <c r="K52" s="4"/>
       <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
+      <c r="M52" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="N52" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="O52" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P52" s="23">
+        <v>237</v>
+      </c>
+      <c r="O52" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>43000304</v>
       </c>
@@ -5341,33 +5188,30 @@
         <v>11000002</v>
       </c>
       <c r="G53" s="4">
-        <v>0</v>
-      </c>
-      <c r="H53" s="4">
         <v>14</v>
       </c>
+      <c r="H53" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="I53" s="4" t="s">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K53" s="4" t="s">
         <v>128</v>
       </c>
+      <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
+      <c r="M53" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="N53" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="O53" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P53" s="23">
+        <v>237</v>
+      </c>
+      <c r="O53" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>43000305</v>
       </c>
@@ -5381,39 +5225,36 @@
         <v>123</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F54">
         <v>11000005</v>
       </c>
       <c r="G54" s="4">
-        <v>0</v>
-      </c>
-      <c r="H54" s="4">
         <v>14</v>
       </c>
+      <c r="H54" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="I54" s="4" t="s">
-        <v>110</v>
+        <v>3</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K54" s="4" t="s">
         <v>130</v>
       </c>
+      <c r="K54" s="4"/>
       <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
+      <c r="M54" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="N54" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="O54" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P54" s="23">
+        <v>237</v>
+      </c>
+      <c r="O54" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>43000306</v>
       </c>
@@ -5433,33 +5274,30 @@
         <v>11000008</v>
       </c>
       <c r="G55" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55" s="4">
-        <v>1</v>
-      </c>
-      <c r="I55" s="4">
         <v>6</v>
       </c>
+      <c r="I55" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J55" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K55" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="K55" s="4"/>
       <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
+      <c r="M55" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="N55" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="O55" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P55" s="23">
+        <v>237</v>
+      </c>
+      <c r="O55" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>43000307</v>
       </c>
@@ -5479,33 +5317,30 @@
         <v>11000001</v>
       </c>
       <c r="G56" s="4">
-        <v>0</v>
-      </c>
-      <c r="H56" s="4">
         <v>10</v>
       </c>
+      <c r="H56" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="I56" s="4" t="s">
-        <v>134</v>
+        <v>3</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K56" s="4" t="s">
         <v>135</v>
       </c>
+      <c r="K56" s="4"/>
       <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
+      <c r="M56" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="N56" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="O56" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P56" s="23">
+        <v>237</v>
+      </c>
+      <c r="O56" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>43000308</v>
       </c>
@@ -5525,33 +5360,30 @@
         <v>11000001</v>
       </c>
       <c r="G57" s="4">
-        <v>0</v>
-      </c>
-      <c r="H57" s="4">
         <v>11</v>
       </c>
+      <c r="H57" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="I57" s="4" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K57" s="4" t="s">
         <v>137</v>
       </c>
+      <c r="K57" s="4"/>
       <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
+      <c r="M57" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="N57" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="O57" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P57" s="23">
+        <v>237</v>
+      </c>
+      <c r="O57" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>43000309</v>
       </c>
@@ -5571,33 +5403,30 @@
         <v>11000004</v>
       </c>
       <c r="G58" s="4">
-        <v>0</v>
-      </c>
-      <c r="H58" s="4">
         <v>13</v>
       </c>
+      <c r="H58" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="I58" s="4" t="s">
-        <v>110</v>
+        <v>3</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K58" s="4" t="s">
         <v>139</v>
       </c>
+      <c r="K58" s="4"/>
       <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
+      <c r="M58" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="N58" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="O58" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P58" s="23">
+        <v>237</v>
+      </c>
+      <c r="O58" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>43000310</v>
       </c>
@@ -5617,33 +5446,30 @@
         <v>11000003</v>
       </c>
       <c r="G59" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H59" s="4">
-        <v>8</v>
-      </c>
-      <c r="I59" s="4">
         <v>2</v>
       </c>
+      <c r="I59" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J59" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K59" s="4" t="s">
         <v>141</v>
       </c>
+      <c r="K59" s="4"/>
       <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
+      <c r="M59" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="N59" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="O59" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P59" s="23">
+        <v>237</v>
+      </c>
+      <c r="O59" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>43000311</v>
       </c>
@@ -5657,39 +5483,36 @@
         <v>123</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F60">
         <v>11000005</v>
       </c>
       <c r="G60" s="4">
-        <v>0</v>
-      </c>
-      <c r="H60" s="4">
         <v>13</v>
       </c>
+      <c r="H60" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="I60" s="4" t="s">
-        <v>84</v>
+        <v>3</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K60" s="4" t="s">
         <v>143</v>
       </c>
+      <c r="K60" s="4"/>
       <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
+      <c r="M60" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="N60" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="O60" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P60" s="23">
+        <v>237</v>
+      </c>
+      <c r="O60" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>43000312</v>
       </c>
@@ -5703,39 +5526,36 @@
         <v>123</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F61">
         <v>11000001</v>
       </c>
       <c r="G61" s="4">
-        <v>0</v>
-      </c>
-      <c r="H61" s="4">
         <v>18</v>
       </c>
+      <c r="H61" s="4" t="s">
+        <v>145</v>
+      </c>
       <c r="I61" s="4" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K61" s="4" t="s">
         <v>146</v>
       </c>
+      <c r="K61" s="4"/>
       <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
+      <c r="M61" s="4" t="s">
+        <v>146</v>
+      </c>
       <c r="N61" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="O61" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P61" s="23">
+        <v>237</v>
+      </c>
+      <c r="O61" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>43000401</v>
       </c>
@@ -5755,33 +5575,30 @@
         <v>11000002</v>
       </c>
       <c r="G62" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H62" s="4">
-        <v>10</v>
-      </c>
-      <c r="I62" s="4">
         <v>6</v>
       </c>
+      <c r="I62" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J62" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K62" s="4" t="s">
         <v>149</v>
       </c>
+      <c r="K62" s="4"/>
       <c r="L62" s="4"/>
-      <c r="M62" s="4"/>
+      <c r="M62" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="N62" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="O62" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P62" s="23">
+        <v>237</v>
+      </c>
+      <c r="O62" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>43000402</v>
       </c>
@@ -5801,33 +5618,30 @@
         <v>11000001</v>
       </c>
       <c r="G63" s="4">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H63" s="4">
-        <v>11</v>
-      </c>
-      <c r="I63" s="4">
         <v>5</v>
       </c>
+      <c r="I63" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J63" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K63" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="K63" s="4"/>
       <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
+      <c r="M63" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="N63" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="O63" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P63" s="23">
+        <v>237</v>
+      </c>
+      <c r="O63" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>43000403</v>
       </c>
@@ -5847,33 +5661,30 @@
         <v>11000002</v>
       </c>
       <c r="G64" s="4">
-        <v>0</v>
-      </c>
-      <c r="H64" s="4">
         <v>13</v>
       </c>
+      <c r="H64" s="4" t="s">
+        <v>153</v>
+      </c>
       <c r="I64" s="4" t="s">
-        <v>153</v>
+        <v>3</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K64" s="4" t="s">
         <v>154</v>
       </c>
+      <c r="K64" s="4"/>
       <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
+      <c r="M64" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="N64" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="O64" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P64" s="23">
+        <v>237</v>
+      </c>
+      <c r="O64" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>43000404</v>
       </c>
@@ -5893,33 +5704,30 @@
         <v>11000001</v>
       </c>
       <c r="G65" s="4">
-        <v>0</v>
-      </c>
-      <c r="H65" s="4">
         <v>14</v>
       </c>
+      <c r="H65" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="I65" s="4" t="s">
-        <v>113</v>
+        <v>3</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K65" s="4" t="s">
         <v>156</v>
       </c>
+      <c r="K65" s="4"/>
       <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
+      <c r="M65" s="4" t="s">
+        <v>156</v>
+      </c>
       <c r="N65" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="O65" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P65" s="23">
+        <v>237</v>
+      </c>
+      <c r="O65" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>43000405</v>
       </c>
@@ -5939,33 +5747,30 @@
         <v>11000007</v>
       </c>
       <c r="G66" s="4">
-        <v>0</v>
-      </c>
-      <c r="H66" s="4">
         <v>18</v>
       </c>
+      <c r="H66" s="4" t="s">
+        <v>145</v>
+      </c>
       <c r="I66" s="4" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K66" s="4" t="s">
         <v>158</v>
       </c>
+      <c r="K66" s="4"/>
       <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
+      <c r="M66" s="4" t="s">
+        <v>158</v>
+      </c>
       <c r="N66" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="O66" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P66" s="23">
+        <v>237</v>
+      </c>
+      <c r="O66" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>43000406</v>
       </c>
@@ -5985,33 +5790,30 @@
         <v>11000006</v>
       </c>
       <c r="G67" s="4">
-        <v>0</v>
-      </c>
-      <c r="H67" s="4">
         <v>15</v>
       </c>
+      <c r="H67" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="I67" s="4" t="s">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K67" s="4" t="s">
         <v>160</v>
       </c>
+      <c r="K67" s="4"/>
       <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
+      <c r="M67" s="4" t="s">
+        <v>160</v>
+      </c>
       <c r="N67" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="O67" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P67" s="23">
+        <v>237</v>
+      </c>
+      <c r="O67" s="23">
         <v>22031003</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>43000407</v>
       </c>
@@ -6031,33 +5833,30 @@
         <v>11000004</v>
       </c>
       <c r="G68" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H68" s="4">
-        <v>10</v>
-      </c>
-      <c r="I68" s="4">
         <v>4</v>
       </c>
+      <c r="I68" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J68" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K68" s="4" t="s">
         <v>162</v>
       </c>
+      <c r="K68" s="4"/>
       <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
+      <c r="M68" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="N68" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="O68" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P68" s="23">
+        <v>237</v>
+      </c>
+      <c r="O68" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>43000408</v>
       </c>
@@ -6077,33 +5876,30 @@
         <v>11000002</v>
       </c>
       <c r="G69" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H69" s="4">
-        <v>7</v>
-      </c>
-      <c r="I69" s="4">
         <v>5</v>
       </c>
+      <c r="I69" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K69" s="4" t="s">
         <v>164</v>
       </c>
+      <c r="K69" s="4"/>
       <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
+      <c r="M69" s="4" t="s">
+        <v>164</v>
+      </c>
       <c r="N69" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="O69" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P69" s="23">
+        <v>237</v>
+      </c>
+      <c r="O69" s="23">
         <v>22031005</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>43000501</v>
       </c>
@@ -6123,33 +5919,30 @@
         <v>11000003</v>
       </c>
       <c r="G70" s="4">
-        <v>0</v>
-      </c>
-      <c r="H70" s="4">
         <v>15</v>
       </c>
+      <c r="H70" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="I70" s="4" t="s">
-        <v>167</v>
+        <v>3</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K70" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="K70" s="4"/>
       <c r="L70" s="4"/>
-      <c r="M70" s="4"/>
+      <c r="M70" s="4" t="s">
+        <v>168</v>
+      </c>
       <c r="N70" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="O70" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P70" s="23">
+        <v>237</v>
+      </c>
+      <c r="O70" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>43000502</v>
       </c>
@@ -6169,33 +5962,30 @@
         <v>11000002</v>
       </c>
       <c r="G71" s="4">
-        <v>0</v>
-      </c>
-      <c r="H71" s="4">
         <v>13</v>
       </c>
+      <c r="H71" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="I71" s="4" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K71" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="K71" s="4"/>
       <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
+      <c r="M71" s="4" t="s">
+        <v>170</v>
+      </c>
       <c r="N71" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="O71" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P71" s="23">
+        <v>237</v>
+      </c>
+      <c r="O71" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>43000503</v>
       </c>
@@ -6215,33 +6005,30 @@
         <v>11000008</v>
       </c>
       <c r="G72" s="4">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H72" s="4">
-        <v>9</v>
-      </c>
-      <c r="I72" s="4">
+        <v>3</v>
+      </c>
+      <c r="I72" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K72" s="4" t="s">
         <v>173</v>
       </c>
+      <c r="K72" s="4"/>
       <c r="L72" s="4"/>
-      <c r="M72" s="4"/>
+      <c r="M72" s="4" t="s">
+        <v>173</v>
+      </c>
       <c r="N72" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="O72" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P72" s="23">
+        <v>237</v>
+      </c>
+      <c r="O72" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>43000504</v>
       </c>
@@ -6261,29 +6048,26 @@
         <v>11000001</v>
       </c>
       <c r="G73" s="4">
-        <v>0</v>
-      </c>
-      <c r="H73" s="4">
         <v>19</v>
       </c>
+      <c r="H73" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="I73" s="4" t="s">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K73" s="4" t="s">
         <v>175</v>
       </c>
+      <c r="K73" s="4"/>
       <c r="L73" s="4"/>
-      <c r="M73" s="4"/>
+      <c r="M73" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="N73" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="O73" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="P73" s="23">
+        <v>237</v>
+      </c>
+      <c r="O73" s="23">
         <v>22031002</v>
       </c>
     </row>
@@ -6299,13 +6083,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6313,16 +6097,15 @@
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="3" max="3" width="5.125" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="9.5" customWidth="1"/>
-    <col min="8" max="8" width="6.125" customWidth="1"/>
-    <col min="9" max="9" width="11.875" customWidth="1"/>
-    <col min="10" max="10" width="9.5" customWidth="1"/>
-    <col min="11" max="13" width="10.625" customWidth="1"/>
-    <col min="15" max="15" width="10.625" customWidth="1"/>
-    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.125" customWidth="1"/>
+    <col min="8" max="8" width="11.875" customWidth="1"/>
+    <col min="9" max="9" width="9.5" customWidth="1"/>
+    <col min="10" max="12" width="10.625" customWidth="1"/>
+    <col min="14" max="14" width="10.625" customWidth="1"/>
+    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>203</v>
       </c>
@@ -6342,37 +6125,34 @@
         <v>208</v>
       </c>
       <c r="G1" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="N1" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="N1" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>236</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="O1" s="21" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>201</v>
       </c>
@@ -6392,37 +6172,34 @@
         <v>201</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>234</v>
+        <v>201</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>202</v>
       </c>
       <c r="K2" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="N2" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="O2" s="22" t="s">
         <v>257</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>214</v>
       </c>
@@ -6442,37 +6219,34 @@
         <v>219</v>
       </c>
       <c r="G3" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="N3" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="L3" s="10" t="s">
+      <c r="O3" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="M3" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="P3" s="20" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43010001</v>
       </c>
@@ -6492,31 +6266,28 @@
         <v>11001002</v>
       </c>
       <c r="G4" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H4" s="4">
         <v>1</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="6" t="s">
-        <v>258</v>
+      <c r="K4" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="L4" s="6"/>
+      <c r="M4" s="4" t="s">
+        <v>236</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="P4" s="19"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="O4" s="19"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43010002</v>
       </c>
@@ -6536,29 +6307,26 @@
         <v>11001002</v>
       </c>
       <c r="G5" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H5" s="4">
         <v>5</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="J5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="M5" s="4" t="s">
+        <v>180</v>
+      </c>
       <c r="N5" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="P5" s="19"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+        <v>239</v>
+      </c>
+      <c r="O5" s="19"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43010003</v>
       </c>
@@ -6578,29 +6346,26 @@
         <v>11001002</v>
       </c>
       <c r="G6" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H6" s="4">
         <v>10</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="J6" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
       <c r="N6" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="P6" s="19"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+        <v>239</v>
+      </c>
+      <c r="O6" s="19"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43010004</v>
       </c>
@@ -6620,29 +6385,26 @@
         <v>11001002</v>
       </c>
       <c r="G7" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H7" s="4">
         <v>10</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="J7" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="K7" s="4" t="s">
         <v>184</v>
       </c>
+      <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="M7" s="4" t="s">
+        <v>184</v>
+      </c>
       <c r="N7" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="P7" s="19"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+        <v>239</v>
+      </c>
+      <c r="O7" s="19"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43010005</v>
       </c>
@@ -6662,33 +6424,28 @@
         <v>11001001</v>
       </c>
       <c r="G8" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H8" s="4">
         <v>1</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="6" t="s">
+        <v>227</v>
+      </c>
       <c r="J8" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="K8" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="L8" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="N8" s="6" t="s">
+      <c r="K8" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="O8" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="P8" s="19"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="N8" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="O8" s="19"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43010006</v>
       </c>
@@ -6708,33 +6465,28 @@
         <v>11001001</v>
       </c>
       <c r="G9" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H9" s="4">
         <v>1</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="6" t="s">
+        <v>232</v>
+      </c>
       <c r="J9" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="K9" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="L9" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="N9" s="6" t="s">
+      <c r="K9" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="O9" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="P9" s="19"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="N9" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="O9" s="19"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43010101</v>
       </c>
@@ -6754,29 +6506,26 @@
         <v>11001001</v>
       </c>
       <c r="G10" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H10" s="4">
         <v>5</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>187</v>
+      </c>
       <c r="J10" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="K10" s="4" t="s">
         <v>188</v>
       </c>
+      <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="N10" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="P10" s="19"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+        <v>239</v>
+      </c>
+      <c r="O10" s="19"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43010102</v>
       </c>
@@ -6796,29 +6545,26 @@
         <v>11001001</v>
       </c>
       <c r="G11" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H11" s="4">
         <v>10</v>
       </c>
-      <c r="I11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4" t="s">
+        <v>191</v>
+      </c>
       <c r="J11" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="K11" s="4" t="s">
         <v>192</v>
       </c>
+      <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+      <c r="M11" s="4" t="s">
+        <v>193</v>
+      </c>
       <c r="N11" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="P11" s="19"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+        <v>239</v>
+      </c>
+      <c r="O11" s="19"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43010103</v>
       </c>
@@ -6838,29 +6584,26 @@
         <v>11001001</v>
       </c>
       <c r="G12" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H12" s="4">
         <v>5</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>195</v>
+      </c>
       <c r="J12" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
       <c r="N12" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="P12" s="19"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+        <v>239</v>
+      </c>
+      <c r="O12" s="19"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43010104</v>
       </c>
@@ -6880,29 +6623,26 @@
         <v>11001001</v>
       </c>
       <c r="G13" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H13" s="4">
         <v>10</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>197</v>
+      </c>
       <c r="J13" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>197</v>
-      </c>
+      <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="M13" s="4" t="s">
+        <v>198</v>
+      </c>
       <c r="N13" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="P13" s="19"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+        <v>239</v>
+      </c>
+      <c r="O13" s="19"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43010105</v>
       </c>
@@ -6922,27 +6662,24 @@
         <v>11001001</v>
       </c>
       <c r="G14" s="4">
-        <v>51018001</v>
-      </c>
-      <c r="H14" s="4">
         <v>25</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>200</v>
+      </c>
       <c r="J14" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
       <c r="N14" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="P14" s="19"/>
+        <v>239</v>
+      </c>
+      <c r="O14" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
magnite will keep after sceneitems reset
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="1" r:id="rId1"/>
     <sheet name="特殊" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="268">
   <si>
     <t>老鼠</t>
   </si>
@@ -869,13 +869,17 @@
   </si>
   <si>
     <t>51000229;4;-1;51000229;4;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51000002;4;-1;51000002;4;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1694,9 +1698,9 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <name val="宋体"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -1724,33 +1728,6 @@
         <color theme="1"/>
         <name val="宋体"/>
         <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -2553,6 +2530,33 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="4"/>
@@ -2610,74 +2614,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2707,51 +2643,51 @@
     <tableColumn id="13" name="Method" dataDxfId="24"/>
     <tableColumn id="14" name="Emethod" dataDxfId="23"/>
     <tableColumn id="15" name="RightMon" dataDxfId="22"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="0"/>
-    <tableColumn id="17" name="Figue" dataDxfId="21"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="20"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="19"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="21"/>
+    <tableColumn id="17" name="Figue" dataDxfId="20"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="19"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:O14" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:O14" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A3:O14"/>
   <sortState ref="A4:O83">
     <sortCondition ref="A3:A83"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="Id" dataDxfId="15"/>
-    <tableColumn id="2" name="Name" dataDxfId="14"/>
-    <tableColumn id="3" name="Type" dataDxfId="13"/>
-    <tableColumn id="6" name="World" dataDxfId="12"/>
-    <tableColumn id="7" name="Deck" dataDxfId="11"/>
-    <tableColumn id="10" name="Job" dataDxfId="10"/>
-    <tableColumn id="11" name="Level" dataDxfId="9"/>
-    <tableColumn id="12" name="Reward" dataDxfId="8"/>
-    <tableColumn id="13" name="Method" dataDxfId="7"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="6"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="5"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="1"/>
-    <tableColumn id="9" name="Figue" dataDxfId="4"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="3"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="2"/>
+    <tableColumn id="1" name="Id" dataDxfId="14"/>
+    <tableColumn id="2" name="Name" dataDxfId="13"/>
+    <tableColumn id="3" name="Type" dataDxfId="12"/>
+    <tableColumn id="6" name="World" dataDxfId="11"/>
+    <tableColumn id="7" name="Deck" dataDxfId="10"/>
+    <tableColumn id="10" name="Job" dataDxfId="9"/>
+    <tableColumn id="11" name="Level" dataDxfId="8"/>
+    <tableColumn id="12" name="Reward" dataDxfId="7"/>
+    <tableColumn id="13" name="Method" dataDxfId="6"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="5"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="4"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="3"/>
+    <tableColumn id="9" name="Figue" dataDxfId="2"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="1"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2819,6 +2755,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2854,6 +2807,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3032,11 +3002,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K24" sqref="K24"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3262,7 +3232,9 @@
         <v>6</v>
       </c>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+      <c r="L5" s="6" t="s">
+        <v>267</v>
+      </c>
       <c r="M5" s="4" t="s">
         <v>6</v>
       </c>
@@ -6085,11 +6057,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
automaticly add people on level up
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,12 +15,12 @@
     <sheet name="People" sheetId="1" r:id="rId1"/>
     <sheet name="特殊" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="274">
   <si>
     <t>老鼠</t>
   </si>
@@ -873,13 +873,35 @@
   </si>
   <si>
     <t>51000002;4;-1;51000002;4;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动开启等级</t>
+  </si>
+  <si>
+    <t>自动开启等级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AutoAddLevel</t>
+  </si>
+  <si>
+    <t>AutoAddLevel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1063,6 +1085,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1070,6 +1093,7 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1077,6 +1101,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1685,7 +1710,61 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="38">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2626,61 +2705,63 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:O73" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
-  <autoFilter ref="A3:O73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:P73" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" tableBorderDxfId="35">
+  <autoFilter ref="A3:P73"/>
   <sortState ref="A4:O83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Id" dataDxfId="32"/>
-    <tableColumn id="2" name="Name" dataDxfId="31"/>
-    <tableColumn id="3" name="Type" dataDxfId="30"/>
-    <tableColumn id="6" name="World" dataDxfId="29"/>
-    <tableColumn id="7" name="Deck" dataDxfId="28"/>
-    <tableColumn id="10" name="Job" dataDxfId="27"/>
-    <tableColumn id="11" name="Level" dataDxfId="26"/>
-    <tableColumn id="12" name="Reward" dataDxfId="25"/>
-    <tableColumn id="13" name="Method" dataDxfId="24"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="23"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="22"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="21"/>
-    <tableColumn id="17" name="Figue" dataDxfId="20"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="19"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="18"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Id" dataDxfId="34"/>
+    <tableColumn id="2" name="Name" dataDxfId="33"/>
+    <tableColumn id="3" name="Type" dataDxfId="32"/>
+    <tableColumn id="6" name="World" dataDxfId="31"/>
+    <tableColumn id="7" name="Deck" dataDxfId="30"/>
+    <tableColumn id="10" name="Job" dataDxfId="29"/>
+    <tableColumn id="11" name="Level" dataDxfId="28"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="0"/>
+    <tableColumn id="12" name="Reward" dataDxfId="27"/>
+    <tableColumn id="13" name="Method" dataDxfId="26"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="25"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="24"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="23"/>
+    <tableColumn id="17" name="Figue" dataDxfId="22"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="21"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:O14" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
-  <autoFilter ref="A3:O14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:P14" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
+  <autoFilter ref="A3:P14"/>
   <sortState ref="A4:O83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Id" dataDxfId="14"/>
-    <tableColumn id="2" name="Name" dataDxfId="13"/>
-    <tableColumn id="3" name="Type" dataDxfId="12"/>
-    <tableColumn id="6" name="World" dataDxfId="11"/>
-    <tableColumn id="7" name="Deck" dataDxfId="10"/>
-    <tableColumn id="10" name="Job" dataDxfId="9"/>
-    <tableColumn id="11" name="Level" dataDxfId="8"/>
-    <tableColumn id="12" name="Reward" dataDxfId="7"/>
-    <tableColumn id="13" name="Method" dataDxfId="6"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="5"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="4"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="3"/>
-    <tableColumn id="9" name="Figue" dataDxfId="2"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="1"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="0"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Id" dataDxfId="16"/>
+    <tableColumn id="2" name="Name" dataDxfId="15"/>
+    <tableColumn id="3" name="Type" dataDxfId="14"/>
+    <tableColumn id="6" name="World" dataDxfId="13"/>
+    <tableColumn id="7" name="Deck" dataDxfId="12"/>
+    <tableColumn id="10" name="Job" dataDxfId="11"/>
+    <tableColumn id="11" name="Level" dataDxfId="10"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="1"/>
+    <tableColumn id="12" name="Reward" dataDxfId="9"/>
+    <tableColumn id="13" name="Method" dataDxfId="8"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="7"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="6"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="5"/>
+    <tableColumn id="9" name="Figue" dataDxfId="4"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="3"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2755,23 +2836,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2807,23 +2871,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3000,13 +3047,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3014,15 +3061,15 @@
     <col min="1" max="1" width="9.25" customWidth="1"/>
     <col min="3" max="3" width="5.25" customWidth="1"/>
     <col min="6" max="6" width="10.125" customWidth="1"/>
-    <col min="7" max="7" width="6.25" customWidth="1"/>
-    <col min="8" max="8" width="11.875" customWidth="1"/>
-    <col min="9" max="9" width="9.5" customWidth="1"/>
-    <col min="10" max="12" width="10.625" customWidth="1"/>
-    <col min="14" max="14" width="10.625" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.25" customWidth="1"/>
+    <col min="9" max="9" width="11.875" customWidth="1"/>
+    <col min="10" max="10" width="9.5" customWidth="1"/>
+    <col min="11" max="13" width="10.625" customWidth="1"/>
+    <col min="15" max="15" width="10.625" customWidth="1"/>
+    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>203</v>
       </c>
@@ -3045,31 +3092,34 @@
         <v>209</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>201</v>
       </c>
@@ -3092,31 +3142,34 @@
         <v>201</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>202</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>214</v>
       </c>
@@ -3139,31 +3192,34 @@
         <v>220</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43000001</v>
       </c>
@@ -3186,23 +3242,24 @@
         <v>1</v>
       </c>
       <c r="H4" s="4"/>
-      <c r="I4" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="4"/>
+      <c r="N4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O4" s="23"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P4" s="23"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43000002</v>
       </c>
@@ -3225,25 +3282,26 @@
         <v>2</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="4"/>
+      <c r="M5" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O5" s="23"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P5" s="23"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43000003</v>
       </c>
@@ -3266,23 +3324,24 @@
         <v>4</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="4"/>
+      <c r="N6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O6" s="23"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P6" s="23"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43000004</v>
       </c>
@@ -3305,23 +3364,24 @@
         <v>5</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="4"/>
+      <c r="N7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="O7" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O7" s="23"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P7" s="23"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43000005</v>
       </c>
@@ -3344,23 +3404,24 @@
         <v>7</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I8" s="4"/>
       <c r="J8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="4"/>
+      <c r="N8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O8" s="23"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P8" s="23"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43000006</v>
       </c>
@@ -3383,23 +3444,24 @@
         <v>11</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="4"/>
+      <c r="N9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="O9" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O9" s="23"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P9" s="23"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43000007</v>
       </c>
@@ -3422,23 +3484,24 @@
         <v>3</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="4"/>
+      <c r="N10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="O10" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O10" s="23"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P10" s="23"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43000008</v>
       </c>
@@ -3461,23 +3524,24 @@
         <v>13</v>
       </c>
       <c r="H11" s="4"/>
-      <c r="I11" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="4"/>
+      <c r="N11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O11" s="23"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P11" s="23"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43000009</v>
       </c>
@@ -3500,23 +3564,24 @@
         <v>13</v>
       </c>
       <c r="H12" s="4"/>
-      <c r="I12" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="4"/>
+      <c r="N12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="O12" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O12" s="23"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P12" s="23"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43000010</v>
       </c>
@@ -3539,23 +3604,24 @@
         <v>6</v>
       </c>
       <c r="H13" s="4"/>
-      <c r="I13" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="4"/>
+      <c r="N13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="O13" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O13" s="23"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P13" s="23"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43000011</v>
       </c>
@@ -3578,23 +3644,24 @@
         <v>5</v>
       </c>
       <c r="H14" s="4"/>
-      <c r="I14" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="4"/>
+      <c r="N14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="O14" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O14" s="23"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P14" s="23"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43000012</v>
       </c>
@@ -3617,23 +3684,24 @@
         <v>12</v>
       </c>
       <c r="H15" s="4"/>
-      <c r="I15" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="4"/>
+      <c r="N15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O15" s="23"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P15" s="23"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43000013</v>
       </c>
@@ -3656,23 +3724,24 @@
         <v>10</v>
       </c>
       <c r="H16" s="4"/>
-      <c r="I16" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="4"/>
+      <c r="N16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N16" s="4" t="s">
+      <c r="O16" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O16" s="23"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P16" s="23"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43000014</v>
       </c>
@@ -3695,23 +3764,24 @@
         <v>12</v>
       </c>
       <c r="H17" s="4"/>
-      <c r="I17" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="4" t="s">
+      <c r="M17" s="4"/>
+      <c r="N17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="O17" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O17" s="23"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P17" s="23"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43000015</v>
       </c>
@@ -3734,23 +3804,24 @@
         <v>12</v>
       </c>
       <c r="H18" s="4"/>
-      <c r="I18" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="4" t="s">
+      <c r="M18" s="4"/>
+      <c r="N18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N18" s="4" t="s">
+      <c r="O18" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O18" s="23"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P18" s="23"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43000016</v>
       </c>
@@ -3773,23 +3844,24 @@
         <v>1</v>
       </c>
       <c r="H19" s="4"/>
-      <c r="I19" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I19" s="4"/>
       <c r="J19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="4"/>
+      <c r="N19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N19" s="4" t="s">
+      <c r="O19" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O19" s="23"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P19" s="23"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43000017</v>
       </c>
@@ -3812,23 +3884,24 @@
         <v>1</v>
       </c>
       <c r="H20" s="4"/>
-      <c r="I20" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I20" s="4"/>
       <c r="J20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="4" t="s">
+      <c r="M20" s="4"/>
+      <c r="N20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N20" s="4" t="s">
+      <c r="O20" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O20" s="23"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P20" s="23"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43000018</v>
       </c>
@@ -3851,23 +3924,24 @@
         <v>9</v>
       </c>
       <c r="H21" s="4"/>
-      <c r="I21" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I21" s="4"/>
       <c r="J21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K21" s="4"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="4" t="s">
+      <c r="M21" s="4"/>
+      <c r="N21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N21" s="4" t="s">
+      <c r="O21" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O21" s="23"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P21" s="23"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43000019</v>
       </c>
@@ -3890,23 +3964,24 @@
         <v>15</v>
       </c>
       <c r="H22" s="4"/>
-      <c r="I22" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I22" s="4"/>
       <c r="J22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="4" t="s">
+      <c r="M22" s="4"/>
+      <c r="N22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="N22" s="4" t="s">
+      <c r="O22" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O22" s="23"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P22" s="23"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43000020</v>
       </c>
@@ -3929,23 +4004,24 @@
         <v>4</v>
       </c>
       <c r="H23" s="4"/>
-      <c r="I23" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I23" s="4"/>
       <c r="J23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K23" s="4"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="4" t="s">
+      <c r="M23" s="4"/>
+      <c r="N23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="O23" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O23" s="23"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P23" s="23"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43000021</v>
       </c>
@@ -3968,23 +4044,24 @@
         <v>15</v>
       </c>
       <c r="H24" s="4"/>
-      <c r="I24" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="4" t="s">
+      <c r="M24" s="4"/>
+      <c r="N24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="N24" s="4" t="s">
+      <c r="O24" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O24" s="23"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P24" s="23"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43000022</v>
       </c>
@@ -4007,23 +4084,24 @@
         <v>14</v>
       </c>
       <c r="H25" s="4"/>
-      <c r="I25" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K25" s="4"/>
       <c r="L25" s="4"/>
-      <c r="M25" s="4" t="s">
+      <c r="M25" s="4"/>
+      <c r="N25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="N25" s="4" t="s">
+      <c r="O25" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O25" s="23"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P25" s="23"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43000023</v>
       </c>
@@ -4046,23 +4124,24 @@
         <v>17</v>
       </c>
       <c r="H26" s="4"/>
-      <c r="I26" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="4" t="s">
+      <c r="M26" s="4"/>
+      <c r="N26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="N26" s="4" t="s">
+      <c r="O26" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O26" s="23"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P26" s="23"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43000024</v>
       </c>
@@ -4085,23 +4164,24 @@
         <v>34</v>
       </c>
       <c r="H27" s="4"/>
-      <c r="I27" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K27" s="4"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="4" t="s">
+      <c r="M27" s="4"/>
+      <c r="N27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="N27" s="4" t="s">
+      <c r="O27" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O27" s="23"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P27" s="23"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43000025</v>
       </c>
@@ -4124,23 +4204,24 @@
         <v>35</v>
       </c>
       <c r="H28" s="4"/>
-      <c r="I28" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K28" s="4"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="4" t="s">
+      <c r="M28" s="4"/>
+      <c r="N28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="N28" s="4" t="s">
+      <c r="O28" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O28" s="23"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P28" s="23"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43000026</v>
       </c>
@@ -4163,23 +4244,24 @@
         <v>35</v>
       </c>
       <c r="H29" s="4"/>
-      <c r="I29" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K29" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="4" t="s">
+      <c r="M29" s="4"/>
+      <c r="N29" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="N29" s="4" t="s">
+      <c r="O29" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O29" s="23"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P29" s="23"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43000027</v>
       </c>
@@ -4202,23 +4284,24 @@
         <v>5</v>
       </c>
       <c r="H30" s="4"/>
-      <c r="I30" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="4" t="s">
+      <c r="M30" s="4"/>
+      <c r="N30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="N30" s="4" t="s">
+      <c r="O30" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O30" s="23"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P30" s="23"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43000028</v>
       </c>
@@ -4241,23 +4324,24 @@
         <v>16</v>
       </c>
       <c r="H31" s="4"/>
-      <c r="I31" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I31" s="4"/>
       <c r="J31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="4" t="s">
+      <c r="M31" s="4"/>
+      <c r="N31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="N31" s="4" t="s">
+      <c r="O31" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O31" s="23"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P31" s="23"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43000029</v>
       </c>
@@ -4280,23 +4364,24 @@
         <v>19</v>
       </c>
       <c r="H32" s="4"/>
-      <c r="I32" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K32" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="4" t="s">
+      <c r="M32" s="4"/>
+      <c r="N32" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="N32" s="4" t="s">
+      <c r="O32" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O32" s="23"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P32" s="23"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43000030</v>
       </c>
@@ -4319,23 +4404,24 @@
         <v>16</v>
       </c>
       <c r="H33" s="4"/>
-      <c r="I33" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="4" t="s">
+      <c r="M33" s="4"/>
+      <c r="N33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="N33" s="4" t="s">
+      <c r="O33" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O33" s="23"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P33" s="23"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43000031</v>
       </c>
@@ -4358,23 +4444,24 @@
         <v>7</v>
       </c>
       <c r="H34" s="4"/>
-      <c r="I34" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I34" s="4"/>
       <c r="J34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K34" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-      <c r="M34" s="4" t="s">
+      <c r="M34" s="4"/>
+      <c r="N34" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N34" s="4" t="s">
+      <c r="O34" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O34" s="23"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P34" s="23"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43000032</v>
       </c>
@@ -4397,23 +4484,24 @@
         <v>18</v>
       </c>
       <c r="H35" s="4"/>
-      <c r="I35" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I35" s="4"/>
       <c r="J35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K35" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="M35" s="4" t="s">
+      <c r="M35" s="4"/>
+      <c r="N35" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="N35" s="4" t="s">
+      <c r="O35" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O35" s="23"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P35" s="23"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43000033</v>
       </c>
@@ -4436,23 +4524,24 @@
         <v>7</v>
       </c>
       <c r="H36" s="4"/>
-      <c r="I36" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="I36" s="4"/>
       <c r="J36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K36" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="K36" s="4"/>
       <c r="L36" s="4"/>
-      <c r="M36" s="4" t="s">
+      <c r="M36" s="4"/>
+      <c r="N36" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="N36" s="4" t="s">
+      <c r="O36" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O36" s="23"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P36" s="23"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43000101</v>
       </c>
@@ -4474,28 +4563,29 @@
       <c r="G37" s="4">
         <v>2</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="4"/>
+      <c r="I37" s="4">
         <v>2</v>
       </c>
-      <c r="I37" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K37" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="K37" s="4"/>
       <c r="L37" s="4"/>
-      <c r="M37" s="4" t="s">
+      <c r="M37" s="4"/>
+      <c r="N37" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="N37" s="4" t="s">
+      <c r="O37" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="O37" s="23">
+      <c r="P37" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43000102</v>
       </c>
@@ -4517,28 +4607,29 @@
       <c r="G38" s="4">
         <v>4</v>
       </c>
-      <c r="H38" s="4">
-        <v>3</v>
-      </c>
-      <c r="I38" s="4" t="s">
+      <c r="H38" s="4"/>
+      <c r="I38" s="4">
         <v>3</v>
       </c>
       <c r="J38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K38" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="K38" s="4"/>
       <c r="L38" s="4"/>
-      <c r="M38" s="4" t="s">
+      <c r="M38" s="4"/>
+      <c r="N38" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N38" s="4" t="s">
+      <c r="O38" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="O38" s="23">
+      <c r="P38" s="23">
         <v>22031004</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>43000103</v>
       </c>
@@ -4560,28 +4651,29 @@
       <c r="G39" s="4">
         <v>7</v>
       </c>
-      <c r="H39" s="4" t="s">
+      <c r="H39" s="4"/>
+      <c r="I39" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I39" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K39" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="K39" s="4"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="4" t="s">
+      <c r="M39" s="4"/>
+      <c r="N39" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="N39" s="4" t="s">
+      <c r="O39" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O39" s="23">
+      <c r="P39" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>43000104</v>
       </c>
@@ -4603,28 +4695,29 @@
       <c r="G40" s="4">
         <v>9</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="H40" s="4"/>
+      <c r="I40" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I40" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K40" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="4" t="s">
+      <c r="M40" s="4"/>
+      <c r="N40" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="N40" s="4" t="s">
+      <c r="O40" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O40" s="23">
+      <c r="P40" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>43000105</v>
       </c>
@@ -4646,28 +4739,29 @@
       <c r="G41" s="4">
         <v>12</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="H41" s="4"/>
+      <c r="I41" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="I41" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K41" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="K41" s="4"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="4" t="s">
+      <c r="M41" s="4"/>
+      <c r="N41" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="N41" s="4" t="s">
+      <c r="O41" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O41" s="23">
+      <c r="P41" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>43000106</v>
       </c>
@@ -4689,28 +4783,29 @@
       <c r="G42" s="4">
         <v>14</v>
       </c>
-      <c r="H42" s="4" t="s">
+      <c r="H42" s="4"/>
+      <c r="I42" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I42" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K42" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K42" s="4"/>
       <c r="L42" s="4"/>
-      <c r="M42" s="4" t="s">
+      <c r="M42" s="4"/>
+      <c r="N42" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="N42" s="4" t="s">
+      <c r="O42" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O42" s="23">
+      <c r="P42" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>43000107</v>
       </c>
@@ -4732,28 +4827,29 @@
       <c r="G43" s="4">
         <v>15</v>
       </c>
-      <c r="H43" s="4" t="s">
+      <c r="H43" s="4"/>
+      <c r="I43" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I43" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K43" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="K43" s="4"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="4" t="s">
+      <c r="M43" s="4"/>
+      <c r="N43" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="N43" s="4" t="s">
+      <c r="O43" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O43" s="23">
+      <c r="P43" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43000108</v>
       </c>
@@ -4775,28 +4871,29 @@
       <c r="G44" s="4">
         <v>18</v>
       </c>
-      <c r="H44" s="4" t="s">
+      <c r="H44" s="4"/>
+      <c r="I44" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I44" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J44" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K44" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="4" t="s">
+      <c r="M44" s="4"/>
+      <c r="N44" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="N44" s="4" t="s">
+      <c r="O44" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O44" s="23">
+      <c r="P44" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>43000109</v>
       </c>
@@ -4818,28 +4915,29 @@
       <c r="G45" s="4">
         <v>21</v>
       </c>
-      <c r="H45" s="4" t="s">
+      <c r="H45" s="4"/>
+      <c r="I45" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I45" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J45" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K45" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K45" s="4"/>
       <c r="L45" s="4"/>
-      <c r="M45" s="4" t="s">
+      <c r="M45" s="4"/>
+      <c r="N45" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="N45" s="4" t="s">
+      <c r="O45" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O45" s="23">
+      <c r="P45" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>43000110</v>
       </c>
@@ -4861,28 +4959,29 @@
       <c r="G46" s="4">
         <v>24</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="H46" s="4"/>
+      <c r="I46" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="I46" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J46" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K46" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="K46" s="4"/>
       <c r="L46" s="4"/>
-      <c r="M46" s="4" t="s">
+      <c r="M46" s="4"/>
+      <c r="N46" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="N46" s="4" t="s">
+      <c r="O46" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O46" s="23">
+      <c r="P46" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>43000201</v>
       </c>
@@ -4904,28 +5003,29 @@
       <c r="G47" s="4">
         <v>22</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="H47" s="4"/>
+      <c r="I47" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I47" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J47" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K47" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="K47" s="4"/>
       <c r="L47" s="4"/>
-      <c r="M47" s="4" t="s">
+      <c r="M47" s="4"/>
+      <c r="N47" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="N47" s="4" t="s">
+      <c r="O47" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O47" s="23">
+      <c r="P47" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>43000202</v>
       </c>
@@ -4947,28 +5047,29 @@
       <c r="G48" s="4">
         <v>17</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="H48" s="4"/>
+      <c r="I48" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="I48" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J48" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K48" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4" t="s">
+      <c r="M48" s="4"/>
+      <c r="N48" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="N48" s="4" t="s">
+      <c r="O48" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O48" s="23">
+      <c r="P48" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>43000203</v>
       </c>
@@ -4990,28 +5091,29 @@
       <c r="G49" s="4">
         <v>22</v>
       </c>
-      <c r="H49" s="4" t="s">
+      <c r="H49" s="4"/>
+      <c r="I49" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I49" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J49" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K49" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="K49" s="4"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="4" t="s">
+      <c r="M49" s="4"/>
+      <c r="N49" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="N49" s="4" t="s">
+      <c r="O49" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O49" s="23">
+      <c r="P49" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>43000301</v>
       </c>
@@ -5033,28 +5135,29 @@
       <c r="G50" s="4">
         <v>7</v>
       </c>
-      <c r="H50" s="4">
+      <c r="H50" s="4"/>
+      <c r="I50" s="4">
         <v>2</v>
       </c>
-      <c r="I50" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J50" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K50" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="K50" s="4"/>
       <c r="L50" s="4"/>
-      <c r="M50" s="4" t="s">
+      <c r="M50" s="4"/>
+      <c r="N50" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="N50" s="4" t="s">
+      <c r="O50" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O50" s="23">
+      <c r="P50" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>43000302</v>
       </c>
@@ -5076,28 +5179,29 @@
       <c r="G51" s="4">
         <v>9</v>
       </c>
-      <c r="H51" s="4">
-        <v>3</v>
-      </c>
-      <c r="I51" s="4" t="s">
+      <c r="H51" s="4"/>
+      <c r="I51" s="4">
         <v>3</v>
       </c>
       <c r="J51" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K51" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="K51" s="4"/>
       <c r="L51" s="4"/>
-      <c r="M51" s="4" t="s">
+      <c r="M51" s="4"/>
+      <c r="N51" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="N51" s="4" t="s">
+      <c r="O51" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O51" s="23">
+      <c r="P51" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>43000303</v>
       </c>
@@ -5119,28 +5223,29 @@
       <c r="G52" s="4">
         <v>5</v>
       </c>
-      <c r="H52" s="4">
+      <c r="H52" s="4"/>
+      <c r="I52" s="4">
         <v>2</v>
       </c>
-      <c r="I52" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J52" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K52" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="K52" s="4"/>
       <c r="L52" s="4"/>
-      <c r="M52" s="4" t="s">
+      <c r="M52" s="4"/>
+      <c r="N52" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="N52" s="4" t="s">
+      <c r="O52" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O52" s="23">
+      <c r="P52" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>43000304</v>
       </c>
@@ -5162,28 +5267,29 @@
       <c r="G53" s="4">
         <v>14</v>
       </c>
-      <c r="H53" s="4" t="s">
+      <c r="H53" s="4"/>
+      <c r="I53" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="I53" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J53" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K53" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="4" t="s">
+      <c r="M53" s="4"/>
+      <c r="N53" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="N53" s="4" t="s">
+      <c r="O53" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O53" s="23">
+      <c r="P53" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>43000305</v>
       </c>
@@ -5205,28 +5311,29 @@
       <c r="G54" s="4">
         <v>14</v>
       </c>
-      <c r="H54" s="4" t="s">
+      <c r="H54" s="4"/>
+      <c r="I54" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="I54" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J54" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K54" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="K54" s="4"/>
       <c r="L54" s="4"/>
-      <c r="M54" s="4" t="s">
+      <c r="M54" s="4"/>
+      <c r="N54" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="N54" s="4" t="s">
+      <c r="O54" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O54" s="23">
+      <c r="P54" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>43000306</v>
       </c>
@@ -5248,28 +5355,29 @@
       <c r="G55" s="4">
         <v>1</v>
       </c>
-      <c r="H55" s="4">
+      <c r="H55" s="4"/>
+      <c r="I55" s="4">
         <v>6</v>
       </c>
-      <c r="I55" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J55" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K55" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="K55" s="4"/>
       <c r="L55" s="4"/>
-      <c r="M55" s="4" t="s">
+      <c r="M55" s="4"/>
+      <c r="N55" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="N55" s="4" t="s">
+      <c r="O55" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O55" s="23">
+      <c r="P55" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>43000307</v>
       </c>
@@ -5291,28 +5399,29 @@
       <c r="G56" s="4">
         <v>10</v>
       </c>
-      <c r="H56" s="4" t="s">
+      <c r="H56" s="4"/>
+      <c r="I56" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="I56" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J56" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K56" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="K56" s="4"/>
       <c r="L56" s="4"/>
-      <c r="M56" s="4" t="s">
+      <c r="M56" s="4"/>
+      <c r="N56" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="N56" s="4" t="s">
+      <c r="O56" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O56" s="23">
+      <c r="P56" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>43000308</v>
       </c>
@@ -5334,28 +5443,29 @@
       <c r="G57" s="4">
         <v>11</v>
       </c>
-      <c r="H57" s="4" t="s">
+      <c r="H57" s="4"/>
+      <c r="I57" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I57" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J57" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K57" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="K57" s="4"/>
       <c r="L57" s="4"/>
-      <c r="M57" s="4" t="s">
+      <c r="M57" s="4"/>
+      <c r="N57" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="N57" s="4" t="s">
+      <c r="O57" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O57" s="23">
+      <c r="P57" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>43000309</v>
       </c>
@@ -5377,28 +5487,29 @@
       <c r="G58" s="4">
         <v>13</v>
       </c>
-      <c r="H58" s="4" t="s">
+      <c r="H58" s="4"/>
+      <c r="I58" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="I58" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J58" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K58" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="K58" s="4"/>
       <c r="L58" s="4"/>
-      <c r="M58" s="4" t="s">
+      <c r="M58" s="4"/>
+      <c r="N58" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="N58" s="4" t="s">
+      <c r="O58" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O58" s="23">
+      <c r="P58" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>43000310</v>
       </c>
@@ -5420,28 +5531,29 @@
       <c r="G59" s="4">
         <v>8</v>
       </c>
-      <c r="H59" s="4">
+      <c r="H59" s="4"/>
+      <c r="I59" s="4">
         <v>2</v>
       </c>
-      <c r="I59" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J59" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K59" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="K59" s="4"/>
       <c r="L59" s="4"/>
-      <c r="M59" s="4" t="s">
+      <c r="M59" s="4"/>
+      <c r="N59" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="N59" s="4" t="s">
+      <c r="O59" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O59" s="23">
+      <c r="P59" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>43000311</v>
       </c>
@@ -5463,28 +5575,29 @@
       <c r="G60" s="4">
         <v>13</v>
       </c>
-      <c r="H60" s="4" t="s">
+      <c r="H60" s="4"/>
+      <c r="I60" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="I60" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J60" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K60" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="K60" s="4"/>
       <c r="L60" s="4"/>
-      <c r="M60" s="4" t="s">
+      <c r="M60" s="4"/>
+      <c r="N60" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="N60" s="4" t="s">
+      <c r="O60" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O60" s="23">
+      <c r="P60" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>43000312</v>
       </c>
@@ -5506,28 +5619,29 @@
       <c r="G61" s="4">
         <v>18</v>
       </c>
-      <c r="H61" s="4" t="s">
+      <c r="H61" s="4"/>
+      <c r="I61" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="I61" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J61" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K61" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K61" s="4"/>
       <c r="L61" s="4"/>
-      <c r="M61" s="4" t="s">
+      <c r="M61" s="4"/>
+      <c r="N61" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="N61" s="4" t="s">
+      <c r="O61" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O61" s="23">
+      <c r="P61" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>43000401</v>
       </c>
@@ -5549,28 +5663,29 @@
       <c r="G62" s="4">
         <v>10</v>
       </c>
-      <c r="H62" s="4">
+      <c r="H62" s="4"/>
+      <c r="I62" s="4">
         <v>6</v>
       </c>
-      <c r="I62" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K62" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="K62" s="4"/>
       <c r="L62" s="4"/>
-      <c r="M62" s="4" t="s">
+      <c r="M62" s="4"/>
+      <c r="N62" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="N62" s="4" t="s">
+      <c r="O62" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O62" s="23">
+      <c r="P62" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>43000402</v>
       </c>
@@ -5592,28 +5707,29 @@
       <c r="G63" s="4">
         <v>11</v>
       </c>
-      <c r="H63" s="4">
+      <c r="H63" s="4"/>
+      <c r="I63" s="4">
         <v>5</v>
       </c>
-      <c r="I63" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J63" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K63" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="K63" s="4"/>
       <c r="L63" s="4"/>
-      <c r="M63" s="4" t="s">
+      <c r="M63" s="4"/>
+      <c r="N63" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="N63" s="4" t="s">
+      <c r="O63" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O63" s="23">
+      <c r="P63" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>43000403</v>
       </c>
@@ -5635,28 +5751,29 @@
       <c r="G64" s="4">
         <v>13</v>
       </c>
-      <c r="H64" s="4" t="s">
+      <c r="H64" s="4"/>
+      <c r="I64" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="I64" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J64" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K64" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="K64" s="4"/>
       <c r="L64" s="4"/>
-      <c r="M64" s="4" t="s">
+      <c r="M64" s="4"/>
+      <c r="N64" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="N64" s="4" t="s">
+      <c r="O64" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O64" s="23">
+      <c r="P64" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>43000404</v>
       </c>
@@ -5678,28 +5795,29 @@
       <c r="G65" s="4">
         <v>14</v>
       </c>
-      <c r="H65" s="4" t="s">
+      <c r="H65" s="4"/>
+      <c r="I65" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I65" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J65" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K65" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="K65" s="4"/>
       <c r="L65" s="4"/>
-      <c r="M65" s="4" t="s">
+      <c r="M65" s="4"/>
+      <c r="N65" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="N65" s="4" t="s">
+      <c r="O65" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O65" s="23">
+      <c r="P65" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>43000405</v>
       </c>
@@ -5721,28 +5839,29 @@
       <c r="G66" s="4">
         <v>18</v>
       </c>
-      <c r="H66" s="4" t="s">
+      <c r="H66" s="4"/>
+      <c r="I66" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="I66" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J66" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K66" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="K66" s="4"/>
       <c r="L66" s="4"/>
-      <c r="M66" s="4" t="s">
+      <c r="M66" s="4"/>
+      <c r="N66" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="N66" s="4" t="s">
+      <c r="O66" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O66" s="23">
+      <c r="P66" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>43000406</v>
       </c>
@@ -5764,28 +5883,29 @@
       <c r="G67" s="4">
         <v>15</v>
       </c>
-      <c r="H67" s="4" t="s">
+      <c r="H67" s="4"/>
+      <c r="I67" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I67" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J67" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K67" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="K67" s="4"/>
       <c r="L67" s="4"/>
-      <c r="M67" s="4" t="s">
+      <c r="M67" s="4"/>
+      <c r="N67" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="N67" s="4" t="s">
+      <c r="O67" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O67" s="23">
+      <c r="P67" s="23">
         <v>22031003</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>43000407</v>
       </c>
@@ -5807,28 +5927,29 @@
       <c r="G68" s="4">
         <v>10</v>
       </c>
-      <c r="H68" s="4">
+      <c r="H68" s="4"/>
+      <c r="I68" s="4">
         <v>4</v>
       </c>
-      <c r="I68" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J68" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K68" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="K68" s="4"/>
       <c r="L68" s="4"/>
-      <c r="M68" s="4" t="s">
+      <c r="M68" s="4"/>
+      <c r="N68" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="N68" s="4" t="s">
+      <c r="O68" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O68" s="23">
+      <c r="P68" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>43000408</v>
       </c>
@@ -5850,28 +5971,29 @@
       <c r="G69" s="4">
         <v>7</v>
       </c>
-      <c r="H69" s="4">
+      <c r="H69" s="4"/>
+      <c r="I69" s="4">
         <v>5</v>
       </c>
-      <c r="I69" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J69" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K69" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="K69" s="4"/>
       <c r="L69" s="4"/>
-      <c r="M69" s="4" t="s">
+      <c r="M69" s="4"/>
+      <c r="N69" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="N69" s="4" t="s">
+      <c r="O69" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O69" s="23">
+      <c r="P69" s="23">
         <v>22031005</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>43000501</v>
       </c>
@@ -5893,28 +6015,29 @@
       <c r="G70" s="4">
         <v>15</v>
       </c>
-      <c r="H70" s="4" t="s">
+      <c r="H70" s="4"/>
+      <c r="I70" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="I70" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K70" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="K70" s="4"/>
       <c r="L70" s="4"/>
-      <c r="M70" s="4" t="s">
+      <c r="M70" s="4"/>
+      <c r="N70" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="N70" s="4" t="s">
+      <c r="O70" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O70" s="23">
+      <c r="P70" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>43000502</v>
       </c>
@@ -5936,28 +6059,29 @@
       <c r="G71" s="4">
         <v>13</v>
       </c>
-      <c r="H71" s="4" t="s">
+      <c r="H71" s="4"/>
+      <c r="I71" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I71" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K71" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="K71" s="4"/>
       <c r="L71" s="4"/>
-      <c r="M71" s="4" t="s">
+      <c r="M71" s="4"/>
+      <c r="N71" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="N71" s="4" t="s">
+      <c r="O71" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O71" s="23">
+      <c r="P71" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>43000503</v>
       </c>
@@ -5979,28 +6103,29 @@
       <c r="G72" s="4">
         <v>9</v>
       </c>
-      <c r="H72" s="4">
-        <v>3</v>
-      </c>
-      <c r="I72" s="4" t="s">
+      <c r="H72" s="4"/>
+      <c r="I72" s="4">
         <v>3</v>
       </c>
       <c r="J72" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K72" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="K72" s="4"/>
       <c r="L72" s="4"/>
-      <c r="M72" s="4" t="s">
+      <c r="M72" s="4"/>
+      <c r="N72" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="N72" s="4" t="s">
+      <c r="O72" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O72" s="23">
+      <c r="P72" s="23">
         <v>22031002</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>43000504</v>
       </c>
@@ -6022,24 +6147,25 @@
       <c r="G73" s="4">
         <v>19</v>
       </c>
-      <c r="H73" s="4" t="s">
+      <c r="H73" s="4"/>
+      <c r="I73" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="I73" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="J73" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K73" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="K73" s="4"/>
       <c r="L73" s="4"/>
-      <c r="M73" s="4" t="s">
+      <c r="M73" s="4"/>
+      <c r="N73" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="N73" s="4" t="s">
+      <c r="O73" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O73" s="23">
+      <c r="P73" s="23">
         <v>22031002</v>
       </c>
     </row>
@@ -6055,13 +6181,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6069,15 +6195,15 @@
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="3" max="3" width="5.125" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="6.125" customWidth="1"/>
-    <col min="8" max="8" width="11.875" customWidth="1"/>
-    <col min="9" max="9" width="9.5" customWidth="1"/>
-    <col min="10" max="12" width="10.625" customWidth="1"/>
-    <col min="14" max="14" width="10.625" customWidth="1"/>
-    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.125" customWidth="1"/>
+    <col min="9" max="9" width="11.875" customWidth="1"/>
+    <col min="10" max="10" width="9.5" customWidth="1"/>
+    <col min="11" max="13" width="10.625" customWidth="1"/>
+    <col min="15" max="15" width="10.625" customWidth="1"/>
+    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>203</v>
       </c>
@@ -6100,31 +6226,34 @@
         <v>209</v>
       </c>
       <c r="H1" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>201</v>
       </c>
@@ -6147,31 +6276,34 @@
         <v>201</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>202</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>202</v>
       </c>
       <c r="K2" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="P2" s="22" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>214</v>
       </c>
@@ -6194,31 +6326,34 @@
         <v>220</v>
       </c>
       <c r="H3" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="P3" s="20" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43010001</v>
       </c>
@@ -6240,26 +6375,29 @@
       <c r="G4" s="4">
         <v>1</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H4" s="4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="6"/>
+      <c r="N4" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="O4" s="19"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P4" s="19"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43010002</v>
       </c>
@@ -6281,24 +6419,27 @@
       <c r="G5" s="4">
         <v>5</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H5" s="4">
+        <v>4</v>
+      </c>
+      <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="L5" s="4"/>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="4"/>
+      <c r="N5" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="O5" s="19"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P5" s="19"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43010003</v>
       </c>
@@ -6320,24 +6461,27 @@
       <c r="G6" s="4">
         <v>10</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4" t="s">
-        <v>182</v>
-      </c>
+      <c r="H6" s="4">
+        <v>10</v>
+      </c>
+      <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="K6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="L6" s="4"/>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="4"/>
+      <c r="N6" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="O6" s="19"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P6" s="19"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43010004</v>
       </c>
@@ -6359,24 +6503,27 @@
       <c r="G7" s="4">
         <v>10</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4" t="s">
+      <c r="H7" s="4">
+        <v>10</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="4"/>
+      <c r="N7" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="O7" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="O7" s="19"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P7" s="19"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43010005</v>
       </c>
@@ -6398,26 +6545,29 @@
       <c r="G8" s="4">
         <v>1</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="6" t="s">
+      <c r="H8" s="4">
+        <v>2</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="K8" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="L8" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="4"/>
+      <c r="N8" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="O8" s="19"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P8" s="19"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43010006</v>
       </c>
@@ -6439,26 +6589,29 @@
       <c r="G9" s="4">
         <v>1</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="6" t="s">
+      <c r="H9" s="4">
+        <v>2</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="K9" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="L9" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="4"/>
+      <c r="N9" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="O9" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="O9" s="19"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P9" s="19"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43010101</v>
       </c>
@@ -6481,23 +6634,24 @@
         <v>5</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="4"/>
+      <c r="N10" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="O10" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="O10" s="19"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P10" s="19"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43010102</v>
       </c>
@@ -6520,23 +6674,24 @@
         <v>10</v>
       </c>
       <c r="H11" s="4"/>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="4"/>
+      <c r="J11" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="K11" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="4"/>
+      <c r="N11" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="O11" s="19"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P11" s="19"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43010103</v>
       </c>
@@ -6559,23 +6714,24 @@
         <v>5</v>
       </c>
       <c r="H12" s="4"/>
-      <c r="I12" s="4" t="s">
-        <v>195</v>
-      </c>
+      <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="K12" s="4"/>
+      <c r="K12" s="4" t="s">
+        <v>195</v>
+      </c>
       <c r="L12" s="4"/>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="4"/>
+      <c r="N12" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="O12" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="O12" s="19"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P12" s="19"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43010104</v>
       </c>
@@ -6598,23 +6754,24 @@
         <v>10</v>
       </c>
       <c r="H13" s="4"/>
-      <c r="I13" s="4" t="s">
-        <v>197</v>
-      </c>
+      <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="K13" s="4"/>
+      <c r="K13" s="4" t="s">
+        <v>197</v>
+      </c>
       <c r="L13" s="4"/>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="4"/>
+      <c r="N13" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="O13" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="O13" s="19"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P13" s="19"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43010105</v>
       </c>
@@ -6637,21 +6794,22 @@
         <v>25</v>
       </c>
       <c r="H14" s="4"/>
-      <c r="I14" s="4" t="s">
-        <v>200</v>
-      </c>
+      <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="K14" s="4"/>
+      <c r="K14" s="4" t="s">
+        <v>200</v>
+      </c>
       <c r="L14" s="4"/>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="4"/>
+      <c r="N14" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="O14" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
new battle map mini
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="275">
   <si>
     <t>老鼠</t>
   </si>
@@ -895,6 +895,10 @@
   </si>
   <si>
     <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mini</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -3050,10 +3054,10 @@
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4579,7 +4583,7 @@
         <v>71</v>
       </c>
       <c r="O37" s="4" t="s">
-        <v>238</v>
+        <v>274</v>
       </c>
       <c r="P37" s="23">
         <v>22031002</v>

</xml_diff>

<commit_message>
fix the people level bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,12 +15,12 @@
     <sheet name="People" sheetId="1" r:id="rId1"/>
     <sheet name="特殊" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="276">
   <si>
     <t>老鼠</t>
   </si>
@@ -899,13 +899,17 @@
   </si>
   <si>
     <t>51000002;4;-1;51000002;4;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>默认对战等级</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2697,74 +2701,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2833,14 +2769,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2908,6 +2844,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2943,6 +2896,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3125,7 +3095,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3161,7 +3131,7 @@
         <v>208</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>209</v>
+        <v>275</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>268</v>

</xml_diff>

<commit_message>
add 2 new scene quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="People" sheetId="1" r:id="rId1"/>
     <sheet name="特殊" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -898,18 +898,18 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51000002;4;-1;51000002;4;1</t>
+    <t>默认对战等级</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>默认对战等级</t>
+    <t>51000002;3;-1;51000002;3;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2769,7 +2769,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2844,23 +2844,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2896,23 +2879,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3095,7 +3061,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3131,7 +3097,7 @@
         <v>208</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>268</v>
@@ -3333,7 +3299,7 @@
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="6" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
add 2 youqiwang people
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="人物" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="279">
   <si>
     <t>老鼠</t>
   </si>
@@ -883,10 +883,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>mini</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>默认对战等级</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -908,6 +904,22 @@
   </si>
   <si>
     <t>土匪</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>chongyue</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>昆虫羽蛾</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhenqi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>真崎杏子</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -3206,10 +3218,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:P40" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A3:P40"/>
-  <sortState ref="A4:O50">
-    <sortCondition ref="A3:A50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:P42" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A3:P42"/>
+  <sortState ref="A4:O52">
+    <sortCondition ref="A3:A52"/>
   </sortState>
   <tableColumns count="16">
     <tableColumn id="1" name="Id" dataDxfId="15"/>
@@ -3610,13 +3622,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3652,7 +3664,7 @@
         <v>204</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>264</v>
@@ -3820,7 +3832,7 @@
         <v>67</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>269</v>
+        <v>234</v>
       </c>
       <c r="P4" s="23">
         <v>22031002</v>
@@ -3908,7 +3920,7 @@
         <v>74</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P6" s="23">
         <v>22031002</v>
@@ -3952,7 +3964,7 @@
         <v>77</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P7" s="23">
         <v>22031002</v>
@@ -3996,7 +4008,7 @@
         <v>81</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P8" s="23">
         <v>22031002</v>
@@ -4040,7 +4052,7 @@
         <v>85</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P9" s="23">
         <v>22031002</v>
@@ -4084,7 +4096,7 @@
         <v>88</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P10" s="23">
         <v>22031002</v>
@@ -4128,7 +4140,7 @@
         <v>92</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P11" s="23">
         <v>22031002</v>
@@ -4172,7 +4184,7 @@
         <v>96</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P12" s="23">
         <v>22031002</v>
@@ -4216,7 +4228,7 @@
         <v>100</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P13" s="23">
         <v>22031002</v>
@@ -4260,7 +4272,7 @@
         <v>104</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P14" s="23">
         <v>22031002</v>
@@ -4304,7 +4316,7 @@
         <v>107</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P15" s="23">
         <v>22031002</v>
@@ -4348,7 +4360,7 @@
         <v>110</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P16" s="23">
         <v>22031002</v>
@@ -4356,43 +4368,41 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>43020301</v>
+        <v>43020204</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>111</v>
+        <v>276</v>
       </c>
       <c r="C17" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F17">
-        <v>11000002</v>
+        <v>11000005</v>
       </c>
       <c r="G17" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H17" s="4"/>
-      <c r="I17" s="4">
-        <v>2</v>
-      </c>
+      <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>114</v>
+        <v>275</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4" t="s">
-        <v>114</v>
+        <v>275</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P17" s="23">
         <v>22031002</v>
@@ -4400,16 +4410,16 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>43020302</v>
+        <v>43020205</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="C18" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>2</v>
@@ -4418,25 +4428,23 @@
         <v>11000008</v>
       </c>
       <c r="G18" s="4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H18" s="4"/>
-      <c r="I18" s="4">
-        <v>3</v>
-      </c>
+      <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>117</v>
+        <v>277</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4" t="s">
-        <v>117</v>
+        <v>277</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P18" s="23">
         <v>22031002</v>
@@ -4444,25 +4452,25 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>43020303</v>
+        <v>43020301</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C19" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>11000004</v>
+        <v>11000002</v>
       </c>
       <c r="G19" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4">
@@ -4472,15 +4480,15 @@
         <v>3</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P19" s="23">
         <v>22031002</v>
@@ -4488,43 +4496,43 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>43020304</v>
+        <v>43020302</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C20" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>122</v>
+        <v>2</v>
       </c>
       <c r="F20">
-        <v>11000002</v>
+        <v>11000008</v>
       </c>
       <c r="G20" s="4">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H20" s="4"/>
-      <c r="I20" s="4" t="s">
-        <v>123</v>
+      <c r="I20" s="4">
+        <v>3</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P20" s="23">
         <v>22031002</v>
@@ -4532,10 +4540,10 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>43020305</v>
+        <v>43020303</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C21" s="4">
         <v>4</v>
@@ -4544,31 +4552,31 @@
         <v>119</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>241</v>
+        <v>69</v>
       </c>
       <c r="F21">
-        <v>11000005</v>
+        <v>11000004</v>
       </c>
       <c r="G21" s="4">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H21" s="4"/>
-      <c r="I21" s="4" t="s">
-        <v>106</v>
+      <c r="I21" s="4">
+        <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P21" s="23">
         <v>22031002</v>
@@ -4576,43 +4584,43 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>43020306</v>
+        <v>43020304</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C22" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>2</v>
+        <v>122</v>
       </c>
       <c r="F22">
-        <v>11000008</v>
+        <v>11000002</v>
       </c>
       <c r="G22" s="4">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="H22" s="4"/>
-      <c r="I22" s="4">
-        <v>6</v>
+      <c r="I22" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P22" s="23">
         <v>22031002</v>
@@ -4620,10 +4628,10 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>43020307</v>
+        <v>43020305</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C23" s="4">
         <v>4</v>
@@ -4632,31 +4640,31 @@
         <v>119</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>2</v>
+        <v>241</v>
       </c>
       <c r="F23">
-        <v>11000001</v>
+        <v>11000005</v>
       </c>
       <c r="G23" s="4">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P23" s="23">
         <v>22031002</v>
@@ -4664,43 +4672,43 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>43020308</v>
+        <v>43020306</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C24" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="F24">
-        <v>11000001</v>
+        <v>11000008</v>
       </c>
       <c r="G24" s="4">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="H24" s="4"/>
-      <c r="I24" s="4" t="s">
-        <v>73</v>
+      <c r="I24" s="4">
+        <v>6</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P24" s="23">
         <v>22031002</v>
@@ -4708,10 +4716,10 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>43020309</v>
+        <v>43020307</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C25" s="4">
         <v>4</v>
@@ -4720,31 +4728,31 @@
         <v>119</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>113</v>
+        <v>2</v>
       </c>
       <c r="F25">
-        <v>11000004</v>
+        <v>11000001</v>
       </c>
       <c r="G25" s="4">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P25" s="23">
         <v>22031002</v>
@@ -4752,10 +4760,10 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>43020310</v>
+        <v>43020308</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C26" s="4">
         <v>4</v>
@@ -4764,31 +4772,31 @@
         <v>119</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="F26">
-        <v>11000003</v>
+        <v>11000001</v>
       </c>
       <c r="G26" s="4">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H26" s="4"/>
-      <c r="I26" s="4">
-        <v>2</v>
+      <c r="I26" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P26" s="23">
         <v>22031002</v>
@@ -4796,10 +4804,10 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>43020311</v>
+        <v>43020309</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C27" s="4">
         <v>4</v>
@@ -4808,31 +4816,31 @@
         <v>119</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>242</v>
+        <v>113</v>
       </c>
       <c r="F27">
-        <v>11000005</v>
+        <v>11000004</v>
       </c>
       <c r="G27" s="4">
         <v>13</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P27" s="23">
         <v>22031002</v>
@@ -4840,10 +4848,10 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>43020312</v>
+        <v>43020310</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C28" s="4">
         <v>4</v>
@@ -4852,31 +4860,31 @@
         <v>119</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>239</v>
+        <v>2</v>
       </c>
       <c r="F28">
-        <v>11000001</v>
+        <v>11000003</v>
       </c>
       <c r="G28" s="4">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H28" s="4"/>
-      <c r="I28" s="4" t="s">
-        <v>141</v>
+      <c r="I28" s="4">
+        <v>2</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P28" s="23">
         <v>22031002</v>
@@ -4884,43 +4892,43 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>43020401</v>
+        <v>43020311</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C29" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>113</v>
+        <v>242</v>
       </c>
       <c r="F29">
-        <v>11000002</v>
+        <v>11000005</v>
       </c>
       <c r="G29" s="4">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H29" s="4"/>
-      <c r="I29" s="4">
-        <v>6</v>
+      <c r="I29" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P29" s="23">
         <v>22031002</v>
@@ -4928,43 +4936,43 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>43020402</v>
+        <v>43020312</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C30" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>94</v>
+        <v>239</v>
       </c>
       <c r="F30">
         <v>11000001</v>
       </c>
       <c r="G30" s="4">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="H30" s="4"/>
-      <c r="I30" s="4">
-        <v>5</v>
+      <c r="I30" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P30" s="23">
         <v>22031002</v>
@@ -4972,10 +4980,10 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>43020403</v>
+        <v>43020401</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C31" s="4">
         <v>5</v>
@@ -4984,31 +4992,31 @@
         <v>144</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>2</v>
+        <v>113</v>
       </c>
       <c r="F31">
         <v>11000002</v>
       </c>
       <c r="G31" s="4">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H31" s="4"/>
-      <c r="I31" s="4" t="s">
-        <v>149</v>
+      <c r="I31" s="4">
+        <v>6</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P31" s="23">
         <v>22031002</v>
@@ -5016,10 +5024,10 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>43020404</v>
+        <v>43020402</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C32" s="4">
         <v>5</v>
@@ -5028,31 +5036,31 @@
         <v>144</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="F32">
         <v>11000001</v>
       </c>
       <c r="G32" s="4">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H32" s="4"/>
-      <c r="I32" s="4" t="s">
-        <v>109</v>
+      <c r="I32" s="4">
+        <v>5</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P32" s="23">
         <v>22031002</v>
@@ -5060,10 +5068,10 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>43020405</v>
+        <v>43020403</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C33" s="4">
         <v>5</v>
@@ -5072,31 +5080,31 @@
         <v>144</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>116</v>
+        <v>2</v>
       </c>
       <c r="F33">
-        <v>11000007</v>
+        <v>11000002</v>
       </c>
       <c r="G33" s="4">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P33" s="23">
         <v>22031002</v>
@@ -5104,10 +5112,10 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>43020406</v>
+        <v>43020404</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C34" s="4">
         <v>5</v>
@@ -5116,42 +5124,42 @@
         <v>144</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F34">
-        <v>11000006</v>
+        <v>11000001</v>
       </c>
       <c r="G34" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="O34" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P34" s="23">
-        <v>22031003</v>
+        <v>22031002</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>43020407</v>
+        <v>43020405</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C35" s="4">
         <v>5</v>
@@ -5160,31 +5168,31 @@
         <v>144</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>2</v>
+        <v>116</v>
       </c>
       <c r="F35">
-        <v>11000004</v>
+        <v>11000007</v>
       </c>
       <c r="G35" s="4">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H35" s="4"/>
-      <c r="I35" s="4">
-        <v>4</v>
+      <c r="I35" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="O35" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P35" s="23">
         <v>22031002</v>
@@ -5192,10 +5200,10 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>43020408</v>
+        <v>43020406</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C36" s="4">
         <v>5</v>
@@ -5204,75 +5212,75 @@
         <v>144</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F36">
-        <v>11000002</v>
+        <v>11000006</v>
       </c>
       <c r="G36" s="4">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H36" s="4"/>
-      <c r="I36" s="4">
-        <v>5</v>
+      <c r="I36" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="O36" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P36" s="23">
-        <v>22031005</v>
+        <v>22031003</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>43020501</v>
+        <v>43020407</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C37" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>116</v>
+        <v>2</v>
       </c>
       <c r="F37">
-        <v>11000003</v>
+        <v>11000004</v>
       </c>
       <c r="G37" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H37" s="4"/>
-      <c r="I37" s="4" t="s">
-        <v>163</v>
+      <c r="I37" s="4">
+        <v>4</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="O37" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P37" s="23">
         <v>22031002</v>
@@ -5280,54 +5288,54 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>43020502</v>
+        <v>43020408</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C38" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="F38">
         <v>11000002</v>
       </c>
       <c r="G38" s="4">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H38" s="4"/>
-      <c r="I38" s="4" t="s">
-        <v>73</v>
+      <c r="I38" s="4">
+        <v>5</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="O38" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P38" s="23">
-        <v>22031002</v>
+        <v>22031005</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>43020503</v>
+        <v>43020501</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C39" s="4">
         <v>6</v>
@@ -5336,31 +5344,31 @@
         <v>162</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="F39">
-        <v>11000008</v>
+        <v>11000003</v>
       </c>
       <c r="G39" s="4">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H39" s="4"/>
-      <c r="I39" s="4">
-        <v>3</v>
+      <c r="I39" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="O39" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P39" s="23">
         <v>22031002</v>
@@ -5368,10 +5376,10 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>43020504</v>
+        <v>43020502</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C40" s="4">
         <v>6</v>
@@ -5383,30 +5391,118 @@
         <v>113</v>
       </c>
       <c r="F40">
-        <v>11000001</v>
+        <v>11000002</v>
       </c>
       <c r="G40" s="4">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="P40" s="23">
+        <v>22031002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>43020503</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" s="4">
+        <v>6</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F41">
+        <v>11000008</v>
+      </c>
+      <c r="G41" s="4">
+        <v>9</v>
+      </c>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4">
+        <v>3</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="P41" s="23">
+        <v>22031002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>43020504</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C42" s="4">
+        <v>6</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42">
+        <v>11000001</v>
+      </c>
+      <c r="G42" s="4">
+        <v>19</v>
+      </c>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K42" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="O40" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="P40" s="23">
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="P42" s="23">
         <v>22031002</v>
       </c>
     </row>
@@ -5424,11 +5520,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5464,7 +5560,7 @@
         <v>204</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>264</v>
@@ -5666,7 +5762,7 @@
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>6</v>
@@ -6201,7 +6297,7 @@
         <v>43000016</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C19" s="4">
         <v>0</v>
@@ -6224,12 +6320,12 @@
         <v>3</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O19" s="4" t="s">
         <v>233</v>
@@ -6241,7 +6337,7 @@
         <v>43000017</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C20" s="4">
         <v>0</v>
@@ -6264,12 +6360,12 @@
         <v>3</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O20" s="4" t="s">
         <v>233</v>

</xml_diff>

<commit_message>
close #96 people met system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="怪物" sheetId="1" r:id="rId2"/>
     <sheet name="特殊" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="286">
   <si>
     <t>老鼠</t>
   </si>
@@ -823,21 +823,111 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>特别怪物</t>
+  </si>
+  <si>
+    <t>特别怪物</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PetMon</t>
+  </si>
+  <si>
+    <t>PetMon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>int[]</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>特别怪物</t>
-  </si>
-  <si>
-    <t>特别怪物</t>
+    <t>RightMon</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>PetMon</t>
-  </si>
-  <si>
-    <t>PetMon</t>
+    <t>51019299;4;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51019298;4;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51000229;4;-1;51000229;4;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动开启等级</t>
+  </si>
+  <si>
+    <t>自动开启等级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AutoAddLevel</t>
+  </si>
+  <si>
+    <t>AutoAddLevel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>默认对战等级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51000002;3;-1;51000002;3;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>山贼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shanzei</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tufei</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>土匪</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>chongyue</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>昆虫羽蛾</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhenqi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>真崎杏子</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机出现</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>InRandomQuest</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -845,89 +935,27 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>RightMon</t>
+    <t>随机出现</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51019299;4;0</t>
+    <t>bool</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51019298;4;0</t>
+    <t>InRandomQuest</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51000229;4;-1;51000229;4;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>自动开启等级</t>
-  </si>
-  <si>
-    <t>自动开启等级</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>AutoAddLevel</t>
-  </si>
-  <si>
-    <t>AutoAddLevel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>默认对战等级</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>51000002;3;-1;51000002;3;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>山贼</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shanzei</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>tufei</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>土匪</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>chongyue</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>昆虫羽蛾</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>zhenqi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>真崎杏子</t>
+    <t>true</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="24" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1114,9 +1142,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1124,9 +1151,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1617,7 +1657,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1675,19 +1715,25 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1735,7 +1781,116 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="60">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2223,33 +2378,6 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -3218,91 +3346,94 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:P42" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A3:P42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:Q42" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+  <autoFilter ref="A3:Q42"/>
   <sortState ref="A4:O52">
     <sortCondition ref="A3:A52"/>
   </sortState>
-  <tableColumns count="16">
-    <tableColumn id="1" name="Id" dataDxfId="15"/>
-    <tableColumn id="2" name="Name" dataDxfId="14"/>
-    <tableColumn id="3" name="Type" dataDxfId="13"/>
-    <tableColumn id="6" name="World" dataDxfId="12"/>
-    <tableColumn id="7" name="Deck" dataDxfId="11"/>
-    <tableColumn id="10" name="Job" dataDxfId="10"/>
-    <tableColumn id="11" name="Level" dataDxfId="9"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="8"/>
-    <tableColumn id="12" name="Reward" dataDxfId="7"/>
-    <tableColumn id="13" name="Method" dataDxfId="6"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="5"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="4"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="3"/>
-    <tableColumn id="17" name="Figue" dataDxfId="2"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="1"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="0"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="Id" dataDxfId="19"/>
+    <tableColumn id="2" name="Name" dataDxfId="18"/>
+    <tableColumn id="3" name="Type" dataDxfId="17"/>
+    <tableColumn id="6" name="World" dataDxfId="16"/>
+    <tableColumn id="7" name="Deck" dataDxfId="15"/>
+    <tableColumn id="10" name="Job" dataDxfId="14"/>
+    <tableColumn id="11" name="Level" dataDxfId="13"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="12"/>
+    <tableColumn id="12" name="Reward" dataDxfId="11"/>
+    <tableColumn id="13" name="Method" dataDxfId="10"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="9"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="8"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="7"/>
+    <tableColumn id="17" name="Figue" dataDxfId="6"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="5"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="4"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:P36" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
-  <autoFilter ref="A3:P36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Q36" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
+  <autoFilter ref="A3:Q36"/>
   <sortState ref="A4:O44">
     <sortCondition ref="A3:A44"/>
   </sortState>
-  <tableColumns count="16">
-    <tableColumn id="1" name="Id" dataDxfId="53"/>
-    <tableColumn id="2" name="Name" dataDxfId="52"/>
-    <tableColumn id="3" name="Type" dataDxfId="51"/>
-    <tableColumn id="6" name="World" dataDxfId="50"/>
-    <tableColumn id="7" name="Deck" dataDxfId="49"/>
-    <tableColumn id="10" name="Job" dataDxfId="48"/>
-    <tableColumn id="11" name="Level" dataDxfId="47"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="46"/>
-    <tableColumn id="12" name="Reward" dataDxfId="45"/>
-    <tableColumn id="13" name="Method" dataDxfId="44"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="43"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="42"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="41"/>
-    <tableColumn id="17" name="Figue" dataDxfId="40"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="39"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="38"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="Id" dataDxfId="56"/>
+    <tableColumn id="2" name="Name" dataDxfId="55"/>
+    <tableColumn id="3" name="Type" dataDxfId="54"/>
+    <tableColumn id="6" name="World" dataDxfId="53"/>
+    <tableColumn id="7" name="Deck" dataDxfId="52"/>
+    <tableColumn id="10" name="Job" dataDxfId="51"/>
+    <tableColumn id="11" name="Level" dataDxfId="50"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="49"/>
+    <tableColumn id="12" name="Reward" dataDxfId="48"/>
+    <tableColumn id="13" name="Method" dataDxfId="47"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="46"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="45"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="44"/>
+    <tableColumn id="17" name="Figue" dataDxfId="43"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="42"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="41"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:P14" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" tableBorderDxfId="35">
-  <autoFilter ref="A3:P14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:Q14" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
+  <autoFilter ref="A3:Q14"/>
   <sortState ref="A4:O83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="16">
-    <tableColumn id="1" name="Id" dataDxfId="34"/>
-    <tableColumn id="2" name="Name" dataDxfId="33"/>
-    <tableColumn id="3" name="Type" dataDxfId="32"/>
-    <tableColumn id="6" name="World" dataDxfId="31"/>
-    <tableColumn id="7" name="Deck" dataDxfId="30"/>
-    <tableColumn id="10" name="Job" dataDxfId="29"/>
-    <tableColumn id="11" name="Level" dataDxfId="28"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="27"/>
-    <tableColumn id="12" name="Reward" dataDxfId="26"/>
-    <tableColumn id="13" name="Method" dataDxfId="25"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="24"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="23"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="22"/>
-    <tableColumn id="9" name="Figue" dataDxfId="21"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="20"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="19"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="Id" dataDxfId="37"/>
+    <tableColumn id="2" name="Name" dataDxfId="36"/>
+    <tableColumn id="3" name="Type" dataDxfId="35"/>
+    <tableColumn id="6" name="World" dataDxfId="34"/>
+    <tableColumn id="7" name="Deck" dataDxfId="33"/>
+    <tableColumn id="10" name="Job" dataDxfId="32"/>
+    <tableColumn id="11" name="Level" dataDxfId="31"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="30"/>
+    <tableColumn id="12" name="Reward" dataDxfId="29"/>
+    <tableColumn id="13" name="Method" dataDxfId="28"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="27"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="26"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="25"/>
+    <tableColumn id="9" name="Figue" dataDxfId="24"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="23"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="2"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3377,23 +3508,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3429,23 +3543,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3622,13 +3719,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3644,7 +3741,7 @@
     <col min="16" max="16" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>199</v>
       </c>
@@ -3664,10 +3761,10 @@
         <v>204</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>236</v>
@@ -3682,7 +3779,7 @@
         <v>243</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>209</v>
@@ -3693,8 +3790,11 @@
       <c r="P1" s="14" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q1" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>197</v>
       </c>
@@ -3743,8 +3843,11 @@
       <c r="P2" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q2" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>210</v>
       </c>
@@ -3767,7 +3870,7 @@
         <v>216</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>217</v>
@@ -3782,7 +3885,7 @@
         <v>245</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>220</v>
@@ -3793,8 +3896,11 @@
       <c r="P3" s="5" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q3" s="22" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43020101</v>
       </c>
@@ -3834,11 +3940,12 @@
       <c r="O4" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P4" s="23">
+      <c r="P4" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q4" s="25"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43020102</v>
       </c>
@@ -3878,11 +3985,14 @@
       <c r="O5" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P5" s="23">
+      <c r="P5" s="19">
         <v>22031004</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q5" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43020103</v>
       </c>
@@ -3922,11 +4032,14 @@
       <c r="O6" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P6" s="23">
+      <c r="P6" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q6" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43020104</v>
       </c>
@@ -3966,11 +4079,14 @@
       <c r="O7" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P7" s="23">
+      <c r="P7" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q7" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43020105</v>
       </c>
@@ -4010,11 +4126,14 @@
       <c r="O8" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P8" s="23">
+      <c r="P8" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q8" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43020106</v>
       </c>
@@ -4054,11 +4173,14 @@
       <c r="O9" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P9" s="23">
+      <c r="P9" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q9" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43020107</v>
       </c>
@@ -4098,11 +4220,14 @@
       <c r="O10" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P10" s="23">
+      <c r="P10" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q10" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43020108</v>
       </c>
@@ -4142,11 +4267,14 @@
       <c r="O11" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P11" s="23">
+      <c r="P11" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q11" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43020109</v>
       </c>
@@ -4186,11 +4314,14 @@
       <c r="O12" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P12" s="23">
+      <c r="P12" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q12" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43020110</v>
       </c>
@@ -4230,11 +4361,14 @@
       <c r="O13" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P13" s="23">
+      <c r="P13" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q13" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43020201</v>
       </c>
@@ -4274,11 +4408,14 @@
       <c r="O14" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P14" s="23">
+      <c r="P14" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q14" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43020202</v>
       </c>
@@ -4318,11 +4455,14 @@
       <c r="O15" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P15" s="23">
+      <c r="P15" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q15" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43020203</v>
       </c>
@@ -4362,16 +4502,19 @@
       <c r="O16" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P16" s="23">
+      <c r="P16" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q16" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43020204</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C17" s="4">
         <v>2</v>
@@ -4394,26 +4537,29 @@
         <v>3</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O17" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P17" s="23">
+      <c r="P17" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q17" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43020205</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C18" s="4">
         <v>2</v>
@@ -4436,21 +4582,24 @@
         <v>3</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="O18" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P18" s="23">
+      <c r="P18" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q18" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43020301</v>
       </c>
@@ -4490,11 +4639,14 @@
       <c r="O19" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P19" s="23">
+      <c r="P19" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q19" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43020302</v>
       </c>
@@ -4534,11 +4686,14 @@
       <c r="O20" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P20" s="23">
+      <c r="P20" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q20" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43020303</v>
       </c>
@@ -4578,11 +4733,14 @@
       <c r="O21" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P21" s="23">
+      <c r="P21" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q21" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43020304</v>
       </c>
@@ -4622,11 +4780,14 @@
       <c r="O22" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P22" s="23">
+      <c r="P22" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q22" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43020305</v>
       </c>
@@ -4666,11 +4827,14 @@
       <c r="O23" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P23" s="23">
+      <c r="P23" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q23" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43020306</v>
       </c>
@@ -4710,11 +4874,14 @@
       <c r="O24" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P24" s="23">
+      <c r="P24" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q24" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43020307</v>
       </c>
@@ -4754,11 +4921,14 @@
       <c r="O25" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P25" s="23">
+      <c r="P25" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q25" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43020308</v>
       </c>
@@ -4798,11 +4968,14 @@
       <c r="O26" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P26" s="23">
+      <c r="P26" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q26" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43020309</v>
       </c>
@@ -4842,11 +5015,14 @@
       <c r="O27" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P27" s="23">
+      <c r="P27" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q27" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43020310</v>
       </c>
@@ -4886,11 +5062,14 @@
       <c r="O28" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P28" s="23">
+      <c r="P28" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q28" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43020311</v>
       </c>
@@ -4930,11 +5109,14 @@
       <c r="O29" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P29" s="23">
+      <c r="P29" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q29" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43020312</v>
       </c>
@@ -4974,11 +5156,14 @@
       <c r="O30" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P30" s="23">
+      <c r="P30" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q30" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43020401</v>
       </c>
@@ -5018,11 +5203,14 @@
       <c r="O31" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P31" s="23">
+      <c r="P31" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q31" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43020402</v>
       </c>
@@ -5062,11 +5250,14 @@
       <c r="O32" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P32" s="23">
+      <c r="P32" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q32" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43020403</v>
       </c>
@@ -5106,11 +5297,14 @@
       <c r="O33" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P33" s="23">
+      <c r="P33" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q33" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43020404</v>
       </c>
@@ -5150,11 +5344,14 @@
       <c r="O34" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P34" s="23">
+      <c r="P34" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q34" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43020405</v>
       </c>
@@ -5194,11 +5391,14 @@
       <c r="O35" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P35" s="23">
+      <c r="P35" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q35" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43020406</v>
       </c>
@@ -5238,11 +5438,14 @@
       <c r="O36" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P36" s="23">
+      <c r="P36" s="19">
         <v>22031003</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q36" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43020407</v>
       </c>
@@ -5282,11 +5485,14 @@
       <c r="O37" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P37" s="23">
+      <c r="P37" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q37" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43020408</v>
       </c>
@@ -5326,11 +5532,14 @@
       <c r="O38" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P38" s="23">
+      <c r="P38" s="19">
         <v>22031005</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q38" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>43020501</v>
       </c>
@@ -5370,11 +5579,14 @@
       <c r="O39" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P39" s="23">
+      <c r="P39" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q39" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>43020502</v>
       </c>
@@ -5414,11 +5626,14 @@
       <c r="O40" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P40" s="23">
+      <c r="P40" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q40" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>43020503</v>
       </c>
@@ -5458,11 +5673,14 @@
       <c r="O41" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P41" s="23">
+      <c r="P41" s="19">
         <v>22031002</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q41" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>43020504</v>
       </c>
@@ -5502,8 +5720,11 @@
       <c r="O42" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="P42" s="23">
+      <c r="P42" s="19">
         <v>22031002</v>
+      </c>
+      <c r="Q42" s="25" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -5518,13 +5739,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G36" sqref="G36"/>
+      <selection pane="bottomRight" activeCell="Q3" sqref="Q1:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5540,7 +5761,7 @@
     <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>199</v>
       </c>
@@ -5560,10 +5781,10 @@
         <v>204</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>236</v>
@@ -5578,7 +5799,7 @@
         <v>243</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>209</v>
@@ -5589,8 +5810,11 @@
       <c r="P1" s="14" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q1" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>197</v>
       </c>
@@ -5613,7 +5837,7 @@
         <v>197</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>221</v>
@@ -5628,7 +5852,7 @@
         <v>244</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>198</v>
@@ -5639,8 +5863,11 @@
       <c r="P2" s="2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q2" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>210</v>
       </c>
@@ -5663,7 +5890,7 @@
         <v>216</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>217</v>
@@ -5678,7 +5905,7 @@
         <v>245</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>220</v>
@@ -5689,8 +5916,11 @@
       <c r="P3" s="5" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q3" s="22" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43000001</v>
       </c>
@@ -5728,9 +5958,10 @@
       <c r="O4" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P4" s="23"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P4" s="19"/>
+      <c r="Q4" s="23"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43000002</v>
       </c>
@@ -5762,7 +5993,7 @@
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>6</v>
@@ -5770,9 +6001,10 @@
       <c r="O5" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P5" s="23"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P5" s="19"/>
+      <c r="Q5" s="23"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43000003</v>
       </c>
@@ -5810,9 +6042,10 @@
       <c r="O6" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P6" s="23"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P6" s="19"/>
+      <c r="Q6" s="23"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43000004</v>
       </c>
@@ -5850,9 +6083,10 @@
       <c r="O7" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P7" s="23"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P7" s="19"/>
+      <c r="Q7" s="23"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43000005</v>
       </c>
@@ -5890,9 +6124,10 @@
       <c r="O8" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P8" s="23"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P8" s="19"/>
+      <c r="Q8" s="23"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43000006</v>
       </c>
@@ -5930,9 +6165,10 @@
       <c r="O9" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P9" s="23"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P9" s="19"/>
+      <c r="Q9" s="23"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43000007</v>
       </c>
@@ -5970,9 +6206,10 @@
       <c r="O10" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P10" s="23"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P10" s="19"/>
+      <c r="Q10" s="23"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43000008</v>
       </c>
@@ -6010,9 +6247,10 @@
       <c r="O11" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P11" s="23"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P11" s="19"/>
+      <c r="Q11" s="23"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43000009</v>
       </c>
@@ -6050,9 +6288,10 @@
       <c r="O12" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P12" s="23"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P12" s="19"/>
+      <c r="Q12" s="23"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43000010</v>
       </c>
@@ -6090,9 +6329,10 @@
       <c r="O13" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P13" s="23"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P13" s="19"/>
+      <c r="Q13" s="23"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43000011</v>
       </c>
@@ -6130,9 +6370,10 @@
       <c r="O14" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P14" s="23"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P14" s="19"/>
+      <c r="Q14" s="23"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43000012</v>
       </c>
@@ -6170,9 +6411,10 @@
       <c r="O15" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P15" s="23"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P15" s="19"/>
+      <c r="Q15" s="23"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43000013</v>
       </c>
@@ -6210,9 +6452,10 @@
       <c r="O16" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P16" s="23"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P16" s="19"/>
+      <c r="Q16" s="23"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43000014</v>
       </c>
@@ -6250,9 +6493,10 @@
       <c r="O17" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P17" s="23"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P17" s="19"/>
+      <c r="Q17" s="23"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43000015</v>
       </c>
@@ -6290,14 +6534,15 @@
       <c r="O18" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P18" s="23"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P18" s="19"/>
+      <c r="Q18" s="23"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43000016</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C19" s="4">
         <v>0</v>
@@ -6320,24 +6565,25 @@
         <v>3</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O19" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P19" s="23"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P19" s="19"/>
+      <c r="Q19" s="23"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43000017</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C20" s="4">
         <v>0</v>
@@ -6360,19 +6606,20 @@
         <v>3</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O20" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P20" s="23"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P20" s="19"/>
+      <c r="Q20" s="23"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43000018</v>
       </c>
@@ -6410,9 +6657,10 @@
       <c r="O21" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P21" s="23"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P21" s="19"/>
+      <c r="Q21" s="23"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43000019</v>
       </c>
@@ -6450,9 +6698,10 @@
       <c r="O22" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P22" s="23"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P22" s="19"/>
+      <c r="Q22" s="23"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43000020</v>
       </c>
@@ -6490,9 +6739,10 @@
       <c r="O23" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P23" s="23"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P23" s="19"/>
+      <c r="Q23" s="23"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43000021</v>
       </c>
@@ -6530,9 +6780,10 @@
       <c r="O24" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P24" s="23"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P24" s="19"/>
+      <c r="Q24" s="23"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43000022</v>
       </c>
@@ -6570,9 +6821,10 @@
       <c r="O25" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P25" s="23"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P25" s="19"/>
+      <c r="Q25" s="23"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43000023</v>
       </c>
@@ -6610,9 +6862,10 @@
       <c r="O26" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P26" s="23"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P26" s="19"/>
+      <c r="Q26" s="23"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43000024</v>
       </c>
@@ -6650,9 +6903,10 @@
       <c r="O27" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P27" s="23"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P27" s="19"/>
+      <c r="Q27" s="23"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43000025</v>
       </c>
@@ -6690,9 +6944,10 @@
       <c r="O28" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P28" s="23"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P28" s="19"/>
+      <c r="Q28" s="23"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43000026</v>
       </c>
@@ -6730,9 +6985,10 @@
       <c r="O29" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P29" s="23"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P29" s="19"/>
+      <c r="Q29" s="23"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43000027</v>
       </c>
@@ -6770,9 +7026,10 @@
       <c r="O30" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P30" s="23"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P30" s="19"/>
+      <c r="Q30" s="23"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43000028</v>
       </c>
@@ -6810,9 +7067,10 @@
       <c r="O31" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P31" s="23"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P31" s="19"/>
+      <c r="Q31" s="23"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43000029</v>
       </c>
@@ -6850,9 +7108,10 @@
       <c r="O32" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P32" s="23"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P32" s="19"/>
+      <c r="Q32" s="23"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43000030</v>
       </c>
@@ -6890,9 +7149,10 @@
       <c r="O33" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P33" s="23"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P33" s="19"/>
+      <c r="Q33" s="23"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43000031</v>
       </c>
@@ -6930,9 +7190,10 @@
       <c r="O34" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P34" s="23"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P34" s="19"/>
+      <c r="Q34" s="23"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43000032</v>
       </c>
@@ -6970,9 +7231,10 @@
       <c r="O35" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P35" s="23"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P35" s="19"/>
+      <c r="Q35" s="23"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43000033</v>
       </c>
@@ -7010,7 +7272,8 @@
       <c r="O36" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="P36" s="23"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -7024,13 +7287,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7046,7 +7309,7 @@
     <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>199</v>
       </c>
@@ -7069,7 +7332,7 @@
         <v>205</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>206</v>
@@ -7084,7 +7347,7 @@
         <v>246</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N1" s="17" t="s">
         <v>209</v>
@@ -7092,11 +7355,14 @@
       <c r="O1" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="16" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q1" s="16" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>197</v>
       </c>
@@ -7119,7 +7385,7 @@
         <v>197</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>221</v>
@@ -7134,7 +7400,7 @@
         <v>247</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>198</v>
@@ -7142,11 +7408,14 @@
       <c r="O2" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="P2" s="22" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P2" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>210</v>
       </c>
@@ -7169,7 +7438,7 @@
         <v>216</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>217</v>
@@ -7181,10 +7450,10 @@
         <v>219</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>220</v>
@@ -7192,11 +7461,14 @@
       <c r="O3" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="P3" s="20" t="s">
+      <c r="P3" s="10" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q3" s="24" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43010001</v>
       </c>
@@ -7229,7 +7501,7 @@
         <v>174</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" s="4" t="s">
@@ -7238,9 +7510,10 @@
       <c r="O4" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="P4" s="19"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P4" s="4"/>
+      <c r="Q4" s="21"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43010002</v>
       </c>
@@ -7280,9 +7553,10 @@
       <c r="O5" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="P5" s="19"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P5" s="4"/>
+      <c r="Q5" s="20"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43010003</v>
       </c>
@@ -7322,9 +7596,10 @@
       <c r="O6" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="P6" s="19"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P6" s="4"/>
+      <c r="Q6" s="20"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43010004</v>
       </c>
@@ -7364,9 +7639,10 @@
       <c r="O7" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="P7" s="19"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P7" s="4"/>
+      <c r="Q7" s="20"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43010005</v>
       </c>
@@ -7399,7 +7675,7 @@
         <v>228</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="6" t="s">
@@ -7408,9 +7684,10 @@
       <c r="O8" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="P8" s="19"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P8" s="4"/>
+      <c r="Q8" s="20"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43010006</v>
       </c>
@@ -7443,7 +7720,7 @@
         <v>223</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="6" t="s">
@@ -7452,9 +7729,10 @@
       <c r="O9" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="P9" s="19"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P9" s="4"/>
+      <c r="Q9" s="20"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43010101</v>
       </c>
@@ -7492,9 +7770,10 @@
       <c r="O10" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="P10" s="19"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P10" s="4"/>
+      <c r="Q10" s="20"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43010102</v>
       </c>
@@ -7532,9 +7811,10 @@
       <c r="O11" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="P11" s="19"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P11" s="4"/>
+      <c r="Q11" s="20"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43010103</v>
       </c>
@@ -7572,9 +7852,10 @@
       <c r="O12" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="P12" s="19"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P12" s="4"/>
+      <c r="Q12" s="20"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43010104</v>
       </c>
@@ -7612,9 +7893,10 @@
       <c r="O13" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="P13" s="19"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P13" s="4"/>
+      <c r="Q13" s="20"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43010105</v>
       </c>
@@ -7652,7 +7934,8 @@
       <c r="O14" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="P14" s="19"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
add new task saiba
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="286">
   <si>
     <t>老鼠</t>
   </si>
@@ -225,9 +225,6 @@
   </si>
   <si>
     <t>sainisi</t>
-  </si>
-  <si>
-    <t>塞巴斯恰恩</t>
   </si>
   <si>
     <t>atr2</t>
@@ -948,6 +945,10 @@
   </si>
   <si>
     <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>塞巴斯恰恩</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1153,6 +1154,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1160,6 +1162,7 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1167,6 +1170,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1798,7 +1802,6 @@
         <name val="宋体"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1836,548 +1839,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF4F81BD"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF4F81BD"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF4F81BD"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF4F81BD"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3277,6 +2738,33 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="4"/>
@@ -3332,6 +2820,522 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF4F81BD"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF4F81BD"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF4F81BD"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF4F81BD"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3346,39 +3350,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:Q42" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:Q42" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
   <autoFilter ref="A3:Q42"/>
   <sortState ref="A4:O52">
     <sortCondition ref="A3:A52"/>
-  </sortState>
-  <tableColumns count="17">
-    <tableColumn id="1" name="Id" dataDxfId="19"/>
-    <tableColumn id="2" name="Name" dataDxfId="18"/>
-    <tableColumn id="3" name="Type" dataDxfId="17"/>
-    <tableColumn id="6" name="World" dataDxfId="16"/>
-    <tableColumn id="7" name="Deck" dataDxfId="15"/>
-    <tableColumn id="10" name="Job" dataDxfId="14"/>
-    <tableColumn id="11" name="Level" dataDxfId="13"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="12"/>
-    <tableColumn id="12" name="Reward" dataDxfId="11"/>
-    <tableColumn id="13" name="Method" dataDxfId="10"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="9"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="8"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="7"/>
-    <tableColumn id="17" name="Figue" dataDxfId="6"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="5"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="4"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Q36" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
-  <autoFilter ref="A3:Q36"/>
-  <sortState ref="A4:O44">
-    <sortCondition ref="A3:A44"/>
   </sortState>
   <tableColumns count="17">
     <tableColumn id="1" name="Id" dataDxfId="56"/>
@@ -3397,36 +3372,65 @@
     <tableColumn id="17" name="Figue" dataDxfId="43"/>
     <tableColumn id="9" name="BattleMap" dataDxfId="42"/>
     <tableColumn id="8" name="DropItem" dataDxfId="41"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="3"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="40"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Q36" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
+  <autoFilter ref="A3:Q36"/>
+  <sortState ref="A4:O44">
+    <sortCondition ref="A3:A44"/>
+  </sortState>
+  <tableColumns count="17">
+    <tableColumn id="1" name="Id" dataDxfId="36"/>
+    <tableColumn id="2" name="Name" dataDxfId="35"/>
+    <tableColumn id="3" name="Type" dataDxfId="34"/>
+    <tableColumn id="6" name="World" dataDxfId="33"/>
+    <tableColumn id="7" name="Deck" dataDxfId="32"/>
+    <tableColumn id="10" name="Job" dataDxfId="31"/>
+    <tableColumn id="11" name="Level" dataDxfId="30"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="29"/>
+    <tableColumn id="12" name="Reward" dataDxfId="28"/>
+    <tableColumn id="13" name="Method" dataDxfId="27"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="26"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="25"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="24"/>
+    <tableColumn id="17" name="Figue" dataDxfId="23"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="22"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="21"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:Q14" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:Q14" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="A3:Q14"/>
   <sortState ref="A4:O83">
     <sortCondition ref="A3:A83"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" name="Id" dataDxfId="37"/>
-    <tableColumn id="2" name="Name" dataDxfId="36"/>
-    <tableColumn id="3" name="Type" dataDxfId="35"/>
-    <tableColumn id="6" name="World" dataDxfId="34"/>
-    <tableColumn id="7" name="Deck" dataDxfId="33"/>
-    <tableColumn id="10" name="Job" dataDxfId="32"/>
-    <tableColumn id="11" name="Level" dataDxfId="31"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="30"/>
-    <tableColumn id="12" name="Reward" dataDxfId="29"/>
-    <tableColumn id="13" name="Method" dataDxfId="28"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="27"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="26"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="25"/>
-    <tableColumn id="9" name="Figue" dataDxfId="24"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="23"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="2"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="1"/>
+    <tableColumn id="1" name="Id" dataDxfId="16"/>
+    <tableColumn id="2" name="Name" dataDxfId="15"/>
+    <tableColumn id="3" name="Type" dataDxfId="14"/>
+    <tableColumn id="6" name="World" dataDxfId="13"/>
+    <tableColumn id="7" name="Deck" dataDxfId="12"/>
+    <tableColumn id="10" name="Job" dataDxfId="11"/>
+    <tableColumn id="11" name="Level" dataDxfId="10"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="9"/>
+    <tableColumn id="12" name="Reward" dataDxfId="8"/>
+    <tableColumn id="13" name="Method" dataDxfId="7"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="6"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="5"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="4"/>
+    <tableColumn id="9" name="Figue" dataDxfId="3"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="2"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="1"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3725,7 +3729,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q5" sqref="Q5"/>
+      <selection pane="bottomRight" activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3743,161 +3747,161 @@
   <sheetData>
     <row r="1" spans="1:17" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>204</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I1" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="O1" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>238</v>
-      </c>
       <c r="P1" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Q1" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="C2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>198</v>
-      </c>
       <c r="O2" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>220</v>
-      </c>
       <c r="O3" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Q3" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.15">
@@ -3938,7 +3942,7 @@
         <v>67</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P4" s="19">
         <v>22031002</v>
@@ -3950,7 +3954,7 @@
         <v>43020102</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>68</v>
+        <v>285</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -3959,7 +3963,7 @@
         <v>66</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5">
         <v>11000003</v>
@@ -3975,29 +3979,27 @@
         <v>3</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P5" s="19">
         <v>22031004</v>
       </c>
-      <c r="Q5" s="25" t="s">
-        <v>285</v>
-      </c>
+      <c r="Q5" s="25"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43020103</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -4006,7 +4008,7 @@
         <v>66</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6">
         <v>11000002</v>
@@ -4016,27 +4018,27 @@
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P6" s="19">
         <v>22031002</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.15">
@@ -4044,7 +4046,7 @@
         <v>43020104</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -4053,7 +4055,7 @@
         <v>66</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F7">
         <v>11000008</v>
@@ -4063,27 +4065,27 @@
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P7" s="19">
         <v>22031002</v>
       </c>
       <c r="Q7" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.15">
@@ -4091,7 +4093,7 @@
         <v>43020105</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -4100,7 +4102,7 @@
         <v>66</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8">
         <v>11000007</v>
@@ -4110,27 +4112,27 @@
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P8" s="19">
         <v>22031002</v>
       </c>
       <c r="Q8" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.15">
@@ -4138,7 +4140,7 @@
         <v>43020106</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -4147,7 +4149,7 @@
         <v>66</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9">
         <v>11000005</v>
@@ -4157,27 +4159,27 @@
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P9" s="19">
         <v>22031002</v>
       </c>
       <c r="Q9" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.15">
@@ -4185,7 +4187,7 @@
         <v>43020107</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -4194,7 +4196,7 @@
         <v>66</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10">
         <v>11000007</v>
@@ -4204,27 +4206,27 @@
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P10" s="19">
         <v>22031002</v>
       </c>
       <c r="Q10" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.15">
@@ -4232,7 +4234,7 @@
         <v>43020108</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -4241,7 +4243,7 @@
         <v>66</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11">
         <v>11000005</v>
@@ -4251,27 +4253,27 @@
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P11" s="19">
         <v>22031002</v>
       </c>
       <c r="Q11" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.15">
@@ -4279,7 +4281,7 @@
         <v>43020109</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
@@ -4288,7 +4290,7 @@
         <v>66</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F12">
         <v>11000006</v>
@@ -4298,27 +4300,27 @@
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P12" s="19">
         <v>22031002</v>
       </c>
       <c r="Q12" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.15">
@@ -4326,7 +4328,7 @@
         <v>43020110</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
@@ -4335,7 +4337,7 @@
         <v>66</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F13">
         <v>11000006</v>
@@ -4345,27 +4347,27 @@
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P13" s="19">
         <v>22031002</v>
       </c>
       <c r="Q13" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.15">
@@ -4373,13 +4375,13 @@
         <v>43020201</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="4">
         <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>2</v>
@@ -4392,27 +4394,27 @@
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P14" s="19">
         <v>22031002</v>
       </c>
       <c r="Q14" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.15">
@@ -4420,13 +4422,13 @@
         <v>43020202</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C15" s="4">
         <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>2</v>
@@ -4439,27 +4441,27 @@
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P15" s="19">
         <v>22031002</v>
       </c>
       <c r="Q15" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.15">
@@ -4467,13 +4469,13 @@
         <v>43020203</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C16" s="4">
         <v>2</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>2</v>
@@ -4486,27 +4488,27 @@
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P16" s="19">
         <v>22031002</v>
       </c>
       <c r="Q16" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.15">
@@ -4514,13 +4516,13 @@
         <v>43020204</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C17" s="4">
         <v>2</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>2</v>
@@ -4537,21 +4539,21 @@
         <v>3</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P17" s="19">
         <v>22031002</v>
       </c>
       <c r="Q17" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.15">
@@ -4559,13 +4561,13 @@
         <v>43020205</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C18" s="4">
         <v>2</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>2</v>
@@ -4582,21 +4584,21 @@
         <v>3</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P18" s="19">
         <v>22031002</v>
       </c>
       <c r="Q18" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.15">
@@ -4604,13 +4606,13 @@
         <v>43020301</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="4">
+        <v>3</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="C19" s="4">
-        <v>3</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>2</v>
@@ -4629,21 +4631,21 @@
         <v>3</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P19" s="19">
         <v>22031002</v>
       </c>
       <c r="Q19" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.15">
@@ -4651,13 +4653,13 @@
         <v>43020302</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20" s="4">
         <v>3</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>2</v>
@@ -4676,21 +4678,21 @@
         <v>3</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P20" s="19">
         <v>22031002</v>
       </c>
       <c r="Q20" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.15">
@@ -4698,16 +4700,16 @@
         <v>43020303</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" s="4">
         <v>4</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F21">
         <v>11000004</v>
@@ -4723,21 +4725,21 @@
         <v>3</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P21" s="19">
         <v>22031002</v>
       </c>
       <c r="Q21" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.15">
@@ -4745,16 +4747,16 @@
         <v>43020304</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C22" s="4">
         <v>4</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F22">
         <v>11000002</v>
@@ -4764,27 +4766,27 @@
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P22" s="19">
         <v>22031002</v>
       </c>
       <c r="Q22" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.15">
@@ -4792,16 +4794,16 @@
         <v>43020305</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C23" s="4">
         <v>4</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F23">
         <v>11000005</v>
@@ -4811,27 +4813,27 @@
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P23" s="19">
         <v>22031002</v>
       </c>
       <c r="Q23" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.15">
@@ -4839,13 +4841,13 @@
         <v>43020306</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C24" s="4">
         <v>3</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>2</v>
@@ -4864,21 +4866,21 @@
         <v>3</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P24" s="19">
         <v>22031002</v>
       </c>
       <c r="Q24" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.15">
@@ -4886,13 +4888,13 @@
         <v>43020307</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C25" s="4">
         <v>4</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>2</v>
@@ -4905,27 +4907,27 @@
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P25" s="19">
         <v>22031002</v>
       </c>
       <c r="Q25" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.15">
@@ -4933,16 +4935,16 @@
         <v>43020308</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C26" s="4">
         <v>4</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F26">
         <v>11000001</v>
@@ -4952,27 +4954,27 @@
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P26" s="19">
         <v>22031002</v>
       </c>
       <c r="Q26" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.15">
@@ -4980,16 +4982,16 @@
         <v>43020309</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27" s="4">
         <v>4</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F27">
         <v>11000004</v>
@@ -4999,27 +5001,27 @@
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P27" s="19">
         <v>22031002</v>
       </c>
       <c r="Q27" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.15">
@@ -5027,13 +5029,13 @@
         <v>43020310</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C28" s="4">
         <v>4</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>2</v>
@@ -5052,21 +5054,21 @@
         <v>3</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P28" s="19">
         <v>22031002</v>
       </c>
       <c r="Q28" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.15">
@@ -5074,16 +5076,16 @@
         <v>43020311</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C29" s="4">
         <v>4</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F29">
         <v>11000005</v>
@@ -5093,27 +5095,27 @@
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P29" s="19">
         <v>22031002</v>
       </c>
       <c r="Q29" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.15">
@@ -5121,16 +5123,16 @@
         <v>43020312</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C30" s="4">
         <v>4</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F30">
         <v>11000001</v>
@@ -5140,27 +5142,27 @@
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>142</v>
       </c>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P30" s="19">
         <v>22031002</v>
       </c>
       <c r="Q30" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.15">
@@ -5168,16 +5170,16 @@
         <v>43020401</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C31" s="4">
         <v>5</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F31">
         <v>11000002</v>
@@ -5193,21 +5195,21 @@
         <v>3</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P31" s="19">
         <v>22031002</v>
       </c>
       <c r="Q31" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.15">
@@ -5215,16 +5217,16 @@
         <v>43020402</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C32" s="4">
         <v>5</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F32">
         <v>11000001</v>
@@ -5240,21 +5242,21 @@
         <v>3</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P32" s="19">
         <v>22031002</v>
       </c>
       <c r="Q32" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.15">
@@ -5262,13 +5264,13 @@
         <v>43020403</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C33" s="4">
         <v>5</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>2</v>
@@ -5281,27 +5283,27 @@
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K33" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P33" s="19">
         <v>22031002</v>
       </c>
       <c r="Q33" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.15">
@@ -5309,16 +5311,16 @@
         <v>43020404</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C34" s="4">
         <v>5</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F34">
         <v>11000001</v>
@@ -5328,27 +5330,27 @@
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O34" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P34" s="19">
         <v>22031002</v>
       </c>
       <c r="Q34" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.15">
@@ -5356,16 +5358,16 @@
         <v>43020405</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C35" s="4">
         <v>5</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F35">
         <v>11000007</v>
@@ -5375,27 +5377,27 @@
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O35" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P35" s="19">
         <v>22031002</v>
       </c>
       <c r="Q35" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.15">
@@ -5403,16 +5405,16 @@
         <v>43020406</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C36" s="4">
         <v>5</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F36">
         <v>11000006</v>
@@ -5422,27 +5424,27 @@
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O36" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P36" s="19">
         <v>22031003</v>
       </c>
       <c r="Q36" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.15">
@@ -5450,13 +5452,13 @@
         <v>43020407</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C37" s="4">
         <v>5</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>2</v>
@@ -5475,21 +5477,21 @@
         <v>3</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O37" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P37" s="19">
         <v>22031002</v>
       </c>
       <c r="Q37" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.15">
@@ -5497,16 +5499,16 @@
         <v>43020408</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C38" s="4">
         <v>5</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F38">
         <v>11000002</v>
@@ -5522,21 +5524,21 @@
         <v>3</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O38" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P38" s="19">
         <v>22031005</v>
       </c>
       <c r="Q38" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.15">
@@ -5544,16 +5546,16 @@
         <v>43020501</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C39" s="4">
         <v>6</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F39">
         <v>11000003</v>
@@ -5563,27 +5565,27 @@
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K39" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O39" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P39" s="19">
         <v>22031002</v>
       </c>
       <c r="Q39" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.15">
@@ -5591,16 +5593,16 @@
         <v>43020502</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C40" s="4">
         <v>6</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F40">
         <v>11000002</v>
@@ -5610,27 +5612,27 @@
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O40" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P40" s="19">
         <v>22031002</v>
       </c>
       <c r="Q40" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.15">
@@ -5638,16 +5640,16 @@
         <v>43020503</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C41" s="4">
         <v>6</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F41">
         <v>11000008</v>
@@ -5663,21 +5665,21 @@
         <v>3</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O41" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P41" s="19">
         <v>22031002</v>
       </c>
       <c r="Q41" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.15">
@@ -5685,16 +5687,16 @@
         <v>43020504</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C42" s="4">
         <v>6</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F42">
         <v>11000001</v>
@@ -5704,27 +5706,27 @@
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
       <c r="N42" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O42" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P42" s="19">
         <v>22031002</v>
       </c>
       <c r="Q42" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -5763,161 +5765,161 @@
   <sheetData>
     <row r="1" spans="1:17" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>204</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I1" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="O1" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>238</v>
-      </c>
       <c r="P1" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Q1" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="C2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>220</v>
-      </c>
       <c r="O3" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Q3" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.15">
@@ -5956,7 +5958,7 @@
         <v>4</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P4" s="19"/>
       <c r="Q4" s="23"/>
@@ -5993,13 +5995,13 @@
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P5" s="19"/>
       <c r="Q5" s="23"/>
@@ -6040,7 +6042,7 @@
         <v>8</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P6" s="19"/>
       <c r="Q6" s="23"/>
@@ -6081,7 +6083,7 @@
         <v>10</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P7" s="19"/>
       <c r="Q7" s="23"/>
@@ -6122,7 +6124,7 @@
         <v>12</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P8" s="19"/>
       <c r="Q8" s="23"/>
@@ -6163,7 +6165,7 @@
         <v>14</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P9" s="19"/>
       <c r="Q9" s="23"/>
@@ -6204,7 +6206,7 @@
         <v>16</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P10" s="19"/>
       <c r="Q10" s="23"/>
@@ -6245,7 +6247,7 @@
         <v>18</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P11" s="19"/>
       <c r="Q11" s="23"/>
@@ -6286,7 +6288,7 @@
         <v>20</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P12" s="19"/>
       <c r="Q12" s="23"/>
@@ -6327,7 +6329,7 @@
         <v>22</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P13" s="19"/>
       <c r="Q13" s="23"/>
@@ -6368,7 +6370,7 @@
         <v>24</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P14" s="19"/>
       <c r="Q14" s="23"/>
@@ -6409,7 +6411,7 @@
         <v>26</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P15" s="19"/>
       <c r="Q15" s="23"/>
@@ -6450,7 +6452,7 @@
         <v>28</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P16" s="19"/>
       <c r="Q16" s="23"/>
@@ -6491,7 +6493,7 @@
         <v>30</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P17" s="19"/>
       <c r="Q17" s="23"/>
@@ -6532,7 +6534,7 @@
         <v>32</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P18" s="19"/>
       <c r="Q18" s="23"/>
@@ -6542,7 +6544,7 @@
         <v>43000016</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C19" s="4">
         <v>0</v>
@@ -6565,15 +6567,15 @@
         <v>3</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P19" s="19"/>
       <c r="Q19" s="23"/>
@@ -6583,7 +6585,7 @@
         <v>43000017</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C20" s="4">
         <v>0</v>
@@ -6606,15 +6608,15 @@
         <v>3</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P20" s="19"/>
       <c r="Q20" s="23"/>
@@ -6655,7 +6657,7 @@
         <v>34</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P21" s="19"/>
       <c r="Q21" s="23"/>
@@ -6696,7 +6698,7 @@
         <v>36</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P22" s="19"/>
       <c r="Q22" s="23"/>
@@ -6737,7 +6739,7 @@
         <v>38</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P23" s="19"/>
       <c r="Q23" s="23"/>
@@ -6778,7 +6780,7 @@
         <v>40</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P24" s="19"/>
       <c r="Q24" s="23"/>
@@ -6819,7 +6821,7 @@
         <v>42</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P25" s="19"/>
       <c r="Q25" s="23"/>
@@ -6860,7 +6862,7 @@
         <v>44</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P26" s="19"/>
       <c r="Q26" s="23"/>
@@ -6901,7 +6903,7 @@
         <v>46</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P27" s="19"/>
       <c r="Q27" s="23"/>
@@ -6942,7 +6944,7 @@
         <v>48</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P28" s="19"/>
       <c r="Q28" s="23"/>
@@ -6983,7 +6985,7 @@
         <v>50</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P29" s="19"/>
       <c r="Q29" s="23"/>
@@ -7024,7 +7026,7 @@
         <v>52</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P30" s="19"/>
       <c r="Q30" s="23"/>
@@ -7065,7 +7067,7 @@
         <v>54</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P31" s="19"/>
       <c r="Q31" s="23"/>
@@ -7106,7 +7108,7 @@
         <v>56</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P32" s="19"/>
       <c r="Q32" s="23"/>
@@ -7147,7 +7149,7 @@
         <v>58</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P33" s="19"/>
       <c r="Q33" s="23"/>
@@ -7188,7 +7190,7 @@
         <v>60</v>
       </c>
       <c r="O34" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P34" s="19"/>
       <c r="Q34" s="23"/>
@@ -7229,7 +7231,7 @@
         <v>62</v>
       </c>
       <c r="O35" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P35" s="19"/>
       <c r="Q35" s="23"/>
@@ -7270,7 +7272,7 @@
         <v>64</v>
       </c>
       <c r="O36" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P36" s="19"/>
       <c r="Q36" s="23"/>
@@ -7311,161 +7313,161 @@
   <sheetData>
     <row r="1" spans="1:17" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="L1" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="N1" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="L1" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="N1" s="17" t="s">
-        <v>209</v>
-      </c>
       <c r="O1" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Q1" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>198</v>
-      </c>
       <c r="C2" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>198</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>198</v>
-      </c>
       <c r="L2" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="N3" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="L3" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>220</v>
-      </c>
       <c r="O3" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Q3" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.15">
@@ -7473,13 +7475,13 @@
         <v>43010001</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C4" s="4">
         <v>101</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>2</v>
@@ -7498,17 +7500,17 @@
         <v>3</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="21"/>
@@ -7518,13 +7520,13 @@
         <v>43010002</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C5" s="4">
         <v>101</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>2</v>
@@ -7548,10 +7550,10 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="20"/>
@@ -7561,13 +7563,13 @@
         <v>43010003</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C6" s="4">
         <v>101</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>2</v>
@@ -7583,18 +7585,18 @@
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="20"/>
@@ -7604,13 +7606,13 @@
         <v>43010004</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C7" s="4">
         <v>101</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>2</v>
@@ -7626,18 +7628,18 @@
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="20"/>
@@ -7647,13 +7649,13 @@
         <v>43010005</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C8" s="4">
         <v>101</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>2</v>
@@ -7669,20 +7671,20 @@
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="20"/>
@@ -7692,13 +7694,13 @@
         <v>43010006</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C9" s="4">
         <v>101</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>2</v>
@@ -7714,20 +7716,20 @@
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="20"/>
@@ -7737,13 +7739,13 @@
         <v>43010101</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C10" s="4">
         <v>102</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>2</v>
@@ -7757,18 +7759,18 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>184</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="20"/>
@@ -7778,13 +7780,13 @@
         <v>43010102</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C11" s="4">
         <v>102</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>2</v>
@@ -7798,18 +7800,18 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="20"/>
@@ -7819,13 +7821,13 @@
         <v>43010103</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C12" s="4">
         <v>102</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>2</v>
@@ -7839,18 +7841,18 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="20"/>
@@ -7860,13 +7862,13 @@
         <v>43010104</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C13" s="4">
         <v>102</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>2</v>
@@ -7880,18 +7882,18 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="20"/>
@@ -7901,13 +7903,13 @@
         <v>43010105</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C14" s="4">
         <v>102</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>2</v>
@@ -7921,18 +7923,18 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="20"/>

</xml_diff>

<commit_message>
add 1 scene quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="人物" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="295">
   <si>
     <t>老鼠</t>
   </si>
@@ -977,6 +977,14 @@
   </si>
   <si>
     <t>string[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛头人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>niutouren</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -3417,8 +3425,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Q38" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
-  <autoFilter ref="A3:Q38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Q39" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
+  <autoFilter ref="A3:Q39"/>
   <sortState ref="A4:O44">
     <sortCondition ref="A3:A44"/>
   </sortState>
@@ -5735,13 +5743,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomRight" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7355,6 +7363,47 @@
       <c r="P38" s="19"/>
       <c r="Q38" s="23"/>
     </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>43000036</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" s="18">
+        <v>11001003</v>
+      </c>
+      <c r="G39" s="4">
+        <v>9</v>
+      </c>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="O39" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="23"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7369,7 +7418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>

</xml_diff>

<commit_message>
new map file format, support no symetric monster layout
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="306">
   <si>
     <t>老鼠</t>
   </si>
@@ -681,9 +681,6 @@
   <si>
     <t>blank</t>
     <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>doublec</t>
   </si>
   <si>
     <t>oneline</t>
@@ -743,13 +740,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>特别怪物</t>
-  </si>
-  <si>
-    <t>特别怪物</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>PetMon</t>
   </si>
   <si>
@@ -765,18 +755,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51019299;4;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>51019298;4;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>51000229;4;-1;51000229;4;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>自动开启等级</t>
   </si>
   <si>
@@ -883,10 +861,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51000080;1;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>bat</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -895,10 +869,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51000002;3;-1;51000002;3;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>string[]</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1022,15 +992,53 @@
     <t>spcentaurs</t>
   </si>
   <si>
-    <t>51000021;4;-1;51000021;4;0;51000021;4;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>spcentaurs</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>centaurs</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>特别怪物（特殊出现）</t>
+  </si>
+  <si>
+    <t>特别怪物（特殊出现）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PetMon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mini</t>
+  </si>
+  <si>
+    <t>round</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51000229;6;3;51000229;6;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51019299;6;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51019298;6;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51000002;7;3;51000002;7;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51000080;9;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51000021;5;4;51000021;7;2;51000021;7;6</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1756,7 +1764,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1790,26 +1798,8 @@
     <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -1840,6 +1830,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1886,7 +1891,14 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="67">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3637,93 +3649,93 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:S42" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:S42" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65" tableBorderDxfId="64">
   <autoFilter ref="A3:S42"/>
   <sortState ref="A4:Q52">
     <sortCondition ref="A3:A52"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" name="Id" dataDxfId="62"/>
-    <tableColumn id="2" name="Name" dataDxfId="61"/>
-    <tableColumn id="18" name="Ename" dataDxfId="60"/>
-    <tableColumn id="3" name="Type" dataDxfId="59"/>
-    <tableColumn id="6" name="World" dataDxfId="58"/>
-    <tableColumn id="7" name="Deck" dataDxfId="57"/>
-    <tableColumn id="10" name="Job" dataDxfId="56"/>
-    <tableColumn id="11" name="Level" dataDxfId="55"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="54"/>
-    <tableColumn id="13" name="Method" dataDxfId="53"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="52"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="51"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="50"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="49"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="48"/>
-    <tableColumn id="17" name="Figue" dataDxfId="47"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="46"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="45"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="44"/>
+    <tableColumn id="1" name="Id" dataDxfId="63"/>
+    <tableColumn id="2" name="Name" dataDxfId="62"/>
+    <tableColumn id="18" name="Ename" dataDxfId="61"/>
+    <tableColumn id="3" name="Type" dataDxfId="60"/>
+    <tableColumn id="6" name="World" dataDxfId="59"/>
+    <tableColumn id="7" name="Deck" dataDxfId="58"/>
+    <tableColumn id="10" name="Job" dataDxfId="57"/>
+    <tableColumn id="11" name="Level" dataDxfId="56"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="55"/>
+    <tableColumn id="13" name="Method" dataDxfId="54"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="53"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="52"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="51"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="50"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="49"/>
+    <tableColumn id="17" name="Figue" dataDxfId="48"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="47"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="46"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:S40" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:S40" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42">
   <autoFilter ref="A3:S40"/>
   <sortState ref="A4:Q44">
     <sortCondition ref="A3:A44"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" name="Id" dataDxfId="40"/>
-    <tableColumn id="2" name="Name" dataDxfId="39"/>
-    <tableColumn id="18" name="Ename" dataDxfId="38"/>
-    <tableColumn id="3" name="Type" dataDxfId="37"/>
-    <tableColumn id="6" name="World" dataDxfId="36"/>
-    <tableColumn id="7" name="Deck" dataDxfId="35"/>
-    <tableColumn id="10" name="Job" dataDxfId="34"/>
-    <tableColumn id="11" name="Level" dataDxfId="33"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="32"/>
-    <tableColumn id="13" name="Method" dataDxfId="31"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="30"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="29"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="28"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="27"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="26"/>
-    <tableColumn id="17" name="Figue" dataDxfId="25"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="24"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="23"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="22"/>
+    <tableColumn id="1" name="Id" dataDxfId="41"/>
+    <tableColumn id="2" name="Name" dataDxfId="40"/>
+    <tableColumn id="18" name="Ename" dataDxfId="39"/>
+    <tableColumn id="3" name="Type" dataDxfId="38"/>
+    <tableColumn id="6" name="World" dataDxfId="37"/>
+    <tableColumn id="7" name="Deck" dataDxfId="36"/>
+    <tableColumn id="10" name="Job" dataDxfId="35"/>
+    <tableColumn id="11" name="Level" dataDxfId="34"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="33"/>
+    <tableColumn id="13" name="Method" dataDxfId="32"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="31"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="30"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="29"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="28"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="27"/>
+    <tableColumn id="17" name="Figue" dataDxfId="26"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="25"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="24"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:S14" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:S14" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="A3:S14"/>
   <sortState ref="A4:Q83">
     <sortCondition ref="A3:A83"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" name="Id" dataDxfId="18"/>
-    <tableColumn id="2" name="Name" dataDxfId="17"/>
-    <tableColumn id="18" name="Ename" dataDxfId="16"/>
-    <tableColumn id="3" name="Type" dataDxfId="15"/>
-    <tableColumn id="6" name="World" dataDxfId="14"/>
-    <tableColumn id="7" name="Deck" dataDxfId="13"/>
-    <tableColumn id="10" name="Job" dataDxfId="12"/>
-    <tableColumn id="11" name="Level" dataDxfId="11"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="10"/>
-    <tableColumn id="13" name="Method" dataDxfId="9"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="8"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="7"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="6"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="5"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="4"/>
-    <tableColumn id="9" name="Figue" dataDxfId="3"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="2"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="1"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="19"/>
+    <tableColumn id="2" name="Name" dataDxfId="18"/>
+    <tableColumn id="18" name="Ename" dataDxfId="17"/>
+    <tableColumn id="3" name="Type" dataDxfId="16"/>
+    <tableColumn id="6" name="World" dataDxfId="15"/>
+    <tableColumn id="7" name="Deck" dataDxfId="14"/>
+    <tableColumn id="10" name="Job" dataDxfId="13"/>
+    <tableColumn id="11" name="Level" dataDxfId="12"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="11"/>
+    <tableColumn id="13" name="Method" dataDxfId="10"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="9"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="8"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="7"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="6"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="5"/>
+    <tableColumn id="9" name="Figue" dataDxfId="4"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="3"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="2"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4053,10 +4065,10 @@
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4072,63 +4084,63 @@
     <col min="18" max="18" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:19" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="J1" s="14" t="s">
+      <c r="H1" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q1" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>252</v>
+      <c r="R1" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
@@ -4139,7 +4151,7 @@
         <v>179</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>178</v>
@@ -4166,10 +4178,10 @@
         <v>179</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>200</v>
@@ -4184,10 +4196,10 @@
         <v>179</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.15">
@@ -4198,7 +4210,7 @@
         <v>191</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>192</v>
@@ -4216,7 +4228,7 @@
         <v>196</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>197</v>
@@ -4225,16 +4237,16 @@
         <v>198</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>230</v>
+        <v>297</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>199</v>
@@ -4243,10 +4255,10 @@
         <v>210</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="S3" s="22" t="s">
-        <v>254</v>
+        <v>224</v>
+      </c>
+      <c r="S3" s="16" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
@@ -4257,7 +4269,7 @@
         <v>63</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -4289,20 +4301,20 @@
         <v>65</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="R4" s="19"/>
-      <c r="S4" s="25"/>
+        <v>212</v>
+      </c>
+      <c r="R4" s="13"/>
+      <c r="S4" s="19"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43020102</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -4334,10 +4346,10 @@
         <v>67</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="R5" s="19"/>
-      <c r="S5" s="25"/>
+        <v>212</v>
+      </c>
+      <c r="R5" s="13"/>
+      <c r="S5" s="19"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6">
@@ -4379,11 +4391,11 @@
         <v>70</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="R6" s="19"/>
-      <c r="S6" s="25" t="s">
-        <v>258</v>
+        <v>212</v>
+      </c>
+      <c r="R6" s="13"/>
+      <c r="S6" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.15">
@@ -4403,7 +4415,7 @@
         <v>64</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G7">
         <v>11000008</v>
@@ -4426,10 +4438,10 @@
         <v>72</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="R7" s="19"/>
-      <c r="S7" s="25"/>
+        <v>212</v>
+      </c>
+      <c r="R7" s="13"/>
+      <c r="S7" s="19"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8">
@@ -4461,7 +4473,7 @@
         <v>3</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -4471,11 +4483,11 @@
         <v>75</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="R8" s="19"/>
-      <c r="S8" s="25" t="s">
-        <v>258</v>
+        <v>212</v>
+      </c>
+      <c r="R8" s="13"/>
+      <c r="S8" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.15">
@@ -4518,11 +4530,11 @@
         <v>78</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="R9" s="19"/>
-      <c r="S9" s="25" t="s">
-        <v>258</v>
+        <v>212</v>
+      </c>
+      <c r="R9" s="13"/>
+      <c r="S9" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.15">
@@ -4565,11 +4577,11 @@
         <v>80</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="R10" s="19"/>
-      <c r="S10" s="25" t="s">
-        <v>258</v>
+        <v>212</v>
+      </c>
+      <c r="R10" s="13"/>
+      <c r="S10" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.15">
@@ -4612,11 +4624,11 @@
         <v>83</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="R11" s="19"/>
-      <c r="S11" s="25" t="s">
-        <v>258</v>
+        <v>212</v>
+      </c>
+      <c r="R11" s="13"/>
+      <c r="S11" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.15">
@@ -4659,11 +4671,11 @@
         <v>86</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="R12" s="19"/>
-      <c r="S12" s="25" t="s">
-        <v>258</v>
+        <v>212</v>
+      </c>
+      <c r="R12" s="13"/>
+      <c r="S12" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.15">
@@ -4706,11 +4718,11 @@
         <v>89</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="R13" s="19"/>
-      <c r="S13" s="25" t="s">
-        <v>258</v>
+        <v>212</v>
+      </c>
+      <c r="R13" s="13"/>
+      <c r="S13" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.15">
@@ -4755,9 +4767,9 @@
       <c r="Q14" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R14" s="19"/>
-      <c r="S14" s="25" t="s">
-        <v>258</v>
+      <c r="R14" s="13"/>
+      <c r="S14" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.15">
@@ -4802,9 +4814,9 @@
       <c r="Q15" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R15" s="19"/>
-      <c r="S15" s="25" t="s">
-        <v>258</v>
+      <c r="R15" s="13"/>
+      <c r="S15" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.15">
@@ -4849,9 +4861,9 @@
       <c r="Q16" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R16" s="19"/>
-      <c r="S16" s="25" t="s">
-        <v>258</v>
+      <c r="R16" s="13"/>
+      <c r="S16" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.15">
@@ -4859,10 +4871,10 @@
         <v>43020204</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D17" s="4">
         <v>2</v>
@@ -4884,21 +4896,21 @@
         <v>3</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="Q17" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R17" s="19"/>
-      <c r="S17" s="25" t="s">
-        <v>258</v>
+      <c r="R17" s="13"/>
+      <c r="S17" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.15">
@@ -4906,10 +4918,10 @@
         <v>43020205</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D18" s="4">
         <v>2</v>
@@ -4931,21 +4943,21 @@
         <v>3</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="Q18" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R18" s="19"/>
-      <c r="S18" s="25" t="s">
-        <v>258</v>
+      <c r="R18" s="13"/>
+      <c r="S18" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.15">
@@ -4990,9 +5002,9 @@
       <c r="Q19" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R19" s="19"/>
-      <c r="S19" s="25" t="s">
-        <v>258</v>
+      <c r="R19" s="13"/>
+      <c r="S19" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.15">
@@ -5037,9 +5049,9 @@
       <c r="Q20" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R20" s="19"/>
-      <c r="S20" s="25" t="s">
-        <v>258</v>
+      <c r="R20" s="13"/>
+      <c r="S20" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.15">
@@ -5084,9 +5096,9 @@
       <c r="Q21" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R21" s="19"/>
-      <c r="S21" s="25" t="s">
-        <v>258</v>
+      <c r="R21" s="13"/>
+      <c r="S21" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.15">
@@ -5131,9 +5143,9 @@
       <c r="Q22" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R22" s="19"/>
-      <c r="S22" s="25" t="s">
-        <v>258</v>
+      <c r="R22" s="13"/>
+      <c r="S22" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.15">
@@ -5153,7 +5165,7 @@
         <v>105</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G23">
         <v>11000005</v>
@@ -5178,9 +5190,9 @@
       <c r="Q23" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R23" s="19"/>
-      <c r="S23" s="25" t="s">
-        <v>258</v>
+      <c r="R23" s="13"/>
+      <c r="S23" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.15">
@@ -5225,9 +5237,9 @@
       <c r="Q24" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R24" s="19"/>
-      <c r="S24" s="25" t="s">
-        <v>258</v>
+      <c r="R24" s="13"/>
+      <c r="S24" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.15">
@@ -5272,9 +5284,9 @@
       <c r="Q25" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R25" s="19"/>
-      <c r="S25" s="25" t="s">
-        <v>258</v>
+      <c r="R25" s="13"/>
+      <c r="S25" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.15">
@@ -5319,9 +5331,9 @@
       <c r="Q26" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R26" s="19"/>
-      <c r="S26" s="25" t="s">
-        <v>258</v>
+      <c r="R26" s="13"/>
+      <c r="S26" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.15">
@@ -5366,9 +5378,9 @@
       <c r="Q27" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R27" s="19"/>
-      <c r="S27" s="25" t="s">
-        <v>258</v>
+      <c r="R27" s="13"/>
+      <c r="S27" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.15">
@@ -5413,9 +5425,9 @@
       <c r="Q28" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R28" s="19"/>
-      <c r="S28" s="25" t="s">
-        <v>258</v>
+      <c r="R28" s="13"/>
+      <c r="S28" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.15">
@@ -5435,7 +5447,7 @@
         <v>105</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G29">
         <v>11000005</v>
@@ -5460,9 +5472,9 @@
       <c r="Q29" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R29" s="19"/>
-      <c r="S29" s="25" t="s">
-        <v>258</v>
+      <c r="R29" s="13"/>
+      <c r="S29" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.15">
@@ -5482,7 +5494,7 @@
         <v>105</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G30">
         <v>11000001</v>
@@ -5507,9 +5519,9 @@
       <c r="Q30" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R30" s="19"/>
-      <c r="S30" s="25" t="s">
-        <v>258</v>
+      <c r="R30" s="13"/>
+      <c r="S30" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.15">
@@ -5554,9 +5566,9 @@
       <c r="Q31" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R31" s="19"/>
-      <c r="S31" s="25" t="s">
-        <v>258</v>
+      <c r="R31" s="13"/>
+      <c r="S31" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.15">
@@ -5601,9 +5613,9 @@
       <c r="Q32" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R32" s="19"/>
-      <c r="S32" s="25" t="s">
-        <v>258</v>
+      <c r="R32" s="13"/>
+      <c r="S32" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.15">
@@ -5648,9 +5660,9 @@
       <c r="Q33" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R33" s="19"/>
-      <c r="S33" s="25" t="s">
-        <v>258</v>
+      <c r="R33" s="13"/>
+      <c r="S33" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.15">
@@ -5695,9 +5707,9 @@
       <c r="Q34" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R34" s="19"/>
-      <c r="S34" s="25" t="s">
-        <v>258</v>
+      <c r="R34" s="13"/>
+      <c r="S34" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.15">
@@ -5742,9 +5754,9 @@
       <c r="Q35" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R35" s="19"/>
-      <c r="S35" s="25" t="s">
-        <v>258</v>
+      <c r="R35" s="13"/>
+      <c r="S35" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.15">
@@ -5789,9 +5801,9 @@
       <c r="Q36" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R36" s="19"/>
-      <c r="S36" s="25" t="s">
-        <v>258</v>
+      <c r="R36" s="13"/>
+      <c r="S36" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.15">
@@ -5836,9 +5848,9 @@
       <c r="Q37" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R37" s="19"/>
-      <c r="S37" s="25" t="s">
-        <v>258</v>
+      <c r="R37" s="13"/>
+      <c r="S37" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.15">
@@ -5883,9 +5895,9 @@
       <c r="Q38" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R38" s="19"/>
-      <c r="S38" s="25" t="s">
-        <v>258</v>
+      <c r="R38" s="13"/>
+      <c r="S38" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.15">
@@ -5930,9 +5942,9 @@
       <c r="Q39" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R39" s="19"/>
-      <c r="S39" s="25" t="s">
-        <v>258</v>
+      <c r="R39" s="13"/>
+      <c r="S39" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.15">
@@ -5977,9 +5989,9 @@
       <c r="Q40" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R40" s="19"/>
-      <c r="S40" s="25" t="s">
-        <v>258</v>
+      <c r="R40" s="13"/>
+      <c r="S40" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.15">
@@ -6024,9 +6036,9 @@
       <c r="Q41" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R41" s="19"/>
-      <c r="S41" s="25" t="s">
-        <v>258</v>
+      <c r="R41" s="13"/>
+      <c r="S41" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.15">
@@ -6071,9 +6083,9 @@
       <c r="Q42" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="R42" s="19"/>
-      <c r="S42" s="25" t="s">
-        <v>258</v>
+      <c r="R42" s="13"/>
+      <c r="S42" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -6091,10 +6103,10 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J39" sqref="J39"/>
+      <selection pane="bottomRight" activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6105,68 +6117,69 @@
     <col min="8" max="9" width="6.25" customWidth="1"/>
     <col min="10" max="10" width="9.5" customWidth="1"/>
     <col min="11" max="11" width="10.625" customWidth="1"/>
-    <col min="12" max="15" width="6.125" customWidth="1"/>
+    <col min="12" max="13" width="6.125" customWidth="1"/>
+    <col min="14" max="15" width="27.125" customWidth="1"/>
     <col min="17" max="17" width="10.625" customWidth="1"/>
     <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:19" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="J1" s="14" t="s">
+      <c r="H1" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q1" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>252</v>
+      <c r="R1" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
@@ -6177,7 +6190,7 @@
         <v>179</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>178</v>
@@ -6195,7 +6208,7 @@
         <v>178</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>179</v>
@@ -6204,16 +6217,16 @@
         <v>179</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>179</v>
@@ -6225,7 +6238,7 @@
         <v>201</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.15">
@@ -6236,7 +6249,7 @@
         <v>191</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>192</v>
@@ -6254,7 +6267,7 @@
         <v>196</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>197</v>
@@ -6263,16 +6276,16 @@
         <v>198</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>199</v>
@@ -6281,17 +6294,17 @@
         <v>210</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="S3" s="22" t="s">
-        <v>254</v>
+        <v>226</v>
+      </c>
+      <c r="S3" s="16" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43000001</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -6306,7 +6319,7 @@
       <c r="F4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="12">
         <v>11001003</v>
       </c>
       <c r="H4" s="4">
@@ -6331,16 +6344,16 @@
         <v>4</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R4" s="19"/>
-      <c r="S4" s="23"/>
+        <v>298</v>
+      </c>
+      <c r="R4" s="13"/>
+      <c r="S4" s="17"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43000002</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -6355,7 +6368,7 @@
       <c r="F5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="12">
         <v>11001003</v>
       </c>
       <c r="H5" s="4">
@@ -6376,22 +6389,22 @@
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="6" t="s">
-        <v>267</v>
+        <v>303</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R5" s="19"/>
-      <c r="S5" s="23"/>
+        <v>298</v>
+      </c>
+      <c r="R5" s="13"/>
+      <c r="S5" s="17"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43000003</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -6406,7 +6419,7 @@
       <c r="F6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="12">
         <v>11001003</v>
       </c>
       <c r="H6" s="4">
@@ -6417,7 +6430,7 @@
         <v>3</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="L6" s="4">
         <v>1</v>
@@ -6431,16 +6444,16 @@
         <v>8</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R6" s="19"/>
-      <c r="S6" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R6" s="13"/>
+      <c r="S6" s="17"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43000004</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -6455,7 +6468,7 @@
       <c r="F7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="12">
         <v>11001003</v>
       </c>
       <c r="H7" s="4">
@@ -6480,16 +6493,16 @@
         <v>10</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R7" s="19"/>
-      <c r="S7" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R7" s="13"/>
+      <c r="S7" s="17"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43000005</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -6504,7 +6517,7 @@
       <c r="F8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="12">
         <v>11001003</v>
       </c>
       <c r="H8" s="4">
@@ -6529,10 +6542,10 @@
         <v>12</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R8" s="19"/>
-      <c r="S8" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R8" s="13"/>
+      <c r="S8" s="17"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9">
@@ -6553,7 +6566,7 @@
       <c r="F9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="12">
         <v>11001003</v>
       </c>
       <c r="H9" s="4">
@@ -6578,16 +6591,16 @@
         <v>14</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R9" s="19"/>
-      <c r="S9" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R9" s="13"/>
+      <c r="S9" s="17"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43000007</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -6602,7 +6615,7 @@
       <c r="F10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="12">
         <v>11001003</v>
       </c>
       <c r="H10" s="4">
@@ -6627,10 +6640,10 @@
         <v>16</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R10" s="19"/>
-      <c r="S10" s="23"/>
+        <v>298</v>
+      </c>
+      <c r="R10" s="13"/>
+      <c r="S10" s="17"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11">
@@ -6651,7 +6664,7 @@
       <c r="F11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="12">
         <v>11001003</v>
       </c>
       <c r="H11" s="4">
@@ -6676,10 +6689,10 @@
         <v>18</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R11" s="19"/>
-      <c r="S11" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R11" s="13"/>
+      <c r="S11" s="17"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12">
@@ -6700,7 +6713,7 @@
       <c r="F12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="12">
         <v>11001003</v>
       </c>
       <c r="H12" s="4">
@@ -6725,17 +6738,17 @@
         <v>20</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R12" s="19"/>
-      <c r="S12" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R12" s="13"/>
+      <c r="S12" s="17"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43000010</v>
       </c>
-      <c r="B13" s="27" t="s">
-        <v>282</v>
+      <c r="B13" s="21" t="s">
+        <v>274</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>21</v>
@@ -6749,7 +6762,7 @@
       <c r="F13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="12">
         <v>11001003</v>
       </c>
       <c r="H13" s="4">
@@ -6774,16 +6787,16 @@
         <v>21</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R13" s="19"/>
-      <c r="S13" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R13" s="13"/>
+      <c r="S13" s="17"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43000011</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -6798,7 +6811,7 @@
       <c r="F14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="12">
         <v>11001003</v>
       </c>
       <c r="H14" s="4">
@@ -6823,10 +6836,10 @@
         <v>23</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R14" s="19"/>
-      <c r="S14" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R14" s="13"/>
+      <c r="S14" s="17"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A15">
@@ -6847,7 +6860,7 @@
       <c r="F15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="12">
         <v>11001003</v>
       </c>
       <c r="H15" s="4">
@@ -6872,10 +6885,10 @@
         <v>25</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R15" s="19"/>
-      <c r="S15" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R15" s="13"/>
+      <c r="S15" s="17"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16">
@@ -6896,7 +6909,7 @@
       <c r="F16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="12">
         <v>11001003</v>
       </c>
       <c r="H16" s="4">
@@ -6921,10 +6934,10 @@
         <v>27</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R16" s="19"/>
-      <c r="S16" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R16" s="13"/>
+      <c r="S16" s="17"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17">
@@ -6945,7 +6958,7 @@
       <c r="F17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="12">
         <v>11001003</v>
       </c>
       <c r="H17" s="4">
@@ -6970,16 +6983,16 @@
         <v>29</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R17" s="19"/>
-      <c r="S17" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R17" s="13"/>
+      <c r="S17" s="17"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43000015</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -6994,7 +7007,7 @@
       <c r="F18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="12">
         <v>11001003</v>
       </c>
       <c r="H18" s="4">
@@ -7015,26 +7028,26 @@
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="6" t="s">
-        <v>264</v>
+        <v>304</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R18" s="19"/>
-      <c r="S18" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R18" s="13"/>
+      <c r="S18" s="17"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43000016</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>244</v>
+      <c r="B19" s="12" t="s">
+        <v>238</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
@@ -7045,7 +7058,7 @@
       <c r="F19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="12">
         <v>11001003</v>
       </c>
       <c r="H19" s="4">
@@ -7056,7 +7069,7 @@
         <v>3</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="L19" s="4">
         <v>1</v>
@@ -7067,23 +7080,23 @@
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R19" s="19"/>
-      <c r="S19" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R19" s="13"/>
+      <c r="S19" s="17"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43000017</v>
       </c>
-      <c r="B20" s="27" t="s">
-        <v>247</v>
+      <c r="B20" s="21" t="s">
+        <v>241</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D20" s="4">
         <v>0</v>
@@ -7094,7 +7107,7 @@
       <c r="F20" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="12">
         <v>11001003</v>
       </c>
       <c r="H20" s="4">
@@ -7105,7 +7118,7 @@
         <v>3</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="L20" s="4">
         <v>1</v>
@@ -7116,20 +7129,20 @@
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R20" s="19"/>
-      <c r="S20" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R20" s="13"/>
+      <c r="S20" s="17"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43000018</v>
       </c>
-      <c r="B21" s="27" t="s">
-        <v>283</v>
+      <c r="B21" s="21" t="s">
+        <v>275</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>32</v>
@@ -7143,7 +7156,7 @@
       <c r="F21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="12">
         <v>11001003</v>
       </c>
       <c r="H21" s="4">
@@ -7168,10 +7181,10 @@
         <v>32</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R21" s="19"/>
-      <c r="S21" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R21" s="13"/>
+      <c r="S21" s="17"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A22">
@@ -7192,7 +7205,7 @@
       <c r="F22" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="12">
         <v>11001003</v>
       </c>
       <c r="H22" s="4">
@@ -7217,16 +7230,16 @@
         <v>34</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R22" s="19"/>
-      <c r="S22" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R22" s="13"/>
+      <c r="S22" s="17"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43000020</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="20" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -7241,7 +7254,7 @@
       <c r="F23" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="18">
+      <c r="G23" s="12">
         <v>11001003</v>
       </c>
       <c r="H23" s="4">
@@ -7266,10 +7279,10 @@
         <v>36</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R23" s="19"/>
-      <c r="S23" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R23" s="13"/>
+      <c r="S23" s="17"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A24">
@@ -7290,7 +7303,7 @@
       <c r="F24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="12">
         <v>11001003</v>
       </c>
       <c r="H24" s="4">
@@ -7315,10 +7328,10 @@
         <v>38</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R24" s="19"/>
-      <c r="S24" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R24" s="13"/>
+      <c r="S24" s="17"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A25">
@@ -7339,7 +7352,7 @@
       <c r="F25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G25" s="12">
         <v>11001003</v>
       </c>
       <c r="H25" s="4">
@@ -7364,10 +7377,10 @@
         <v>40</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R25" s="19"/>
-      <c r="S25" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R25" s="13"/>
+      <c r="S25" s="17"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A26">
@@ -7388,7 +7401,7 @@
       <c r="F26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G26" s="12">
         <v>11001003</v>
       </c>
       <c r="H26" s="4">
@@ -7413,10 +7426,10 @@
         <v>42</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R26" s="19"/>
-      <c r="S26" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R26" s="13"/>
+      <c r="S26" s="17"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A27">
@@ -7437,7 +7450,7 @@
       <c r="F27" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="18">
+      <c r="G27" s="12">
         <v>11001003</v>
       </c>
       <c r="H27" s="4">
@@ -7462,10 +7475,10 @@
         <v>44</v>
       </c>
       <c r="Q27" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R27" s="19"/>
-      <c r="S27" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R27" s="13"/>
+      <c r="S27" s="17"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A28">
@@ -7486,7 +7499,7 @@
       <c r="F28" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="12">
         <v>11001003</v>
       </c>
       <c r="H28" s="4">
@@ -7511,10 +7524,10 @@
         <v>46</v>
       </c>
       <c r="Q28" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R28" s="19"/>
-      <c r="S28" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R28" s="13"/>
+      <c r="S28" s="17"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A29">
@@ -7535,7 +7548,7 @@
       <c r="F29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="18">
+      <c r="G29" s="12">
         <v>11001003</v>
       </c>
       <c r="H29" s="4">
@@ -7560,10 +7573,10 @@
         <v>48</v>
       </c>
       <c r="Q29" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R29" s="19"/>
-      <c r="S29" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R29" s="13"/>
+      <c r="S29" s="17"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A30">
@@ -7584,7 +7597,7 @@
       <c r="F30" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G30" s="18">
+      <c r="G30" s="12">
         <v>11001003</v>
       </c>
       <c r="H30" s="4">
@@ -7609,10 +7622,10 @@
         <v>50</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R30" s="19"/>
-      <c r="S30" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R30" s="13"/>
+      <c r="S30" s="17"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A31">
@@ -7633,7 +7646,7 @@
       <c r="F31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G31" s="18">
+      <c r="G31" s="12">
         <v>11001003</v>
       </c>
       <c r="H31" s="4">
@@ -7658,10 +7671,10 @@
         <v>52</v>
       </c>
       <c r="Q31" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R31" s="19"/>
-      <c r="S31" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R31" s="13"/>
+      <c r="S31" s="17"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A32">
@@ -7682,7 +7695,7 @@
       <c r="F32" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G32" s="18">
+      <c r="G32" s="12">
         <v>11001003</v>
       </c>
       <c r="H32" s="4">
@@ -7707,10 +7720,10 @@
         <v>54</v>
       </c>
       <c r="Q32" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R32" s="19"/>
-      <c r="S32" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R32" s="13"/>
+      <c r="S32" s="17"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A33">
@@ -7731,7 +7744,7 @@
       <c r="F33" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G33" s="18">
+      <c r="G33" s="12">
         <v>11001003</v>
       </c>
       <c r="H33" s="4">
@@ -7756,10 +7769,10 @@
         <v>56</v>
       </c>
       <c r="Q33" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R33" s="19"/>
-      <c r="S33" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R33" s="13"/>
+      <c r="S33" s="17"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A34">
@@ -7780,7 +7793,7 @@
       <c r="F34" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G34" s="18">
+      <c r="G34" s="12">
         <v>11001003</v>
       </c>
       <c r="H34" s="4">
@@ -7805,10 +7818,10 @@
         <v>58</v>
       </c>
       <c r="Q34" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R34" s="19"/>
-      <c r="S34" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R34" s="13"/>
+      <c r="S34" s="17"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A35">
@@ -7829,7 +7842,7 @@
       <c r="F35" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G35" s="18">
+      <c r="G35" s="12">
         <v>11001003</v>
       </c>
       <c r="H35" s="4">
@@ -7854,10 +7867,10 @@
         <v>60</v>
       </c>
       <c r="Q35" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R35" s="19"/>
-      <c r="S35" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R35" s="13"/>
+      <c r="S35" s="17"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A36">
@@ -7878,7 +7891,7 @@
       <c r="F36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G36" s="18">
+      <c r="G36" s="12">
         <v>11001003</v>
       </c>
       <c r="H36" s="4">
@@ -7903,20 +7916,20 @@
         <v>62</v>
       </c>
       <c r="Q36" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R36" s="19"/>
-      <c r="S36" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R36" s="13"/>
+      <c r="S36" s="17"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43000034</v>
       </c>
-      <c r="B37" s="18" t="s">
-        <v>260</v>
+      <c r="B37" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D37" s="4">
         <v>0</v>
@@ -7925,9 +7938,9 @@
         <v>1</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="G37" s="18">
+        <v>255</v>
+      </c>
+      <c r="G37" s="12">
         <v>11001003</v>
       </c>
       <c r="H37" s="4">
@@ -7938,7 +7951,7 @@
         <v>3</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="L37" s="4">
         <v>1</v>
@@ -7949,23 +7962,23 @@
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="4" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="Q37" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R37" s="19"/>
-      <c r="S37" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R37" s="13"/>
+      <c r="S37" s="17"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43000035</v>
       </c>
-      <c r="B38" s="18" t="s">
-        <v>266</v>
+      <c r="B38" s="12" t="s">
+        <v>259</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D38" s="4">
         <v>0</v>
@@ -7976,7 +7989,7 @@
       <c r="F38" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G38" s="18">
+      <c r="G38" s="12">
         <v>11001003</v>
       </c>
       <c r="H38" s="4">
@@ -7987,7 +8000,7 @@
         <v>3</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="L38" s="4">
         <v>1</v>
@@ -7998,23 +8011,23 @@
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
       <c r="P38" s="4" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="Q38" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R38" s="19"/>
-      <c r="S38" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R38" s="13"/>
+      <c r="S38" s="17"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>43000036</v>
       </c>
-      <c r="B39" s="18" t="s">
-        <v>270</v>
+      <c r="B39" s="12" t="s">
+        <v>262</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="D39" s="4">
         <v>0</v>
@@ -8025,7 +8038,7 @@
       <c r="F39" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G39" s="18">
+      <c r="G39" s="12">
         <v>11001003</v>
       </c>
       <c r="H39" s="4">
@@ -8036,7 +8049,7 @@
         <v>3</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="L39" s="4">
         <v>1</v>
@@ -8047,23 +8060,23 @@
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
       <c r="P39" s="4" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="Q39" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R39" s="19"/>
-      <c r="S39" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="R39" s="13"/>
+      <c r="S39" s="17"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>43001001</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>299</v>
+      <c r="B40" s="12" t="s">
+        <v>291</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D40" s="4">
         <v>0</v>
@@ -8074,7 +8087,7 @@
       <c r="F40" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G40" s="18">
+      <c r="G40" s="12">
         <v>11001003</v>
       </c>
       <c r="H40" s="4">
@@ -8085,7 +8098,7 @@
         <v>3</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="L40" s="4">
         <v>1</v>
@@ -8094,22 +8107,25 @@
         <v>24</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="O40" s="4">
-        <v>51000021</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="O40" s="4"/>
       <c r="P40" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="Q40" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="R40" s="19"/>
-      <c r="S40" s="23"/>
+        <v>294</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>299</v>
+      </c>
+      <c r="R40" s="13"/>
+      <c r="S40" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="Q40">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(Q40))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -8126,7 +8142,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
+      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8137,68 +8153,70 @@
     <col min="8" max="9" width="6.125" customWidth="1"/>
     <col min="10" max="10" width="9.5" customWidth="1"/>
     <col min="11" max="11" width="10.625" customWidth="1"/>
-    <col min="12" max="15" width="6.125" customWidth="1"/>
+    <col min="12" max="13" width="6.125" customWidth="1"/>
+    <col min="14" max="14" width="28.375" customWidth="1"/>
+    <col min="15" max="15" width="19.5" customWidth="1"/>
     <col min="17" max="17" width="10.625" customWidth="1"/>
     <col min="19" max="19" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>272</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="I1" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="J1" s="16" t="s">
+      <c r="I1" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="J1" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="L1" s="16" t="s">
-        <v>288</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>291</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>286</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="P1" s="17" t="s">
+      <c r="L1" s="25" t="s">
+        <v>280</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>295</v>
+      </c>
+      <c r="P1" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="R1" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="S1" s="16" t="s">
-        <v>255</v>
+      <c r="R1" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
@@ -8209,7 +8227,7 @@
         <v>179</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>178</v>
@@ -8227,7 +8245,7 @@
         <v>178</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>179</v>
@@ -8236,16 +8254,16 @@
         <v>179</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>179</v>
@@ -8254,10 +8272,10 @@
         <v>209</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.15">
@@ -8268,7 +8286,7 @@
         <v>191</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>192</v>
@@ -8286,7 +8304,7 @@
         <v>196</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>197</v>
@@ -8295,16 +8313,16 @@
         <v>198</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="P3" s="10" t="s">
         <v>199</v>
@@ -8313,10 +8331,10 @@
         <v>210</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="S3" s="24" t="s">
-        <v>257</v>
+        <v>224</v>
+      </c>
+      <c r="S3" s="18" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
@@ -8338,7 +8356,7 @@
       <c r="F4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="12">
         <v>11001002</v>
       </c>
       <c r="H4" s="4">
@@ -8356,17 +8374,17 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="6" t="s">
-        <v>236</v>
+        <v>300</v>
       </c>
       <c r="O4" s="6"/>
       <c r="P4" s="4" t="s">
         <v>211</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R4" s="4"/>
-      <c r="S4" s="21"/>
+      <c r="S4" s="15"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5">
@@ -8387,7 +8405,7 @@
       <c r="F5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="12">
         <v>11001002</v>
       </c>
       <c r="H5" s="4">
@@ -8410,10 +8428,10 @@
         <v>157</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R5" s="4"/>
-      <c r="S5" s="20"/>
+      <c r="S5" s="14"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6">
@@ -8434,7 +8452,7 @@
       <c r="F6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="12">
         <v>11001002</v>
       </c>
       <c r="H6" s="4">
@@ -8457,10 +8475,10 @@
         <v>159</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R6" s="4"/>
-      <c r="S6" s="20"/>
+      <c r="S6" s="14"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7">
@@ -8481,7 +8499,7 @@
       <c r="F7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="12">
         <v>11001002</v>
       </c>
       <c r="H7" s="4">
@@ -8504,10 +8522,10 @@
         <v>161</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R7" s="4"/>
-      <c r="S7" s="20"/>
+      <c r="S7" s="14"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8">
@@ -8528,7 +8546,7 @@
       <c r="F8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="12">
         <v>11001001</v>
       </c>
       <c r="H8" s="4">
@@ -8546,17 +8564,17 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="4" t="s">
-        <v>234</v>
+        <v>301</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="6" t="s">
         <v>203</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R8" s="4"/>
-      <c r="S8" s="20"/>
+      <c r="S8" s="14"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9">
@@ -8577,7 +8595,7 @@
       <c r="F9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="12">
         <v>11001001</v>
       </c>
       <c r="H9" s="4">
@@ -8595,17 +8613,17 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="4" t="s">
-        <v>235</v>
+        <v>302</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="6" t="s">
         <v>206</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R9" s="4"/>
-      <c r="S9" s="20"/>
+      <c r="S9" s="14"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10">
@@ -8626,7 +8644,7 @@
       <c r="F10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="12">
         <v>11001001</v>
       </c>
       <c r="H10" s="4">
@@ -8647,10 +8665,10 @@
         <v>166</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R10" s="4"/>
-      <c r="S10" s="20"/>
+      <c r="S10" s="14"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11">
@@ -8671,7 +8689,7 @@
       <c r="F11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="12">
         <v>11001001</v>
       </c>
       <c r="H11" s="4">
@@ -8692,10 +8710,10 @@
         <v>170</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R11" s="4"/>
-      <c r="S11" s="20"/>
+      <c r="S11" s="14"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12">
@@ -8716,7 +8734,7 @@
       <c r="F12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="12">
         <v>11001001</v>
       </c>
       <c r="H12" s="4">
@@ -8737,10 +8755,10 @@
         <v>172</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R12" s="4"/>
-      <c r="S12" s="20"/>
+      <c r="S12" s="14"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13">
@@ -8761,7 +8779,7 @@
       <c r="F13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="12">
         <v>11001001</v>
       </c>
       <c r="H13" s="4">
@@ -8782,10 +8800,10 @@
         <v>175</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R13" s="4"/>
-      <c r="S13" s="20"/>
+      <c r="S13" s="14"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14">
@@ -8806,7 +8824,7 @@
       <c r="F14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="12">
         <v>11001001</v>
       </c>
       <c r="H14" s="4">
@@ -8827,10 +8845,10 @@
         <v>177</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R14" s="4"/>
-      <c r="S14" s="20"/>
+      <c r="S14" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
no cardout punish on monster
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -16,7 +16,7 @@
     <sheet name="怪物" sheetId="1" r:id="rId2"/>
     <sheet name="特殊" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -1038,7 +1038,7 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51000021;5;4;51000021;7;2;51000021;7;6</t>
+    <t>51000021;5;4;51000021;7;2;51000021;7;6;51000021;12;3;51000021;12;5</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1892,13 +1892,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="67">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3060,6 +3053,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -3680,62 +3680,62 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:S40" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:S40" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
   <autoFilter ref="A3:S40"/>
   <sortState ref="A4:Q44">
     <sortCondition ref="A3:A44"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" name="Id" dataDxfId="41"/>
-    <tableColumn id="2" name="Name" dataDxfId="40"/>
-    <tableColumn id="18" name="Ename" dataDxfId="39"/>
-    <tableColumn id="3" name="Type" dataDxfId="38"/>
-    <tableColumn id="6" name="World" dataDxfId="37"/>
-    <tableColumn id="7" name="Deck" dataDxfId="36"/>
-    <tableColumn id="10" name="Job" dataDxfId="35"/>
-    <tableColumn id="11" name="Level" dataDxfId="34"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="33"/>
-    <tableColumn id="13" name="Method" dataDxfId="32"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="31"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="30"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="29"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="28"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="27"/>
-    <tableColumn id="17" name="Figue" dataDxfId="26"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="25"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="24"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="23"/>
+    <tableColumn id="1" name="Id" dataDxfId="40"/>
+    <tableColumn id="2" name="Name" dataDxfId="39"/>
+    <tableColumn id="18" name="Ename" dataDxfId="38"/>
+    <tableColumn id="3" name="Type" dataDxfId="37"/>
+    <tableColumn id="6" name="World" dataDxfId="36"/>
+    <tableColumn id="7" name="Deck" dataDxfId="35"/>
+    <tableColumn id="10" name="Job" dataDxfId="34"/>
+    <tableColumn id="11" name="Level" dataDxfId="33"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="32"/>
+    <tableColumn id="13" name="Method" dataDxfId="31"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="30"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="29"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="28"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="27"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="26"/>
+    <tableColumn id="17" name="Figue" dataDxfId="25"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="24"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="23"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:S14" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:S14" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" tableBorderDxfId="19">
   <autoFilter ref="A3:S14"/>
   <sortState ref="A4:Q83">
     <sortCondition ref="A3:A83"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" name="Id" dataDxfId="19"/>
-    <tableColumn id="2" name="Name" dataDxfId="18"/>
-    <tableColumn id="18" name="Ename" dataDxfId="17"/>
-    <tableColumn id="3" name="Type" dataDxfId="16"/>
-    <tableColumn id="6" name="World" dataDxfId="15"/>
-    <tableColumn id="7" name="Deck" dataDxfId="14"/>
-    <tableColumn id="10" name="Job" dataDxfId="13"/>
-    <tableColumn id="11" name="Level" dataDxfId="12"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="11"/>
-    <tableColumn id="13" name="Method" dataDxfId="10"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="9"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="8"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="7"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="6"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="5"/>
-    <tableColumn id="9" name="Figue" dataDxfId="4"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="3"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="2"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="1"/>
+    <tableColumn id="1" name="Id" dataDxfId="18"/>
+    <tableColumn id="2" name="Name" dataDxfId="17"/>
+    <tableColumn id="18" name="Ename" dataDxfId="16"/>
+    <tableColumn id="3" name="Type" dataDxfId="15"/>
+    <tableColumn id="6" name="World" dataDxfId="14"/>
+    <tableColumn id="7" name="Deck" dataDxfId="13"/>
+    <tableColumn id="10" name="Job" dataDxfId="12"/>
+    <tableColumn id="11" name="Level" dataDxfId="11"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="10"/>
+    <tableColumn id="13" name="Method" dataDxfId="9"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="8"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="7"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="6"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="5"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="4"/>
+    <tableColumn id="9" name="Figue" dataDxfId="3"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="2"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="1"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6106,7 +6106,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N40" sqref="N40"/>
+      <selection pane="bottomRight" activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8104,7 +8104,7 @@
         <v>1</v>
       </c>
       <c r="M40" s="4">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>305</v>
@@ -8122,7 +8122,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="Q40">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="44" priority="1">
       <formula>LEN(TRIM(Q40))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
clean the id of special decks
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="人物" sheetId="4" r:id="rId1"/>
@@ -1022,14 +1022,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51019299;6;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>51019298;6;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>51000002;7;3;51000002;7;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1039,6 +1031,14 @@
   </si>
   <si>
     <t>51000021;5;4;51000021;7;2;51000021;7;6;51000021;12;3;51000021;12;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51019002;6;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51019001;6;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6102,11 +6102,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N33" sqref="N33"/>
+      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6389,7 +6389,7 @@
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>6</v>
@@ -7028,7 +7028,7 @@
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="P18" s="4" t="s">
         <v>257</v>
@@ -8107,7 +8107,7 @@
         <v>20</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="O40" s="4"/>
       <c r="P40" s="4" t="s">
@@ -8138,11 +8138,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
+      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8564,7 +8564,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="4" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="6" t="s">
@@ -8613,7 +8613,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="4" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="6" t="s">

</xml_diff>

<commit_message>
show item quliaty on material view
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="人物" sheetId="4" r:id="rId1"/>
@@ -1030,16 +1030,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51000021;5;4;51000021;7;2;51000021;7;6;51000021;12;3;51000021;12;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>51019002;6;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>51019001;6;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51000021;5;4;51000021;7;2;51000021;7;6</t>
   </si>
 </sst>
 </file>
@@ -6102,11 +6101,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
+      <selection pane="bottomRight" activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8107,7 +8106,7 @@
         <v>20</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="O40" s="4"/>
       <c r="P40" s="4" t="s">
@@ -8138,11 +8137,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8564,7 +8563,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="6" t="s">
@@ -8613,7 +8612,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="6" t="s">

</xml_diff>

<commit_message>
add a monster bee
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="怪物" sheetId="1" r:id="rId2"/>
     <sheet name="特殊" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="312">
   <si>
     <t>老鼠</t>
   </si>
@@ -1039,6 +1039,30 @@
   </si>
   <si>
     <t>51000021;5;4;51000021;7;2;51000021;7;6</t>
+  </si>
+  <si>
+    <t>lang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>honglang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>feichong</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mifeng</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>蜜蜂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bee</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1763,7 +1787,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1845,6 +1869,9 @@
     <xf numFmtId="0" fontId="20" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1891,6 +1918,13 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="67">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3052,13 +3086,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -3679,62 +3706,62 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:S40" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
-  <autoFilter ref="A3:S40"/>
-  <sortState ref="A4:Q44">
-    <sortCondition ref="A3:A44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:S41" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42">
+  <autoFilter ref="A3:S41"/>
+  <sortState ref="A4:Q45">
+    <sortCondition ref="A3:A45"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" name="Id" dataDxfId="40"/>
-    <tableColumn id="2" name="Name" dataDxfId="39"/>
-    <tableColumn id="18" name="Ename" dataDxfId="38"/>
-    <tableColumn id="3" name="Type" dataDxfId="37"/>
-    <tableColumn id="6" name="World" dataDxfId="36"/>
-    <tableColumn id="7" name="Deck" dataDxfId="35"/>
-    <tableColumn id="10" name="Job" dataDxfId="34"/>
-    <tableColumn id="11" name="Level" dataDxfId="33"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="32"/>
-    <tableColumn id="13" name="Method" dataDxfId="31"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="30"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="29"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="28"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="27"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="26"/>
-    <tableColumn id="17" name="Figue" dataDxfId="25"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="24"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="23"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="22"/>
+    <tableColumn id="1" name="Id" dataDxfId="41"/>
+    <tableColumn id="2" name="Name" dataDxfId="40"/>
+    <tableColumn id="18" name="Ename" dataDxfId="39"/>
+    <tableColumn id="3" name="Type" dataDxfId="38"/>
+    <tableColumn id="6" name="World" dataDxfId="37"/>
+    <tableColumn id="7" name="Deck" dataDxfId="36"/>
+    <tableColumn id="10" name="Job" dataDxfId="35"/>
+    <tableColumn id="11" name="Level" dataDxfId="34"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="33"/>
+    <tableColumn id="13" name="Method" dataDxfId="32"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="31"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="30"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="29"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="28"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="27"/>
+    <tableColumn id="17" name="Figue" dataDxfId="26"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="25"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="24"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:S14" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:S14" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="A3:S14"/>
   <sortState ref="A4:Q83">
     <sortCondition ref="A3:A83"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" name="Id" dataDxfId="18"/>
-    <tableColumn id="2" name="Name" dataDxfId="17"/>
-    <tableColumn id="18" name="Ename" dataDxfId="16"/>
-    <tableColumn id="3" name="Type" dataDxfId="15"/>
-    <tableColumn id="6" name="World" dataDxfId="14"/>
-    <tableColumn id="7" name="Deck" dataDxfId="13"/>
-    <tableColumn id="10" name="Job" dataDxfId="12"/>
-    <tableColumn id="11" name="Level" dataDxfId="11"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="10"/>
-    <tableColumn id="13" name="Method" dataDxfId="9"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="8"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="7"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="6"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="5"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="4"/>
-    <tableColumn id="9" name="Figue" dataDxfId="3"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="2"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="1"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="19"/>
+    <tableColumn id="2" name="Name" dataDxfId="18"/>
+    <tableColumn id="18" name="Ename" dataDxfId="17"/>
+    <tableColumn id="3" name="Type" dataDxfId="16"/>
+    <tableColumn id="6" name="World" dataDxfId="15"/>
+    <tableColumn id="7" name="Deck" dataDxfId="14"/>
+    <tableColumn id="10" name="Job" dataDxfId="13"/>
+    <tableColumn id="11" name="Level" dataDxfId="12"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="11"/>
+    <tableColumn id="13" name="Method" dataDxfId="10"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="9"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="8"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="7"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="6"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="5"/>
+    <tableColumn id="9" name="Figue" dataDxfId="4"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="3"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="2"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6099,13 +6126,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N38" sqref="N38"/>
+      <selection pane="bottomRight" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6332,7 +6359,7 @@
         <v>4</v>
       </c>
       <c r="L4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M4" s="4">
         <v>15</v>
@@ -6356,7 +6383,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>6</v>
+        <v>306</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -6381,10 +6408,10 @@
         <v>6</v>
       </c>
       <c r="L5" s="4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="M5" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="6" t="s">
@@ -6603,7 +6630,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>16</v>
+        <v>308</v>
       </c>
       <c r="D10" s="4">
         <v>0</v>
@@ -6628,10 +6655,10 @@
         <v>16</v>
       </c>
       <c r="L10" s="4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="M10" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -7140,11 +7167,11 @@
       <c r="A21">
         <v>43000018</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="12" t="s">
         <v>275</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>32</v>
+        <v>307</v>
       </c>
       <c r="D21" s="4">
         <v>0</v>
@@ -8069,13 +8096,13 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>43001001</v>
+        <v>43000037</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="D40" s="4">
         <v>0</v>
@@ -8090,39 +8117,88 @@
         <v>11001003</v>
       </c>
       <c r="H40" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>292</v>
+        <v>311</v>
       </c>
       <c r="L40" s="4">
         <v>1</v>
       </c>
       <c r="M40" s="4">
-        <v>20</v>
-      </c>
-      <c r="N40" s="4" t="s">
-        <v>305</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="N40" s="4"/>
       <c r="O40" s="4"/>
       <c r="P40" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q40" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="R40" s="27"/>
+      <c r="S40" s="27"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>43001001</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G41" s="12">
+        <v>11001003</v>
+      </c>
+      <c r="H41" s="4">
+        <v>10</v>
+      </c>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="L41" s="4">
+        <v>1</v>
+      </c>
+      <c r="M41" s="4">
+        <v>20</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="Q41" t="s">
         <v>299</v>
       </c>
-      <c r="R40" s="13"/>
-      <c r="S40" s="17"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="Q40">
-    <cfRule type="containsBlanks" dxfId="44" priority="1">
-      <formula>LEN(TRIM(Q40))=0</formula>
+  <conditionalFormatting sqref="Q41">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(Q41))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add a new event of blockway
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="320">
   <si>
     <t>老鼠</t>
   </si>
@@ -1079,6 +1079,21 @@
   <si>
     <t>海盗</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>士兵</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>soldier</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>soldier</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51000010;0;0;51000010;2;2;51000010;0;4;51000009;7;2</t>
   </si>
 </sst>
 </file>
@@ -1314,6 +1329,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1944,13 +1960,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="67">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3112,6 +3121,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -3732,62 +3748,62 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表2" displayName="表2" ref="A3:S42" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42">
-  <autoFilter ref="A3:S42" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表2" displayName="表2" ref="A3:S43" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
+  <autoFilter ref="A3:S43" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:Q46">
     <sortCondition ref="A3:A46"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="40"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Ename" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="World" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Deck" dataDxfId="36"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Job" dataDxfId="35"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Level" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="AutoAddLevel" dataDxfId="33"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Method" dataDxfId="32"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Emethod" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="EpSlow" dataDxfId="30"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="CardReduce" dataDxfId="29"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="RightMon" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PetMon" dataDxfId="27"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Figue" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BattleMap" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="DropItem" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="InRandomQuest" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="39"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Ename" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="World" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Deck" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Job" dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Level" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="AutoAddLevel" dataDxfId="32"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Method" dataDxfId="31"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Emethod" dataDxfId="30"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="EpSlow" dataDxfId="29"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="CardReduce" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="RightMon" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PetMon" dataDxfId="26"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Figue" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BattleMap" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="DropItem" dataDxfId="23"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="InRandomQuest" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表2_2" displayName="表2_2" ref="A3:S14" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表2_2" displayName="表2_2" ref="A3:S14" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" tableBorderDxfId="19">
   <autoFilter ref="A3:S14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:Q83">
     <sortCondition ref="A3:A83"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="18"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Ename" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="World" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Deck" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Job" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Level" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="AutoAddLevel" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Method" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Emethod" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="EpSlow" dataDxfId="8"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="CardReduce" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="RightMon" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="PetMon" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Figue" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="BattleMap" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="DropItem" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="InRandomQuest" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Ename" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="World" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Deck" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Job" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Level" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="AutoAddLevel" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Method" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Emethod" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="EpSlow" dataDxfId="7"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="CardReduce" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="RightMon" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="PetMon" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Figue" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="BattleMap" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="DropItem" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="InRandomQuest" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6152,13 +6168,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8269,10 +8285,61 @@
       <c r="R42" s="13"/>
       <c r="S42" s="17"/>
     </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>43001002</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G43" s="12">
+        <v>11001003</v>
+      </c>
+      <c r="H43" s="4">
+        <v>12</v>
+      </c>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="L43" s="4">
+        <v>1</v>
+      </c>
+      <c r="M43" s="4">
+        <v>20</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q43" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="R43" s="13"/>
+      <c r="S43" s="17"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="Q42">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="44" priority="1">
       <formula>LEN(TRIM(Q42))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
optimise the codes implement
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -2032,7 +2032,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="87">
+  <dxfs count="80">
     <dxf>
       <font>
         <b val="0"/>
@@ -2183,75 +2183,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4026,96 +3957,96 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:T42" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85" tableBorderDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:T42" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" tableBorderDxfId="77">
   <autoFilter ref="A3:T42"/>
   <sortState ref="A4:T42">
-    <sortCondition ref="H3:H42"/>
+    <sortCondition ref="A3:A42"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="83"/>
-    <tableColumn id="2" name="Name" dataDxfId="82"/>
-    <tableColumn id="18" name="Ename" dataDxfId="81"/>
-    <tableColumn id="3" name="Type" dataDxfId="80"/>
-    <tableColumn id="21" name="Quality" dataDxfId="20"/>
-    <tableColumn id="6" name="World" dataDxfId="79"/>
-    <tableColumn id="10" name="Job" dataDxfId="78"/>
-    <tableColumn id="11" name="Level" dataDxfId="77"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="76"/>
-    <tableColumn id="13" name="Method" dataDxfId="75"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="74"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="73"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="72"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="71"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="70"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="69"/>
-    <tableColumn id="17" name="Figue" dataDxfId="68"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="67"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="66"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="65"/>
+    <tableColumn id="1" name="Id" dataDxfId="76"/>
+    <tableColumn id="2" name="Name" dataDxfId="75"/>
+    <tableColumn id="18" name="Ename" dataDxfId="74"/>
+    <tableColumn id="3" name="Type" dataDxfId="73"/>
+    <tableColumn id="21" name="Quality" dataDxfId="13"/>
+    <tableColumn id="6" name="World" dataDxfId="72"/>
+    <tableColumn id="10" name="Job" dataDxfId="71"/>
+    <tableColumn id="11" name="Level" dataDxfId="70"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="69"/>
+    <tableColumn id="13" name="Method" dataDxfId="68"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="67"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="66"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="65"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="64"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="63"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="62"/>
+    <tableColumn id="17" name="Figue" dataDxfId="61"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="60"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="59"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55">
   <autoFilter ref="A3:T50"/>
   <sortState ref="A4:R48">
     <sortCondition ref="A3:A48"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="61"/>
-    <tableColumn id="2" name="Name" dataDxfId="60"/>
-    <tableColumn id="18" name="Ename" dataDxfId="59"/>
-    <tableColumn id="3" name="Type" dataDxfId="58"/>
+    <tableColumn id="1" name="Id" dataDxfId="54"/>
+    <tableColumn id="2" name="Name" dataDxfId="53"/>
+    <tableColumn id="18" name="Ename" dataDxfId="52"/>
+    <tableColumn id="3" name="Type" dataDxfId="51"/>
     <tableColumn id="7" name="Quality" dataDxfId="12"/>
-    <tableColumn id="6" name="World" dataDxfId="57"/>
-    <tableColumn id="10" name="Job" dataDxfId="56"/>
-    <tableColumn id="11" name="Level" dataDxfId="55"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="54"/>
-    <tableColumn id="13" name="Method" dataDxfId="53"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="52"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="51"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="50"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="49"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="48"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="47"/>
-    <tableColumn id="17" name="Figue" dataDxfId="46"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="45"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="44"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="43"/>
+    <tableColumn id="6" name="World" dataDxfId="50"/>
+    <tableColumn id="10" name="Job" dataDxfId="49"/>
+    <tableColumn id="11" name="Level" dataDxfId="48"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="47"/>
+    <tableColumn id="13" name="Method" dataDxfId="46"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="45"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="44"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="43"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="42"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="41"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="40"/>
+    <tableColumn id="17" name="Figue" dataDxfId="39"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="38"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="37"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:T14" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" tableBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:T14" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
   <autoFilter ref="A3:T14"/>
   <sortState ref="A4:R83">
     <sortCondition ref="A3:A83"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="39"/>
-    <tableColumn id="2" name="Name" dataDxfId="38"/>
-    <tableColumn id="18" name="Ename" dataDxfId="37"/>
-    <tableColumn id="3" name="Type" dataDxfId="36"/>
+    <tableColumn id="1" name="Id" dataDxfId="32"/>
+    <tableColumn id="2" name="Name" dataDxfId="31"/>
+    <tableColumn id="18" name="Ename" dataDxfId="30"/>
+    <tableColumn id="3" name="Type" dataDxfId="29"/>
     <tableColumn id="7" name="Quality" dataDxfId="0"/>
-    <tableColumn id="6" name="World" dataDxfId="35"/>
-    <tableColumn id="10" name="Job" dataDxfId="34"/>
-    <tableColumn id="11" name="Level" dataDxfId="33"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="32"/>
-    <tableColumn id="13" name="Method" dataDxfId="31"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="30"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="29"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="28"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="27"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="26"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="25"/>
-    <tableColumn id="9" name="Figue" dataDxfId="24"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="23"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="22"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="21"/>
+    <tableColumn id="6" name="World" dataDxfId="28"/>
+    <tableColumn id="10" name="Job" dataDxfId="27"/>
+    <tableColumn id="11" name="Level" dataDxfId="26"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="25"/>
+    <tableColumn id="13" name="Method" dataDxfId="24"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="23"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="22"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="21"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="20"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="19"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="18"/>
+    <tableColumn id="9" name="Figue" dataDxfId="17"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="16"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="15"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4448,7 +4379,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4652,33 +4583,33 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4">
-        <v>43020306</v>
+        <v>43020101</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>102</v>
+        <v>252</v>
       </c>
       <c r="D4" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="33"/>
       <c r="F4" s="4" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="G4">
-        <v>11000008</v>
+        <v>11000001</v>
       </c>
       <c r="H4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -4686,25 +4617,23 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>198</v>
       </c>
       <c r="S4" s="13"/>
-      <c r="T4" s="19" t="s">
-        <v>233</v>
-      </c>
+      <c r="T4" s="19"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5">
-        <v>43020101</v>
+        <v>43020102</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>234</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -4714,17 +4643,17 @@
         <v>63</v>
       </c>
       <c r="G5">
-        <v>11000001</v>
+        <v>11000003</v>
       </c>
       <c r="H5" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -4732,7 +4661,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R5" s="4" t="s">
         <v>198</v>
@@ -4742,33 +4671,35 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>43020102</v>
+        <v>43020103</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>234</v>
+        <v>66</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>253</v>
+        <v>67</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="33"/>
+      <c r="E6" s="33">
+        <v>1</v>
+      </c>
       <c r="F6" s="4" t="s">
         <v>63</v>
       </c>
       <c r="G6">
-        <v>11000003</v>
+        <v>11000002</v>
       </c>
       <c r="H6" s="4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -4776,43 +4707,47 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>198</v>
       </c>
       <c r="S6" s="13"/>
-      <c r="T6" s="19"/>
+      <c r="T6" s="19" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>43020205</v>
+        <v>43020104</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>226</v>
+        <v>68</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>225</v>
+        <v>69</v>
       </c>
       <c r="D7" s="4">
-        <v>2</v>
-      </c>
-      <c r="E7" s="33"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="33">
+        <v>1</v>
+      </c>
       <c r="F7" s="4" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="G7">
         <v>11000008</v>
       </c>
       <c r="H7" s="4">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>225</v>
+        <v>69</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -4820,45 +4755,45 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>225</v>
+        <v>69</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>198</v>
       </c>
       <c r="S7" s="13"/>
-      <c r="T7" s="19" t="s">
-        <v>233</v>
-      </c>
+      <c r="T7" s="19"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>43020303</v>
+        <v>43020105</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="D8" s="4">
-        <v>4</v>
-      </c>
-      <c r="E8" s="33"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="33">
+        <v>2</v>
+      </c>
       <c r="F8" s="4" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="G8">
-        <v>11000004</v>
+        <v>11000007</v>
       </c>
       <c r="H8" s="4">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>96</v>
+        <v>251</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -4866,7 +4801,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>198</v>
@@ -4878,35 +4813,35 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>43020204</v>
+        <v>43020106</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>224</v>
+        <v>72</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>223</v>
+        <v>73</v>
       </c>
       <c r="D9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="G9">
         <v>11000005</v>
       </c>
       <c r="H9" s="4">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>223</v>
+        <v>73</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -4914,7 +4849,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="s">
-        <v>223</v>
+        <v>73</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>198</v>
@@ -4926,35 +4861,35 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>43020103</v>
+        <v>43020107</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
       <c r="E10" s="33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>63</v>
       </c>
       <c r="G10">
-        <v>11000002</v>
+        <v>11000007</v>
       </c>
       <c r="H10" s="4">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -4962,7 +4897,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>198</v>
@@ -4974,35 +4909,35 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>43020301</v>
+        <v>43020108</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="33">
         <v>3</v>
       </c>
-      <c r="E11" s="33">
-        <v>1</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="G11">
-        <v>11000002</v>
+        <v>11000005</v>
       </c>
       <c r="H11" s="4">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -5010,7 +4945,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>198</v>
@@ -5022,35 +4957,35 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>43020408</v>
+        <v>43020109</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>130</v>
+        <v>78</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="D12" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E12" s="33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="G12">
-        <v>11000002</v>
+        <v>11000006</v>
       </c>
       <c r="H12" s="4">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -5058,7 +4993,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="R12" s="4" t="s">
         <v>198</v>
@@ -5070,35 +5005,35 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>43020310</v>
+        <v>43020110</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="33">
         <v>4</v>
       </c>
-      <c r="E13" s="33">
-        <v>1</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="G13">
-        <v>11000003</v>
+        <v>11000006</v>
       </c>
       <c r="H13" s="4">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
@@ -5106,7 +5041,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>198</v>
@@ -5118,35 +5053,35 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>43020104</v>
+        <v>43020201</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D14" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="G14">
-        <v>11000008</v>
+        <v>11000007</v>
       </c>
       <c r="H14" s="4">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
@@ -5154,45 +5089,47 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>198</v>
       </c>
       <c r="S14" s="13"/>
-      <c r="T14" s="19"/>
+      <c r="T14" s="19" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>43020302</v>
+        <v>43020202</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D15" s="4">
+        <v>2</v>
+      </c>
+      <c r="E15" s="33">
         <v>3</v>
       </c>
-      <c r="E15" s="33">
-        <v>1</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G15">
-        <v>11000008</v>
+        <v>11000001</v>
       </c>
       <c r="H15" s="4">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
@@ -5200,7 +5137,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="R15" s="4" t="s">
         <v>198</v>
@@ -5212,35 +5149,35 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>43020503</v>
+        <v>43020203</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="D16" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E16" s="33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="G16">
-        <v>11000008</v>
+        <v>11000002</v>
       </c>
       <c r="H16" s="4">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -5248,7 +5185,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>198</v>
@@ -5260,35 +5197,35 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>43020307</v>
+        <v>43020204</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>103</v>
+        <v>224</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>104</v>
+        <v>223</v>
       </c>
       <c r="D17" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E17" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="G17">
-        <v>11000001</v>
+        <v>11000005</v>
       </c>
       <c r="H17" s="4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>104</v>
+        <v>223</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
@@ -5296,7 +5233,7 @@
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4" t="s">
-        <v>104</v>
+        <v>223</v>
       </c>
       <c r="R17" s="4" t="s">
         <v>198</v>
@@ -5308,35 +5245,33 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>43020401</v>
+        <v>43020205</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>115</v>
+        <v>226</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>117</v>
+        <v>225</v>
       </c>
       <c r="D18" s="4">
-        <v>5</v>
-      </c>
-      <c r="E18" s="33">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E18" s="33"/>
       <c r="F18" s="4" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="G18">
-        <v>11000002</v>
+        <v>11000008</v>
       </c>
       <c r="H18" s="4">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>117</v>
+        <v>225</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -5344,7 +5279,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4" t="s">
-        <v>117</v>
+        <v>225</v>
       </c>
       <c r="R18" s="4" t="s">
         <v>198</v>
@@ -5356,35 +5291,35 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>43020407</v>
+        <v>43020301</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="D19" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E19" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="G19">
-        <v>11000004</v>
+        <v>11000002</v>
       </c>
       <c r="H19" s="4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
@@ -5392,7 +5327,7 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="R19" s="4" t="s">
         <v>198</v>
@@ -5404,35 +5339,35 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>43020308</v>
+        <v>43020302</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D20" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G20">
-        <v>11000001</v>
+        <v>11000008</v>
       </c>
       <c r="H20" s="4">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
@@ -5440,7 +5375,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="R20" s="4" t="s">
         <v>198</v>
@@ -5452,35 +5387,33 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>43020402</v>
+        <v>43020303</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="D21" s="4">
+        <v>4</v>
+      </c>
+      <c r="E21" s="33"/>
+      <c r="F21" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21">
+        <v>11000004</v>
+      </c>
+      <c r="H21" s="4">
         <v>5</v>
-      </c>
-      <c r="E21" s="33">
-        <v>2</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G21">
-        <v>11000001</v>
-      </c>
-      <c r="H21" s="4">
-        <v>11</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
@@ -5488,7 +5421,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="R21" s="4" t="s">
         <v>198</v>
@@ -5500,35 +5433,35 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>43020105</v>
+        <v>43020304</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="D22" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E22" s="33">
         <v>2</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="G22">
-        <v>11000007</v>
+        <v>11000002</v>
       </c>
       <c r="H22" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>251</v>
+        <v>98</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -5536,7 +5469,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="R22" s="4" t="s">
         <v>198</v>
@@ -5548,13 +5481,13 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>43020309</v>
+        <v>43020305</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D23" s="4">
         <v>4</v>
@@ -5566,17 +5499,17 @@
         <v>95</v>
       </c>
       <c r="G23">
-        <v>11000004</v>
+        <v>11000005</v>
       </c>
       <c r="H23" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -5584,7 +5517,7 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="R23" s="4" t="s">
         <v>198</v>
@@ -5596,35 +5529,33 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>43020311</v>
+        <v>43020306</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D24" s="4">
-        <v>4</v>
-      </c>
-      <c r="E24" s="33">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E24" s="33"/>
       <c r="F24" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G24">
-        <v>11000005</v>
+        <v>11000008</v>
       </c>
       <c r="H24" s="4">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
@@ -5632,7 +5563,7 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="R24" s="4" t="s">
         <v>198</v>
@@ -5644,35 +5575,35 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>43020403</v>
+        <v>43020307</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="D25" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E25" s="33">
         <v>2</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="G25">
-        <v>11000002</v>
+        <v>11000001</v>
       </c>
       <c r="H25" s="4">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -5680,7 +5611,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="R25" s="4" t="s">
         <v>198</v>
@@ -5692,35 +5623,35 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>43020502</v>
+        <v>43020308</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="D26" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E26" s="33">
         <v>2</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="G26">
-        <v>11000002</v>
+        <v>11000001</v>
       </c>
       <c r="H26" s="4">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
@@ -5728,7 +5659,7 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="R26" s="4" t="s">
         <v>198</v>
@@ -5740,35 +5671,35 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>43020106</v>
+        <v>43020309</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="D27" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E27" s="33">
         <v>2</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="G27">
-        <v>11000005</v>
+        <v>11000004</v>
       </c>
       <c r="H27" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -5776,7 +5707,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="R27" s="4" t="s">
         <v>198</v>
@@ -5788,35 +5719,35 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>43020304</v>
+        <v>43020310</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="D28" s="4">
         <v>4</v>
       </c>
       <c r="E28" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>95</v>
       </c>
       <c r="G28">
-        <v>11000002</v>
+        <v>11000003</v>
       </c>
       <c r="H28" s="4">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -5824,7 +5755,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>198</v>
@@ -5836,13 +5767,13 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>43020305</v>
+        <v>43020311</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="D29" s="4">
         <v>4</v>
@@ -5857,14 +5788,14 @@
         <v>11000005</v>
       </c>
       <c r="H29" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
@@ -5872,7 +5803,7 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="R29" s="4" t="s">
         <v>198</v>
@@ -5884,35 +5815,35 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>43020404</v>
+        <v>43020312</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D30" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E30" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="G30">
         <v>11000001</v>
       </c>
       <c r="H30" s="4">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
@@ -5920,7 +5851,7 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>198</v>
@@ -5932,35 +5863,35 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>43020107</v>
+        <v>43020401</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="D31" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E31" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="G31">
-        <v>11000007</v>
+        <v>11000002</v>
       </c>
       <c r="H31" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
@@ -5968,7 +5899,7 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="R31" s="4" t="s">
         <v>198</v>
@@ -5980,35 +5911,35 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>43020406</v>
+        <v>43020402</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D32" s="4">
         <v>5</v>
       </c>
       <c r="E32" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>116</v>
       </c>
       <c r="G32">
-        <v>11000006</v>
+        <v>11000001</v>
       </c>
       <c r="H32" s="4">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
@@ -6016,7 +5947,7 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="R32" s="4" t="s">
         <v>198</v>
@@ -6028,35 +5959,35 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>43020501</v>
+        <v>43020403</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="D33" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E33" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="G33">
-        <v>11000003</v>
+        <v>11000002</v>
       </c>
       <c r="H33" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -6064,7 +5995,7 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="R33" s="4" t="s">
         <v>198</v>
@@ -6076,35 +6007,35 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>43020202</v>
+        <v>43020404</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="D34" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E34" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="G34">
         <v>11000001</v>
       </c>
       <c r="H34" s="4">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -6112,7 +6043,7 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="R34" s="4" t="s">
         <v>198</v>
@@ -6124,25 +6055,25 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>43020108</v>
+        <v>43020405</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="D35" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E35" s="33">
         <v>3</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="G35">
-        <v>11000005</v>
+        <v>11000007</v>
       </c>
       <c r="H35" s="4">
         <v>18</v>
@@ -6152,7 +6083,7 @@
         <v>2</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
@@ -6160,7 +6091,7 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>198</v>
@@ -6172,35 +6103,35 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>43020312</v>
+        <v>43020406</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="D36" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E36" s="33">
         <v>3</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="G36">
-        <v>11000001</v>
+        <v>11000006</v>
       </c>
       <c r="H36" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
@@ -6208,7 +6139,7 @@
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="R36" s="4" t="s">
         <v>198</v>
@@ -6220,35 +6151,35 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>43020405</v>
+        <v>43020407</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D37" s="4">
         <v>5</v>
       </c>
       <c r="E37" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>116</v>
       </c>
       <c r="G37">
-        <v>11000007</v>
+        <v>11000004</v>
       </c>
       <c r="H37" s="4">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
@@ -6256,7 +6187,7 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>198</v>
@@ -6268,35 +6199,35 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>43020504</v>
+        <v>43020408</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D38" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E38" s="33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="G38">
-        <v>11000001</v>
+        <v>11000002</v>
       </c>
       <c r="H38" s="4">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
@@ -6304,7 +6235,7 @@
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="R38" s="4" t="s">
         <v>198</v>
@@ -6316,35 +6247,35 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>43020109</v>
+        <v>43020501</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="D39" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E39" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="G39">
-        <v>11000006</v>
+        <v>11000003</v>
       </c>
       <c r="H39" s="4">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -6352,7 +6283,7 @@
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="R39" s="4" t="s">
         <v>198</v>
@@ -6364,35 +6295,35 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>43020201</v>
+        <v>43020502</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="D40" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E40" s="33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="G40">
-        <v>11000007</v>
+        <v>11000002</v>
       </c>
       <c r="H40" s="4">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -6400,7 +6331,7 @@
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="R40" s="4" t="s">
         <v>198</v>
@@ -6412,35 +6343,35 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>43020203</v>
+        <v>43020503</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="D41" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E41" s="33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="G41">
-        <v>11000002</v>
+        <v>11000008</v>
       </c>
       <c r="H41" s="4">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
@@ -6448,7 +6379,7 @@
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="4" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="R41" s="4" t="s">
         <v>198</v>
@@ -6460,35 +6391,35 @@
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A42">
-        <v>43020110</v>
+        <v>43020504</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
       <c r="D42" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E42" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="G42">
-        <v>11000006</v>
+        <v>11000001</v>
       </c>
       <c r="H42" s="4">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
@@ -6496,7 +6427,7 @@
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
       <c r="R42" s="4" t="s">
         <v>198</v>

</xml_diff>

<commit_message>
add a new people
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="人物" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="333">
   <si>
     <t>老鼠</t>
   </si>
@@ -1145,6 +1145,18 @@
   </si>
   <si>
     <t>品质</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kini</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>基尼星</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cai</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2032,35 +2044,50 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="84">
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2154,62 +2181,6 @@
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2613,6 +2584,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -3180,6 +3180,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -3791,6 +3820,33 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -3957,96 +4013,96 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:T42" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" tableBorderDxfId="77">
-  <autoFilter ref="A3:T42"/>
-  <sortState ref="A4:T42">
-    <sortCondition ref="A3:A42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:T43" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" tableBorderDxfId="81">
+  <autoFilter ref="A3:T43"/>
+  <sortState ref="A4:T43">
+    <sortCondition ref="A3:A43"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="76"/>
-    <tableColumn id="2" name="Name" dataDxfId="75"/>
-    <tableColumn id="18" name="Ename" dataDxfId="74"/>
-    <tableColumn id="3" name="Type" dataDxfId="73"/>
-    <tableColumn id="21" name="Quality" dataDxfId="13"/>
-    <tableColumn id="6" name="World" dataDxfId="72"/>
-    <tableColumn id="10" name="Job" dataDxfId="71"/>
-    <tableColumn id="11" name="Level" dataDxfId="70"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="69"/>
-    <tableColumn id="13" name="Method" dataDxfId="68"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="67"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="66"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="65"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="64"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="63"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="62"/>
-    <tableColumn id="17" name="Figue" dataDxfId="61"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="60"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="59"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="58"/>
+    <tableColumn id="1" name="Id" dataDxfId="80"/>
+    <tableColumn id="2" name="Name" dataDxfId="79"/>
+    <tableColumn id="18" name="Ename" dataDxfId="78"/>
+    <tableColumn id="3" name="Type" dataDxfId="77"/>
+    <tableColumn id="21" name="Quality" dataDxfId="76"/>
+    <tableColumn id="6" name="World" dataDxfId="75"/>
+    <tableColumn id="10" name="Job" dataDxfId="74"/>
+    <tableColumn id="11" name="Level" dataDxfId="73"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="72"/>
+    <tableColumn id="13" name="Method" dataDxfId="71"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="70"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="69"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="68"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="67"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="66"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="65"/>
+    <tableColumn id="17" name="Figue" dataDxfId="64"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="63"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="62"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58">
   <autoFilter ref="A3:T50"/>
   <sortState ref="A4:R48">
     <sortCondition ref="A3:A48"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="54"/>
-    <tableColumn id="2" name="Name" dataDxfId="53"/>
-    <tableColumn id="18" name="Ename" dataDxfId="52"/>
-    <tableColumn id="3" name="Type" dataDxfId="51"/>
-    <tableColumn id="7" name="Quality" dataDxfId="12"/>
-    <tableColumn id="6" name="World" dataDxfId="50"/>
-    <tableColumn id="10" name="Job" dataDxfId="49"/>
-    <tableColumn id="11" name="Level" dataDxfId="48"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="47"/>
-    <tableColumn id="13" name="Method" dataDxfId="46"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="45"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="44"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="43"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="42"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="41"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="40"/>
-    <tableColumn id="17" name="Figue" dataDxfId="39"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="38"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="37"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="36"/>
+    <tableColumn id="1" name="Id" dataDxfId="57"/>
+    <tableColumn id="2" name="Name" dataDxfId="56"/>
+    <tableColumn id="18" name="Ename" dataDxfId="55"/>
+    <tableColumn id="3" name="Type" dataDxfId="54"/>
+    <tableColumn id="7" name="Quality" dataDxfId="53"/>
+    <tableColumn id="6" name="World" dataDxfId="52"/>
+    <tableColumn id="10" name="Job" dataDxfId="51"/>
+    <tableColumn id="11" name="Level" dataDxfId="50"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="49"/>
+    <tableColumn id="13" name="Method" dataDxfId="48"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="47"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="46"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="45"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="44"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="43"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="42"/>
+    <tableColumn id="17" name="Figue" dataDxfId="41"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="40"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="39"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:T14" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:T14" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" tableBorderDxfId="35">
   <autoFilter ref="A3:T14"/>
   <sortState ref="A4:R83">
     <sortCondition ref="A3:A83"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="32"/>
-    <tableColumn id="2" name="Name" dataDxfId="31"/>
-    <tableColumn id="18" name="Ename" dataDxfId="30"/>
-    <tableColumn id="3" name="Type" dataDxfId="29"/>
-    <tableColumn id="7" name="Quality" dataDxfId="0"/>
-    <tableColumn id="6" name="World" dataDxfId="28"/>
-    <tableColumn id="10" name="Job" dataDxfId="27"/>
-    <tableColumn id="11" name="Level" dataDxfId="26"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="25"/>
-    <tableColumn id="13" name="Method" dataDxfId="24"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="23"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="22"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="21"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="20"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="19"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="18"/>
-    <tableColumn id="9" name="Figue" dataDxfId="17"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="16"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="15"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="14"/>
+    <tableColumn id="1" name="Id" dataDxfId="34"/>
+    <tableColumn id="2" name="Name" dataDxfId="33"/>
+    <tableColumn id="18" name="Ename" dataDxfId="32"/>
+    <tableColumn id="3" name="Type" dataDxfId="31"/>
+    <tableColumn id="7" name="Quality" dataDxfId="30"/>
+    <tableColumn id="6" name="World" dataDxfId="29"/>
+    <tableColumn id="10" name="Job" dataDxfId="28"/>
+    <tableColumn id="11" name="Level" dataDxfId="27"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="26"/>
+    <tableColumn id="13" name="Method" dataDxfId="25"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="24"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="23"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="22"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="21"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="20"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="19"/>
+    <tableColumn id="9" name="Figue" dataDxfId="18"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="17"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="16"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4373,13 +4429,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T42"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O3" sqref="O1:O3"/>
+      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6205,7 +6261,7 @@
         <v>130</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>131</v>
+        <v>332</v>
       </c>
       <c r="D38" s="4">
         <v>5</v>
@@ -6247,35 +6303,35 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>43020501</v>
+        <v>43020409</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>132</v>
+        <v>331</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>134</v>
+        <v>330</v>
       </c>
       <c r="D39" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E39" s="33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="G39">
-        <v>11000003</v>
+        <v>11000002</v>
       </c>
       <c r="H39" s="4">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>134</v>
+        <v>330</v>
       </c>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -6283,7 +6339,7 @@
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4" t="s">
-        <v>134</v>
+        <v>330</v>
       </c>
       <c r="R39" s="4" t="s">
         <v>198</v>
@@ -6295,35 +6351,35 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>43020502</v>
+        <v>43020501</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D40" s="4">
         <v>6</v>
       </c>
       <c r="E40" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>133</v>
       </c>
       <c r="G40">
-        <v>11000002</v>
+        <v>11000003</v>
       </c>
       <c r="H40" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -6331,7 +6387,7 @@
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R40" s="4" t="s">
         <v>198</v>
@@ -6343,35 +6399,35 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>43020503</v>
+        <v>43020502</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D41" s="4">
         <v>6</v>
       </c>
       <c r="E41" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>133</v>
       </c>
       <c r="G41">
-        <v>11000008</v>
+        <v>11000002</v>
       </c>
       <c r="H41" s="4">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
@@ -6379,7 +6435,7 @@
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R41" s="4" t="s">
         <v>198</v>
@@ -6391,35 +6447,35 @@
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A42">
-        <v>43020504</v>
+        <v>43020503</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D42" s="4">
         <v>6</v>
       </c>
       <c r="E42" s="33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>133</v>
       </c>
       <c r="G42">
-        <v>11000001</v>
+        <v>11000008</v>
       </c>
       <c r="H42" s="4">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
@@ -6427,7 +6483,7 @@
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="R42" s="4" t="s">
         <v>198</v>
@@ -6437,19 +6493,81 @@
         <v>233</v>
       </c>
     </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>43020504</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="4">
+        <v>6</v>
+      </c>
+      <c r="E43" s="33">
+        <v>3</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G43">
+        <v>11000001</v>
+      </c>
+      <c r="H43" s="4">
+        <v>19</v>
+      </c>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="R43" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="S43" s="13"/>
+      <c r="T43" s="19" t="s">
+        <v>233</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="E4:E42">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+  <conditionalFormatting sqref="E4:E38 E40:E43">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6465,11 +6583,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O3" sqref="O1:O3"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9036,37 +9154,37 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="R42">
-    <cfRule type="containsBlanks" dxfId="7" priority="7">
+    <cfRule type="containsBlanks" dxfId="10" priority="7">
       <formula>LEN(TRIM(R42))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsBlanks" dxfId="6" priority="6">
+    <cfRule type="containsBlanks" dxfId="9" priority="6">
       <formula>LEN(TRIM(C47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="containsBlanks" dxfId="5" priority="5">
+    <cfRule type="containsBlanks" dxfId="8" priority="5">
       <formula>LEN(TRIM(K47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q47">
-    <cfRule type="containsBlanks" dxfId="4" priority="4">
+    <cfRule type="containsBlanks" dxfId="7" priority="4">
       <formula>LEN(TRIM(Q47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C50">
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
+    <cfRule type="containsBlanks" dxfId="6" priority="3">
       <formula>LEN(TRIM(C48))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:K50">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
+    <cfRule type="containsBlanks" dxfId="5" priority="2">
       <formula>LEN(TRIM(K48))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q48:Q50">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="4" priority="1">
       <formula>LEN(TRIM(Q48))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add some new decks
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="437">
   <si>
     <t>老鼠</t>
   </si>
@@ -1450,6 +1450,42 @@
   </si>
   <si>
     <t>humagat</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>humkongque</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kongque</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>孔雀舞</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>十六夜秋</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shiliu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>humshiliu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>roy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>罗伊</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>humroy</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2340,7 +2376,51 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="100">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4439,96 +4519,96 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:T48" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94" tableBorderDxfId="93">
-  <autoFilter ref="A3:T48"/>
-  <sortState ref="A4:T48">
-    <sortCondition ref="A3:A48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:T51" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98" tableBorderDxfId="97">
+  <autoFilter ref="A3:T51"/>
+  <sortState ref="A4:T50">
+    <sortCondition ref="A3:A50"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="92"/>
-    <tableColumn id="2" name="Name" dataDxfId="91"/>
-    <tableColumn id="18" name="Ename" dataDxfId="90"/>
-    <tableColumn id="3" name="Type" dataDxfId="89"/>
-    <tableColumn id="21" name="Quality" dataDxfId="88"/>
-    <tableColumn id="6" name="World" dataDxfId="87"/>
-    <tableColumn id="10" name="Job" dataDxfId="86"/>
-    <tableColumn id="11" name="Level" dataDxfId="85"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="84"/>
-    <tableColumn id="13" name="Method" dataDxfId="83"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="82"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="81"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="80"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="79"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="78"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="77"/>
-    <tableColumn id="17" name="Figue" dataDxfId="76"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="75"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="74"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="73"/>
+    <tableColumn id="1" name="Id" dataDxfId="96"/>
+    <tableColumn id="2" name="Name" dataDxfId="95"/>
+    <tableColumn id="18" name="Ename" dataDxfId="94"/>
+    <tableColumn id="3" name="Type" dataDxfId="93"/>
+    <tableColumn id="21" name="Quality" dataDxfId="92"/>
+    <tableColumn id="6" name="World" dataDxfId="91"/>
+    <tableColumn id="10" name="Job" dataDxfId="90"/>
+    <tableColumn id="11" name="Level" dataDxfId="89"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="88"/>
+    <tableColumn id="13" name="Method" dataDxfId="87"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="86"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="85"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="84"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="83"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="82"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="81"/>
+    <tableColumn id="17" name="Figue" dataDxfId="80"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="79"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="78"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75" tableBorderDxfId="74">
   <autoFilter ref="A3:T50"/>
   <sortState ref="A4:R48">
     <sortCondition ref="A3:A48"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="69"/>
-    <tableColumn id="2" name="Name" dataDxfId="68"/>
-    <tableColumn id="18" name="Ename" dataDxfId="67"/>
-    <tableColumn id="3" name="Type" dataDxfId="66"/>
-    <tableColumn id="7" name="Quality" dataDxfId="65"/>
-    <tableColumn id="6" name="World" dataDxfId="64"/>
-    <tableColumn id="10" name="Job" dataDxfId="63"/>
-    <tableColumn id="11" name="Level" dataDxfId="62"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="61"/>
-    <tableColumn id="13" name="Method" dataDxfId="60"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="59"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="58"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="57"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="56"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="55"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="54"/>
-    <tableColumn id="17" name="Figue" dataDxfId="53"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="52"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="51"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="50"/>
+    <tableColumn id="1" name="Id" dataDxfId="73"/>
+    <tableColumn id="2" name="Name" dataDxfId="72"/>
+    <tableColumn id="18" name="Ename" dataDxfId="71"/>
+    <tableColumn id="3" name="Type" dataDxfId="70"/>
+    <tableColumn id="7" name="Quality" dataDxfId="69"/>
+    <tableColumn id="6" name="World" dataDxfId="68"/>
+    <tableColumn id="10" name="Job" dataDxfId="67"/>
+    <tableColumn id="11" name="Level" dataDxfId="66"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="65"/>
+    <tableColumn id="13" name="Method" dataDxfId="64"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="63"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="62"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="61"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="60"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="59"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="58"/>
+    <tableColumn id="17" name="Figue" dataDxfId="57"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="56"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="55"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:T14" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48" tableBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:T14" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52" tableBorderDxfId="51">
   <autoFilter ref="A3:T14"/>
   <sortState ref="A4:R83">
     <sortCondition ref="A3:A83"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="46"/>
-    <tableColumn id="2" name="Name" dataDxfId="45"/>
-    <tableColumn id="18" name="Ename" dataDxfId="44"/>
-    <tableColumn id="3" name="Type" dataDxfId="43"/>
-    <tableColumn id="7" name="Quality" dataDxfId="42"/>
-    <tableColumn id="6" name="World" dataDxfId="41"/>
-    <tableColumn id="10" name="Job" dataDxfId="40"/>
-    <tableColumn id="11" name="Level" dataDxfId="39"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="38"/>
-    <tableColumn id="13" name="Method" dataDxfId="37"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="36"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="35"/>
-    <tableColumn id="12" name="EpSlow" dataDxfId="34"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="33"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="32"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="31"/>
-    <tableColumn id="9" name="Figue" dataDxfId="30"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="29"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="28"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="27"/>
+    <tableColumn id="1" name="Id" dataDxfId="50"/>
+    <tableColumn id="2" name="Name" dataDxfId="49"/>
+    <tableColumn id="18" name="Ename" dataDxfId="48"/>
+    <tableColumn id="3" name="Type" dataDxfId="47"/>
+    <tableColumn id="7" name="Quality" dataDxfId="46"/>
+    <tableColumn id="6" name="World" dataDxfId="45"/>
+    <tableColumn id="10" name="Job" dataDxfId="44"/>
+    <tableColumn id="11" name="Level" dataDxfId="43"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="42"/>
+    <tableColumn id="13" name="Method" dataDxfId="41"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="40"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="39"/>
+    <tableColumn id="12" name="EpSlow" dataDxfId="38"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="37"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="36"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="35"/>
+    <tableColumn id="9" name="Figue" dataDxfId="34"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="33"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="32"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4855,13 +4935,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T48"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G43" sqref="G43"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5773,35 +5853,35 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>43020301</v>
+        <v>43020206</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>412</v>
+        <v>430</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>411</v>
+        <v>429</v>
       </c>
       <c r="D19" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" s="33">
         <v>1</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G19" s="34">
-        <v>11000005</v>
+        <v>11000003</v>
       </c>
       <c r="H19" s="4">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
@@ -5809,7 +5889,7 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
       <c r="R19" s="4" t="s">
         <v>179</v>
@@ -5821,35 +5901,35 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>43020302</v>
+        <v>43020207</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>414</v>
+        <v>432</v>
       </c>
       <c r="D20" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G20" s="34">
-        <v>11000006</v>
+        <v>11000007</v>
       </c>
       <c r="H20" s="4">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>415</v>
+        <v>433</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
@@ -5857,7 +5937,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4" t="s">
-        <v>415</v>
+        <v>433</v>
       </c>
       <c r="R20" s="4" t="s">
         <v>179</v>
@@ -5869,33 +5949,35 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>43020303</v>
+        <v>43020301</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>85</v>
+        <v>412</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>87</v>
+        <v>411</v>
       </c>
       <c r="D21" s="4">
         <v>3</v>
       </c>
-      <c r="E21" s="33"/>
+      <c r="E21" s="33">
+        <v>1</v>
+      </c>
       <c r="F21" s="4" t="s">
         <v>86</v>
       </c>
       <c r="G21" s="34">
-        <v>11000004</v>
+        <v>11000005</v>
       </c>
       <c r="H21" s="4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>378</v>
+        <v>420</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
@@ -5903,7 +5985,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4" t="s">
-        <v>378</v>
+        <v>410</v>
       </c>
       <c r="R21" s="4" t="s">
         <v>179</v>
@@ -5915,35 +5997,35 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>43020304</v>
+        <v>43020302</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>88</v>
+        <v>413</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>89</v>
+        <v>414</v>
       </c>
       <c r="D22" s="4">
         <v>3</v>
       </c>
       <c r="E22" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>86</v>
       </c>
       <c r="G22" s="34">
-        <v>11000002</v>
+        <v>11000006</v>
       </c>
       <c r="H22" s="4">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>379</v>
+        <v>415</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -5951,7 +6033,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4" t="s">
-        <v>379</v>
+        <v>415</v>
       </c>
       <c r="R22" s="4" t="s">
         <v>179</v>
@@ -5963,35 +6045,33 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>43020305</v>
+        <v>43020303</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D23" s="4">
         <v>3</v>
       </c>
-      <c r="E23" s="33">
-        <v>2</v>
-      </c>
+      <c r="E23" s="33"/>
       <c r="F23" s="4" t="s">
         <v>86</v>
       </c>
       <c r="G23" s="34">
-        <v>11000005</v>
+        <v>11000004</v>
       </c>
       <c r="H23" s="4">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -5999,7 +6079,7 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="R23" s="4" t="s">
         <v>179</v>
@@ -6011,35 +6091,35 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>43020306</v>
+        <v>43020304</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>419</v>
+        <v>88</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>417</v>
+        <v>89</v>
       </c>
       <c r="D24" s="4">
         <v>3</v>
       </c>
       <c r="E24" s="33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>86</v>
       </c>
       <c r="G24" s="34">
-        <v>11000004</v>
+        <v>11000002</v>
       </c>
       <c r="H24" s="4">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>421</v>
+        <v>379</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
@@ -6047,7 +6127,7 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4" t="s">
-        <v>416</v>
+        <v>379</v>
       </c>
       <c r="R24" s="4" t="s">
         <v>179</v>
@@ -6059,13 +6139,13 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>43020307</v>
+        <v>43020305</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>418</v>
+        <v>90</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D25" s="4">
         <v>3</v>
@@ -6077,17 +6157,17 @@
         <v>86</v>
       </c>
       <c r="G25" s="34">
-        <v>11000001</v>
+        <v>11000005</v>
       </c>
       <c r="H25" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -6095,7 +6175,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="R25" s="4" t="s">
         <v>179</v>
@@ -6107,35 +6187,35 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>43020308</v>
+        <v>43020306</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>95</v>
+        <v>419</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>96</v>
+        <v>417</v>
       </c>
       <c r="D26" s="4">
         <v>3</v>
       </c>
       <c r="E26" s="33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>86</v>
       </c>
       <c r="G26" s="34">
-        <v>11000001</v>
+        <v>11000004</v>
       </c>
       <c r="H26" s="4">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>383</v>
+        <v>421</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
@@ -6143,7 +6223,7 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4" t="s">
-        <v>383</v>
+        <v>416</v>
       </c>
       <c r="R26" s="4" t="s">
         <v>179</v>
@@ -6155,13 +6235,13 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>43020309</v>
+        <v>43020307</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>97</v>
+        <v>418</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D27" s="4">
         <v>3</v>
@@ -6173,17 +6253,17 @@
         <v>86</v>
       </c>
       <c r="G27" s="34">
-        <v>11000004</v>
+        <v>11000001</v>
       </c>
       <c r="H27" s="4">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -6191,7 +6271,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="R27" s="4" t="s">
         <v>179</v>
@@ -6203,35 +6283,35 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>43020310</v>
+        <v>43020308</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D28" s="4">
         <v>3</v>
       </c>
       <c r="E28" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>86</v>
       </c>
       <c r="G28" s="34">
-        <v>11000003</v>
+        <v>11000001</v>
       </c>
       <c r="H28" s="4">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -6239,7 +6319,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>179</v>
@@ -6251,13 +6331,13 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>43020311</v>
+        <v>43020309</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D29" s="4">
         <v>3</v>
@@ -6269,7 +6349,7 @@
         <v>86</v>
       </c>
       <c r="G29" s="34">
-        <v>11000005</v>
+        <v>11000004</v>
       </c>
       <c r="H29" s="4">
         <v>19</v>
@@ -6279,7 +6359,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
@@ -6287,7 +6367,7 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="R29" s="4" t="s">
         <v>179</v>
@@ -6299,35 +6379,35 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>43020312</v>
+        <v>43020310</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D30" s="4">
         <v>3</v>
       </c>
       <c r="E30" s="33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>86</v>
       </c>
       <c r="G30" s="34">
-        <v>11000001</v>
+        <v>11000003</v>
       </c>
       <c r="H30" s="4">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
@@ -6335,7 +6415,7 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>179</v>
@@ -6347,35 +6427,35 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>43020401</v>
+        <v>43020311</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D31" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31" s="33">
         <v>2</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="G31" s="34">
-        <v>11000002</v>
+        <v>11000005</v>
       </c>
       <c r="H31" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
@@ -6383,7 +6463,7 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="R31" s="4" t="s">
         <v>179</v>
@@ -6395,35 +6475,35 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>43020402</v>
+        <v>43020312</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D32" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E32" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="G32" s="34">
-        <v>11000005</v>
+        <v>11000001</v>
       </c>
       <c r="H32" s="4">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
@@ -6431,7 +6511,7 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="R32" s="4" t="s">
         <v>179</v>
@@ -6443,13 +6523,13 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>43020403</v>
+        <v>43020401</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D33" s="4">
         <v>4</v>
@@ -6461,17 +6541,17 @@
         <v>106</v>
       </c>
       <c r="G33" s="34">
-        <v>11000010</v>
+        <v>11000002</v>
       </c>
       <c r="H33" s="4">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -6479,7 +6559,7 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="R33" s="4" t="s">
         <v>179</v>
@@ -6491,13 +6571,13 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>43020404</v>
+        <v>43020402</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D34" s="4">
         <v>4</v>
@@ -6509,17 +6589,17 @@
         <v>106</v>
       </c>
       <c r="G34" s="34">
-        <v>11000001</v>
+        <v>11000005</v>
       </c>
       <c r="H34" s="4">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -6527,7 +6607,7 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="R34" s="4" t="s">
         <v>179</v>
@@ -6539,35 +6619,35 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>43020405</v>
+        <v>43020403</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D35" s="4">
         <v>4</v>
       </c>
       <c r="E35" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>106</v>
       </c>
       <c r="G35" s="34">
-        <v>11000008</v>
+        <v>11000010</v>
       </c>
       <c r="H35" s="4">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
@@ -6575,7 +6655,7 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>179</v>
@@ -6587,35 +6667,35 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>43020406</v>
+        <v>43020404</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D36" s="4">
         <v>4</v>
       </c>
       <c r="E36" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>106</v>
       </c>
       <c r="G36" s="34">
-        <v>11000010</v>
+        <v>11000001</v>
       </c>
       <c r="H36" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
@@ -6623,7 +6703,7 @@
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="R36" s="4" t="s">
         <v>179</v>
@@ -6635,35 +6715,35 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>43020407</v>
+        <v>43020405</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D37" s="4">
         <v>4</v>
       </c>
       <c r="E37" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>106</v>
       </c>
       <c r="G37" s="34">
-        <v>11000004</v>
+        <v>11000008</v>
       </c>
       <c r="H37" s="4">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
@@ -6671,7 +6751,7 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>179</v>
@@ -6683,35 +6763,35 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>43020408</v>
+        <v>43020406</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>302</v>
+        <v>117</v>
       </c>
       <c r="D38" s="4">
         <v>4</v>
       </c>
       <c r="E38" s="33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>106</v>
       </c>
       <c r="G38" s="34">
-        <v>11000002</v>
+        <v>11000010</v>
       </c>
       <c r="H38" s="4">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
@@ -6719,7 +6799,7 @@
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="R38" s="4" t="s">
         <v>179</v>
@@ -6731,19 +6811,19 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>43020409</v>
+        <v>43020407</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>301</v>
+        <v>118</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>300</v>
+        <v>119</v>
       </c>
       <c r="D39" s="4">
         <v>4</v>
       </c>
       <c r="E39" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>106</v>
@@ -6752,14 +6832,14 @@
         <v>11000004</v>
       </c>
       <c r="H39" s="4">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -6767,7 +6847,7 @@
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="R39" s="4" t="s">
         <v>179</v>
@@ -6779,35 +6859,35 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>43020501</v>
+        <v>43020408</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>123</v>
+        <v>302</v>
       </c>
       <c r="D40" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E40" s="33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="G40" s="34">
-        <v>11000003</v>
+        <v>11000002</v>
       </c>
       <c r="H40" s="4">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -6815,7 +6895,7 @@
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="R40" s="4" t="s">
         <v>179</v>
@@ -6827,35 +6907,35 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>43020502</v>
+        <v>43020409</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>124</v>
+        <v>301</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>125</v>
+        <v>300</v>
       </c>
       <c r="D41" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E41" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="G41" s="34">
-        <v>11000002</v>
+        <v>11000004</v>
       </c>
       <c r="H41" s="4">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
@@ -6863,7 +6943,7 @@
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="R41" s="4" t="s">
         <v>179</v>
@@ -6875,35 +6955,35 @@
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A42">
-        <v>43020503</v>
+        <v>43020501</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D42" s="4">
         <v>5</v>
       </c>
       <c r="E42" s="33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>122</v>
       </c>
       <c r="G42" s="34">
-        <v>11000008</v>
+        <v>11000003</v>
       </c>
       <c r="H42" s="4">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
@@ -6911,7 +6991,7 @@
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="R42" s="4" t="s">
         <v>179</v>
@@ -6923,35 +7003,35 @@
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A43">
-        <v>43020504</v>
+        <v>43020502</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D43" s="4">
         <v>5</v>
       </c>
       <c r="E43" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>122</v>
       </c>
       <c r="G43" s="34">
-        <v>11000005</v>
+        <v>11000002</v>
       </c>
       <c r="H43" s="4">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
@@ -6959,7 +7039,7 @@
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="R43" s="4" t="s">
         <v>179</v>
@@ -6971,43 +7051,43 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A44">
-        <v>43020505</v>
+        <v>43020503</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>423</v>
+        <v>126</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="D44" s="27">
+        <v>127</v>
+      </c>
+      <c r="D44" s="4">
         <v>5</v>
       </c>
-      <c r="E44" s="4">
-        <v>2</v>
+      <c r="E44" s="33">
+        <v>1</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G44" s="29">
-        <v>11000001</v>
-      </c>
-      <c r="H44" s="27">
-        <v>16</v>
-      </c>
-      <c r="I44" s="27"/>
+      <c r="G44" s="34">
+        <v>11000008</v>
+      </c>
+      <c r="H44" s="4">
+        <v>13</v>
+      </c>
+      <c r="I44" s="4"/>
       <c r="J44" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K44" s="27" t="s">
-        <v>427</v>
+      <c r="K44" s="4" t="s">
+        <v>399</v>
       </c>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
-      <c r="O44" s="27"/>
-      <c r="P44" s="27"/>
-      <c r="Q44" s="27" t="s">
-        <v>427</v>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4" t="s">
+        <v>399</v>
       </c>
       <c r="R44" s="4" t="s">
         <v>179</v>
@@ -7019,43 +7099,43 @@
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A45">
-        <v>43020506</v>
+        <v>43020504</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>424</v>
+        <v>128</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="D45" s="27">
+        <v>129</v>
+      </c>
+      <c r="D45" s="4">
         <v>5</v>
       </c>
-      <c r="E45" s="4">
-        <v>1</v>
+      <c r="E45" s="33">
+        <v>3</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G45" s="29">
-        <v>11000004</v>
-      </c>
-      <c r="H45" s="27">
-        <v>10</v>
-      </c>
-      <c r="I45" s="27"/>
+      <c r="G45" s="34">
+        <v>11000005</v>
+      </c>
+      <c r="H45" s="4">
+        <v>28</v>
+      </c>
+      <c r="I45" s="4"/>
       <c r="J45" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K45" s="27" t="s">
-        <v>426</v>
+      <c r="K45" s="4" t="s">
+        <v>400</v>
       </c>
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
-      <c r="O45" s="27"/>
-      <c r="P45" s="27"/>
-      <c r="Q45" s="27" t="s">
-        <v>426</v>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4" t="s">
+        <v>400</v>
       </c>
       <c r="R45" s="4" t="s">
         <v>179</v>
@@ -7067,43 +7147,43 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A46">
-        <v>43020601</v>
+        <v>43020505</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>81</v>
+        <v>423</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="4">
-        <v>6</v>
-      </c>
-      <c r="E46" s="33">
-        <v>1</v>
+        <v>422</v>
+      </c>
+      <c r="D46" s="27">
+        <v>5</v>
+      </c>
+      <c r="E46" s="4">
+        <v>2</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="G46" s="34">
-        <v>11000002</v>
-      </c>
-      <c r="H46" s="4">
-        <v>7</v>
-      </c>
-      <c r="I46" s="4"/>
+        <v>122</v>
+      </c>
+      <c r="G46" s="29">
+        <v>11000001</v>
+      </c>
+      <c r="H46" s="27">
+        <v>16</v>
+      </c>
+      <c r="I46" s="27"/>
       <c r="J46" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K46" s="4" t="s">
-        <v>376</v>
+      <c r="K46" s="27" t="s">
+        <v>427</v>
       </c>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
-      <c r="Q46" s="4" t="s">
-        <v>376</v>
+      <c r="O46" s="27"/>
+      <c r="P46" s="27"/>
+      <c r="Q46" s="27" t="s">
+        <v>427</v>
       </c>
       <c r="R46" s="4" t="s">
         <v>179</v>
@@ -7115,41 +7195,43 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A47">
-        <v>43020602</v>
+        <v>43020506</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>83</v>
+        <v>424</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D47" s="4">
-        <v>6</v>
-      </c>
-      <c r="E47" s="33"/>
+        <v>425</v>
+      </c>
+      <c r="D47" s="27">
+        <v>5</v>
+      </c>
+      <c r="E47" s="4">
+        <v>1</v>
+      </c>
       <c r="F47" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="G47" s="34">
-        <v>11000010</v>
-      </c>
-      <c r="H47" s="4">
-        <v>4</v>
-      </c>
-      <c r="I47" s="4"/>
+        <v>122</v>
+      </c>
+      <c r="G47" s="29">
+        <v>11000004</v>
+      </c>
+      <c r="H47" s="27">
+        <v>10</v>
+      </c>
+      <c r="I47" s="27"/>
       <c r="J47" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K47" s="4" t="s">
-        <v>377</v>
+      <c r="K47" s="27" t="s">
+        <v>426</v>
       </c>
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4" t="s">
-        <v>377</v>
+      <c r="O47" s="27"/>
+      <c r="P47" s="27"/>
+      <c r="Q47" s="27" t="s">
+        <v>426</v>
       </c>
       <c r="R47" s="4" t="s">
         <v>179</v>
@@ -7161,18 +7243,20 @@
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A48">
-        <v>43020603</v>
+        <v>43020601</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="D48" s="4">
         <v>6</v>
       </c>
-      <c r="E48" s="33"/>
+      <c r="E48" s="33">
+        <v>1</v>
+      </c>
       <c r="F48" s="4" t="s">
         <v>409</v>
       </c>
@@ -7180,14 +7264,14 @@
         <v>11000002</v>
       </c>
       <c r="H48" s="4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
@@ -7195,7 +7279,7 @@
       <c r="O48" s="4"/>
       <c r="P48" s="4"/>
       <c r="Q48" s="4" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="R48" s="4" t="s">
         <v>179</v>
@@ -7205,75 +7289,229 @@
         <v>213</v>
       </c>
     </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>43020602</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" s="4">
+        <v>6</v>
+      </c>
+      <c r="E49" s="33"/>
+      <c r="F49" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="G49" s="34">
+        <v>11000010</v>
+      </c>
+      <c r="H49" s="4">
+        <v>4</v>
+      </c>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="R49" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="S49" s="13"/>
+      <c r="T49" s="19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>43020603</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="4">
+        <v>6</v>
+      </c>
+      <c r="E50" s="33"/>
+      <c r="F50" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="G50" s="34">
+        <v>11000002</v>
+      </c>
+      <c r="H50" s="4">
+        <v>1</v>
+      </c>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="R50" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="S50" s="13"/>
+      <c r="T50" s="19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>43020604</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="D51" s="4">
+        <v>6</v>
+      </c>
+      <c r="E51" s="33">
+        <v>1</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="G51" s="34">
+        <v>11000001</v>
+      </c>
+      <c r="H51" s="4">
+        <v>11</v>
+      </c>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="R51" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="S51" s="13"/>
+      <c r="T51" s="19" t="s">
+        <v>213</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="E4:E18 E21:E23 E25:E41 E43:E48">
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
+  <conditionalFormatting sqref="E23:E25 E27:E43 E4:E19 E45:E51">
+    <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="37" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
+  <conditionalFormatting sqref="E44">
+    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="31" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9860,37 +10098,37 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="R42">
-    <cfRule type="containsBlanks" dxfId="6" priority="9">
+    <cfRule type="containsBlanks" dxfId="10" priority="9">
       <formula>LEN(TRIM(R42))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsBlanks" dxfId="5" priority="8">
+    <cfRule type="containsBlanks" dxfId="9" priority="8">
       <formula>LEN(TRIM(C47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q47">
-    <cfRule type="containsBlanks" dxfId="4" priority="6">
+    <cfRule type="containsBlanks" dxfId="8" priority="6">
       <formula>LEN(TRIM(Q47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C50">
-    <cfRule type="containsBlanks" dxfId="3" priority="5">
+    <cfRule type="containsBlanks" dxfId="7" priority="5">
       <formula>LEN(TRIM(C48))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q48:Q50">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="6" priority="3">
       <formula>LEN(TRIM(Q48))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="5" priority="2">
       <formula>LEN(TRIM(K47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:K50">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="4" priority="1">
       <formula>LEN(TRIM(K48))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
optimise the elite and common
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D6C1358A-188C-469E-A316-37FCEFB3DAD6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EDF7F513-1A4C-4607-A86C-F500BE256CB7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2227,7 +2227,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2312,9 +2312,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -2331,6 +2328,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4555,8 +4561,8 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
   <autoFilter ref="A3:T50" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState ref="A4:R48">
-    <sortCondition ref="A3:A48"/>
+  <sortState ref="A4:T50">
+    <sortCondition ref="A3:A50"/>
   </sortState>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="42"/>
@@ -4940,7 +4946,7 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
@@ -5158,11 +5164,11 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="33">
         <v>11000001</v>
       </c>
       <c r="H4" s="4">
@@ -5202,11 +5208,11 @@
       <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="32"/>
       <c r="F5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="33">
         <v>11000003</v>
       </c>
       <c r="H5" s="4">
@@ -5246,13 +5252,13 @@
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="32">
         <v>1</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="33">
         <v>11000001</v>
       </c>
       <c r="H6" s="4">
@@ -5294,13 +5300,13 @@
       <c r="D7" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="32">
         <v>1</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="33">
         <v>11000008</v>
       </c>
       <c r="H7" s="4">
@@ -5340,13 +5346,13 @@
       <c r="D8" s="4">
         <v>1</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="32">
         <v>2</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="33">
         <v>11000002</v>
       </c>
       <c r="H8" s="4">
@@ -5388,13 +5394,13 @@
       <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="32">
         <v>2</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="33">
         <v>11000003</v>
       </c>
       <c r="H9" s="4">
@@ -5436,13 +5442,13 @@
       <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="32">
         <v>3</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="33">
         <v>11000007</v>
       </c>
       <c r="H10" s="4">
@@ -5484,13 +5490,13 @@
       <c r="D11" s="4">
         <v>1</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="32">
         <v>3</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="33">
         <v>11000009</v>
       </c>
       <c r="H11" s="4">
@@ -5532,13 +5538,13 @@
       <c r="D12" s="4">
         <v>1</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="32">
         <v>4</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="33">
         <v>11000004</v>
       </c>
       <c r="H12" s="4">
@@ -5580,13 +5586,13 @@
       <c r="D13" s="4">
         <v>1</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="32">
         <v>4</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="33">
         <v>11000006</v>
       </c>
       <c r="H13" s="4">
@@ -5628,13 +5634,13 @@
       <c r="D14" s="4">
         <v>2</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="32">
         <v>4</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="33">
         <v>11000007</v>
       </c>
       <c r="H14" s="4">
@@ -5676,13 +5682,13 @@
       <c r="D15" s="4">
         <v>2</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E15" s="32">
         <v>3</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="33">
         <v>11000001</v>
       </c>
       <c r="H15" s="4">
@@ -5724,13 +5730,13 @@
       <c r="D16" s="4">
         <v>2</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="32">
         <v>4</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="33">
         <v>11000002</v>
       </c>
       <c r="H16" s="4">
@@ -5772,13 +5778,13 @@
       <c r="D17" s="4">
         <v>2</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="32">
         <v>1</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="33">
         <v>11000009</v>
       </c>
       <c r="H17" s="4">
@@ -5820,11 +5826,11 @@
       <c r="D18" s="4">
         <v>2</v>
       </c>
-      <c r="E18" s="33"/>
+      <c r="E18" s="32"/>
       <c r="F18" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="33">
         <v>11000008</v>
       </c>
       <c r="H18" s="4">
@@ -5866,13 +5872,13 @@
       <c r="D19" s="4">
         <v>2</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="32">
         <v>1</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G19" s="33">
         <v>11000003</v>
       </c>
       <c r="H19" s="4">
@@ -5914,13 +5920,13 @@
       <c r="D20" s="4">
         <v>2</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="32">
         <v>2</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="33">
         <v>11000007</v>
       </c>
       <c r="H20" s="4">
@@ -5962,13 +5968,13 @@
       <c r="D21" s="4">
         <v>3</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="32">
         <v>1</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="33">
         <v>11000005</v>
       </c>
       <c r="H21" s="4">
@@ -6010,13 +6016,13 @@
       <c r="D22" s="4">
         <v>3</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="32">
         <v>3</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="33">
         <v>11000006</v>
       </c>
       <c r="H22" s="4">
@@ -6058,11 +6064,11 @@
       <c r="D23" s="4">
         <v>3</v>
       </c>
-      <c r="E23" s="33"/>
+      <c r="E23" s="32"/>
       <c r="F23" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="33">
         <v>11000004</v>
       </c>
       <c r="H23" s="4">
@@ -6104,13 +6110,13 @@
       <c r="D24" s="4">
         <v>3</v>
       </c>
-      <c r="E24" s="33">
+      <c r="E24" s="32">
         <v>2</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G24" s="34">
+      <c r="G24" s="33">
         <v>11000002</v>
       </c>
       <c r="H24" s="4">
@@ -6152,13 +6158,13 @@
       <c r="D25" s="4">
         <v>3</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="32">
         <v>2</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="33">
         <v>11000005</v>
       </c>
       <c r="H25" s="4">
@@ -6200,13 +6206,13 @@
       <c r="D26" s="4">
         <v>3</v>
       </c>
-      <c r="E26" s="33">
+      <c r="E26" s="32">
         <v>4</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G26" s="34">
+      <c r="G26" s="33">
         <v>11000004</v>
       </c>
       <c r="H26" s="4">
@@ -6248,13 +6254,13 @@
       <c r="D27" s="4">
         <v>3</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="32">
         <v>2</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G27" s="33">
         <v>11000001</v>
       </c>
       <c r="H27" s="4">
@@ -6296,13 +6302,13 @@
       <c r="D28" s="4">
         <v>3</v>
       </c>
-      <c r="E28" s="33">
+      <c r="E28" s="32">
         <v>2</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G28" s="34">
+      <c r="G28" s="33">
         <v>11000001</v>
       </c>
       <c r="H28" s="4">
@@ -6344,13 +6350,13 @@
       <c r="D29" s="4">
         <v>3</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E29" s="32">
         <v>2</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G29" s="34">
+      <c r="G29" s="33">
         <v>11000004</v>
       </c>
       <c r="H29" s="4">
@@ -6392,13 +6398,13 @@
       <c r="D30" s="4">
         <v>3</v>
       </c>
-      <c r="E30" s="33">
+      <c r="E30" s="32">
         <v>1</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G30" s="34">
+      <c r="G30" s="33">
         <v>11000003</v>
       </c>
       <c r="H30" s="4">
@@ -6440,13 +6446,13 @@
       <c r="D31" s="4">
         <v>3</v>
       </c>
-      <c r="E31" s="33">
+      <c r="E31" s="32">
         <v>2</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G31" s="34">
+      <c r="G31" s="33">
         <v>11000005</v>
       </c>
       <c r="H31" s="4">
@@ -6488,13 +6494,13 @@
       <c r="D32" s="4">
         <v>3</v>
       </c>
-      <c r="E32" s="33">
+      <c r="E32" s="32">
         <v>3</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G32" s="34">
+      <c r="G32" s="33">
         <v>11000001</v>
       </c>
       <c r="H32" s="4">
@@ -6536,13 +6542,13 @@
       <c r="D33" s="4">
         <v>4</v>
       </c>
-      <c r="E33" s="33">
+      <c r="E33" s="32">
         <v>2</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G33" s="34">
+      <c r="G33" s="33">
         <v>11000002</v>
       </c>
       <c r="H33" s="4">
@@ -6584,13 +6590,13 @@
       <c r="D34" s="4">
         <v>4</v>
       </c>
-      <c r="E34" s="33">
+      <c r="E34" s="32">
         <v>2</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G34" s="34">
+      <c r="G34" s="33">
         <v>11000005</v>
       </c>
       <c r="H34" s="4">
@@ -6632,13 +6638,13 @@
       <c r="D35" s="4">
         <v>4</v>
       </c>
-      <c r="E35" s="33">
+      <c r="E35" s="32">
         <v>2</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G35" s="34">
+      <c r="G35" s="33">
         <v>11000010</v>
       </c>
       <c r="H35" s="4">
@@ -6680,13 +6686,13 @@
       <c r="D36" s="4">
         <v>4</v>
       </c>
-      <c r="E36" s="33">
+      <c r="E36" s="32">
         <v>2</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G36" s="34">
+      <c r="G36" s="33">
         <v>11000001</v>
       </c>
       <c r="H36" s="4">
@@ -6728,13 +6734,13 @@
       <c r="D37" s="4">
         <v>4</v>
       </c>
-      <c r="E37" s="33">
+      <c r="E37" s="32">
         <v>3</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G37" s="34">
+      <c r="G37" s="33">
         <v>11000008</v>
       </c>
       <c r="H37" s="4">
@@ -6776,13 +6782,13 @@
       <c r="D38" s="4">
         <v>4</v>
       </c>
-      <c r="E38" s="33">
+      <c r="E38" s="32">
         <v>3</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G38" s="34">
+      <c r="G38" s="33">
         <v>11000010</v>
       </c>
       <c r="H38" s="4">
@@ -6824,13 +6830,13 @@
       <c r="D39" s="4">
         <v>4</v>
       </c>
-      <c r="E39" s="33">
+      <c r="E39" s="32">
         <v>2</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G39" s="34">
+      <c r="G39" s="33">
         <v>11000004</v>
       </c>
       <c r="H39" s="4">
@@ -6872,13 +6878,13 @@
       <c r="D40" s="4">
         <v>4</v>
       </c>
-      <c r="E40" s="33">
+      <c r="E40" s="32">
         <v>1</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G40" s="34">
+      <c r="G40" s="33">
         <v>11000002</v>
       </c>
       <c r="H40" s="4">
@@ -6920,13 +6926,13 @@
       <c r="D41" s="4">
         <v>4</v>
       </c>
-      <c r="E41" s="33">
+      <c r="E41" s="32">
         <v>1</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G41" s="34">
+      <c r="G41" s="33">
         <v>11000004</v>
       </c>
       <c r="H41" s="4">
@@ -6968,13 +6974,13 @@
       <c r="D42" s="4">
         <v>5</v>
       </c>
-      <c r="E42" s="33">
+      <c r="E42" s="32">
         <v>3</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G42" s="34">
+      <c r="G42" s="33">
         <v>11000003</v>
       </c>
       <c r="H42" s="4">
@@ -7016,13 +7022,13 @@
       <c r="D43" s="4">
         <v>5</v>
       </c>
-      <c r="E43" s="33">
+      <c r="E43" s="32">
         <v>2</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G43" s="34">
+      <c r="G43" s="33">
         <v>11000002</v>
       </c>
       <c r="H43" s="4">
@@ -7064,13 +7070,13 @@
       <c r="D44" s="4">
         <v>5</v>
       </c>
-      <c r="E44" s="33">
+      <c r="E44" s="32">
         <v>1</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G44" s="34">
+      <c r="G44" s="33">
         <v>11000008</v>
       </c>
       <c r="H44" s="4">
@@ -7112,13 +7118,13 @@
       <c r="D45" s="4">
         <v>5</v>
       </c>
-      <c r="E45" s="33">
+      <c r="E45" s="32">
         <v>3</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G45" s="34">
+      <c r="G45" s="33">
         <v>11000005</v>
       </c>
       <c r="H45" s="4">
@@ -7166,7 +7172,7 @@
       <c r="F46" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G46" s="29">
+      <c r="G46" s="28">
         <v>11000001</v>
       </c>
       <c r="H46" s="27">
@@ -7214,7 +7220,7 @@
       <c r="F47" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G47" s="29">
+      <c r="G47" s="28">
         <v>11000004</v>
       </c>
       <c r="H47" s="27">
@@ -7256,13 +7262,13 @@
       <c r="D48" s="4">
         <v>6</v>
       </c>
-      <c r="E48" s="33">
+      <c r="E48" s="32">
         <v>1</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="G48" s="34">
+      <c r="G48" s="33">
         <v>11000002</v>
       </c>
       <c r="H48" s="4">
@@ -7304,11 +7310,11 @@
       <c r="D49" s="4">
         <v>6</v>
       </c>
-      <c r="E49" s="33"/>
+      <c r="E49" s="32"/>
       <c r="F49" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="G49" s="34">
+      <c r="G49" s="33">
         <v>11000010</v>
       </c>
       <c r="H49" s="4">
@@ -7350,11 +7356,11 @@
       <c r="D50" s="4">
         <v>6</v>
       </c>
-      <c r="E50" s="33"/>
+      <c r="E50" s="32"/>
       <c r="F50" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="G50" s="34">
+      <c r="G50" s="33">
         <v>11000002</v>
       </c>
       <c r="H50" s="4">
@@ -7396,13 +7402,13 @@
       <c r="D51" s="4">
         <v>6</v>
       </c>
-      <c r="E51" s="33">
+      <c r="E51" s="32">
         <v>1</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="G51" s="34">
+      <c r="G51" s="33">
         <v>11000001</v>
       </c>
       <c r="H51" s="4">
@@ -7533,7 +7539,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K41" sqref="K41"/>
+      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7588,10 +7594,10 @@
       <c r="L1" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="29" t="s">
         <v>241</v>
       </c>
       <c r="O1" s="11" t="s">
@@ -7650,10 +7656,10 @@
       <c r="L2" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="30" t="s">
         <v>149</v>
       </c>
       <c r="O2" s="2" t="s">
@@ -7991,13 +7997,13 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>43000006</v>
+        <v>43000007</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
@@ -8010,44 +8016,44 @@
         <v>11001003</v>
       </c>
       <c r="H9" s="4">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="L9">
-        <v>51018006</v>
+        <v>51018005</v>
       </c>
       <c r="M9" s="4">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="N9" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>180</v>
+        <v>253</v>
       </c>
       <c r="S9" s="13"/>
       <c r="T9" s="17"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>43000007</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>12</v>
+        <v>43000008</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>263</v>
+        <v>14</v>
       </c>
       <c r="D10" s="4">
         <v>0</v>
@@ -8060,44 +8066,44 @@
         <v>11001003</v>
       </c>
       <c r="H10" s="4">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="L10">
-        <v>51018005</v>
+        <v>51018006</v>
       </c>
       <c r="M10" s="4">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="N10" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>253</v>
+        <v>180</v>
       </c>
       <c r="S10" s="13"/>
       <c r="T10" s="17"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>43000008</v>
+        <v>43000009</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11" s="4">
         <v>0</v>
@@ -8117,10 +8123,10 @@
         <v>2</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L11">
-        <v>51018006</v>
+        <v>51018005</v>
       </c>
       <c r="M11" s="4">
         <v>1</v>
@@ -8131,7 +8137,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>180</v>
@@ -8141,13 +8147,13 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>43000009</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>15</v>
+        <v>43000010</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>231</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D12" s="4">
         <v>0</v>
@@ -8160,14 +8166,14 @@
         <v>11001003</v>
       </c>
       <c r="H12" s="4">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="L12">
         <v>51018005</v>
@@ -8181,7 +8187,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="R12" s="4" t="s">
         <v>180</v>
@@ -8191,13 +8197,13 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>43000010</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>231</v>
+        <v>43000011</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D13" s="4">
         <v>0</v>
@@ -8210,14 +8216,14 @@
         <v>11001003</v>
       </c>
       <c r="H13" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="L13">
         <v>51018005</v>
@@ -8231,7 +8237,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>180</v>
@@ -8241,13 +8247,13 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>43000011</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>18</v>
+        <v>43000012</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D14" s="4">
         <v>0</v>
@@ -8260,14 +8266,14 @@
         <v>11001003</v>
       </c>
       <c r="H14" s="4">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="L14">
         <v>51018005</v>
@@ -8281,7 +8287,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>180</v>
@@ -8291,13 +8297,13 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>43000012</v>
+        <v>43000013</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D15" s="4">
         <v>0</v>
@@ -8310,14 +8316,14 @@
         <v>11001003</v>
       </c>
       <c r="H15" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="L15">
         <v>51018005</v>
@@ -8331,7 +8337,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="R15" s="4" t="s">
         <v>180</v>
@@ -8341,13 +8347,13 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>43000013</v>
+        <v>43000014</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D16" s="4">
         <v>0</v>
@@ -8360,14 +8366,14 @@
         <v>11001003</v>
       </c>
       <c r="H16" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="L16">
         <v>51018005</v>
@@ -8381,7 +8387,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>180</v>
@@ -8391,13 +8397,13 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>43000014</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>24</v>
+        <v>43000015</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D17" s="4">
         <v>0</v>
@@ -8417,7 +8423,7 @@
         <v>2</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="L17">
         <v>51018005</v>
@@ -8429,9 +8435,11 @@
         <v>15</v>
       </c>
       <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
+      <c r="P17" s="6" t="s">
+        <v>257</v>
+      </c>
       <c r="Q17" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="R17" s="4" t="s">
         <v>180</v>
@@ -8441,13 +8449,13 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>43000015</v>
+        <v>43000016</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>26</v>
+        <v>201</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>27</v>
+        <v>202</v>
       </c>
       <c r="D18" s="4">
         <v>0</v>
@@ -8460,17 +8468,17 @@
         <v>11001003</v>
       </c>
       <c r="H18" s="4">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="L18">
-        <v>51018005</v>
+        <v>51018007</v>
       </c>
       <c r="M18" s="4">
         <v>1</v>
@@ -8479,11 +8487,9 @@
         <v>15</v>
       </c>
       <c r="O18" s="4"/>
-      <c r="P18" s="6" t="s">
-        <v>257</v>
-      </c>
+      <c r="P18" s="4"/>
       <c r="Q18" s="4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="R18" s="4" t="s">
         <v>180</v>
@@ -8493,13 +8499,13 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>43000016</v>
+        <v>43000017</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>201</v>
+        <v>270</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>202</v>
+        <v>269</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
@@ -8512,14 +8518,14 @@
         <v>11001003</v>
       </c>
       <c r="H19" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L19">
         <v>51018007</v>
@@ -8533,7 +8539,7 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="R19" s="4" t="s">
         <v>180</v>
@@ -8543,13 +8549,13 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>43000017</v>
+        <v>43000018</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D20" s="4">
         <v>0</v>
@@ -8562,17 +8568,17 @@
         <v>11001003</v>
       </c>
       <c r="H20" s="4">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="L20">
-        <v>51018007</v>
+        <v>51018005</v>
       </c>
       <c r="M20" s="4">
         <v>1</v>
@@ -8583,7 +8589,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="R20" s="4" t="s">
         <v>180</v>
@@ -8593,13 +8599,13 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>43000018</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>232</v>
+        <v>43000019</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>262</v>
+        <v>29</v>
       </c>
       <c r="D21" s="4">
         <v>0</v>
@@ -8612,14 +8618,14 @@
         <v>11001003</v>
       </c>
       <c r="H21" s="4">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="L21">
         <v>51018005</v>
@@ -8633,7 +8639,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="R21" s="4" t="s">
         <v>180</v>
@@ -8643,13 +8649,13 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>43000019</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>28</v>
+        <v>43000020</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D22" s="4">
         <v>0</v>
@@ -8662,17 +8668,17 @@
         <v>11001003</v>
       </c>
       <c r="H22" s="4">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="L22">
-        <v>51018005</v>
+        <v>51018007</v>
       </c>
       <c r="M22" s="4">
         <v>1</v>
@@ -8683,7 +8689,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="R22" s="4" t="s">
         <v>180</v>
@@ -8693,13 +8699,13 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>43000020</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>30</v>
+        <v>43000021</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D23" s="4">
         <v>0</v>
@@ -8712,17 +8718,17 @@
         <v>11001003</v>
       </c>
       <c r="H23" s="4">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="L23">
-        <v>51018007</v>
+        <v>51018005</v>
       </c>
       <c r="M23" s="4">
         <v>1</v>
@@ -8733,7 +8739,7 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="R23" s="4" t="s">
         <v>180</v>
@@ -8743,13 +8749,13 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>43000021</v>
+        <v>43000022</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D24" s="4">
         <v>0</v>
@@ -8762,17 +8768,17 @@
         <v>11001003</v>
       </c>
       <c r="H24" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="L24">
-        <v>51018005</v>
+        <v>51018006</v>
       </c>
       <c r="M24" s="4">
         <v>1</v>
@@ -8783,7 +8789,7 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="R24" s="4" t="s">
         <v>180</v>
@@ -8793,13 +8799,13 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>43000022</v>
+        <v>43000023</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D25" s="4">
         <v>0</v>
@@ -8812,17 +8818,17 @@
         <v>11001003</v>
       </c>
       <c r="H25" s="4">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="L25">
-        <v>51018006</v>
+        <v>51018005</v>
       </c>
       <c r="M25" s="4">
         <v>1</v>
@@ -8833,7 +8839,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="R25" s="4" t="s">
         <v>180</v>
@@ -8843,13 +8849,13 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>43000023</v>
+        <v>43000024</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D26" s="4">
         <v>0</v>
@@ -8862,14 +8868,14 @@
         <v>11001003</v>
       </c>
       <c r="H26" s="4">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="L26">
         <v>51018005</v>
@@ -8883,7 +8889,7 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="R26" s="4" t="s">
         <v>180</v>
@@ -8893,13 +8899,13 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>43000024</v>
+        <v>43000025</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D27" s="4">
         <v>0</v>
@@ -8912,14 +8918,14 @@
         <v>11001003</v>
       </c>
       <c r="H27" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="L27">
         <v>51018005</v>
@@ -8933,7 +8939,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="R27" s="4" t="s">
         <v>180</v>
@@ -8943,13 +8949,13 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>43000025</v>
+        <v>43000026</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D28" s="4">
         <v>0</v>
@@ -8969,7 +8975,7 @@
         <v>2</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="L28">
         <v>51018005</v>
@@ -8983,7 +8989,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>180</v>
@@ -8993,13 +8999,13 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>43000026</v>
+        <v>43000027</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D29" s="4">
         <v>0</v>
@@ -9012,17 +9018,17 @@
         <v>11001003</v>
       </c>
       <c r="H29" s="4">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="L29">
-        <v>51018005</v>
+        <v>51018006</v>
       </c>
       <c r="M29" s="4">
         <v>1</v>
@@ -9033,7 +9039,7 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="R29" s="4" t="s">
         <v>180</v>
@@ -9043,13 +9049,13 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>43000027</v>
+        <v>43000028</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D30" s="4">
         <v>0</v>
@@ -9062,14 +9068,14 @@
         <v>11001003</v>
       </c>
       <c r="H30" s="4">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="L30">
         <v>51018006</v>
@@ -9083,7 +9089,7 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>180</v>
@@ -9093,13 +9099,13 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>43000028</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>46</v>
+        <v>43000029</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>47</v>
+        <v>273</v>
       </c>
       <c r="D31" s="4">
         <v>0</v>
@@ -9112,17 +9118,17 @@
         <v>11001003</v>
       </c>
       <c r="H31" s="4">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="L31">
-        <v>51018006</v>
+        <v>51018005</v>
       </c>
       <c r="M31" s="4">
         <v>1</v>
@@ -9133,7 +9139,7 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="R31" s="4" t="s">
         <v>180</v>
@@ -9143,13 +9149,13 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>43000029</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>48</v>
+        <v>43000030</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>273</v>
+        <v>50</v>
       </c>
       <c r="D32" s="4">
         <v>0</v>
@@ -9162,14 +9168,14 @@
         <v>11001003</v>
       </c>
       <c r="H32" s="4">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L32">
         <v>51018005</v>
@@ -9183,7 +9189,7 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="R32" s="4" t="s">
         <v>180</v>
@@ -9193,13 +9199,13 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>43000030</v>
+        <v>43000031</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D33" s="4">
         <v>0</v>
@@ -9212,14 +9218,14 @@
         <v>11001003</v>
       </c>
       <c r="H33" s="4">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="L33">
         <v>51018005</v>
@@ -9233,7 +9239,7 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="R33" s="4" t="s">
         <v>180</v>
@@ -9243,13 +9249,13 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>43000031</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>51</v>
+        <v>43000032</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>52</v>
+        <v>266</v>
       </c>
       <c r="D34" s="4">
         <v>0</v>
@@ -9262,14 +9268,14 @@
         <v>11001003</v>
       </c>
       <c r="H34" s="4">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L34">
         <v>51018005</v>
@@ -9283,7 +9289,7 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="R34" s="4" t="s">
         <v>180</v>
@@ -9293,13 +9299,13 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>43000032</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>53</v>
+        <v>43000033</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>266</v>
+        <v>55</v>
       </c>
       <c r="D35" s="4">
         <v>0</v>
@@ -9312,14 +9318,14 @@
         <v>11001003</v>
       </c>
       <c r="H35" s="4">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="L35">
         <v>51018005</v>
@@ -9333,7 +9339,7 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>180</v>
@@ -9343,13 +9349,13 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>43000033</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>54</v>
+        <v>43000035</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>55</v>
+        <v>217</v>
       </c>
       <c r="D36" s="4">
         <v>0</v>
@@ -9362,14 +9368,14 @@
         <v>11001003</v>
       </c>
       <c r="H36" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="L36">
         <v>51018005</v>
@@ -9383,7 +9389,7 @@
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="R36" s="4" t="s">
         <v>180</v>
@@ -9393,13 +9399,13 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>43000034</v>
+        <v>43000037</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>215</v>
+        <v>264</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>216</v>
+        <v>265</v>
       </c>
       <c r="D37" s="4">
         <v>0</v>
@@ -9419,7 +9425,7 @@
         <v>2</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>347</v>
+        <v>436</v>
       </c>
       <c r="L37">
         <v>51018005</v>
@@ -9433,23 +9439,23 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>180</v>
       </c>
       <c r="S37" s="13"/>
-      <c r="T37" s="17"/>
+      <c r="T37" s="13"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>43000035</v>
+        <v>43000038</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>218</v>
+        <v>267</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>217</v>
+        <v>268</v>
       </c>
       <c r="D38" s="4">
         <v>0</v>
@@ -9462,14 +9468,14 @@
         <v>11001003</v>
       </c>
       <c r="H38" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="L38">
         <v>51018005</v>
@@ -9483,23 +9489,23 @@
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="R38" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="S38" s="13"/>
-      <c r="T38" s="17"/>
+      <c r="S38" s="35"/>
+      <c r="T38" s="35"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>43000036</v>
+        <v>43001001</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>221</v>
+        <v>248</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>222</v>
+        <v>249</v>
       </c>
       <c r="D39" s="4">
         <v>0</v>
@@ -9512,14 +9518,14 @@
         <v>11001003</v>
       </c>
       <c r="H39" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="L39">
         <v>51018007</v>
@@ -9528,28 +9534,30 @@
         <v>1</v>
       </c>
       <c r="N39" s="4">
-        <v>15</v>
-      </c>
-      <c r="O39" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="O39" s="4" t="s">
+        <v>260</v>
+      </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="R39" s="4" t="s">
-        <v>180</v>
+        <v>352</v>
+      </c>
+      <c r="R39" s="6" t="s">
+        <v>254</v>
       </c>
       <c r="S39" s="13"/>
       <c r="T39" s="17"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>43000037</v>
+        <v>43001002</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="D40" s="4">
         <v>0</v>
@@ -9562,44 +9570,46 @@
         <v>11001003</v>
       </c>
       <c r="H40" s="4">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>436</v>
+        <v>353</v>
       </c>
       <c r="L40">
-        <v>51018005</v>
+        <v>51018007</v>
       </c>
       <c r="M40" s="4">
         <v>1</v>
       </c>
       <c r="N40" s="4">
-        <v>15</v>
-      </c>
-      <c r="O40" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>278</v>
+      </c>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="R40" s="4" t="s">
         <v>180</v>
       </c>
       <c r="S40" s="27"/>
-      <c r="T40" s="27"/>
+      <c r="T40" s="36"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>43000038</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>267</v>
+        <v>43001003</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>277</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="D41" s="4">
         <v>0</v>
@@ -9612,44 +9622,46 @@
         <v>11001003</v>
       </c>
       <c r="H41" s="4">
-        <v>7</v>
-      </c>
-      <c r="I41" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="I41" s="27"/>
       <c r="J41" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="L41">
-        <v>51018005</v>
+        <v>51018007</v>
       </c>
       <c r="M41" s="4">
         <v>1</v>
       </c>
       <c r="N41" s="4">
-        <v>15</v>
-      </c>
-      <c r="O41" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="P41" s="4"/>
       <c r="Q41" s="4" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="R41" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="S41" s="28"/>
-      <c r="T41" s="28"/>
+      <c r="S41" s="27"/>
+      <c r="T41" s="27"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A42">
-        <v>43001001</v>
+        <v>43001004</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>248</v>
+        <v>215</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
       <c r="D42" s="4">
         <v>0</v>
@@ -9662,46 +9674,44 @@
         <v>11001003</v>
       </c>
       <c r="H42" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="L42">
-        <v>51018007</v>
+        <v>51018005</v>
       </c>
       <c r="M42" s="4">
         <v>1</v>
       </c>
       <c r="N42" s="4">
-        <v>20</v>
-      </c>
-      <c r="O42" s="4" t="s">
-        <v>260</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="R42" t="s">
-        <v>254</v>
+        <v>347</v>
+      </c>
+      <c r="R42" s="34" t="s">
+        <v>180</v>
       </c>
       <c r="S42" s="13"/>
       <c r="T42" s="17"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A43">
-        <v>43001002</v>
+        <v>43001005</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>271</v>
+        <v>221</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>272</v>
+        <v>222</v>
       </c>
       <c r="D43" s="4">
         <v>0</v>
@@ -9714,14 +9724,14 @@
         <v>11001003</v>
       </c>
       <c r="H43" s="4">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="L43">
         <v>51018007</v>
@@ -9730,14 +9740,12 @@
         <v>1</v>
       </c>
       <c r="N43" s="4">
-        <v>20</v>
-      </c>
-      <c r="O43" s="4" t="s">
-        <v>278</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="O43" s="4"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="R43" s="4" t="s">
         <v>180</v>
@@ -9747,13 +9755,13 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A44">
-        <v>43001003</v>
-      </c>
-      <c r="B44" s="29" t="s">
-        <v>277</v>
+        <v>43001006</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D44" s="4">
         <v>0</v>
@@ -9766,36 +9774,34 @@
         <v>11001003</v>
       </c>
       <c r="H44" s="4">
-        <v>12</v>
-      </c>
-      <c r="I44" s="27"/>
+        <v>11</v>
+      </c>
+      <c r="I44" s="4"/>
       <c r="J44" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>354</v>
+        <v>319</v>
       </c>
       <c r="L44">
-        <v>51018007</v>
+        <v>51018006</v>
       </c>
       <c r="M44" s="4">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="N44" s="4">
-        <v>10</v>
-      </c>
-      <c r="O44" s="4" t="s">
-        <v>279</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="O44" s="4"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="4" t="s">
-        <v>354</v>
+        <v>319</v>
       </c>
       <c r="R44" s="4" t="s">
         <v>180</v>
       </c>
       <c r="S44" s="27"/>
-      <c r="T44" s="27"/>
+      <c r="T44" s="36"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A45" s="27">
@@ -9814,7 +9820,7 @@
       <c r="F45" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G45" s="29">
+      <c r="G45" s="28">
         <v>11001003</v>
       </c>
       <c r="H45" s="27">
@@ -9864,7 +9870,7 @@
       <c r="F46" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G46" s="29">
+      <c r="G46" s="28">
         <v>11001003</v>
       </c>
       <c r="H46" s="27">
@@ -9914,7 +9920,7 @@
       <c r="F47" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G47" s="29">
+      <c r="G47" s="28">
         <v>11001003</v>
       </c>
       <c r="H47" s="27">
@@ -9954,7 +9960,7 @@
       <c r="B48" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="C48" s="32" t="s">
+      <c r="C48" s="31" t="s">
         <v>285</v>
       </c>
       <c r="D48" s="27">
@@ -9964,7 +9970,7 @@
       <c r="F48" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G48" s="29">
+      <c r="G48" s="28">
         <v>11001003</v>
       </c>
       <c r="H48" s="27">
@@ -9974,7 +9980,7 @@
       <c r="J48" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="K48" s="32" t="s">
+      <c r="K48" s="31" t="s">
         <v>358</v>
       </c>
       <c r="L48">
@@ -9988,7 +9994,7 @@
       </c>
       <c r="O48" s="27"/>
       <c r="P48" s="27"/>
-      <c r="Q48" s="32" t="s">
+      <c r="Q48" s="31" t="s">
         <v>358</v>
       </c>
       <c r="R48" s="27" t="s">
@@ -10004,7 +10010,7 @@
       <c r="B49" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="C49" s="32" t="s">
+      <c r="C49" s="31" t="s">
         <v>289</v>
       </c>
       <c r="D49" s="27">
@@ -10014,7 +10020,7 @@
       <c r="F49" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G49" s="29">
+      <c r="G49" s="28">
         <v>11001003</v>
       </c>
       <c r="H49" s="27">
@@ -10024,7 +10030,7 @@
       <c r="J49" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="K49" s="32" t="s">
+      <c r="K49" s="31" t="s">
         <v>359</v>
       </c>
       <c r="L49">
@@ -10038,7 +10044,7 @@
       </c>
       <c r="O49" s="27"/>
       <c r="P49" s="27"/>
-      <c r="Q49" s="32" t="s">
+      <c r="Q49" s="31" t="s">
         <v>359</v>
       </c>
       <c r="R49" s="27" t="s">
@@ -10054,7 +10060,7 @@
       <c r="B50" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="C50" s="32" t="s">
+      <c r="C50" s="31" t="s">
         <v>290</v>
       </c>
       <c r="D50" s="27">
@@ -10064,7 +10070,7 @@
       <c r="F50" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G50" s="29">
+      <c r="G50" s="28">
         <v>11001003</v>
       </c>
       <c r="H50" s="27">
@@ -10074,7 +10080,7 @@
       <c r="J50" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="K50" s="32" t="s">
+      <c r="K50" s="31" t="s">
         <v>360</v>
       </c>
       <c r="L50">
@@ -10088,7 +10094,7 @@
       </c>
       <c r="O50" s="27"/>
       <c r="P50" s="27"/>
-      <c r="Q50" s="32" t="s">
+      <c r="Q50" s="31" t="s">
         <v>360</v>
       </c>
       <c r="R50" s="27" t="s">

</xml_diff>

<commit_message>
ep recover speed upgrade
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EDF7F513-1A4C-4607-A86C-F500BE256CB7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F204BAB0-4755-401C-B01F-5CADA48F9FAE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="434">
   <si>
     <t>老鼠</t>
   </si>
@@ -793,14 +793,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>能量速度降低</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>EpSlow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>右方Add</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -809,12 +801,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>能量速度降低</t>
-  </si>
-  <si>
-    <t>EpSlow</t>
-  </si>
-  <si>
     <t>右方Add</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -844,10 +830,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>double</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>半人马</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1488,6 +1470,14 @@
   </si>
   <si>
     <t>monbee</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EpRecoverRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ep恢复速度</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4545,7 +4535,7 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Method" dataDxfId="63"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Emethod" dataDxfId="62"/>
     <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="KingTowerId" dataDxfId="61"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="EpSlow" dataDxfId="60"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="EpRecoverRate" dataDxfId="60"/>
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="CardReduce" dataDxfId="59"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="RightMon" dataDxfId="58"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="PetMon" dataDxfId="57"/>
@@ -4577,7 +4567,7 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Method" dataDxfId="33"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Emethod" dataDxfId="32"/>
     <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="KingTowerId" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="EpSlow" dataDxfId="30"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="EpRecoverRate" dataDxfId="30"/>
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="CardReduce" dataDxfId="29"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="RightMon" dataDxfId="28"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PetMon" dataDxfId="27"/>
@@ -4609,7 +4599,7 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Method" dataDxfId="10"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Emethod" dataDxfId="9"/>
     <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="KingTowerId" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="EpSlow" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="EpRecoverRate" dataDxfId="7"/>
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="CardReduce" dataDxfId="6"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="RightMon" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="PetMon" dataDxfId="4"/>
@@ -4946,10 +4936,10 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4:M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4979,7 +4969,7 @@
         <v>153</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>154</v>
@@ -5000,19 +4990,19 @@
         <v>158</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>233</v>
+        <v>433</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="Q1" s="23" t="s">
         <v>159</v>
@@ -5041,7 +5031,7 @@
         <v>149</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>150</v>
@@ -5062,13 +5052,13 @@
         <v>150</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>169</v>
@@ -5103,7 +5093,7 @@
         <v>162</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>163</v>
@@ -5124,19 +5114,19 @@
         <v>167</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>234</v>
+        <v>432</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>184</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>168</v>
@@ -5179,15 +5169,17 @@
         <v>2</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>179</v>
@@ -5223,15 +5215,17 @@
         <v>2</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="R5" s="4" t="s">
         <v>179</v>
@@ -5269,15 +5263,17 @@
         <v>2</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>179</v>
@@ -5317,15 +5313,17 @@
         <v>2</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>179</v>
@@ -5363,15 +5361,17 @@
         <v>2</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>179</v>
@@ -5411,15 +5411,17 @@
         <v>2</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>179</v>
@@ -5459,15 +5461,17 @@
         <v>2</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>179</v>
@@ -5507,15 +5511,17 @@
         <v>2</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+      <c r="M11" s="4">
+        <v>1</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>179</v>
@@ -5555,15 +5561,17 @@
         <v>2</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="R12" s="4" t="s">
         <v>179</v>
@@ -5603,15 +5611,17 @@
         <v>2</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>179</v>
@@ -5651,15 +5661,17 @@
         <v>2</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>179</v>
@@ -5699,15 +5711,17 @@
         <v>2</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="M15" s="4">
+        <v>1</v>
+      </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="R15" s="4" t="s">
         <v>179</v>
@@ -5747,15 +5761,17 @@
         <v>2</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="M16" s="4">
+        <v>1</v>
+      </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>179</v>
@@ -5795,15 +5811,17 @@
         <v>2</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+      <c r="M17" s="4">
+        <v>1</v>
+      </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="R17" s="4" t="s">
         <v>179</v>
@@ -5841,15 +5859,17 @@
         <v>2</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
+      <c r="M18" s="4">
+        <v>1</v>
+      </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="R18" s="4" t="s">
         <v>179</v>
@@ -5864,10 +5884,10 @@
         <v>43020206</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D19" s="4">
         <v>2</v>
@@ -5889,15 +5909,17 @@
         <v>2</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
+      <c r="M19" s="4">
+        <v>1</v>
+      </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="R19" s="4" t="s">
         <v>179</v>
@@ -5912,10 +5934,10 @@
         <v>43020207</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D20" s="4">
         <v>2</v>
@@ -5937,15 +5959,17 @@
         <v>2</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="M20" s="4">
+        <v>1</v>
+      </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="R20" s="4" t="s">
         <v>179</v>
@@ -5960,10 +5984,10 @@
         <v>43020301</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D21" s="4">
         <v>3</v>
@@ -5985,15 +6009,17 @@
         <v>2</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
+      <c r="M21" s="4">
+        <v>1</v>
+      </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="R21" s="4" t="s">
         <v>179</v>
@@ -6008,10 +6034,10 @@
         <v>43020302</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D22" s="4">
         <v>3</v>
@@ -6033,15 +6059,17 @@
         <v>2</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
+      <c r="M22" s="4">
+        <v>1</v>
+      </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="R22" s="4" t="s">
         <v>179</v>
@@ -6079,15 +6107,17 @@
         <v>2</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
+      <c r="M23" s="4">
+        <v>1</v>
+      </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="R23" s="4" t="s">
         <v>179</v>
@@ -6127,15 +6157,17 @@
         <v>2</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
+      <c r="M24" s="4">
+        <v>1</v>
+      </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="R24" s="4" t="s">
         <v>179</v>
@@ -6175,15 +6207,17 @@
         <v>2</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
+      <c r="M25" s="4">
+        <v>1</v>
+      </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="R25" s="4" t="s">
         <v>179</v>
@@ -6198,10 +6232,10 @@
         <v>43020306</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="D26" s="4">
         <v>3</v>
@@ -6223,15 +6257,17 @@
         <v>2</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
+      <c r="M26" s="4">
+        <v>1</v>
+      </c>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="R26" s="4" t="s">
         <v>179</v>
@@ -6246,7 +6282,7 @@
         <v>43020307</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>94</v>
@@ -6271,15 +6307,17 @@
         <v>2</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
+      <c r="M27" s="4">
+        <v>1</v>
+      </c>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="R27" s="4" t="s">
         <v>179</v>
@@ -6319,15 +6357,17 @@
         <v>2</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
+      <c r="M28" s="4">
+        <v>1</v>
+      </c>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>179</v>
@@ -6367,15 +6407,17 @@
         <v>2</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
+      <c r="M29" s="4">
+        <v>1</v>
+      </c>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="R29" s="4" t="s">
         <v>179</v>
@@ -6415,15 +6457,17 @@
         <v>2</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="M30" s="4">
+        <v>1</v>
+      </c>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>179</v>
@@ -6463,15 +6507,17 @@
         <v>2</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
+      <c r="M31" s="4">
+        <v>1</v>
+      </c>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="R31" s="4" t="s">
         <v>179</v>
@@ -6511,15 +6557,17 @@
         <v>2</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
+      <c r="M32" s="4">
+        <v>1</v>
+      </c>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="R32" s="4" t="s">
         <v>179</v>
@@ -6559,15 +6607,17 @@
         <v>2</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
+      <c r="M33" s="4">
+        <v>1</v>
+      </c>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="R33" s="4" t="s">
         <v>179</v>
@@ -6607,15 +6657,17 @@
         <v>2</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
+      <c r="M34" s="4">
+        <v>1</v>
+      </c>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="R34" s="4" t="s">
         <v>179</v>
@@ -6655,15 +6707,17 @@
         <v>2</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
+      <c r="M35" s="4">
+        <v>1</v>
+      </c>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>179</v>
@@ -6703,15 +6757,17 @@
         <v>2</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
+      <c r="M36" s="4">
+        <v>1</v>
+      </c>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="R36" s="4" t="s">
         <v>179</v>
@@ -6751,15 +6807,17 @@
         <v>2</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
+      <c r="M37" s="4">
+        <v>1</v>
+      </c>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>179</v>
@@ -6799,15 +6857,17 @@
         <v>2</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
+      <c r="M38" s="4">
+        <v>1</v>
+      </c>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="R38" s="4" t="s">
         <v>179</v>
@@ -6847,15 +6907,17 @@
         <v>2</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
+      <c r="M39" s="4">
+        <v>1</v>
+      </c>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="R39" s="4" t="s">
         <v>179</v>
@@ -6873,7 +6935,7 @@
         <v>120</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="D40" s="4">
         <v>4</v>
@@ -6895,15 +6957,17 @@
         <v>2</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
+      <c r="M40" s="4">
+        <v>1</v>
+      </c>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="R40" s="4" t="s">
         <v>179</v>
@@ -6918,10 +6982,10 @@
         <v>43020409</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D41" s="4">
         <v>4</v>
@@ -6943,15 +7007,17 @@
         <v>2</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
+      <c r="M41" s="4">
+        <v>1</v>
+      </c>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="4" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="R41" s="4" t="s">
         <v>179</v>
@@ -6991,15 +7057,17 @@
         <v>2</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
+      <c r="M42" s="4">
+        <v>1</v>
+      </c>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="R42" s="4" t="s">
         <v>179</v>
@@ -7039,15 +7107,17 @@
         <v>2</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
+      <c r="M43" s="4">
+        <v>1</v>
+      </c>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="R43" s="4" t="s">
         <v>179</v>
@@ -7087,15 +7157,17 @@
         <v>2</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
+      <c r="M44" s="4">
+        <v>1</v>
+      </c>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="4" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="R44" s="4" t="s">
         <v>179</v>
@@ -7135,15 +7207,17 @@
         <v>2</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
+      <c r="M45" s="4">
+        <v>1</v>
+      </c>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
       <c r="P45" s="4"/>
       <c r="Q45" s="4" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="R45" s="4" t="s">
         <v>179</v>
@@ -7158,10 +7232,10 @@
         <v>43020505</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D46" s="27">
         <v>5</v>
@@ -7183,15 +7257,17 @@
         <v>2</v>
       </c>
       <c r="K46" s="27" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
+      <c r="M46" s="4">
+        <v>1</v>
+      </c>
       <c r="N46" s="4"/>
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
       <c r="Q46" s="27" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="R46" s="4" t="s">
         <v>179</v>
@@ -7206,10 +7282,10 @@
         <v>43020506</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D47" s="27">
         <v>5</v>
@@ -7231,15 +7307,17 @@
         <v>2</v>
       </c>
       <c r="K47" s="27" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
+      <c r="M47" s="4">
+        <v>1</v>
+      </c>
       <c r="N47" s="4"/>
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
       <c r="Q47" s="27" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="R47" s="4" t="s">
         <v>179</v>
@@ -7266,7 +7344,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="G48" s="33">
         <v>11000002</v>
@@ -7279,15 +7357,17 @@
         <v>2</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
+      <c r="M48" s="4">
+        <v>1</v>
+      </c>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
       <c r="P48" s="4"/>
       <c r="Q48" s="4" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="R48" s="4" t="s">
         <v>179</v>
@@ -7312,7 +7392,7 @@
       </c>
       <c r="E49" s="32"/>
       <c r="F49" s="4" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="G49" s="33">
         <v>11000010</v>
@@ -7325,15 +7405,17 @@
         <v>2</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
+      <c r="M49" s="4">
+        <v>1</v>
+      </c>
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
       <c r="P49" s="4"/>
       <c r="Q49" s="4" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="R49" s="4" t="s">
         <v>179</v>
@@ -7358,7 +7440,7 @@
       </c>
       <c r="E50" s="32"/>
       <c r="F50" s="4" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="G50" s="33">
         <v>11000002</v>
@@ -7371,15 +7453,17 @@
         <v>2</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
+      <c r="M50" s="4">
+        <v>1</v>
+      </c>
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
       <c r="P50" s="4"/>
       <c r="Q50" s="4" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="R50" s="4" t="s">
         <v>179</v>
@@ -7394,10 +7478,10 @@
         <v>43020604</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D51" s="4">
         <v>6</v>
@@ -7406,7 +7490,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="G51" s="33">
         <v>11000001</v>
@@ -7419,15 +7503,17 @@
         <v>2</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
+      <c r="M51" s="4">
+        <v>1</v>
+      </c>
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
       <c r="Q51" s="4" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="R51" s="4" t="s">
         <v>179</v>
@@ -7536,10 +7622,10 @@
   <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomRight" activeCell="M39" sqref="M39:M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7571,7 +7657,7 @@
         <v>153</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>154</v>
@@ -7592,19 +7678,19 @@
         <v>158</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>233</v>
+        <v>433</v>
       </c>
       <c r="N1" s="29" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="Q1" s="23" t="s">
         <v>159</v>
@@ -7633,7 +7719,7 @@
         <v>149</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>150</v>
@@ -7654,10 +7740,10 @@
         <v>150</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="M2" s="30" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="N2" s="30" t="s">
         <v>149</v>
@@ -7695,7 +7781,7 @@
         <v>162</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>163</v>
@@ -7716,13 +7802,13 @@
         <v>167</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>234</v>
+        <v>432</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>184</v>
@@ -7771,13 +7857,13 @@
         <v>2</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="L4">
         <v>51018005</v>
       </c>
       <c r="M4" s="4">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="N4" s="4">
         <v>15</v>
@@ -7785,10 +7871,10 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="S4" s="13"/>
       <c r="T4" s="17"/>
@@ -7801,7 +7887,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -7821,26 +7907,26 @@
         <v>2</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="L5">
         <v>51018005</v>
       </c>
       <c r="M5" s="4">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="N5" s="4">
         <v>18</v>
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="6" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="S5" s="13"/>
       <c r="T5" s="17"/>
@@ -7873,13 +7959,13 @@
         <v>2</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="L6">
         <v>51018005</v>
       </c>
       <c r="M6" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N6" s="4">
         <v>15</v>
@@ -7887,7 +7973,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>180</v>
@@ -7923,13 +8009,13 @@
         <v>2</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="L7">
         <v>51018006</v>
       </c>
       <c r="M7" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N7" s="4">
         <v>15</v>
@@ -7937,7 +8023,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>180</v>
@@ -7973,13 +8059,13 @@
         <v>2</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L8">
         <v>51018006</v>
       </c>
       <c r="M8" s="4">
-        <v>1.5</v>
+        <v>0.4</v>
       </c>
       <c r="N8" s="4">
         <v>15</v>
@@ -7987,7 +8073,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>180</v>
@@ -8003,7 +8089,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
@@ -8023,13 +8109,13 @@
         <v>2</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="L9">
         <v>51018005</v>
       </c>
       <c r="M9" s="4">
-        <v>1.5</v>
+        <v>0.4</v>
       </c>
       <c r="N9" s="4">
         <v>18</v>
@@ -8037,10 +8123,10 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="S9" s="13"/>
       <c r="T9" s="17"/>
@@ -8073,13 +8159,13 @@
         <v>2</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="L10">
         <v>51018006</v>
       </c>
       <c r="M10" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N10" s="4">
         <v>15</v>
@@ -8087,7 +8173,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>180</v>
@@ -8123,13 +8209,13 @@
         <v>2</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="L11">
         <v>51018005</v>
       </c>
       <c r="M11" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N11" s="4">
         <v>15</v>
@@ -8137,7 +8223,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>180</v>
@@ -8173,13 +8259,13 @@
         <v>2</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="L12">
         <v>51018005</v>
       </c>
       <c r="M12" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N12" s="4">
         <v>15</v>
@@ -8187,7 +8273,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="R12" s="4" t="s">
         <v>180</v>
@@ -8223,13 +8309,13 @@
         <v>2</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="L13">
         <v>51018005</v>
       </c>
       <c r="M13" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N13" s="4">
         <v>15</v>
@@ -8237,7 +8323,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>180</v>
@@ -8273,13 +8359,13 @@
         <v>2</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="L14">
         <v>51018005</v>
       </c>
       <c r="M14" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N14" s="4">
         <v>15</v>
@@ -8287,7 +8373,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>180</v>
@@ -8323,13 +8409,13 @@
         <v>2</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="L15">
         <v>51018005</v>
       </c>
       <c r="M15" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N15" s="4">
         <v>15</v>
@@ -8337,7 +8423,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="R15" s="4" t="s">
         <v>180</v>
@@ -8373,13 +8459,13 @@
         <v>2</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="L16">
         <v>51018005</v>
       </c>
       <c r="M16" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N16" s="4">
         <v>15</v>
@@ -8387,7 +8473,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>180</v>
@@ -8423,23 +8509,23 @@
         <v>2</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="L17">
         <v>51018005</v>
       </c>
       <c r="M17" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N17" s="4">
         <v>15</v>
       </c>
       <c r="O17" s="4"/>
       <c r="P17" s="6" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="R17" s="4" t="s">
         <v>180</v>
@@ -8475,13 +8561,13 @@
         <v>2</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="L18">
         <v>51018007</v>
       </c>
       <c r="M18" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N18" s="4">
         <v>15</v>
@@ -8489,7 +8575,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="R18" s="4" t="s">
         <v>180</v>
@@ -8502,10 +8588,10 @@
         <v>43000017</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
@@ -8525,13 +8611,13 @@
         <v>2</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="L19">
         <v>51018007</v>
       </c>
       <c r="M19" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N19" s="4">
         <v>15</v>
@@ -8539,7 +8625,7 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="R19" s="4" t="s">
         <v>180</v>
@@ -8555,7 +8641,7 @@
         <v>232</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D20" s="4">
         <v>0</v>
@@ -8575,13 +8661,13 @@
         <v>2</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="L20">
         <v>51018005</v>
       </c>
       <c r="M20" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N20" s="4">
         <v>15</v>
@@ -8589,7 +8675,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="R20" s="4" t="s">
         <v>180</v>
@@ -8625,13 +8711,13 @@
         <v>2</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="L21">
         <v>51018005</v>
       </c>
       <c r="M21" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N21" s="4">
         <v>15</v>
@@ -8639,7 +8725,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="R21" s="4" t="s">
         <v>180</v>
@@ -8675,13 +8761,13 @@
         <v>2</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="L22">
         <v>51018007</v>
       </c>
       <c r="M22" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N22" s="4">
         <v>15</v>
@@ -8689,7 +8775,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="R22" s="4" t="s">
         <v>180</v>
@@ -8725,13 +8811,13 @@
         <v>2</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="L23">
         <v>51018005</v>
       </c>
       <c r="M23" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N23" s="4">
         <v>15</v>
@@ -8739,7 +8825,7 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="R23" s="4" t="s">
         <v>180</v>
@@ -8775,13 +8861,13 @@
         <v>2</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="L24">
         <v>51018006</v>
       </c>
       <c r="M24" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N24" s="4">
         <v>15</v>
@@ -8789,7 +8875,7 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="R24" s="4" t="s">
         <v>180</v>
@@ -8825,13 +8911,13 @@
         <v>2</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="L25">
         <v>51018005</v>
       </c>
       <c r="M25" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N25" s="4">
         <v>15</v>
@@ -8839,7 +8925,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="R25" s="4" t="s">
         <v>180</v>
@@ -8875,13 +8961,13 @@
         <v>2</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="L26">
         <v>51018005</v>
       </c>
       <c r="M26" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N26" s="4">
         <v>15</v>
@@ -8889,7 +8975,7 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="R26" s="4" t="s">
         <v>180</v>
@@ -8925,13 +9011,13 @@
         <v>2</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="L27">
         <v>51018005</v>
       </c>
       <c r="M27" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N27" s="4">
         <v>15</v>
@@ -8939,7 +9025,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="R27" s="4" t="s">
         <v>180</v>
@@ -8975,13 +9061,13 @@
         <v>2</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="L28">
         <v>51018005</v>
       </c>
       <c r="M28" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N28" s="4">
         <v>15</v>
@@ -8989,7 +9075,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>180</v>
@@ -9025,13 +9111,13 @@
         <v>2</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="L29">
         <v>51018006</v>
       </c>
       <c r="M29" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N29" s="4">
         <v>15</v>
@@ -9039,7 +9125,7 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="R29" s="4" t="s">
         <v>180</v>
@@ -9075,13 +9161,13 @@
         <v>2</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="L30">
         <v>51018006</v>
       </c>
       <c r="M30" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N30" s="4">
         <v>15</v>
@@ -9089,7 +9175,7 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>180</v>
@@ -9105,7 +9191,7 @@
         <v>48</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D31" s="4">
         <v>0</v>
@@ -9125,13 +9211,13 @@
         <v>2</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="L31">
         <v>51018005</v>
       </c>
       <c r="M31" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N31" s="4">
         <v>15</v>
@@ -9139,7 +9225,7 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="R31" s="4" t="s">
         <v>180</v>
@@ -9175,13 +9261,13 @@
         <v>2</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="L32">
         <v>51018005</v>
       </c>
       <c r="M32" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N32" s="4">
         <v>15</v>
@@ -9189,7 +9275,7 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="R32" s="4" t="s">
         <v>180</v>
@@ -9225,13 +9311,13 @@
         <v>2</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="L33">
         <v>51018005</v>
       </c>
       <c r="M33" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N33" s="4">
         <v>15</v>
@@ -9239,7 +9325,7 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="R33" s="4" t="s">
         <v>180</v>
@@ -9255,7 +9341,7 @@
         <v>53</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D34" s="4">
         <v>0</v>
@@ -9275,13 +9361,13 @@
         <v>2</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="L34">
         <v>51018005</v>
       </c>
       <c r="M34" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N34" s="4">
         <v>15</v>
@@ -9289,7 +9375,7 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="R34" s="4" t="s">
         <v>180</v>
@@ -9325,13 +9411,13 @@
         <v>2</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="L35">
         <v>51018005</v>
       </c>
       <c r="M35" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N35" s="4">
         <v>15</v>
@@ -9339,7 +9425,7 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>180</v>
@@ -9375,13 +9461,13 @@
         <v>2</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="L36">
         <v>51018005</v>
       </c>
       <c r="M36" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N36" s="4">
         <v>15</v>
@@ -9389,7 +9475,7 @@
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="R36" s="4" t="s">
         <v>180</v>
@@ -9402,10 +9488,10 @@
         <v>43000037</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D37" s="4">
         <v>0</v>
@@ -9425,13 +9511,13 @@
         <v>2</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="L37">
         <v>51018005</v>
       </c>
       <c r="M37" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N37" s="4">
         <v>15</v>
@@ -9439,7 +9525,7 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>180</v>
@@ -9452,10 +9538,10 @@
         <v>43000038</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D38" s="4">
         <v>0</v>
@@ -9475,13 +9561,13 @@
         <v>2</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="L38">
         <v>51018005</v>
       </c>
       <c r="M38" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N38" s="4">
         <v>15</v>
@@ -9489,7 +9575,7 @@
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="R38" s="4" t="s">
         <v>180</v>
@@ -9502,10 +9588,10 @@
         <v>43001001</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D39" s="4">
         <v>0</v>
@@ -9525,26 +9611,26 @@
         <v>2</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="L39">
         <v>51018007</v>
       </c>
       <c r="M39" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="N39" s="4">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="O39" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="4" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="R39" s="6" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="S39" s="13"/>
       <c r="T39" s="17"/>
@@ -9554,10 +9640,10 @@
         <v>43001002</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D40" s="4">
         <v>0</v>
@@ -9577,23 +9663,23 @@
         <v>2</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="L40">
         <v>51018007</v>
       </c>
       <c r="M40" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="N40" s="4">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="O40" s="4" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="R40" s="4" t="s">
         <v>180</v>
@@ -9606,10 +9692,10 @@
         <v>43001003</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D41" s="4">
         <v>0</v>
@@ -9629,23 +9715,23 @@
         <v>2</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="L41">
         <v>51018007</v>
       </c>
       <c r="M41" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="N41" s="4">
         <v>10</v>
       </c>
       <c r="O41" s="4" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="P41" s="4"/>
       <c r="Q41" s="4" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="R41" s="4" t="s">
         <v>180</v>
@@ -9681,7 +9767,7 @@
         <v>2</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="L42">
         <v>51018005</v>
@@ -9690,12 +9776,12 @@
         <v>1</v>
       </c>
       <c r="N42" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="R42" s="34" t="s">
         <v>180</v>
@@ -9731,7 +9817,7 @@
         <v>2</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="L43">
         <v>51018007</v>
@@ -9740,12 +9826,12 @@
         <v>1</v>
       </c>
       <c r="N43" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="R43" s="4" t="s">
         <v>180</v>
@@ -9761,7 +9847,7 @@
         <v>11</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D44" s="4">
         <v>0</v>
@@ -9781,21 +9867,21 @@
         <v>2</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="L44">
         <v>51018006</v>
       </c>
       <c r="M44" s="4">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="N44" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="O44" s="4"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="4" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="R44" s="4" t="s">
         <v>180</v>
@@ -9808,10 +9894,10 @@
         <v>43002001</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D45" s="27">
         <v>0</v>
@@ -9831,13 +9917,13 @@
         <v>2</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="L45">
         <v>51018005</v>
       </c>
       <c r="M45" s="4">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="N45" s="4">
         <v>10</v>
@@ -9845,7 +9931,7 @@
       <c r="O45" s="27"/>
       <c r="P45" s="27"/>
       <c r="Q45" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="R45" s="27" t="s">
         <v>180</v>
@@ -9858,10 +9944,10 @@
         <v>43002002</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D46" s="27">
         <v>0</v>
@@ -9881,13 +9967,13 @@
         <v>2</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="L46">
         <v>51018005</v>
       </c>
       <c r="M46" s="4">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="N46" s="4">
         <v>10</v>
@@ -9895,7 +9981,7 @@
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
       <c r="Q46" s="4" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="R46" s="27" t="s">
         <v>180</v>
@@ -9908,10 +9994,10 @@
         <v>43002003</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D47" s="27">
         <v>0</v>
@@ -9931,13 +10017,13 @@
         <v>2</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="L47">
         <v>51018005</v>
       </c>
       <c r="M47" s="4">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="N47" s="4">
         <v>10</v>
@@ -9945,7 +10031,7 @@
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
       <c r="Q47" s="4" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="R47" s="27" t="s">
         <v>180</v>
@@ -9958,10 +10044,10 @@
         <v>43002004</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D48" s="27">
         <v>0</v>
@@ -9981,13 +10067,13 @@
         <v>2</v>
       </c>
       <c r="K48" s="31" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="L48">
         <v>51018005</v>
       </c>
       <c r="M48" s="4">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="N48" s="4">
         <v>10</v>
@@ -9995,7 +10081,7 @@
       <c r="O48" s="27"/>
       <c r="P48" s="27"/>
       <c r="Q48" s="31" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="R48" s="27" t="s">
         <v>180</v>
@@ -10008,10 +10094,10 @@
         <v>43002005</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D49" s="27">
         <v>0</v>
@@ -10031,13 +10117,13 @@
         <v>2</v>
       </c>
       <c r="K49" s="31" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="L49">
         <v>51018005</v>
       </c>
       <c r="M49" s="4">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="N49" s="4">
         <v>10</v>
@@ -10045,7 +10131,7 @@
       <c r="O49" s="27"/>
       <c r="P49" s="27"/>
       <c r="Q49" s="31" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="R49" s="27" t="s">
         <v>180</v>
@@ -10058,10 +10144,10 @@
         <v>43002006</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D50" s="27">
         <v>0</v>
@@ -10081,13 +10167,13 @@
         <v>2</v>
       </c>
       <c r="K50" s="31" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="L50">
         <v>51018005</v>
       </c>
       <c r="M50" s="4">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="N50" s="4">
         <v>10</v>
@@ -10095,7 +10181,7 @@
       <c r="O50" s="27"/>
       <c r="P50" s="27"/>
       <c r="Q50" s="31" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="R50" s="27" t="s">
         <v>180</v>
@@ -10156,7 +10242,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10188,7 +10274,7 @@
         <v>153</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F1" s="25" t="s">
         <v>154</v>
@@ -10209,19 +10295,19 @@
         <v>158</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>291</v>
-      </c>
-      <c r="M1" s="25" t="s">
-        <v>237</v>
+        <v>286</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>433</v>
       </c>
       <c r="N1" s="25" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="O1" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="Q1" s="26" t="s">
         <v>159</v>
@@ -10271,13 +10357,13 @@
         <v>150</v>
       </c>
       <c r="L2" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="M2" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>247</v>
-      </c>
       <c r="N2" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="O2" s="8" t="s">
         <v>185</v>
@@ -10312,7 +10398,7 @@
         <v>162</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>163</v>
@@ -10333,13 +10419,13 @@
         <v>167</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>238</v>
+        <v>432</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="O3" s="10" t="s">
         <v>193</v>
@@ -10390,17 +10476,19 @@
         <v>2</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
       <c r="N4" s="4"/>
       <c r="O4" s="6" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="4" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>180</v>
@@ -10441,12 +10529,14 @@
         <v>2</v>
       </c>
       <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="R5" s="4" t="s">
         <v>180</v>
@@ -10481,18 +10571,20 @@
         <v>10</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>180</v>
@@ -10527,18 +10619,20 @@
         <v>10</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>180</v>
@@ -10573,20 +10667,22 @@
         <v>2</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
       <c r="N8" s="6"/>
       <c r="O8" s="4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="6" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>180</v>
@@ -10621,20 +10717,22 @@
         <v>2</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
       <c r="N9" s="6"/>
       <c r="O9" s="4" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="6" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>180</v>
@@ -10667,18 +10765,20 @@
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>180</v>
@@ -10711,18 +10811,20 @@
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+      <c r="M11" s="4">
+        <v>1</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>180</v>
@@ -10755,18 +10857,20 @@
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="R12" s="4" t="s">
         <v>180</v>
@@ -10799,18 +10903,20 @@
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>180</v>
@@ -10843,18 +10949,20 @@
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>180</v>

</xml_diff>

<commit_message>
format the code of trap
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F204BAB0-4755-401C-B01F-5CADA48F9FAE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="人物" sheetId="4" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="432">
   <si>
     <t>老鼠</t>
   </si>
@@ -857,14 +856,6 @@
   </si>
   <si>
     <t>51000229;6;3;51000229;6;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>51000002;7;3;51000002;7;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>51000080;9;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1484,7 +1475,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4505,6 +4496,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4517,96 +4576,96 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2_4" displayName="表2_4" ref="A3:T51" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74" tableBorderDxfId="73">
-  <autoFilter ref="A3:T51" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:T51" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74" tableBorderDxfId="73">
+  <autoFilter ref="A3:T51"/>
   <sortState ref="A4:T50">
     <sortCondition ref="A3:A50"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="71"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Ename" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="69"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Quality" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="World" dataDxfId="67"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Job" dataDxfId="66"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Level" dataDxfId="65"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="AutoAddLevel" dataDxfId="64"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Method" dataDxfId="63"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Emethod" dataDxfId="62"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="KingTowerId" dataDxfId="61"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="EpRecoverRate" dataDxfId="60"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="CardReduce" dataDxfId="59"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="RightMon" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="PetMon" dataDxfId="57"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Figue" dataDxfId="56"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BattleMap" dataDxfId="55"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="DropItem" dataDxfId="54"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="InRandomQuest" dataDxfId="53"/>
+    <tableColumn id="1" name="Id" dataDxfId="72"/>
+    <tableColumn id="2" name="Name" dataDxfId="71"/>
+    <tableColumn id="18" name="Ename" dataDxfId="70"/>
+    <tableColumn id="3" name="Type" dataDxfId="69"/>
+    <tableColumn id="21" name="Quality" dataDxfId="68"/>
+    <tableColumn id="6" name="World" dataDxfId="67"/>
+    <tableColumn id="10" name="Job" dataDxfId="66"/>
+    <tableColumn id="11" name="Level" dataDxfId="65"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="64"/>
+    <tableColumn id="13" name="Method" dataDxfId="63"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="62"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="61"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="60"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="59"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="58"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="57"/>
+    <tableColumn id="17" name="Figue" dataDxfId="56"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="55"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="54"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
-  <autoFilter ref="A3:T50" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
+  <autoFilter ref="A3:T50"/>
   <sortState ref="A4:T50">
     <sortCondition ref="A3:A50"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="41"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Ename" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Quality" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="World" dataDxfId="37"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Job" dataDxfId="36"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Level" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="AutoAddLevel" dataDxfId="34"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Method" dataDxfId="33"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Emethod" dataDxfId="32"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="KingTowerId" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="EpRecoverRate" dataDxfId="30"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="CardReduce" dataDxfId="29"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="RightMon" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PetMon" dataDxfId="27"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Figue" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BattleMap" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="DropItem" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="InRandomQuest" dataDxfId="23"/>
+    <tableColumn id="1" name="Id" dataDxfId="42"/>
+    <tableColumn id="2" name="Name" dataDxfId="41"/>
+    <tableColumn id="18" name="Ename" dataDxfId="40"/>
+    <tableColumn id="3" name="Type" dataDxfId="39"/>
+    <tableColumn id="7" name="Quality" dataDxfId="38"/>
+    <tableColumn id="6" name="World" dataDxfId="37"/>
+    <tableColumn id="10" name="Job" dataDxfId="36"/>
+    <tableColumn id="11" name="Level" dataDxfId="35"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="34"/>
+    <tableColumn id="13" name="Method" dataDxfId="33"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="32"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="31"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="30"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="29"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="28"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="27"/>
+    <tableColumn id="17" name="Figue" dataDxfId="26"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="25"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="24"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表2_2" displayName="表2_2" ref="A3:T14" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
-  <autoFilter ref="A3:T14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:T14" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+  <autoFilter ref="A3:T14"/>
   <sortState ref="A4:R83">
     <sortCondition ref="A3:A83"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="18"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Ename" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Quality" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="World" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Job" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Level" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="AutoAddLevel" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Method" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Emethod" dataDxfId="9"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="KingTowerId" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="EpRecoverRate" dataDxfId="7"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="CardReduce" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="RightMon" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="PetMon" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Figue" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="BattleMap" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="DropItem" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="InRandomQuest" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="19"/>
+    <tableColumn id="2" name="Name" dataDxfId="18"/>
+    <tableColumn id="18" name="Ename" dataDxfId="17"/>
+    <tableColumn id="3" name="Type" dataDxfId="16"/>
+    <tableColumn id="7" name="Quality" dataDxfId="15"/>
+    <tableColumn id="6" name="World" dataDxfId="14"/>
+    <tableColumn id="10" name="Job" dataDxfId="13"/>
+    <tableColumn id="11" name="Level" dataDxfId="12"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="11"/>
+    <tableColumn id="13" name="Method" dataDxfId="10"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="9"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="8"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="7"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="6"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="5"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="4"/>
+    <tableColumn id="9" name="Figue" dataDxfId="3"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="2"/>
+    <tableColumn id="8" name="DropItem" dataDxfId="1"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4620,7 +4679,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -4932,7 +4991,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4969,7 +5028,7 @@
         <v>153</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>154</v>
@@ -4990,10 +5049,10 @@
         <v>158</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="N1" s="11" t="s">
         <v>237</v>
@@ -5031,7 +5090,7 @@
         <v>149</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>150</v>
@@ -5052,7 +5111,7 @@
         <v>150</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>242</v>
@@ -5093,7 +5152,7 @@
         <v>162</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>163</v>
@@ -5114,10 +5173,10 @@
         <v>167</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>241</v>
@@ -5169,7 +5228,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4">
@@ -5179,7 +5238,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>179</v>
@@ -5215,7 +5274,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4">
@@ -5225,7 +5284,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="R5" s="4" t="s">
         <v>179</v>
@@ -5263,7 +5322,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4">
@@ -5273,7 +5332,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>179</v>
@@ -5313,7 +5372,7 @@
         <v>2</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4">
@@ -5323,7 +5382,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>179</v>
@@ -5361,7 +5420,7 @@
         <v>2</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4">
@@ -5371,7 +5430,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>179</v>
@@ -5411,7 +5470,7 @@
         <v>2</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4">
@@ -5421,7 +5480,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>179</v>
@@ -5461,7 +5520,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4">
@@ -5471,7 +5530,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>179</v>
@@ -5511,7 +5570,7 @@
         <v>2</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4">
@@ -5521,7 +5580,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>179</v>
@@ -5561,7 +5620,7 @@
         <v>2</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4">
@@ -5571,7 +5630,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="R12" s="4" t="s">
         <v>179</v>
@@ -5611,7 +5670,7 @@
         <v>2</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4">
@@ -5621,7 +5680,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>179</v>
@@ -5661,7 +5720,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4">
@@ -5671,7 +5730,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>179</v>
@@ -5711,7 +5770,7 @@
         <v>2</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4">
@@ -5721,7 +5780,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="R15" s="4" t="s">
         <v>179</v>
@@ -5761,7 +5820,7 @@
         <v>2</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4">
@@ -5771,7 +5830,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>179</v>
@@ -5811,7 +5870,7 @@
         <v>2</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4">
@@ -5821,7 +5880,7 @@
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="R17" s="4" t="s">
         <v>179</v>
@@ -5859,7 +5918,7 @@
         <v>2</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4">
@@ -5869,7 +5928,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="R18" s="4" t="s">
         <v>179</v>
@@ -5884,10 +5943,10 @@
         <v>43020206</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D19" s="4">
         <v>2</v>
@@ -5909,7 +5968,7 @@
         <v>2</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4">
@@ -5919,7 +5978,7 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="R19" s="4" t="s">
         <v>179</v>
@@ -5934,10 +5993,10 @@
         <v>43020207</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D20" s="4">
         <v>2</v>
@@ -5959,7 +6018,7 @@
         <v>2</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4">
@@ -5969,7 +6028,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="R20" s="4" t="s">
         <v>179</v>
@@ -5984,10 +6043,10 @@
         <v>43020301</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D21" s="4">
         <v>3</v>
@@ -6009,7 +6068,7 @@
         <v>2</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4">
@@ -6019,7 +6078,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="R21" s="4" t="s">
         <v>179</v>
@@ -6034,10 +6093,10 @@
         <v>43020302</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D22" s="4">
         <v>3</v>
@@ -6059,7 +6118,7 @@
         <v>2</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4">
@@ -6069,7 +6128,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="R22" s="4" t="s">
         <v>179</v>
@@ -6107,7 +6166,7 @@
         <v>2</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4">
@@ -6117,7 +6176,7 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="R23" s="4" t="s">
         <v>179</v>
@@ -6157,7 +6216,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4">
@@ -6167,7 +6226,7 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="R24" s="4" t="s">
         <v>179</v>
@@ -6207,7 +6266,7 @@
         <v>2</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4">
@@ -6217,7 +6276,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="R25" s="4" t="s">
         <v>179</v>
@@ -6232,10 +6291,10 @@
         <v>43020306</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D26" s="4">
         <v>3</v>
@@ -6257,7 +6316,7 @@
         <v>2</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4">
@@ -6267,7 +6326,7 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="R26" s="4" t="s">
         <v>179</v>
@@ -6282,7 +6341,7 @@
         <v>43020307</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>94</v>
@@ -6307,7 +6366,7 @@
         <v>2</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4">
@@ -6317,7 +6376,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="R27" s="4" t="s">
         <v>179</v>
@@ -6357,7 +6416,7 @@
         <v>2</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="4">
@@ -6367,7 +6426,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>179</v>
@@ -6407,7 +6466,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4">
@@ -6417,7 +6476,7 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="R29" s="4" t="s">
         <v>179</v>
@@ -6457,7 +6516,7 @@
         <v>2</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L30" s="4"/>
       <c r="M30" s="4">
@@ -6467,7 +6526,7 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>179</v>
@@ -6507,7 +6566,7 @@
         <v>2</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L31" s="4"/>
       <c r="M31" s="4">
@@ -6517,7 +6576,7 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="R31" s="4" t="s">
         <v>179</v>
@@ -6557,7 +6616,7 @@
         <v>2</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="4">
@@ -6567,7 +6626,7 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="R32" s="4" t="s">
         <v>179</v>
@@ -6607,7 +6666,7 @@
         <v>2</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L33" s="4"/>
       <c r="M33" s="4">
@@ -6617,7 +6676,7 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="R33" s="4" t="s">
         <v>179</v>
@@ -6657,7 +6716,7 @@
         <v>2</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4">
@@ -6667,7 +6726,7 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="R34" s="4" t="s">
         <v>179</v>
@@ -6707,7 +6766,7 @@
         <v>2</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L35" s="4"/>
       <c r="M35" s="4">
@@ -6717,7 +6776,7 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>179</v>
@@ -6757,7 +6816,7 @@
         <v>2</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L36" s="4"/>
       <c r="M36" s="4">
@@ -6767,7 +6826,7 @@
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="R36" s="4" t="s">
         <v>179</v>
@@ -6807,7 +6866,7 @@
         <v>2</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L37" s="4"/>
       <c r="M37" s="4">
@@ -6817,7 +6876,7 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>179</v>
@@ -6857,7 +6916,7 @@
         <v>2</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="L38" s="4"/>
       <c r="M38" s="4">
@@ -6867,7 +6926,7 @@
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="R38" s="4" t="s">
         <v>179</v>
@@ -6907,7 +6966,7 @@
         <v>2</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L39" s="4"/>
       <c r="M39" s="4">
@@ -6917,7 +6976,7 @@
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="R39" s="4" t="s">
         <v>179</v>
@@ -6935,7 +6994,7 @@
         <v>120</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D40" s="4">
         <v>4</v>
@@ -6957,7 +7016,7 @@
         <v>2</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="4">
@@ -6967,7 +7026,7 @@
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="R40" s="4" t="s">
         <v>179</v>
@@ -6982,10 +7041,10 @@
         <v>43020409</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D41" s="4">
         <v>4</v>
@@ -7007,7 +7066,7 @@
         <v>2</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L41" s="4"/>
       <c r="M41" s="4">
@@ -7017,7 +7076,7 @@
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="R41" s="4" t="s">
         <v>179</v>
@@ -7057,7 +7116,7 @@
         <v>2</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="4">
@@ -7067,7 +7126,7 @@
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="R42" s="4" t="s">
         <v>179</v>
@@ -7107,7 +7166,7 @@
         <v>2</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="L43" s="4"/>
       <c r="M43" s="4">
@@ -7117,7 +7176,7 @@
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="R43" s="4" t="s">
         <v>179</v>
@@ -7157,7 +7216,7 @@
         <v>2</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L44" s="4"/>
       <c r="M44" s="4">
@@ -7167,7 +7226,7 @@
       <c r="O44" s="4"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="R44" s="4" t="s">
         <v>179</v>
@@ -7207,7 +7266,7 @@
         <v>2</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="L45" s="4"/>
       <c r="M45" s="4">
@@ -7217,7 +7276,7 @@
       <c r="O45" s="4"/>
       <c r="P45" s="4"/>
       <c r="Q45" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="R45" s="4" t="s">
         <v>179</v>
@@ -7232,10 +7291,10 @@
         <v>43020505</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D46" s="27">
         <v>5</v>
@@ -7257,7 +7316,7 @@
         <v>2</v>
       </c>
       <c r="K46" s="27" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="L46" s="4"/>
       <c r="M46" s="4">
@@ -7267,7 +7326,7 @@
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
       <c r="Q46" s="27" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="R46" s="4" t="s">
         <v>179</v>
@@ -7282,10 +7341,10 @@
         <v>43020506</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D47" s="27">
         <v>5</v>
@@ -7307,7 +7366,7 @@
         <v>2</v>
       </c>
       <c r="K47" s="27" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="L47" s="4"/>
       <c r="M47" s="4">
@@ -7317,7 +7376,7 @@
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
       <c r="Q47" s="27" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="R47" s="4" t="s">
         <v>179</v>
@@ -7344,7 +7403,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G48" s="33">
         <v>11000002</v>
@@ -7357,7 +7416,7 @@
         <v>2</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L48" s="4"/>
       <c r="M48" s="4">
@@ -7367,7 +7426,7 @@
       <c r="O48" s="4"/>
       <c r="P48" s="4"/>
       <c r="Q48" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="R48" s="4" t="s">
         <v>179</v>
@@ -7392,7 +7451,7 @@
       </c>
       <c r="E49" s="32"/>
       <c r="F49" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G49" s="33">
         <v>11000010</v>
@@ -7405,7 +7464,7 @@
         <v>2</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L49" s="4"/>
       <c r="M49" s="4">
@@ -7415,7 +7474,7 @@
       <c r="O49" s="4"/>
       <c r="P49" s="4"/>
       <c r="Q49" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="R49" s="4" t="s">
         <v>179</v>
@@ -7440,7 +7499,7 @@
       </c>
       <c r="E50" s="32"/>
       <c r="F50" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G50" s="33">
         <v>11000002</v>
@@ -7453,7 +7512,7 @@
         <v>2</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="L50" s="4"/>
       <c r="M50" s="4">
@@ -7463,7 +7522,7 @@
       <c r="O50" s="4"/>
       <c r="P50" s="4"/>
       <c r="Q50" s="4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="R50" s="4" t="s">
         <v>179</v>
@@ -7478,10 +7537,10 @@
         <v>43020604</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D51" s="4">
         <v>6</v>
@@ -7490,7 +7549,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G51" s="33">
         <v>11000001</v>
@@ -7503,7 +7562,7 @@
         <v>2</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="L51" s="4"/>
       <c r="M51" s="4">
@@ -7513,7 +7572,7 @@
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
       <c r="Q51" s="4" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="R51" s="4" t="s">
         <v>179</v>
@@ -7618,14 +7677,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M39" sqref="M39:M41"/>
+      <selection pane="bottomRight" activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7657,7 +7716,7 @@
         <v>153</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>154</v>
@@ -7678,10 +7737,10 @@
         <v>158</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="N1" s="29" t="s">
         <v>237</v>
@@ -7719,7 +7778,7 @@
         <v>149</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>150</v>
@@ -7740,7 +7799,7 @@
         <v>150</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M2" s="30" t="s">
         <v>242</v>
@@ -7781,7 +7840,7 @@
         <v>162</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>163</v>
@@ -7802,10 +7861,10 @@
         <v>167</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>241</v>
@@ -7857,7 +7916,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L4">
         <v>51018005</v>
@@ -7871,7 +7930,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>248</v>
@@ -7887,7 +7946,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -7907,7 +7966,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L5">
         <v>51018005</v>
@@ -7919,11 +7978,9 @@
         <v>18</v>
       </c>
       <c r="O5" s="4"/>
-      <c r="P5" s="6" t="s">
-        <v>251</v>
-      </c>
+      <c r="P5" s="6"/>
       <c r="Q5" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="R5" s="4" t="s">
         <v>248</v>
@@ -7959,7 +8016,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="L6">
         <v>51018005</v>
@@ -7973,7 +8030,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>180</v>
@@ -8009,7 +8066,7 @@
         <v>2</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="L7">
         <v>51018006</v>
@@ -8023,7 +8080,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>180</v>
@@ -8059,7 +8116,7 @@
         <v>2</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L8">
         <v>51018006</v>
@@ -8073,7 +8130,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>180</v>
@@ -8089,7 +8146,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
@@ -8109,7 +8166,7 @@
         <v>2</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="L9">
         <v>51018005</v>
@@ -8123,7 +8180,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>248</v>
@@ -8159,7 +8216,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="L10">
         <v>51018006</v>
@@ -8173,7 +8230,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>180</v>
@@ -8209,7 +8266,7 @@
         <v>2</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L11">
         <v>51018005</v>
@@ -8223,7 +8280,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>180</v>
@@ -8259,7 +8316,7 @@
         <v>2</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L12">
         <v>51018005</v>
@@ -8273,7 +8330,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="R12" s="4" t="s">
         <v>180</v>
@@ -8309,7 +8366,7 @@
         <v>2</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L13">
         <v>51018005</v>
@@ -8323,7 +8380,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>180</v>
@@ -8359,7 +8416,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="L14">
         <v>51018005</v>
@@ -8373,7 +8430,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>180</v>
@@ -8409,7 +8466,7 @@
         <v>2</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="L15">
         <v>51018005</v>
@@ -8423,7 +8480,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="R15" s="4" t="s">
         <v>180</v>
@@ -8459,7 +8516,7 @@
         <v>2</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="L16">
         <v>51018005</v>
@@ -8473,7 +8530,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>180</v>
@@ -8509,7 +8566,7 @@
         <v>2</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L17">
         <v>51018005</v>
@@ -8521,11 +8578,9 @@
         <v>15</v>
       </c>
       <c r="O17" s="4"/>
-      <c r="P17" s="6" t="s">
-        <v>252</v>
-      </c>
+      <c r="P17" s="6"/>
       <c r="Q17" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="R17" s="4" t="s">
         <v>180</v>
@@ -8561,7 +8616,7 @@
         <v>2</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="L18">
         <v>51018007</v>
@@ -8575,7 +8630,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="R18" s="4" t="s">
         <v>180</v>
@@ -8588,10 +8643,10 @@
         <v>43000017</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
@@ -8611,7 +8666,7 @@
         <v>2</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="L19">
         <v>51018007</v>
@@ -8625,7 +8680,7 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="R19" s="4" t="s">
         <v>180</v>
@@ -8641,7 +8696,7 @@
         <v>232</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D20" s="4">
         <v>0</v>
@@ -8661,7 +8716,7 @@
         <v>2</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="L20">
         <v>51018005</v>
@@ -8675,7 +8730,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="R20" s="4" t="s">
         <v>180</v>
@@ -8711,7 +8766,7 @@
         <v>2</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="L21">
         <v>51018005</v>
@@ -8725,7 +8780,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="R21" s="4" t="s">
         <v>180</v>
@@ -8761,7 +8816,7 @@
         <v>2</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="L22">
         <v>51018007</v>
@@ -8775,7 +8830,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="R22" s="4" t="s">
         <v>180</v>
@@ -8811,7 +8866,7 @@
         <v>2</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="L23">
         <v>51018005</v>
@@ -8825,7 +8880,7 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="R23" s="4" t="s">
         <v>180</v>
@@ -8861,7 +8916,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L24">
         <v>51018006</v>
@@ -8875,7 +8930,7 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="R24" s="4" t="s">
         <v>180</v>
@@ -8911,7 +8966,7 @@
         <v>2</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L25">
         <v>51018005</v>
@@ -8925,7 +8980,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="R25" s="4" t="s">
         <v>180</v>
@@ -8961,7 +9016,7 @@
         <v>2</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="L26">
         <v>51018005</v>
@@ -8975,7 +9030,7 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="R26" s="4" t="s">
         <v>180</v>
@@ -9011,7 +9066,7 @@
         <v>2</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="L27">
         <v>51018005</v>
@@ -9025,7 +9080,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="R27" s="4" t="s">
         <v>180</v>
@@ -9061,7 +9116,7 @@
         <v>2</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="L28">
         <v>51018005</v>
@@ -9075,7 +9130,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>180</v>
@@ -9111,7 +9166,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="L29">
         <v>51018006</v>
@@ -9125,7 +9180,7 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="R29" s="4" t="s">
         <v>180</v>
@@ -9161,7 +9216,7 @@
         <v>2</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="L30">
         <v>51018006</v>
@@ -9175,7 +9230,7 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>180</v>
@@ -9191,7 +9246,7 @@
         <v>48</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D31" s="4">
         <v>0</v>
@@ -9211,7 +9266,7 @@
         <v>2</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="L31">
         <v>51018005</v>
@@ -9225,7 +9280,7 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="R31" s="4" t="s">
         <v>180</v>
@@ -9261,7 +9316,7 @@
         <v>2</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="L32">
         <v>51018005</v>
@@ -9275,7 +9330,7 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="R32" s="4" t="s">
         <v>180</v>
@@ -9311,7 +9366,7 @@
         <v>2</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="L33">
         <v>51018005</v>
@@ -9325,7 +9380,7 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="R33" s="4" t="s">
         <v>180</v>
@@ -9341,7 +9396,7 @@
         <v>53</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D34" s="4">
         <v>0</v>
@@ -9361,7 +9416,7 @@
         <v>2</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L34">
         <v>51018005</v>
@@ -9375,7 +9430,7 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="R34" s="4" t="s">
         <v>180</v>
@@ -9411,7 +9466,7 @@
         <v>2</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="L35">
         <v>51018005</v>
@@ -9425,7 +9480,7 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>180</v>
@@ -9461,7 +9516,7 @@
         <v>2</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="L36">
         <v>51018005</v>
@@ -9475,7 +9530,7 @@
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="R36" s="4" t="s">
         <v>180</v>
@@ -9488,10 +9543,10 @@
         <v>43000037</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D37" s="4">
         <v>0</v>
@@ -9511,7 +9566,7 @@
         <v>2</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="L37">
         <v>51018005</v>
@@ -9525,7 +9580,7 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>180</v>
@@ -9538,10 +9593,10 @@
         <v>43000038</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D38" s="4">
         <v>0</v>
@@ -9561,7 +9616,7 @@
         <v>2</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="L38">
         <v>51018005</v>
@@ -9575,7 +9630,7 @@
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="R38" s="4" t="s">
         <v>180</v>
@@ -9611,7 +9666,7 @@
         <v>2</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L39">
         <v>51018007</v>
@@ -9623,11 +9678,11 @@
         <v>15</v>
       </c>
       <c r="O39" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="R39" s="6" t="s">
         <v>249</v>
@@ -9640,10 +9695,10 @@
         <v>43001002</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D40" s="4">
         <v>0</v>
@@ -9663,7 +9718,7 @@
         <v>2</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L40">
         <v>51018007</v>
@@ -9675,11 +9730,11 @@
         <v>15</v>
       </c>
       <c r="O40" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="R40" s="4" t="s">
         <v>180</v>
@@ -9692,10 +9747,10 @@
         <v>43001003</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D41" s="4">
         <v>0</v>
@@ -9715,7 +9770,7 @@
         <v>2</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L41">
         <v>51018007</v>
@@ -9727,11 +9782,11 @@
         <v>10</v>
       </c>
       <c r="O41" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="P41" s="4"/>
       <c r="Q41" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="R41" s="4" t="s">
         <v>180</v>
@@ -9767,7 +9822,7 @@
         <v>2</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="L42">
         <v>51018005</v>
@@ -9781,7 +9836,7 @@
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="R42" s="34" t="s">
         <v>180</v>
@@ -9817,7 +9872,7 @@
         <v>2</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="L43">
         <v>51018007</v>
@@ -9831,7 +9886,7 @@
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="R43" s="4" t="s">
         <v>180</v>
@@ -9847,7 +9902,7 @@
         <v>11</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D44" s="4">
         <v>0</v>
@@ -9867,7 +9922,7 @@
         <v>2</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L44">
         <v>51018006</v>
@@ -9881,7 +9936,7 @@
       <c r="O44" s="4"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="R44" s="4" t="s">
         <v>180</v>
@@ -9894,10 +9949,10 @@
         <v>43002001</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D45" s="27">
         <v>0</v>
@@ -9917,7 +9972,7 @@
         <v>2</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L45">
         <v>51018005</v>
@@ -9931,7 +9986,7 @@
       <c r="O45" s="27"/>
       <c r="P45" s="27"/>
       <c r="Q45" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="R45" s="27" t="s">
         <v>180</v>
@@ -9944,10 +9999,10 @@
         <v>43002002</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D46" s="27">
         <v>0</v>
@@ -9967,7 +10022,7 @@
         <v>2</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L46">
         <v>51018005</v>
@@ -9981,7 +10036,7 @@
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
       <c r="Q46" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="R46" s="27" t="s">
         <v>180</v>
@@ -9994,10 +10049,10 @@
         <v>43002003</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D47" s="27">
         <v>0</v>
@@ -10017,7 +10072,7 @@
         <v>2</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="L47">
         <v>51018005</v>
@@ -10031,7 +10086,7 @@
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
       <c r="Q47" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="R47" s="27" t="s">
         <v>180</v>
@@ -10044,10 +10099,10 @@
         <v>43002004</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D48" s="27">
         <v>0</v>
@@ -10067,7 +10122,7 @@
         <v>2</v>
       </c>
       <c r="K48" s="31" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="L48">
         <v>51018005</v>
@@ -10081,7 +10136,7 @@
       <c r="O48" s="27"/>
       <c r="P48" s="27"/>
       <c r="Q48" s="31" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="R48" s="27" t="s">
         <v>180</v>
@@ -10094,10 +10149,10 @@
         <v>43002005</v>
       </c>
       <c r="B49" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C49" s="31" t="s">
         <v>282</v>
-      </c>
-      <c r="C49" s="31" t="s">
-        <v>284</v>
       </c>
       <c r="D49" s="27">
         <v>0</v>
@@ -10117,7 +10172,7 @@
         <v>2</v>
       </c>
       <c r="K49" s="31" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="L49">
         <v>51018005</v>
@@ -10131,7 +10186,7 @@
       <c r="O49" s="27"/>
       <c r="P49" s="27"/>
       <c r="Q49" s="31" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="R49" s="27" t="s">
         <v>180</v>
@@ -10144,10 +10199,10 @@
         <v>43002006</v>
       </c>
       <c r="B50" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C50" s="31" t="s">
         <v>283</v>
-      </c>
-      <c r="C50" s="31" t="s">
-        <v>285</v>
       </c>
       <c r="D50" s="27">
         <v>0</v>
@@ -10167,7 +10222,7 @@
         <v>2</v>
       </c>
       <c r="K50" s="31" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="L50">
         <v>51018005</v>
@@ -10181,7 +10236,7 @@
       <c r="O50" s="27"/>
       <c r="P50" s="27"/>
       <c r="Q50" s="31" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="R50" s="27" t="s">
         <v>180</v>
@@ -10235,7 +10290,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10274,7 +10329,7 @@
         <v>153</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F1" s="25" t="s">
         <v>154</v>
@@ -10295,10 +10350,10 @@
         <v>158</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="N1" s="25" t="s">
         <v>236</v>
@@ -10398,7 +10453,7 @@
         <v>162</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>163</v>
@@ -10419,10 +10474,10 @@
         <v>167</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>240</v>
@@ -10476,7 +10531,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4">
@@ -10488,7 +10543,7 @@
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>180</v>
@@ -10536,7 +10591,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="R5" s="4" t="s">
         <v>180</v>
@@ -10571,10 +10626,10 @@
         <v>10</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4">
@@ -10584,7 +10639,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>180</v>
@@ -10619,10 +10674,10 @@
         <v>10</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4">
@@ -10632,7 +10687,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>180</v>
@@ -10667,10 +10722,10 @@
         <v>2</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="4">
@@ -10678,11 +10733,11 @@
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>180</v>
@@ -10717,10 +10772,10 @@
         <v>2</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="4">
@@ -10728,11 +10783,11 @@
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>180</v>
@@ -10765,10 +10820,10 @@
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4">
@@ -10778,7 +10833,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>180</v>
@@ -10811,10 +10866,10 @@
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4">
@@ -10824,7 +10879,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>180</v>
@@ -10857,10 +10912,10 @@
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4">
@@ -10870,7 +10925,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="R12" s="4" t="s">
         <v>180</v>
@@ -10903,10 +10958,10 @@
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4">
@@ -10916,7 +10971,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>180</v>
@@ -10949,10 +11004,10 @@
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4">
@@ -10962,7 +11017,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>180</v>

</xml_diff>

<commit_message>
optimise the ground tool
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{881AA608-30AF-41AF-967C-564ACC941FCD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="人物" sheetId="4" r:id="rId1"/>
@@ -1469,14 +1470,14 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51000021;5;4;51000021;7;2;51000021;7;6</t>
+    <t>51000021;5;3;51000021;4;1;51000021;4;5</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1711,7 +1712,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1930,6 +1931,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2209,7 +2222,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2319,6 +2332,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4497,74 +4516,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4577,96 +4528,96 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:T51" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74" tableBorderDxfId="73">
-  <autoFilter ref="A3:T51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2_4" displayName="表2_4" ref="A3:T51" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74" tableBorderDxfId="73">
+  <autoFilter ref="A3:T51" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState ref="A4:T50">
     <sortCondition ref="A3:A50"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="72"/>
-    <tableColumn id="2" name="Name" dataDxfId="71"/>
-    <tableColumn id="18" name="Ename" dataDxfId="70"/>
-    <tableColumn id="3" name="Type" dataDxfId="69"/>
-    <tableColumn id="21" name="Quality" dataDxfId="68"/>
-    <tableColumn id="6" name="World" dataDxfId="67"/>
-    <tableColumn id="10" name="Job" dataDxfId="66"/>
-    <tableColumn id="11" name="Level" dataDxfId="65"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="64"/>
-    <tableColumn id="13" name="Method" dataDxfId="63"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="62"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="61"/>
-    <tableColumn id="12" name="EpRecoverRate" dataDxfId="60"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="59"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="58"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="57"/>
-    <tableColumn id="17" name="Figue" dataDxfId="56"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="55"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="54"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="71"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Ename" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="69"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Quality" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="World" dataDxfId="67"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Job" dataDxfId="66"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Level" dataDxfId="65"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="AutoAddLevel" dataDxfId="64"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Method" dataDxfId="63"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Emethod" dataDxfId="62"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="KingTowerId" dataDxfId="61"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="EpRecoverRate" dataDxfId="60"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="CardReduce" dataDxfId="59"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="RightMon" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="PetMon" dataDxfId="57"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Figue" dataDxfId="56"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BattleMap" dataDxfId="55"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="DropItem" dataDxfId="54"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="InRandomQuest" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
-  <autoFilter ref="A3:T50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
+  <autoFilter ref="A3:T50" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:T50">
     <sortCondition ref="A3:A50"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="42"/>
-    <tableColumn id="2" name="Name" dataDxfId="41"/>
-    <tableColumn id="18" name="Ename" dataDxfId="40"/>
-    <tableColumn id="3" name="Type" dataDxfId="39"/>
-    <tableColumn id="7" name="Quality" dataDxfId="38"/>
-    <tableColumn id="6" name="World" dataDxfId="37"/>
-    <tableColumn id="10" name="Job" dataDxfId="36"/>
-    <tableColumn id="11" name="Level" dataDxfId="35"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="34"/>
-    <tableColumn id="13" name="Method" dataDxfId="33"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="32"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="31"/>
-    <tableColumn id="12" name="EpRecoverRate" dataDxfId="30"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="29"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="28"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="27"/>
-    <tableColumn id="17" name="Figue" dataDxfId="26"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="25"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="24"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="41"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Ename" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Quality" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="World" dataDxfId="37"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Job" dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Level" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="AutoAddLevel" dataDxfId="34"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Method" dataDxfId="33"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Emethod" dataDxfId="32"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="KingTowerId" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="EpRecoverRate" dataDxfId="30"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="CardReduce" dataDxfId="29"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="RightMon" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PetMon" dataDxfId="27"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Figue" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BattleMap" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="DropItem" dataDxfId="24"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="InRandomQuest" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:T14" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
-  <autoFilter ref="A3:T14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表2_2" displayName="表2_2" ref="A3:T14" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+  <autoFilter ref="A3:T14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:R83">
     <sortCondition ref="A3:A83"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="19"/>
-    <tableColumn id="2" name="Name" dataDxfId="18"/>
-    <tableColumn id="18" name="Ename" dataDxfId="17"/>
-    <tableColumn id="3" name="Type" dataDxfId="16"/>
-    <tableColumn id="7" name="Quality" dataDxfId="15"/>
-    <tableColumn id="6" name="World" dataDxfId="14"/>
-    <tableColumn id="10" name="Job" dataDxfId="13"/>
-    <tableColumn id="11" name="Level" dataDxfId="12"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="11"/>
-    <tableColumn id="13" name="Method" dataDxfId="10"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="9"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="8"/>
-    <tableColumn id="12" name="EpRecoverRate" dataDxfId="7"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="6"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="5"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="4"/>
-    <tableColumn id="9" name="Figue" dataDxfId="3"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="2"/>
-    <tableColumn id="8" name="DropItem" dataDxfId="1"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="18"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Ename" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Quality" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="World" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Job" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Level" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="AutoAddLevel" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Method" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Emethod" dataDxfId="9"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="KingTowerId" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="EpRecoverRate" dataDxfId="7"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="CardReduce" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="RightMon" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="PetMon" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Figue" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="BattleMap" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="DropItem" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="InRandomQuest" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4680,7 +4631,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -4992,7 +4943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7678,14 +7629,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O40" sqref="O40"/>
+      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9640,7 +9591,7 @@
       <c r="T38" s="35"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A39">
+      <c r="A39" s="37">
         <v>43001001</v>
       </c>
       <c r="B39" s="12" t="s">
@@ -9692,7 +9643,7 @@
       <c r="T39" s="17"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A40">
+      <c r="A40" s="37">
         <v>43001002</v>
       </c>
       <c r="B40" s="12" t="s">
@@ -9744,7 +9695,7 @@
       <c r="T40" s="36"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A41">
+      <c r="A41" s="37">
         <v>43001003</v>
       </c>
       <c r="B41" s="28" t="s">
@@ -9796,7 +9747,7 @@
       <c r="T41" s="27"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A42">
+      <c r="A42" s="37">
         <v>43001004</v>
       </c>
       <c r="B42" s="12" t="s">
@@ -9846,7 +9797,7 @@
       <c r="T42" s="17"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A43">
+      <c r="A43" s="37">
         <v>43001005</v>
       </c>
       <c r="B43" s="12" t="s">
@@ -9896,7 +9847,7 @@
       <c r="T43" s="17"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A44">
+      <c r="A44" s="37">
         <v>43001006</v>
       </c>
       <c r="B44" s="12" t="s">
@@ -9946,7 +9897,7 @@
       <c r="T44" s="36"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A45" s="27">
+      <c r="A45" s="38">
         <v>43002001</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -9996,7 +9947,7 @@
       <c r="T45" s="27"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A46" s="27">
+      <c r="A46" s="38">
         <v>43002002</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -10046,7 +9997,7 @@
       <c r="T46" s="27"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A47" s="27">
+      <c r="A47" s="38">
         <v>43002003</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -10096,7 +10047,7 @@
       <c r="T47" s="27"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A48" s="27">
+      <c r="A48" s="38">
         <v>43002004</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -10146,7 +10097,7 @@
       <c r="T48" s="27"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A49" s="27">
+      <c r="A49" s="38">
         <v>43002005</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -10196,7 +10147,7 @@
       <c r="T49" s="27"/>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A50" s="27">
+      <c r="A50" s="38">
         <v>43002006</v>
       </c>
       <c r="B50" s="4" t="s">
@@ -10291,7 +10242,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
config the elite monster
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{881AA608-30AF-41AF-967C-564ACC941FCD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E691F7B3-4E83-4028-A51F-4CBE0D0E898D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="436">
   <si>
     <t>老鼠</t>
   </si>
@@ -936,10 +936,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51000010;0;0;51000010;2;2;51000010;0;4;51000009;7;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>51000031;7;1;51000258;7;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1472,6 +1468,23 @@
   <si>
     <t>51000021;5;3;51000021;4;1;51000021;4;5</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jungle</t>
+  </si>
+  <si>
+    <t>51000093;7;0;51000093;7;4;51000106;9;0;51000106;9;4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51000010;6;0;51000010;6;2;51000010;6;4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51000024;3;2</t>
+  </si>
+  <si>
+    <t>51000216;10;2;51000216;10;4</t>
   </si>
 </sst>
 </file>
@@ -4980,7 +4993,7 @@
         <v>153</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>154</v>
@@ -5001,10 +5014,10 @@
         <v>158</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="N1" s="11" t="s">
         <v>237</v>
@@ -5042,7 +5055,7 @@
         <v>149</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>150</v>
@@ -5063,7 +5076,7 @@
         <v>150</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>242</v>
@@ -5104,7 +5117,7 @@
         <v>162</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>163</v>
@@ -5125,10 +5138,10 @@
         <v>167</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>241</v>
@@ -5180,7 +5193,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4">
@@ -5190,7 +5203,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>179</v>
@@ -5226,7 +5239,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4">
@@ -5236,7 +5249,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="R5" s="4" t="s">
         <v>179</v>
@@ -5274,7 +5287,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4">
@@ -5284,7 +5297,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>179</v>
@@ -5324,7 +5337,7 @@
         <v>2</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4">
@@ -5334,7 +5347,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>179</v>
@@ -5372,7 +5385,7 @@
         <v>2</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4">
@@ -5382,7 +5395,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>179</v>
@@ -5422,7 +5435,7 @@
         <v>2</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4">
@@ -5432,7 +5445,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>179</v>
@@ -5472,7 +5485,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4">
@@ -5482,7 +5495,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>179</v>
@@ -5522,7 +5535,7 @@
         <v>2</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4">
@@ -5532,7 +5545,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>179</v>
@@ -5572,7 +5585,7 @@
         <v>2</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4">
@@ -5582,7 +5595,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="R12" s="4" t="s">
         <v>179</v>
@@ -5622,7 +5635,7 @@
         <v>2</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4">
@@ -5632,7 +5645,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>179</v>
@@ -5672,7 +5685,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4">
@@ -5682,7 +5695,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>179</v>
@@ -5722,7 +5735,7 @@
         <v>2</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4">
@@ -5732,7 +5745,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R15" s="4" t="s">
         <v>179</v>
@@ -5772,7 +5785,7 @@
         <v>2</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4">
@@ -5782,7 +5795,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>179</v>
@@ -5822,7 +5835,7 @@
         <v>2</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4">
@@ -5832,7 +5845,7 @@
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="R17" s="4" t="s">
         <v>179</v>
@@ -5870,7 +5883,7 @@
         <v>2</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4">
@@ -5880,7 +5893,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="R18" s="4" t="s">
         <v>179</v>
@@ -5895,10 +5908,10 @@
         <v>43020206</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D19" s="4">
         <v>2</v>
@@ -5920,7 +5933,7 @@
         <v>2</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4">
@@ -5930,7 +5943,7 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="R19" s="4" t="s">
         <v>179</v>
@@ -5945,10 +5958,10 @@
         <v>43020207</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>422</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>423</v>
       </c>
       <c r="D20" s="4">
         <v>2</v>
@@ -5970,7 +5983,7 @@
         <v>2</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4">
@@ -5980,7 +5993,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="R20" s="4" t="s">
         <v>179</v>
@@ -5995,10 +6008,10 @@
         <v>43020301</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D21" s="4">
         <v>3</v>
@@ -6020,7 +6033,7 @@
         <v>2</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4">
@@ -6030,7 +6043,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="R21" s="4" t="s">
         <v>179</v>
@@ -6045,10 +6058,10 @@
         <v>43020302</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>404</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>405</v>
       </c>
       <c r="D22" s="4">
         <v>3</v>
@@ -6070,7 +6083,7 @@
         <v>2</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4">
@@ -6080,7 +6093,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="R22" s="4" t="s">
         <v>179</v>
@@ -6118,7 +6131,7 @@
         <v>2</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4">
@@ -6128,7 +6141,7 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="R23" s="4" t="s">
         <v>179</v>
@@ -6168,7 +6181,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4">
@@ -6178,7 +6191,7 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="R24" s="4" t="s">
         <v>179</v>
@@ -6218,7 +6231,7 @@
         <v>2</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4">
@@ -6228,7 +6241,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="R25" s="4" t="s">
         <v>179</v>
@@ -6243,10 +6256,10 @@
         <v>43020306</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D26" s="4">
         <v>3</v>
@@ -6268,7 +6281,7 @@
         <v>2</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4">
@@ -6278,7 +6291,7 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="R26" s="4" t="s">
         <v>179</v>
@@ -6293,7 +6306,7 @@
         <v>43020307</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>94</v>
@@ -6318,7 +6331,7 @@
         <v>2</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4">
@@ -6328,7 +6341,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="R27" s="4" t="s">
         <v>179</v>
@@ -6368,7 +6381,7 @@
         <v>2</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="4">
@@ -6378,7 +6391,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>179</v>
@@ -6418,7 +6431,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4">
@@ -6428,7 +6441,7 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="R29" s="4" t="s">
         <v>179</v>
@@ -6468,7 +6481,7 @@
         <v>2</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L30" s="4"/>
       <c r="M30" s="4">
@@ -6478,7 +6491,7 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>179</v>
@@ -6518,7 +6531,7 @@
         <v>2</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L31" s="4"/>
       <c r="M31" s="4">
@@ -6528,7 +6541,7 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="R31" s="4" t="s">
         <v>179</v>
@@ -6568,7 +6581,7 @@
         <v>2</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="4">
@@ -6578,7 +6591,7 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="R32" s="4" t="s">
         <v>179</v>
@@ -6618,7 +6631,7 @@
         <v>2</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L33" s="4"/>
       <c r="M33" s="4">
@@ -6628,7 +6641,7 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="R33" s="4" t="s">
         <v>179</v>
@@ -6668,7 +6681,7 @@
         <v>2</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4">
@@ -6678,7 +6691,7 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="R34" s="4" t="s">
         <v>179</v>
@@ -6718,7 +6731,7 @@
         <v>2</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="L35" s="4"/>
       <c r="M35" s="4">
@@ -6728,7 +6741,7 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>179</v>
@@ -6768,7 +6781,7 @@
         <v>2</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="L36" s="4"/>
       <c r="M36" s="4">
@@ -6778,7 +6791,7 @@
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="R36" s="4" t="s">
         <v>179</v>
@@ -6818,7 +6831,7 @@
         <v>2</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="L37" s="4"/>
       <c r="M37" s="4">
@@ -6828,7 +6841,7 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>179</v>
@@ -6868,7 +6881,7 @@
         <v>2</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="L38" s="4"/>
       <c r="M38" s="4">
@@ -6878,7 +6891,7 @@
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R38" s="4" t="s">
         <v>179</v>
@@ -6918,7 +6931,7 @@
         <v>2</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L39" s="4"/>
       <c r="M39" s="4">
@@ -6928,7 +6941,7 @@
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="R39" s="4" t="s">
         <v>179</v>
@@ -6946,7 +6959,7 @@
         <v>120</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D40" s="4">
         <v>4</v>
@@ -6968,7 +6981,7 @@
         <v>2</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="4">
@@ -6978,7 +6991,7 @@
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="R40" s="4" t="s">
         <v>179</v>
@@ -6993,10 +7006,10 @@
         <v>43020409</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D41" s="4">
         <v>4</v>
@@ -7018,7 +7031,7 @@
         <v>2</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L41" s="4"/>
       <c r="M41" s="4">
@@ -7028,7 +7041,7 @@
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="R41" s="4" t="s">
         <v>179</v>
@@ -7068,7 +7081,7 @@
         <v>2</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="4">
@@ -7078,7 +7091,7 @@
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="R42" s="4" t="s">
         <v>179</v>
@@ -7118,7 +7131,7 @@
         <v>2</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L43" s="4"/>
       <c r="M43" s="4">
@@ -7128,7 +7141,7 @@
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="R43" s="4" t="s">
         <v>179</v>
@@ -7168,7 +7181,7 @@
         <v>2</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L44" s="4"/>
       <c r="M44" s="4">
@@ -7178,7 +7191,7 @@
       <c r="O44" s="4"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="R44" s="4" t="s">
         <v>179</v>
@@ -7218,7 +7231,7 @@
         <v>2</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L45" s="4"/>
       <c r="M45" s="4">
@@ -7228,7 +7241,7 @@
       <c r="O45" s="4"/>
       <c r="P45" s="4"/>
       <c r="Q45" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="R45" s="4" t="s">
         <v>179</v>
@@ -7243,10 +7256,10 @@
         <v>43020505</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D46" s="27">
         <v>5</v>
@@ -7268,7 +7281,7 @@
         <v>2</v>
       </c>
       <c r="K46" s="27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L46" s="4"/>
       <c r="M46" s="4">
@@ -7278,7 +7291,7 @@
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
       <c r="Q46" s="27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R46" s="4" t="s">
         <v>179</v>
@@ -7293,10 +7306,10 @@
         <v>43020506</v>
       </c>
       <c r="B47" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>415</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>416</v>
       </c>
       <c r="D47" s="27">
         <v>5</v>
@@ -7318,7 +7331,7 @@
         <v>2</v>
       </c>
       <c r="K47" s="27" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L47" s="4"/>
       <c r="M47" s="4">
@@ -7328,7 +7341,7 @@
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
       <c r="Q47" s="27" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="R47" s="4" t="s">
         <v>179</v>
@@ -7355,7 +7368,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G48" s="33">
         <v>11000002</v>
@@ -7368,7 +7381,7 @@
         <v>2</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="L48" s="4"/>
       <c r="M48" s="4">
@@ -7378,7 +7391,7 @@
       <c r="O48" s="4"/>
       <c r="P48" s="4"/>
       <c r="Q48" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="R48" s="4" t="s">
         <v>179</v>
@@ -7403,7 +7416,7 @@
       </c>
       <c r="E49" s="32"/>
       <c r="F49" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G49" s="33">
         <v>11000010</v>
@@ -7416,7 +7429,7 @@
         <v>2</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L49" s="4"/>
       <c r="M49" s="4">
@@ -7426,7 +7439,7 @@
       <c r="O49" s="4"/>
       <c r="P49" s="4"/>
       <c r="Q49" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="R49" s="4" t="s">
         <v>179</v>
@@ -7451,7 +7464,7 @@
       </c>
       <c r="E50" s="32"/>
       <c r="F50" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G50" s="33">
         <v>11000002</v>
@@ -7464,7 +7477,7 @@
         <v>2</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L50" s="4"/>
       <c r="M50" s="4">
@@ -7474,7 +7487,7 @@
       <c r="O50" s="4"/>
       <c r="P50" s="4"/>
       <c r="Q50" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="R50" s="4" t="s">
         <v>179</v>
@@ -7489,10 +7502,10 @@
         <v>43020604</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D51" s="4">
         <v>6</v>
@@ -7501,7 +7514,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G51" s="33">
         <v>11000001</v>
@@ -7514,7 +7527,7 @@
         <v>2</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L51" s="4"/>
       <c r="M51" s="4">
@@ -7524,7 +7537,7 @@
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
       <c r="Q51" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="R51" s="4" t="s">
         <v>179</v>
@@ -7633,10 +7646,10 @@
   <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="I28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomRight" activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7668,7 +7681,7 @@
         <v>153</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>154</v>
@@ -7689,10 +7702,10 @@
         <v>158</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="N1" s="29" t="s">
         <v>237</v>
@@ -7730,7 +7743,7 @@
         <v>149</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>150</v>
@@ -7751,7 +7764,7 @@
         <v>150</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M2" s="30" t="s">
         <v>242</v>
@@ -7792,7 +7805,7 @@
         <v>162</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>163</v>
@@ -7813,10 +7826,10 @@
         <v>167</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>241</v>
@@ -7868,7 +7881,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L4">
         <v>51018005</v>
@@ -7882,7 +7895,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>248</v>
@@ -7918,7 +7931,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L5">
         <v>51018005</v>
@@ -7932,7 +7945,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="R5" s="4" t="s">
         <v>248</v>
@@ -7968,7 +7981,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L6">
         <v>51018005</v>
@@ -7982,7 +7995,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>180</v>
@@ -8018,7 +8031,7 @@
         <v>2</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L7">
         <v>51018006</v>
@@ -8032,7 +8045,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>180</v>
@@ -8068,7 +8081,7 @@
         <v>2</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L8">
         <v>51018006</v>
@@ -8082,7 +8095,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>180</v>
@@ -8118,7 +8131,7 @@
         <v>2</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L9">
         <v>51018005</v>
@@ -8132,7 +8145,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>248</v>
@@ -8168,7 +8181,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L10">
         <v>51018006</v>
@@ -8182,7 +8195,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>180</v>
@@ -8218,7 +8231,7 @@
         <v>2</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L11">
         <v>51018005</v>
@@ -8232,7 +8245,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>180</v>
@@ -8268,7 +8281,7 @@
         <v>2</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L12">
         <v>51018005</v>
@@ -8282,7 +8295,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="R12" s="4" t="s">
         <v>180</v>
@@ -8318,7 +8331,7 @@
         <v>2</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L13">
         <v>51018005</v>
@@ -8332,7 +8345,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>180</v>
@@ -8368,7 +8381,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L14">
         <v>51018005</v>
@@ -8382,7 +8395,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>180</v>
@@ -8418,7 +8431,7 @@
         <v>2</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L15">
         <v>51018005</v>
@@ -8432,7 +8445,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R15" s="4" t="s">
         <v>180</v>
@@ -8468,7 +8481,7 @@
         <v>2</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L16">
         <v>51018005</v>
@@ -8482,7 +8495,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>180</v>
@@ -8518,7 +8531,7 @@
         <v>2</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L17">
         <v>51018005</v>
@@ -8532,7 +8545,7 @@
       <c r="O17" s="4"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="R17" s="4" t="s">
         <v>180</v>
@@ -8568,7 +8581,7 @@
         <v>2</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L18">
         <v>51018007</v>
@@ -8582,7 +8595,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R18" s="4" t="s">
         <v>180</v>
@@ -8618,7 +8631,7 @@
         <v>2</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L19">
         <v>51018007</v>
@@ -8632,7 +8645,7 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="R19" s="4" t="s">
         <v>180</v>
@@ -8668,7 +8681,7 @@
         <v>2</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L20">
         <v>51018005</v>
@@ -8682,7 +8695,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="R20" s="4" t="s">
         <v>180</v>
@@ -8718,7 +8731,7 @@
         <v>2</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L21">
         <v>51018005</v>
@@ -8732,7 +8745,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="R21" s="4" t="s">
         <v>180</v>
@@ -8768,7 +8781,7 @@
         <v>2</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L22">
         <v>51018007</v>
@@ -8782,7 +8795,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="R22" s="4" t="s">
         <v>180</v>
@@ -8818,7 +8831,7 @@
         <v>2</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L23">
         <v>51018005</v>
@@ -8832,7 +8845,7 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="R23" s="4" t="s">
         <v>180</v>
@@ -8868,7 +8881,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L24">
         <v>51018006</v>
@@ -8882,7 +8895,7 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R24" s="4" t="s">
         <v>180</v>
@@ -8918,7 +8931,7 @@
         <v>2</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L25">
         <v>51018005</v>
@@ -8932,7 +8945,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="R25" s="4" t="s">
         <v>180</v>
@@ -8968,7 +8981,7 @@
         <v>2</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L26">
         <v>51018005</v>
@@ -8982,7 +8995,7 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="R26" s="4" t="s">
         <v>180</v>
@@ -9018,7 +9031,7 @@
         <v>2</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L27">
         <v>51018005</v>
@@ -9032,7 +9045,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="R27" s="4" t="s">
         <v>180</v>
@@ -9068,7 +9081,7 @@
         <v>2</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L28">
         <v>51018005</v>
@@ -9082,7 +9095,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>180</v>
@@ -9118,7 +9131,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L29">
         <v>51018006</v>
@@ -9132,7 +9145,7 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="R29" s="4" t="s">
         <v>180</v>
@@ -9168,7 +9181,7 @@
         <v>2</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="L30">
         <v>51018006</v>
@@ -9182,7 +9195,7 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>180</v>
@@ -9218,7 +9231,7 @@
         <v>2</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="L31">
         <v>51018005</v>
@@ -9232,7 +9245,7 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="R31" s="4" t="s">
         <v>180</v>
@@ -9268,7 +9281,7 @@
         <v>2</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="L32">
         <v>51018005</v>
@@ -9282,7 +9295,7 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="R32" s="4" t="s">
         <v>180</v>
@@ -9318,7 +9331,7 @@
         <v>2</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L33">
         <v>51018005</v>
@@ -9332,7 +9345,7 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="R33" s="4" t="s">
         <v>180</v>
@@ -9368,7 +9381,7 @@
         <v>2</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L34">
         <v>51018005</v>
@@ -9382,7 +9395,7 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="R34" s="4" t="s">
         <v>180</v>
@@ -9418,7 +9431,7 @@
         <v>2</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L35">
         <v>51018005</v>
@@ -9432,7 +9445,7 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>180</v>
@@ -9468,7 +9481,7 @@
         <v>2</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L36">
         <v>51018005</v>
@@ -9482,7 +9495,7 @@
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="R36" s="4" t="s">
         <v>180</v>
@@ -9518,7 +9531,7 @@
         <v>2</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L37">
         <v>51018005</v>
@@ -9532,7 +9545,7 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>180</v>
@@ -9568,7 +9581,7 @@
         <v>2</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L38">
         <v>51018005</v>
@@ -9582,7 +9595,7 @@
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="R38" s="4" t="s">
         <v>180</v>
@@ -9618,7 +9631,7 @@
         <v>2</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L39">
         <v>51018007</v>
@@ -9630,11 +9643,11 @@
         <v>15</v>
       </c>
       <c r="O39" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="R39" s="6" t="s">
         <v>249</v>
@@ -9670,7 +9683,7 @@
         <v>2</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L40">
         <v>51018007</v>
@@ -9682,11 +9695,11 @@
         <v>15</v>
       </c>
       <c r="O40" s="4" t="s">
-        <v>270</v>
+        <v>433</v>
       </c>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="R40" s="4" t="s">
         <v>180</v>
@@ -9702,7 +9715,7 @@
         <v>269</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D41" s="4">
         <v>0</v>
@@ -9722,7 +9735,7 @@
         <v>2</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L41">
         <v>51018007</v>
@@ -9734,11 +9747,11 @@
         <v>10</v>
       </c>
       <c r="O41" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="P41" s="4"/>
       <c r="Q41" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="R41" s="4" t="s">
         <v>180</v>
@@ -9774,7 +9787,7 @@
         <v>2</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="L42">
         <v>51018005</v>
@@ -9785,13 +9798,15 @@
       <c r="N42" s="4">
         <v>10</v>
       </c>
-      <c r="O42" s="4"/>
+      <c r="O42" s="4" t="s">
+        <v>432</v>
+      </c>
       <c r="P42" s="4"/>
       <c r="Q42" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="R42" s="34" t="s">
-        <v>180</v>
+        <v>431</v>
       </c>
       <c r="S42" s="13"/>
       <c r="T42" s="17"/>
@@ -9824,7 +9839,7 @@
         <v>2</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L43">
         <v>51018007</v>
@@ -9835,10 +9850,12 @@
       <c r="N43" s="4">
         <v>10</v>
       </c>
-      <c r="O43" s="4"/>
+      <c r="O43" s="4" t="s">
+        <v>434</v>
+      </c>
       <c r="P43" s="4"/>
       <c r="Q43" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="R43" s="4" t="s">
         <v>180</v>
@@ -9874,7 +9891,7 @@
         <v>2</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L44">
         <v>51018006</v>
@@ -9885,13 +9902,15 @@
       <c r="N44" s="4">
         <v>10</v>
       </c>
-      <c r="O44" s="4"/>
+      <c r="O44" s="4" t="s">
+        <v>435</v>
+      </c>
       <c r="P44" s="4"/>
       <c r="Q44" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="R44" s="4" t="s">
-        <v>180</v>
+        <v>310</v>
+      </c>
+      <c r="R44" s="6" t="s">
+        <v>249</v>
       </c>
       <c r="S44" s="27"/>
       <c r="T44" s="36"/>
@@ -9904,7 +9923,7 @@
         <v>267</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D45" s="27">
         <v>0</v>
@@ -9924,7 +9943,7 @@
         <v>2</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L45">
         <v>51018005</v>
@@ -9938,7 +9957,7 @@
       <c r="O45" s="27"/>
       <c r="P45" s="27"/>
       <c r="Q45" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="R45" s="27" t="s">
         <v>180</v>
@@ -9954,7 +9973,7 @@
         <v>266</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D46" s="27">
         <v>0</v>
@@ -9974,7 +9993,7 @@
         <v>2</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L46">
         <v>51018005</v>
@@ -9988,7 +10007,7 @@
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
       <c r="Q46" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="R46" s="27" t="s">
         <v>180</v>
@@ -10001,10 +10020,10 @@
         <v>43002003</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D47" s="27">
         <v>0</v>
@@ -10024,7 +10043,7 @@
         <v>2</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L47">
         <v>51018005</v>
@@ -10038,7 +10057,7 @@
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
       <c r="Q47" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="R47" s="27" t="s">
         <v>180</v>
@@ -10051,10 +10070,10 @@
         <v>43002004</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D48" s="27">
         <v>0</v>
@@ -10074,7 +10093,7 @@
         <v>2</v>
       </c>
       <c r="K48" s="31" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L48">
         <v>51018005</v>
@@ -10088,7 +10107,7 @@
       <c r="O48" s="27"/>
       <c r="P48" s="27"/>
       <c r="Q48" s="31" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="R48" s="27" t="s">
         <v>180</v>
@@ -10101,10 +10120,10 @@
         <v>43002005</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D49" s="27">
         <v>0</v>
@@ -10124,7 +10143,7 @@
         <v>2</v>
       </c>
       <c r="K49" s="31" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L49">
         <v>51018005</v>
@@ -10138,7 +10157,7 @@
       <c r="O49" s="27"/>
       <c r="P49" s="27"/>
       <c r="Q49" s="31" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="R49" s="27" t="s">
         <v>180</v>
@@ -10151,10 +10170,10 @@
         <v>43002006</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D50" s="27">
         <v>0</v>
@@ -10174,7 +10193,7 @@
         <v>2</v>
       </c>
       <c r="K50" s="31" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L50">
         <v>51018005</v>
@@ -10188,7 +10207,7 @@
       <c r="O50" s="27"/>
       <c r="P50" s="27"/>
       <c r="Q50" s="31" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="R50" s="27" t="s">
         <v>180</v>
@@ -10281,7 +10300,7 @@
         <v>153</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F1" s="25" t="s">
         <v>154</v>
@@ -10302,10 +10321,10 @@
         <v>158</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="N1" s="25" t="s">
         <v>236</v>
@@ -10405,7 +10424,7 @@
         <v>162</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>163</v>
@@ -10426,10 +10445,10 @@
         <v>167</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>240</v>
@@ -10483,7 +10502,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4">
@@ -10495,7 +10514,7 @@
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>180</v>
@@ -10543,7 +10562,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="R5" s="4" t="s">
         <v>180</v>
@@ -10578,10 +10597,10 @@
         <v>10</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4">
@@ -10591,7 +10610,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>180</v>
@@ -10626,10 +10645,10 @@
         <v>10</v>
       </c>
       <c r="J7" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>297</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>298</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4">
@@ -10639,7 +10658,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>180</v>
@@ -10674,10 +10693,10 @@
         <v>2</v>
       </c>
       <c r="J8" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="K8" s="6" t="s">
         <v>398</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>399</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="4">
@@ -10689,7 +10708,7 @@
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>180</v>
@@ -10724,10 +10743,10 @@
         <v>2</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="4">
@@ -10739,7 +10758,7 @@
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>180</v>
@@ -10772,10 +10791,10 @@
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4">
@@ -10785,7 +10804,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>180</v>
@@ -10818,10 +10837,10 @@
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4">
@@ -10831,7 +10850,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>180</v>
@@ -10864,10 +10883,10 @@
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4">
@@ -10877,7 +10896,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="R12" s="4" t="s">
         <v>180</v>
@@ -10910,10 +10929,10 @@
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4">
@@ -10923,7 +10942,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>180</v>
@@ -10956,10 +10975,10 @@
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4">
@@ -10969,7 +10988,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>180</v>

</xml_diff>

<commit_message>
optimise the chess move method
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{695370B1-8981-4826-9B73-022240911C69}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="人物" sheetId="4" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="435">
   <si>
     <t>老鼠</t>
   </si>
@@ -1457,12 +1456,34 @@
   </si>
   <si>
     <t>51000216;10;2;51000216;10;4</t>
+  </si>
+  <si>
+    <t>初始场景id</t>
+  </si>
+  <si>
+    <t>初始场景id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BornSceneId</t>
+  </si>
+  <si>
+    <t>BornSceneId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Figue</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2370,7 +2391,36 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="97">
+  <dxfs count="100">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2683,6 +2733,54 @@
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -4420,6 +4518,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4432,93 +4598,96 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2_4" displayName="表2_4" ref="A3:S51" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95" tableBorderDxfId="94">
-  <autoFilter ref="A3:S51" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState ref="A4:S50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:T51" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98" tableBorderDxfId="97">
+  <autoFilter ref="A3:T51"/>
+  <sortState ref="A4:T50">
     <sortCondition ref="A3:A50"/>
   </sortState>
-  <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="92"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Ename" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="90"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Quality" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="World" dataDxfId="88"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Job" dataDxfId="87"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Level" dataDxfId="86"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="AutoAddLevel" dataDxfId="85"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Method" dataDxfId="84"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Emethod" dataDxfId="83"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="KingTowerId" dataDxfId="82"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="EpRecoverRate" dataDxfId="81"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="CardReduce" dataDxfId="80"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="RightMon" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="PetMon" dataDxfId="78"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Figue" dataDxfId="77"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BattleMap" dataDxfId="76"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="InRandomQuest" dataDxfId="75"/>
+  <tableColumns count="20">
+    <tableColumn id="1" name="Id" dataDxfId="96"/>
+    <tableColumn id="2" name="Name" dataDxfId="95"/>
+    <tableColumn id="18" name="Ename" dataDxfId="94"/>
+    <tableColumn id="3" name="Type" dataDxfId="93"/>
+    <tableColumn id="21" name="Quality" dataDxfId="92"/>
+    <tableColumn id="6" name="World" dataDxfId="91"/>
+    <tableColumn id="10" name="Job" dataDxfId="90"/>
+    <tableColumn id="11" name="Level" dataDxfId="89"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="88"/>
+    <tableColumn id="13" name="Method" dataDxfId="87"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="86"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="85"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="84"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="83"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="82"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="81"/>
+    <tableColumn id="7" name="BornSceneId" dataDxfId="33"/>
+    <tableColumn id="17" name="Figue" dataDxfId="80"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="79"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表2" displayName="表2" ref="A3:S50" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72">
-  <autoFilter ref="A3:S50" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState ref="A4:S50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75">
+  <autoFilter ref="A3:T50"/>
+  <sortState ref="A4:T50">
     <sortCondition ref="A3:A50"/>
   </sortState>
-  <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="70"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Ename" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="68"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Quality" dataDxfId="67"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="World" dataDxfId="66"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Job" dataDxfId="65"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Level" dataDxfId="64"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="AutoAddLevel" dataDxfId="63"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Method" dataDxfId="62"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Emethod" dataDxfId="61"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="KingTowerId" dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="EpRecoverRate" dataDxfId="59"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="CardReduce" dataDxfId="58"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="RightMon" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PetMon" dataDxfId="56"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Figue" dataDxfId="55"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BattleMap" dataDxfId="54"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="InRandomQuest" dataDxfId="53"/>
+  <tableColumns count="20">
+    <tableColumn id="1" name="Id" dataDxfId="74"/>
+    <tableColumn id="2" name="Name" dataDxfId="73"/>
+    <tableColumn id="18" name="Ename" dataDxfId="72"/>
+    <tableColumn id="3" name="Type" dataDxfId="71"/>
+    <tableColumn id="7" name="Quality" dataDxfId="70"/>
+    <tableColumn id="6" name="World" dataDxfId="69"/>
+    <tableColumn id="10" name="Job" dataDxfId="68"/>
+    <tableColumn id="11" name="Level" dataDxfId="67"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="66"/>
+    <tableColumn id="13" name="Method" dataDxfId="65"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="64"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="63"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="62"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="61"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="60"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="59"/>
+    <tableColumn id="8" name="BornSceneId" dataDxfId="32"/>
+    <tableColumn id="17" name="Figue" dataDxfId="58"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="57"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表2_2" displayName="表2_2" ref="A3:S14" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51" tableBorderDxfId="50">
-  <autoFilter ref="A3:S14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A4:R83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:T14" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53">
+  <autoFilter ref="A3:T14"/>
+  <sortState ref="A4:S83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="48"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Ename" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type" dataDxfId="46"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Quality" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="World" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Job" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Level" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="AutoAddLevel" dataDxfId="41"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Method" dataDxfId="40"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Emethod" dataDxfId="39"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="KingTowerId" dataDxfId="38"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="EpRecoverRate" dataDxfId="37"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="CardReduce" dataDxfId="36"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="RightMon" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="PetMon" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Figue" dataDxfId="33"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="BattleMap" dataDxfId="32"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="InRandomQuest" dataDxfId="31"/>
+  <tableColumns count="20">
+    <tableColumn id="1" name="Id" dataDxfId="52"/>
+    <tableColumn id="2" name="Name" dataDxfId="51"/>
+    <tableColumn id="18" name="Ename" dataDxfId="50"/>
+    <tableColumn id="3" name="Type" dataDxfId="49"/>
+    <tableColumn id="7" name="Quality" dataDxfId="48"/>
+    <tableColumn id="6" name="World" dataDxfId="47"/>
+    <tableColumn id="10" name="Job" dataDxfId="46"/>
+    <tableColumn id="11" name="Level" dataDxfId="45"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="44"/>
+    <tableColumn id="13" name="Method" dataDxfId="43"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="42"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="41"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="40"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="39"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="38"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="37"/>
+    <tableColumn id="8" name="BornSceneId" dataDxfId="0"/>
+    <tableColumn id="9" name="Figue" dataDxfId="36"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="35"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4532,7 +4701,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -4844,14 +5013,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R34" sqref="R34"/>
+      <selection pane="bottomRight" activeCell="Q45" sqref="Q45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4863,10 +5032,11 @@
     <col min="10" max="10" width="9.5" customWidth="1"/>
     <col min="11" max="12" width="10.625" customWidth="1"/>
     <col min="13" max="16" width="5.875" customWidth="1"/>
-    <col min="18" max="18" width="10.625" customWidth="1"/>
+    <col min="17" max="17" width="9.75" customWidth="1"/>
+    <col min="19" max="19" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" ht="72" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>151</v>
       </c>
@@ -4915,17 +5085,20 @@
       <c r="P1" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="R1" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>149</v>
       </c>
@@ -4974,17 +5147,20 @@
       <c r="P2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>160</v>
       </c>
@@ -5034,16 +5210,19 @@
         <v>240</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>168</v>
+        <v>433</v>
       </c>
       <c r="R3" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="S3" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43020101</v>
       </c>
@@ -5080,15 +5259,18 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="4">
+        <v>13010002</v>
+      </c>
+      <c r="R4" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S4" s="19"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T4" s="19"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43020102</v>
       </c>
@@ -5125,15 +5307,18 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="4">
+        <v>13010003</v>
+      </c>
+      <c r="R5" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S5" s="19"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T5" s="19"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43020103</v>
       </c>
@@ -5172,17 +5357,20 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="4" t="s">
+      <c r="Q6" s="4">
+        <v>13010004</v>
+      </c>
+      <c r="R6" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="S6" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S6" s="19" t="s">
+      <c r="T6" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43020104</v>
       </c>
@@ -5221,15 +5409,18 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="4" t="s">
+      <c r="Q7" s="4">
+        <v>13010007</v>
+      </c>
+      <c r="R7" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="S7" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S7" s="19"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T7" s="19"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43020105</v>
       </c>
@@ -5268,17 +5459,20 @@
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="4" t="s">
+      <c r="Q8" s="4">
+        <v>13010009</v>
+      </c>
+      <c r="R8" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="S8" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S8" s="19" t="s">
+      <c r="T8" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43020106</v>
       </c>
@@ -5317,17 +5511,20 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="4" t="s">
+      <c r="Q9" s="4">
+        <v>13010008</v>
+      </c>
+      <c r="R9" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="S9" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S9" s="19" t="s">
+      <c r="T9" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43020107</v>
       </c>
@@ -5366,17 +5563,18 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="4" t="s">
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="R10" s="4" t="s">
+      <c r="S10" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S10" s="19" t="s">
+      <c r="T10" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43020108</v>
       </c>
@@ -5415,17 +5613,20 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="4" t="s">
+      <c r="Q11" s="4">
+        <v>13010203</v>
+      </c>
+      <c r="R11" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="S11" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S11" s="19" t="s">
+      <c r="T11" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43020109</v>
       </c>
@@ -5464,17 +5665,20 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="4" t="s">
+      <c r="Q12" s="4">
+        <v>13010202</v>
+      </c>
+      <c r="R12" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="R12" s="4" t="s">
+      <c r="S12" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S12" s="19" t="s">
+      <c r="T12" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43020110</v>
       </c>
@@ -5513,17 +5717,20 @@
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="4" t="s">
+      <c r="Q13" s="4">
+        <v>13010203</v>
+      </c>
+      <c r="R13" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="R13" s="4" t="s">
+      <c r="S13" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S13" s="19" t="s">
+      <c r="T13" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43020201</v>
       </c>
@@ -5562,17 +5769,20 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="4" t="s">
+      <c r="Q14" s="4">
+        <v>13010103</v>
+      </c>
+      <c r="R14" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="R14" s="4" t="s">
+      <c r="S14" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S14" s="19" t="s">
+      <c r="T14" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43020202</v>
       </c>
@@ -5611,17 +5821,18 @@
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
-      <c r="Q15" s="4" t="s">
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="R15" s="4" t="s">
+      <c r="S15" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S15" s="19" t="s">
+      <c r="T15" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43020203</v>
       </c>
@@ -5660,17 +5871,18 @@
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
-      <c r="Q16" s="4" t="s">
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="R16" s="4" t="s">
+      <c r="S16" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S16" s="19" t="s">
+      <c r="T16" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43020204</v>
       </c>
@@ -5709,17 +5921,20 @@
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="4" t="s">
+      <c r="Q17" s="4">
+        <v>13010107</v>
+      </c>
+      <c r="R17" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="R17" s="4" t="s">
+      <c r="S17" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S17" s="19" t="s">
+      <c r="T17" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43020205</v>
       </c>
@@ -5756,17 +5971,20 @@
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
-      <c r="Q18" s="4" t="s">
+      <c r="Q18" s="4">
+        <v>13010202</v>
+      </c>
+      <c r="R18" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="R18" s="4" t="s">
+      <c r="S18" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S18" s="19" t="s">
+      <c r="T18" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43020206</v>
       </c>
@@ -5805,17 +6023,20 @@
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="4" t="s">
+      <c r="Q19" s="4">
+        <v>13010205</v>
+      </c>
+      <c r="R19" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="R19" s="4" t="s">
+      <c r="S19" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S19" s="19" t="s">
+      <c r="T19" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43020207</v>
       </c>
@@ -5854,17 +6075,18 @@
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="4" t="s">
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="R20" s="4" t="s">
+      <c r="S20" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S20" s="19" t="s">
+      <c r="T20" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43020301</v>
       </c>
@@ -5903,17 +6125,20 @@
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
-      <c r="Q21" s="4" t="s">
+      <c r="Q21" s="4">
+        <v>13010102</v>
+      </c>
+      <c r="R21" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="R21" s="4" t="s">
+      <c r="S21" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S21" s="19" t="s">
+      <c r="T21" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43020302</v>
       </c>
@@ -5952,17 +6177,18 @@
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
-      <c r="Q22" s="4" t="s">
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="R22" s="4" t="s">
+      <c r="S22" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S22" s="19" t="s">
+      <c r="T22" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43020303</v>
       </c>
@@ -5999,17 +6225,20 @@
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
-      <c r="Q23" s="4" t="s">
+      <c r="Q23" s="4">
+        <v>13010106</v>
+      </c>
+      <c r="R23" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="R23" s="4" t="s">
+      <c r="S23" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S23" s="19" t="s">
+      <c r="T23" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43020304</v>
       </c>
@@ -6048,17 +6277,18 @@
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
-      <c r="Q24" s="4" t="s">
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="R24" s="4" t="s">
+      <c r="S24" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S24" s="19" t="s">
+      <c r="T24" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43020305</v>
       </c>
@@ -6097,17 +6327,20 @@
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
-      <c r="Q25" s="4" t="s">
+      <c r="Q25" s="4">
+        <v>13010204</v>
+      </c>
+      <c r="R25" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="R25" s="4" t="s">
+      <c r="S25" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S25" s="19" t="s">
+      <c r="T25" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43020306</v>
       </c>
@@ -6146,17 +6379,20 @@
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
-      <c r="Q26" s="4" t="s">
+      <c r="Q26" s="4">
+        <v>13010204</v>
+      </c>
+      <c r="R26" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="R26" s="4" t="s">
+      <c r="S26" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S26" s="19" t="s">
+      <c r="T26" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43020307</v>
       </c>
@@ -6195,17 +6431,20 @@
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
-      <c r="Q27" s="4" t="s">
+      <c r="Q27" s="4">
+        <v>13010102</v>
+      </c>
+      <c r="R27" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="R27" s="4" t="s">
+      <c r="S27" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S27" s="19" t="s">
+      <c r="T27" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43020308</v>
       </c>
@@ -6244,17 +6483,18 @@
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
-      <c r="Q28" s="4" t="s">
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="R28" s="4" t="s">
+      <c r="S28" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S28" s="19" t="s">
+      <c r="T28" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43020309</v>
       </c>
@@ -6293,17 +6533,20 @@
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
-      <c r="Q29" s="4" t="s">
+      <c r="Q29" s="4">
+        <v>13010105</v>
+      </c>
+      <c r="R29" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="R29" s="4" t="s">
+      <c r="S29" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S29" s="19" t="s">
+      <c r="T29" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43020310</v>
       </c>
@@ -6342,17 +6585,20 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
-      <c r="Q30" s="4" t="s">
+      <c r="Q30" s="4">
+        <v>13010105</v>
+      </c>
+      <c r="R30" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="R30" s="4" t="s">
+      <c r="S30" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S30" s="19" t="s">
+      <c r="T30" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43020311</v>
       </c>
@@ -6391,17 +6637,18 @@
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
-      <c r="Q31" s="4" t="s">
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="R31" s="4" t="s">
+      <c r="S31" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S31" s="19" t="s">
+      <c r="T31" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43020312</v>
       </c>
@@ -6440,17 +6687,18 @@
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
-      <c r="Q32" s="4" t="s">
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="R32" s="4" t="s">
+      <c r="S32" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S32" s="19" t="s">
+      <c r="T32" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43020401</v>
       </c>
@@ -6489,17 +6737,20 @@
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
-      <c r="Q33" s="4" t="s">
+      <c r="Q33" s="4">
+        <v>13010108</v>
+      </c>
+      <c r="R33" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="R33" s="4" t="s">
+      <c r="S33" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S33" s="19" t="s">
+      <c r="T33" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43020402</v>
       </c>
@@ -6538,17 +6789,20 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
-      <c r="Q34" s="4" t="s">
+      <c r="Q34" s="4">
+        <v>13010103</v>
+      </c>
+      <c r="R34" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="R34" s="4" t="s">
+      <c r="S34" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S34" s="19" t="s">
+      <c r="T34" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43020403</v>
       </c>
@@ -6587,17 +6841,18 @@
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
-      <c r="Q35" s="4" t="s">
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="R35" s="4" t="s">
+      <c r="S35" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S35" s="19" t="s">
+      <c r="T35" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43020404</v>
       </c>
@@ -6636,17 +6891,20 @@
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
-      <c r="Q36" s="4" t="s">
+      <c r="Q36" s="4">
+        <v>13010208</v>
+      </c>
+      <c r="R36" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="R36" s="4" t="s">
+      <c r="S36" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S36" s="19" t="s">
+      <c r="T36" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43020405</v>
       </c>
@@ -6685,17 +6943,20 @@
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
-      <c r="Q37" s="4" t="s">
+      <c r="Q37" s="4">
+        <v>13010108</v>
+      </c>
+      <c r="R37" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="R37" s="4" t="s">
+      <c r="S37" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S37" s="19" t="s">
+      <c r="T37" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43020406</v>
       </c>
@@ -6734,17 +6995,20 @@
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
-      <c r="Q38" s="4" t="s">
+      <c r="Q38" s="4">
+        <v>13010104</v>
+      </c>
+      <c r="R38" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="R38" s="4" t="s">
+      <c r="S38" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S38" s="19" t="s">
+      <c r="T38" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>43020407</v>
       </c>
@@ -6783,17 +7047,20 @@
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
-      <c r="Q39" s="4" t="s">
+      <c r="Q39" s="4">
+        <v>13010209</v>
+      </c>
+      <c r="R39" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="R39" s="4" t="s">
+      <c r="S39" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S39" s="19" t="s">
+      <c r="T39" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>43020408</v>
       </c>
@@ -6832,17 +7099,20 @@
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
-      <c r="Q40" s="4" t="s">
+      <c r="Q40" s="4">
+        <v>13010205</v>
+      </c>
+      <c r="R40" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="R40" s="4" t="s">
+      <c r="S40" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S40" s="19" t="s">
+      <c r="T40" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>43020409</v>
       </c>
@@ -6881,17 +7151,18 @@
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
-      <c r="Q41" s="4" t="s">
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="R41" s="4" t="s">
+      <c r="S41" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S41" s="19" t="s">
+      <c r="T41" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>43020501</v>
       </c>
@@ -6930,17 +7201,18 @@
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
-      <c r="Q42" s="4" t="s">
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="R42" s="4" t="s">
+      <c r="S42" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S42" s="19" t="s">
+      <c r="T42" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>43020502</v>
       </c>
@@ -6979,17 +7251,20 @@
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
-      <c r="Q43" s="4" t="s">
+      <c r="Q43" s="4">
+        <v>13010109</v>
+      </c>
+      <c r="R43" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="R43" s="4" t="s">
+      <c r="S43" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S43" s="19" t="s">
+      <c r="T43" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43020503</v>
       </c>
@@ -7028,17 +7303,20 @@
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
       <c r="P44" s="4"/>
-      <c r="Q44" s="4" t="s">
+      <c r="Q44" s="4">
+        <v>13010207</v>
+      </c>
+      <c r="R44" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="R44" s="4" t="s">
+      <c r="S44" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S44" s="19" t="s">
+      <c r="T44" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>43020504</v>
       </c>
@@ -7077,17 +7355,20 @@
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
       <c r="P45" s="4"/>
-      <c r="Q45" s="4" t="s">
+      <c r="Q45" s="4">
+        <v>13010209</v>
+      </c>
+      <c r="R45" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="R45" s="4" t="s">
+      <c r="S45" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S45" s="19" t="s">
+      <c r="T45" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>43020505</v>
       </c>
@@ -7126,17 +7407,20 @@
       <c r="N46" s="4"/>
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
-      <c r="Q46" s="27" t="s">
+      <c r="Q46" s="4">
+        <v>13010206</v>
+      </c>
+      <c r="R46" s="27" t="s">
         <v>410</v>
       </c>
-      <c r="R46" s="4" t="s">
+      <c r="S46" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S46" s="19" t="s">
+      <c r="T46" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>43020506</v>
       </c>
@@ -7175,17 +7459,18 @@
       <c r="N47" s="4"/>
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
-      <c r="Q47" s="27" t="s">
+      <c r="Q47" s="27"/>
+      <c r="R47" s="27" t="s">
         <v>409</v>
       </c>
-      <c r="R47" s="4" t="s">
+      <c r="S47" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S47" s="19" t="s">
+      <c r="T47" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>43020601</v>
       </c>
@@ -7224,17 +7509,18 @@
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
       <c r="P48" s="4"/>
-      <c r="Q48" s="4" t="s">
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="R48" s="4" t="s">
+      <c r="S48" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S48" s="19" t="s">
+      <c r="T48" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>43020602</v>
       </c>
@@ -7271,17 +7557,20 @@
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
       <c r="P49" s="4"/>
-      <c r="Q49" s="4" t="s">
+      <c r="Q49" s="4">
+        <v>13010110</v>
+      </c>
+      <c r="R49" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="R49" s="4" t="s">
+      <c r="S49" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S49" s="19" t="s">
+      <c r="T49" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>43020603</v>
       </c>
@@ -7318,17 +7607,18 @@
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
       <c r="P50" s="4"/>
-      <c r="Q50" s="4" t="s">
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="R50" s="4" t="s">
+      <c r="S50" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S50" s="19" t="s">
+      <c r="T50" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>43020604</v>
       </c>
@@ -7367,99 +7657,100 @@
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
-      <c r="Q51" s="4" t="s">
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="R51" s="4" t="s">
+      <c r="S51" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="S51" s="19" t="s">
+      <c r="T51" s="19" t="s">
         <v>208</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E23:E25 E27:E43 E4:E19 E45:E51">
-    <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="35" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="36" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="37" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="32" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7472,14 +7763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="I22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S1" sqref="S1:S1048576"/>
+      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7492,11 +7783,12 @@
     <col min="11" max="12" width="10.625" customWidth="1"/>
     <col min="13" max="14" width="6.125" customWidth="1"/>
     <col min="15" max="16" width="27.125" customWidth="1"/>
-    <col min="18" max="18" width="10.625" customWidth="1"/>
-    <col min="19" max="19" width="8" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
+    <col min="19" max="19" width="10.625" customWidth="1"/>
+    <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>151</v>
       </c>
@@ -7545,17 +7837,20 @@
       <c r="P1" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="11" t="s">
+        <v>429</v>
+      </c>
+      <c r="R1" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>149</v>
       </c>
@@ -7604,17 +7899,20 @@
       <c r="P2" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>160</v>
       </c>
@@ -7664,16 +7962,19 @@
         <v>185</v>
       </c>
       <c r="Q3" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43000001</v>
       </c>
@@ -7714,15 +8015,16 @@
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="S4" s="17"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T4" s="17"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43000002</v>
       </c>
@@ -7763,15 +8065,16 @@
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="6"/>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="6"/>
+      <c r="R5" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="S5" s="17"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T5" s="17"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43000003</v>
       </c>
@@ -7812,15 +8115,16 @@
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="4" t="s">
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="S6" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S6" s="17"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T6" s="17"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43000004</v>
       </c>
@@ -7861,15 +8165,16 @@
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="4" t="s">
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="S7" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S7" s="17"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T7" s="17"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43000005</v>
       </c>
@@ -7910,15 +8215,16 @@
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="4" t="s">
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="S8" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S8" s="17"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T8" s="17"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43000007</v>
       </c>
@@ -7959,15 +8265,16 @@
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="4" t="s">
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="S9" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="S9" s="17"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T9" s="17"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43000008</v>
       </c>
@@ -8008,15 +8315,16 @@
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="4" t="s">
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="R10" s="4" t="s">
+      <c r="S10" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S10" s="17"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T10" s="17"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43000009</v>
       </c>
@@ -8057,15 +8365,16 @@
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="4" t="s">
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="S11" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S11" s="17"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T11" s="17"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43000010</v>
       </c>
@@ -8106,15 +8415,16 @@
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="4" t="s">
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="R12" s="4" t="s">
+      <c r="S12" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S12" s="17"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T12" s="17"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43000011</v>
       </c>
@@ -8155,15 +8465,16 @@
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="4" t="s">
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="R13" s="4" t="s">
+      <c r="S13" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S13" s="17"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T13" s="17"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43000012</v>
       </c>
@@ -8204,15 +8515,16 @@
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="4" t="s">
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="R14" s="4" t="s">
+      <c r="S14" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S14" s="17"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T14" s="17"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43000013</v>
       </c>
@@ -8253,15 +8565,16 @@
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
-      <c r="Q15" s="4" t="s">
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="R15" s="4" t="s">
+      <c r="S15" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S15" s="17"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T15" s="17"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43000014</v>
       </c>
@@ -8302,15 +8615,16 @@
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
-      <c r="Q16" s="4" t="s">
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="R16" s="4" t="s">
+      <c r="S16" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S16" s="17"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T16" s="17"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43000015</v>
       </c>
@@ -8351,15 +8665,16 @@
       </c>
       <c r="O17" s="4"/>
       <c r="P17" s="6"/>
-      <c r="Q17" s="4" t="s">
+      <c r="Q17" s="6"/>
+      <c r="R17" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="R17" s="4" t="s">
+      <c r="S17" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S17" s="17"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T17" s="17"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43000016</v>
       </c>
@@ -8400,15 +8715,16 @@
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
-      <c r="Q18" s="4" t="s">
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="R18" s="4" t="s">
+      <c r="S18" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S18" s="17"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T18" s="17"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43000017</v>
       </c>
@@ -8449,15 +8765,16 @@
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="4" t="s">
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="R19" s="4" t="s">
+      <c r="S19" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S19" s="17"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T19" s="17"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43000018</v>
       </c>
@@ -8498,15 +8815,16 @@
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="4" t="s">
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="R20" s="4" t="s">
+      <c r="S20" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S20" s="17"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T20" s="17"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43000019</v>
       </c>
@@ -8547,15 +8865,16 @@
       </c>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
-      <c r="Q21" s="4" t="s">
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="R21" s="4" t="s">
+      <c r="S21" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S21" s="17"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T21" s="17"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43000020</v>
       </c>
@@ -8596,15 +8915,16 @@
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
-      <c r="Q22" s="4" t="s">
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="R22" s="4" t="s">
+      <c r="S22" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S22" s="17"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T22" s="17"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43000021</v>
       </c>
@@ -8645,15 +8965,16 @@
       </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
-      <c r="Q23" s="4" t="s">
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="R23" s="4" t="s">
+      <c r="S23" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S23" s="17"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T23" s="17"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43000022</v>
       </c>
@@ -8694,15 +9015,16 @@
       </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
-      <c r="Q24" s="4" t="s">
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="R24" s="4" t="s">
+      <c r="S24" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S24" s="17"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T24" s="17"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43000023</v>
       </c>
@@ -8743,15 +9065,16 @@
       </c>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
-      <c r="Q25" s="4" t="s">
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="R25" s="4" t="s">
+      <c r="S25" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S25" s="17"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T25" s="17"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43000024</v>
       </c>
@@ -8792,15 +9115,16 @@
       </c>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
-      <c r="Q26" s="4" t="s">
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="R26" s="4" t="s">
+      <c r="S26" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S26" s="17"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T26" s="17"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43000025</v>
       </c>
@@ -8841,15 +9165,16 @@
       </c>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
-      <c r="Q27" s="4" t="s">
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="R27" s="4" t="s">
+      <c r="S27" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S27" s="17"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T27" s="17"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43000026</v>
       </c>
@@ -8890,15 +9215,16 @@
       </c>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
-      <c r="Q28" s="4" t="s">
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="R28" s="4" t="s">
+      <c r="S28" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S28" s="17"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T28" s="17"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43000027</v>
       </c>
@@ -8939,15 +9265,16 @@
       </c>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
-      <c r="Q29" s="4" t="s">
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="R29" s="4" t="s">
+      <c r="S29" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S29" s="17"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T29" s="17"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43000028</v>
       </c>
@@ -8988,15 +9315,16 @@
       </c>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
-      <c r="Q30" s="4" t="s">
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="R30" s="4" t="s">
+      <c r="S30" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S30" s="17"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T30" s="17"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43000029</v>
       </c>
@@ -9037,15 +9365,16 @@
       </c>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
-      <c r="Q31" s="4" t="s">
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="R31" s="4" t="s">
+      <c r="S31" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S31" s="17"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T31" s="17"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43000030</v>
       </c>
@@ -9086,15 +9415,16 @@
       </c>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
-      <c r="Q32" s="4" t="s">
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="R32" s="4" t="s">
+      <c r="S32" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S32" s="17"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T32" s="17"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43000031</v>
       </c>
@@ -9135,15 +9465,16 @@
       </c>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
-      <c r="Q33" s="4" t="s">
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="R33" s="4" t="s">
+      <c r="S33" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S33" s="17"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T33" s="17"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43000032</v>
       </c>
@@ -9184,15 +9515,16 @@
       </c>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
-      <c r="Q34" s="4" t="s">
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="R34" s="4" t="s">
+      <c r="S34" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S34" s="17"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T34" s="17"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43000033</v>
       </c>
@@ -9233,15 +9565,16 @@
       </c>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
-      <c r="Q35" s="4" t="s">
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="R35" s="4" t="s">
+      <c r="S35" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S35" s="17"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T35" s="17"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43000035</v>
       </c>
@@ -9282,15 +9615,16 @@
       </c>
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
-      <c r="Q36" s="4" t="s">
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="R36" s="4" t="s">
+      <c r="S36" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S36" s="17"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T36" s="17"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43000037</v>
       </c>
@@ -9331,15 +9665,16 @@
       </c>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
-      <c r="Q37" s="4" t="s">
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="R37" s="4" t="s">
+      <c r="S37" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S37" s="13"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T37" s="13"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43000038</v>
       </c>
@@ -9380,15 +9715,16 @@
       </c>
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
-      <c r="Q38" s="4" t="s">
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="R38" s="4" t="s">
+      <c r="S38" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S38" s="35"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T38" s="35"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A39" s="37">
         <v>43001001</v>
       </c>
@@ -9431,15 +9767,16 @@
         <v>423</v>
       </c>
       <c r="P39" s="4"/>
-      <c r="Q39" s="4" t="s">
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="R39" s="6" t="s">
+      <c r="S39" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="S39" s="17"/>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T39" s="17"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A40" s="37">
         <v>43001002</v>
       </c>
@@ -9482,15 +9819,16 @@
         <v>426</v>
       </c>
       <c r="P40" s="4"/>
-      <c r="Q40" s="4" t="s">
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="R40" s="4" t="s">
+      <c r="S40" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S40" s="36"/>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T40" s="36"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A41" s="37">
         <v>43001003</v>
       </c>
@@ -9533,15 +9871,16 @@
         <v>263</v>
       </c>
       <c r="P41" s="4"/>
-      <c r="Q41" s="4" t="s">
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="R41" s="4" t="s">
+      <c r="S41" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S41" s="27"/>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T41" s="27"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A42" s="37">
         <v>43001004</v>
       </c>
@@ -9584,15 +9923,16 @@
         <v>425</v>
       </c>
       <c r="P42" s="4"/>
-      <c r="Q42" s="4" t="s">
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="R42" s="34" t="s">
+      <c r="S42" s="34" t="s">
         <v>424</v>
       </c>
-      <c r="S42" s="17"/>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T42" s="17"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A43" s="37">
         <v>43001005</v>
       </c>
@@ -9635,15 +9975,16 @@
         <v>427</v>
       </c>
       <c r="P43" s="4"/>
-      <c r="Q43" s="4" t="s">
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="R43" s="4" t="s">
+      <c r="S43" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S43" s="17"/>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T43" s="17"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A44" s="37">
         <v>43001006</v>
       </c>
@@ -9686,15 +10027,16 @@
         <v>428</v>
       </c>
       <c r="P44" s="4"/>
-      <c r="Q44" s="4" t="s">
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="R44" s="6" t="s">
+      <c r="S44" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="S44" s="36"/>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T44" s="36"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A45" s="38">
         <v>43002001</v>
       </c>
@@ -9735,15 +10077,16 @@
       </c>
       <c r="O45" s="27"/>
       <c r="P45" s="27"/>
-      <c r="Q45" s="4" t="s">
+      <c r="Q45" s="27"/>
+      <c r="R45" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="R45" s="27" t="s">
+      <c r="S45" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="S45" s="27"/>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T45" s="27"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A46" s="38">
         <v>43002002</v>
       </c>
@@ -9784,15 +10127,16 @@
       </c>
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
-      <c r="Q46" s="4" t="s">
+      <c r="Q46" s="27"/>
+      <c r="R46" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="R46" s="27" t="s">
+      <c r="S46" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="S46" s="27"/>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T46" s="27"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A47" s="38">
         <v>43002003</v>
       </c>
@@ -9833,15 +10177,16 @@
       </c>
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
-      <c r="Q47" s="4" t="s">
+      <c r="Q47" s="27"/>
+      <c r="R47" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="R47" s="27" t="s">
+      <c r="S47" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="S47" s="27"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T47" s="27"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A48" s="38">
         <v>43002004</v>
       </c>
@@ -9882,15 +10227,16 @@
       </c>
       <c r="O48" s="27"/>
       <c r="P48" s="27"/>
-      <c r="Q48" s="31" t="s">
+      <c r="Q48" s="13"/>
+      <c r="R48" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="R48" s="27" t="s">
+      <c r="S48" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="S48" s="27"/>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T48" s="27"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A49" s="38">
         <v>43002005</v>
       </c>
@@ -9931,15 +10277,16 @@
       </c>
       <c r="O49" s="27"/>
       <c r="P49" s="27"/>
-      <c r="Q49" s="31" t="s">
+      <c r="Q49" s="13"/>
+      <c r="R49" s="31" t="s">
         <v>343</v>
       </c>
-      <c r="R49" s="27" t="s">
+      <c r="S49" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="S49" s="27"/>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T49" s="27"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A50" s="38">
         <v>43002006</v>
       </c>
@@ -9980,48 +10327,49 @@
       </c>
       <c r="O50" s="27"/>
       <c r="P50" s="27"/>
-      <c r="Q50" s="31" t="s">
+      <c r="Q50" s="13"/>
+      <c r="R50" s="31" t="s">
         <v>344</v>
       </c>
-      <c r="R50" s="27" t="s">
+      <c r="S50" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="S50" s="27"/>
+      <c r="T50" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="R42">
-    <cfRule type="containsBlanks" dxfId="6" priority="9">
-      <formula>LEN(TRIM(R42))=0</formula>
+  <conditionalFormatting sqref="S42">
+    <cfRule type="containsBlanks" dxfId="7" priority="9">
+      <formula>LEN(TRIM(S42))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsBlanks" dxfId="5" priority="8">
+    <cfRule type="containsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(C47))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q47">
-    <cfRule type="containsBlanks" dxfId="4" priority="6">
-      <formula>LEN(TRIM(Q47))=0</formula>
+  <conditionalFormatting sqref="R47">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(R47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C50">
-    <cfRule type="containsBlanks" dxfId="3" priority="5">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(C48))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q48:Q50">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(Q48))=0</formula>
+  <conditionalFormatting sqref="R48:R50">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
+      <formula>LEN(TRIM(R48))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(K47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:K50">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(K48))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10034,14 +10382,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:S14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S1" sqref="S1:S1048576"/>
+      <selection pane="bottomRight" activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10055,11 +10403,12 @@
     <col min="13" max="14" width="6.125" customWidth="1"/>
     <col min="15" max="15" width="28.375" customWidth="1"/>
     <col min="16" max="16" width="19.5" customWidth="1"/>
-    <col min="18" max="18" width="10.625" customWidth="1"/>
-    <col min="19" max="19" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.875" customWidth="1"/>
+    <col min="19" max="19" width="10.625" customWidth="1"/>
+    <col min="20" max="20" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>151</v>
       </c>
@@ -10108,17 +10457,20 @@
       <c r="P1" s="25" t="s">
         <v>238</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="25" t="s">
+        <v>429</v>
+      </c>
+      <c r="R1" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="R1" s="25" t="s">
+      <c r="S1" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="T1" s="25" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>149</v>
       </c>
@@ -10167,17 +10519,20 @@
       <c r="P2" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="R2" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>160</v>
       </c>
@@ -10227,16 +10582,19 @@
         <v>186</v>
       </c>
       <c r="Q3" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="R3" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="S3" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="S3" s="18" t="s">
+      <c r="T3" s="18" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43010001</v>
       </c>
@@ -10277,15 +10635,16 @@
         <v>243</v>
       </c>
       <c r="P4" s="6"/>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="6"/>
+      <c r="R4" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S4" s="15"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T4" s="15"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43010002</v>
       </c>
@@ -10324,15 +10683,16 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S5" s="14"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T5" s="14"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43010003</v>
       </c>
@@ -10371,15 +10731,16 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="4" t="s">
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="S6" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S6" s="14"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T6" s="14"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43010004</v>
       </c>
@@ -10418,15 +10779,16 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="4" t="s">
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="S7" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S7" s="14"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T7" s="14"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43010005</v>
       </c>
@@ -10467,15 +10829,16 @@
         <v>244</v>
       </c>
       <c r="P8" s="4"/>
-      <c r="Q8" s="6" t="s">
+      <c r="Q8" s="4"/>
+      <c r="R8" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="S8" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S8" s="14"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T8" s="14"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43010006</v>
       </c>
@@ -10516,15 +10879,16 @@
         <v>245</v>
       </c>
       <c r="P9" s="4"/>
-      <c r="Q9" s="6" t="s">
+      <c r="Q9" s="4"/>
+      <c r="R9" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="S9" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S9" s="14"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T9" s="14"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43010101</v>
       </c>
@@ -10561,15 +10925,16 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="4" t="s">
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="R10" s="4" t="s">
+      <c r="S10" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S10" s="14"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T10" s="14"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43010102</v>
       </c>
@@ -10606,15 +10971,16 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="4" t="s">
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="S11" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S11" s="14"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T11" s="14"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43010103</v>
       </c>
@@ -10651,15 +11017,16 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="4" t="s">
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="R12" s="4" t="s">
+      <c r="S12" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S12" s="14"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T12" s="14"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43010104</v>
       </c>
@@ -10696,15 +11063,16 @@
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="4" t="s">
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="R13" s="4" t="s">
+      <c r="S13" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S13" s="14"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T13" s="14"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43010105</v>
       </c>
@@ -10741,13 +11109,14 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="4" t="s">
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="R14" s="4" t="s">
+      <c r="S14" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
event happen on catch chess
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="人物" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="449">
   <si>
     <t>老鼠</t>
   </si>
@@ -1478,6 +1478,55 @@
   <si>
     <t>Figue</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>綁定事件</t>
+  </si>
+  <si>
+    <t>綁定事件</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BindQuest</t>
+  </si>
+  <si>
+    <t>BindQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcsainisi</t>
+  </si>
+  <si>
+    <t>npcsaibasi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcaolai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npckedi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcweia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcmilanda</t>
+  </si>
+  <si>
+    <t>npcbeilukai</t>
+  </si>
+  <si>
+    <t>npcleiluo</t>
+  </si>
+  <si>
+    <t>npcbaludi</t>
   </si>
 </sst>
 </file>
@@ -2391,7 +2440,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="100">
+  <dxfs count="111">
     <dxf>
       <font>
         <b val="0"/>
@@ -2420,6 +2469,62 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2850,6 +2955,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -3460,6 +3594,25 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -4007,6 +4160,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -4598,96 +4780,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:T51" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98" tableBorderDxfId="97">
-  <autoFilter ref="A3:T51"/>
-  <sortState ref="A4:T50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:U51" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109" tableBorderDxfId="108">
+  <autoFilter ref="A3:U51"/>
+  <sortState ref="A4:U50">
     <sortCondition ref="A3:A50"/>
   </sortState>
-  <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="96"/>
-    <tableColumn id="2" name="Name" dataDxfId="95"/>
-    <tableColumn id="18" name="Ename" dataDxfId="94"/>
-    <tableColumn id="3" name="Type" dataDxfId="93"/>
-    <tableColumn id="21" name="Quality" dataDxfId="92"/>
-    <tableColumn id="6" name="World" dataDxfId="91"/>
-    <tableColumn id="10" name="Job" dataDxfId="90"/>
-    <tableColumn id="11" name="Level" dataDxfId="89"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="88"/>
-    <tableColumn id="13" name="Method" dataDxfId="87"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="86"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="85"/>
-    <tableColumn id="12" name="EpRecoverRate" dataDxfId="84"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="83"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="82"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="81"/>
-    <tableColumn id="7" name="BornSceneId" dataDxfId="33"/>
-    <tableColumn id="17" name="Figue" dataDxfId="80"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="79"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="78"/>
+  <tableColumns count="21">
+    <tableColumn id="1" name="Id" dataDxfId="107"/>
+    <tableColumn id="2" name="Name" dataDxfId="106"/>
+    <tableColumn id="18" name="Ename" dataDxfId="105"/>
+    <tableColumn id="3" name="Type" dataDxfId="104"/>
+    <tableColumn id="21" name="Quality" dataDxfId="103"/>
+    <tableColumn id="6" name="World" dataDxfId="102"/>
+    <tableColumn id="10" name="Job" dataDxfId="101"/>
+    <tableColumn id="11" name="Level" dataDxfId="100"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="99"/>
+    <tableColumn id="13" name="Method" dataDxfId="98"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="97"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="96"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="95"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="94"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="93"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="92"/>
+    <tableColumn id="7" name="BornSceneId" dataDxfId="91"/>
+    <tableColumn id="8" name="BindQuest" dataDxfId="41"/>
+    <tableColumn id="17" name="Figue" dataDxfId="90"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="89"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75">
-  <autoFilter ref="A3:T50"/>
-  <sortState ref="A4:T50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:U50" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86" tableBorderDxfId="85">
+  <autoFilter ref="A3:U50"/>
+  <sortState ref="A4:U50">
     <sortCondition ref="A3:A50"/>
   </sortState>
-  <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="74"/>
-    <tableColumn id="2" name="Name" dataDxfId="73"/>
-    <tableColumn id="18" name="Ename" dataDxfId="72"/>
-    <tableColumn id="3" name="Type" dataDxfId="71"/>
-    <tableColumn id="7" name="Quality" dataDxfId="70"/>
-    <tableColumn id="6" name="World" dataDxfId="69"/>
-    <tableColumn id="10" name="Job" dataDxfId="68"/>
-    <tableColumn id="11" name="Level" dataDxfId="67"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="66"/>
-    <tableColumn id="13" name="Method" dataDxfId="65"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="64"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="63"/>
-    <tableColumn id="12" name="EpRecoverRate" dataDxfId="62"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="61"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="60"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="59"/>
-    <tableColumn id="8" name="BornSceneId" dataDxfId="32"/>
-    <tableColumn id="17" name="Figue" dataDxfId="58"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="57"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="56"/>
+  <tableColumns count="21">
+    <tableColumn id="1" name="Id" dataDxfId="84"/>
+    <tableColumn id="2" name="Name" dataDxfId="83"/>
+    <tableColumn id="18" name="Ename" dataDxfId="82"/>
+    <tableColumn id="3" name="Type" dataDxfId="81"/>
+    <tableColumn id="7" name="Quality" dataDxfId="80"/>
+    <tableColumn id="6" name="World" dataDxfId="79"/>
+    <tableColumn id="10" name="Job" dataDxfId="78"/>
+    <tableColumn id="11" name="Level" dataDxfId="77"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="76"/>
+    <tableColumn id="13" name="Method" dataDxfId="75"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="74"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="73"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="72"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="71"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="70"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="69"/>
+    <tableColumn id="8" name="BornSceneId" dataDxfId="68"/>
+    <tableColumn id="21" name="BindQuest" dataDxfId="40"/>
+    <tableColumn id="17" name="Figue" dataDxfId="67"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="66"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:T14" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53">
-  <autoFilter ref="A3:T14"/>
-  <sortState ref="A4:S83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:U14" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
+  <autoFilter ref="A3:U14"/>
+  <sortState ref="A4:T83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="52"/>
-    <tableColumn id="2" name="Name" dataDxfId="51"/>
-    <tableColumn id="18" name="Ename" dataDxfId="50"/>
-    <tableColumn id="3" name="Type" dataDxfId="49"/>
-    <tableColumn id="7" name="Quality" dataDxfId="48"/>
-    <tableColumn id="6" name="World" dataDxfId="47"/>
-    <tableColumn id="10" name="Job" dataDxfId="46"/>
-    <tableColumn id="11" name="Level" dataDxfId="45"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="44"/>
-    <tableColumn id="13" name="Method" dataDxfId="43"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="42"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="41"/>
-    <tableColumn id="12" name="EpRecoverRate" dataDxfId="40"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="39"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="38"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="37"/>
-    <tableColumn id="8" name="BornSceneId" dataDxfId="0"/>
-    <tableColumn id="9" name="Figue" dataDxfId="36"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="35"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="34"/>
+  <tableColumns count="21">
+    <tableColumn id="1" name="Id" dataDxfId="61"/>
+    <tableColumn id="2" name="Name" dataDxfId="60"/>
+    <tableColumn id="18" name="Ename" dataDxfId="59"/>
+    <tableColumn id="3" name="Type" dataDxfId="58"/>
+    <tableColumn id="7" name="Quality" dataDxfId="57"/>
+    <tableColumn id="6" name="World" dataDxfId="56"/>
+    <tableColumn id="10" name="Job" dataDxfId="55"/>
+    <tableColumn id="11" name="Level" dataDxfId="54"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="53"/>
+    <tableColumn id="13" name="Method" dataDxfId="52"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="51"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="50"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="49"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="48"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="47"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="46"/>
+    <tableColumn id="8" name="BornSceneId" dataDxfId="45"/>
+    <tableColumn id="21" name="BindQuest" dataDxfId="0"/>
+    <tableColumn id="9" name="Figue" dataDxfId="44"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="43"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5014,13 +5199,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T51"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q45" sqref="Q45"/>
+      <selection pane="bottomRight" activeCell="R1" sqref="R1:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5032,11 +5217,11 @@
     <col min="10" max="10" width="9.5" customWidth="1"/>
     <col min="11" max="12" width="10.625" customWidth="1"/>
     <col min="13" max="16" width="5.875" customWidth="1"/>
-    <col min="17" max="17" width="9.75" customWidth="1"/>
-    <col min="19" max="19" width="10.625" customWidth="1"/>
+    <col min="17" max="18" width="9.75" customWidth="1"/>
+    <col min="20" max="20" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" ht="72" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>151</v>
       </c>
@@ -5088,17 +5273,20 @@
       <c r="Q1" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="11" t="s">
+        <v>436</v>
+      </c>
+      <c r="S1" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>149</v>
       </c>
@@ -5150,17 +5338,20 @@
       <c r="Q2" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>160</v>
       </c>
@@ -5213,16 +5404,19 @@
         <v>433</v>
       </c>
       <c r="R3" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="S3" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43020101</v>
       </c>
@@ -5263,14 +5457,17 @@
         <v>13010002</v>
       </c>
       <c r="R4" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="S4" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43020102</v>
       </c>
@@ -5310,15 +5507,18 @@
       <c r="Q5" s="4">
         <v>13010003</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="32" t="s">
+        <v>441</v>
+      </c>
+      <c r="S5" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43020103</v>
       </c>
@@ -5360,17 +5560,20 @@
       <c r="Q6" s="4">
         <v>13010004</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="R6" s="32" t="s">
+        <v>443</v>
+      </c>
+      <c r="S6" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="T6" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T6" s="19" t="s">
+      <c r="U6" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43020104</v>
       </c>
@@ -5412,15 +5615,18 @@
       <c r="Q7" s="4">
         <v>13010007</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="32" t="s">
+        <v>444</v>
+      </c>
+      <c r="S7" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="S7" s="4" t="s">
+      <c r="T7" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43020105</v>
       </c>
@@ -5462,17 +5668,20 @@
       <c r="Q8" s="4">
         <v>13010009</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="R8" s="32" t="s">
+        <v>442</v>
+      </c>
+      <c r="S8" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="T8" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T8" s="19" t="s">
+      <c r="U8" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43020106</v>
       </c>
@@ -5514,17 +5723,20 @@
       <c r="Q9" s="4">
         <v>13010008</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="32" t="s">
+        <v>445</v>
+      </c>
+      <c r="S9" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="T9" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T9" s="19" t="s">
+      <c r="U9" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43020107</v>
       </c>
@@ -5564,17 +5776,18 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-      <c r="R10" s="4" t="s">
+      <c r="R10" s="4"/>
+      <c r="S10" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="S10" s="4" t="s">
+      <c r="T10" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T10" s="19" t="s">
+      <c r="U10" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43020108</v>
       </c>
@@ -5616,17 +5829,20 @@
       <c r="Q11" s="4">
         <v>13010203</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="32" t="s">
+        <v>446</v>
+      </c>
+      <c r="S11" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="T11" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T11" s="19" t="s">
+      <c r="U11" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43020109</v>
       </c>
@@ -5668,17 +5884,20 @@
       <c r="Q12" s="4">
         <v>13010202</v>
       </c>
-      <c r="R12" s="4" t="s">
+      <c r="R12" s="32" t="s">
+        <v>447</v>
+      </c>
+      <c r="S12" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="S12" s="4" t="s">
+      <c r="T12" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T12" s="19" t="s">
+      <c r="U12" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43020110</v>
       </c>
@@ -5720,17 +5939,20 @@
       <c r="Q13" s="4">
         <v>13010203</v>
       </c>
-      <c r="R13" s="4" t="s">
+      <c r="R13" s="32" t="s">
+        <v>448</v>
+      </c>
+      <c r="S13" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="S13" s="4" t="s">
+      <c r="T13" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T13" s="19" t="s">
+      <c r="U13" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43020201</v>
       </c>
@@ -5772,17 +5994,18 @@
       <c r="Q14" s="4">
         <v>13010103</v>
       </c>
-      <c r="R14" s="4" t="s">
+      <c r="R14" s="4"/>
+      <c r="S14" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="S14" s="4" t="s">
+      <c r="T14" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T14" s="19" t="s">
+      <c r="U14" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43020202</v>
       </c>
@@ -5822,17 +6045,18 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
-      <c r="R15" s="4" t="s">
+      <c r="R15" s="4"/>
+      <c r="S15" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="S15" s="4" t="s">
+      <c r="T15" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T15" s="19" t="s">
+      <c r="U15" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43020203</v>
       </c>
@@ -5872,17 +6096,18 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-      <c r="R16" s="4" t="s">
+      <c r="R16" s="4"/>
+      <c r="S16" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="S16" s="4" t="s">
+      <c r="T16" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T16" s="19" t="s">
+      <c r="U16" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43020204</v>
       </c>
@@ -5924,17 +6149,18 @@
       <c r="Q17" s="4">
         <v>13010107</v>
       </c>
-      <c r="R17" s="4" t="s">
+      <c r="R17" s="4"/>
+      <c r="S17" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="S17" s="4" t="s">
+      <c r="T17" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T17" s="19" t="s">
+      <c r="U17" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43020205</v>
       </c>
@@ -5974,17 +6200,18 @@
       <c r="Q18" s="4">
         <v>13010202</v>
       </c>
-      <c r="R18" s="4" t="s">
+      <c r="R18" s="4"/>
+      <c r="S18" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="S18" s="4" t="s">
+      <c r="T18" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T18" s="19" t="s">
+      <c r="U18" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43020206</v>
       </c>
@@ -6026,17 +6253,18 @@
       <c r="Q19" s="4">
         <v>13010205</v>
       </c>
-      <c r="R19" s="4" t="s">
+      <c r="R19" s="4"/>
+      <c r="S19" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="S19" s="4" t="s">
+      <c r="T19" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T19" s="19" t="s">
+      <c r="U19" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43020207</v>
       </c>
@@ -6076,17 +6304,18 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
-      <c r="R20" s="4" t="s">
+      <c r="R20" s="4"/>
+      <c r="S20" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="S20" s="4" t="s">
+      <c r="T20" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T20" s="19" t="s">
+      <c r="U20" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43020301</v>
       </c>
@@ -6128,17 +6357,18 @@
       <c r="Q21" s="4">
         <v>13010102</v>
       </c>
-      <c r="R21" s="4" t="s">
+      <c r="R21" s="4"/>
+      <c r="S21" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="S21" s="4" t="s">
+      <c r="T21" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T21" s="19" t="s">
+      <c r="U21" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43020302</v>
       </c>
@@ -6178,17 +6408,18 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
-      <c r="R22" s="4" t="s">
+      <c r="R22" s="4"/>
+      <c r="S22" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="S22" s="4" t="s">
+      <c r="T22" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T22" s="19" t="s">
+      <c r="U22" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43020303</v>
       </c>
@@ -6228,17 +6459,18 @@
       <c r="Q23" s="4">
         <v>13010106</v>
       </c>
-      <c r="R23" s="4" t="s">
+      <c r="R23" s="4"/>
+      <c r="S23" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="S23" s="4" t="s">
+      <c r="T23" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T23" s="19" t="s">
+      <c r="U23" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43020304</v>
       </c>
@@ -6278,17 +6510,18 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
-      <c r="R24" s="4" t="s">
+      <c r="R24" s="4"/>
+      <c r="S24" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="S24" s="4" t="s">
+      <c r="T24" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T24" s="19" t="s">
+      <c r="U24" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43020305</v>
       </c>
@@ -6330,17 +6563,18 @@
       <c r="Q25" s="4">
         <v>13010204</v>
       </c>
-      <c r="R25" s="4" t="s">
+      <c r="R25" s="4"/>
+      <c r="S25" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="S25" s="4" t="s">
+      <c r="T25" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T25" s="19" t="s">
+      <c r="U25" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43020306</v>
       </c>
@@ -6382,17 +6616,18 @@
       <c r="Q26" s="4">
         <v>13010204</v>
       </c>
-      <c r="R26" s="4" t="s">
+      <c r="R26" s="4"/>
+      <c r="S26" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="S26" s="4" t="s">
+      <c r="T26" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T26" s="19" t="s">
+      <c r="U26" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43020307</v>
       </c>
@@ -6434,17 +6669,18 @@
       <c r="Q27" s="4">
         <v>13010102</v>
       </c>
-      <c r="R27" s="4" t="s">
+      <c r="R27" s="4"/>
+      <c r="S27" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="S27" s="4" t="s">
+      <c r="T27" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T27" s="19" t="s">
+      <c r="U27" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43020308</v>
       </c>
@@ -6484,17 +6720,18 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
-      <c r="R28" s="4" t="s">
+      <c r="R28" s="4"/>
+      <c r="S28" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="S28" s="4" t="s">
+      <c r="T28" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T28" s="19" t="s">
+      <c r="U28" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43020309</v>
       </c>
@@ -6536,17 +6773,18 @@
       <c r="Q29" s="4">
         <v>13010105</v>
       </c>
-      <c r="R29" s="4" t="s">
+      <c r="R29" s="4"/>
+      <c r="S29" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="S29" s="4" t="s">
+      <c r="T29" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T29" s="19" t="s">
+      <c r="U29" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43020310</v>
       </c>
@@ -6588,17 +6826,18 @@
       <c r="Q30" s="4">
         <v>13010105</v>
       </c>
-      <c r="R30" s="4" t="s">
+      <c r="R30" s="4"/>
+      <c r="S30" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="S30" s="4" t="s">
+      <c r="T30" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T30" s="19" t="s">
+      <c r="U30" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43020311</v>
       </c>
@@ -6638,17 +6877,18 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
-      <c r="R31" s="4" t="s">
+      <c r="R31" s="4"/>
+      <c r="S31" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="S31" s="4" t="s">
+      <c r="T31" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T31" s="19" t="s">
+      <c r="U31" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43020312</v>
       </c>
@@ -6688,17 +6928,18 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
-      <c r="R32" s="4" t="s">
+      <c r="R32" s="4"/>
+      <c r="S32" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="S32" s="4" t="s">
+      <c r="T32" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T32" s="19" t="s">
+      <c r="U32" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43020401</v>
       </c>
@@ -6740,17 +6981,18 @@
       <c r="Q33" s="4">
         <v>13010108</v>
       </c>
-      <c r="R33" s="4" t="s">
+      <c r="R33" s="4"/>
+      <c r="S33" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="S33" s="4" t="s">
+      <c r="T33" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T33" s="19" t="s">
+      <c r="U33" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43020402</v>
       </c>
@@ -6792,17 +7034,18 @@
       <c r="Q34" s="4">
         <v>13010103</v>
       </c>
-      <c r="R34" s="4" t="s">
+      <c r="R34" s="4"/>
+      <c r="S34" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="S34" s="4" t="s">
+      <c r="T34" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T34" s="19" t="s">
+      <c r="U34" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43020403</v>
       </c>
@@ -6842,17 +7085,18 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
-      <c r="R35" s="4" t="s">
+      <c r="R35" s="4"/>
+      <c r="S35" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="S35" s="4" t="s">
+      <c r="T35" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T35" s="19" t="s">
+      <c r="U35" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43020404</v>
       </c>
@@ -6894,17 +7138,18 @@
       <c r="Q36" s="4">
         <v>13010208</v>
       </c>
-      <c r="R36" s="4" t="s">
+      <c r="R36" s="4"/>
+      <c r="S36" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="S36" s="4" t="s">
+      <c r="T36" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T36" s="19" t="s">
+      <c r="U36" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43020405</v>
       </c>
@@ -6946,17 +7191,18 @@
       <c r="Q37" s="4">
         <v>13010108</v>
       </c>
-      <c r="R37" s="4" t="s">
+      <c r="R37" s="4"/>
+      <c r="S37" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="S37" s="4" t="s">
+      <c r="T37" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T37" s="19" t="s">
+      <c r="U37" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43020406</v>
       </c>
@@ -6998,17 +7244,18 @@
       <c r="Q38" s="4">
         <v>13010104</v>
       </c>
-      <c r="R38" s="4" t="s">
+      <c r="R38" s="4"/>
+      <c r="S38" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="S38" s="4" t="s">
+      <c r="T38" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T38" s="19" t="s">
+      <c r="U38" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>43020407</v>
       </c>
@@ -7050,17 +7297,18 @@
       <c r="Q39" s="4">
         <v>13010209</v>
       </c>
-      <c r="R39" s="4" t="s">
+      <c r="R39" s="4"/>
+      <c r="S39" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="S39" s="4" t="s">
+      <c r="T39" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T39" s="19" t="s">
+      <c r="U39" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>43020408</v>
       </c>
@@ -7102,17 +7350,18 @@
       <c r="Q40" s="4">
         <v>13010205</v>
       </c>
-      <c r="R40" s="4" t="s">
+      <c r="R40" s="4"/>
+      <c r="S40" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="S40" s="4" t="s">
+      <c r="T40" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T40" s="19" t="s">
+      <c r="U40" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>43020409</v>
       </c>
@@ -7152,17 +7401,18 @@
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
-      <c r="R41" s="4" t="s">
+      <c r="R41" s="4"/>
+      <c r="S41" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="S41" s="4" t="s">
+      <c r="T41" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T41" s="19" t="s">
+      <c r="U41" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>43020501</v>
       </c>
@@ -7202,17 +7452,18 @@
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
-      <c r="R42" s="4" t="s">
+      <c r="R42" s="4"/>
+      <c r="S42" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="S42" s="4" t="s">
+      <c r="T42" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T42" s="19" t="s">
+      <c r="U42" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>43020502</v>
       </c>
@@ -7254,17 +7505,18 @@
       <c r="Q43" s="4">
         <v>13010109</v>
       </c>
-      <c r="R43" s="4" t="s">
+      <c r="R43" s="4"/>
+      <c r="S43" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="S43" s="4" t="s">
+      <c r="T43" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T43" s="19" t="s">
+      <c r="U43" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43020503</v>
       </c>
@@ -7306,17 +7558,18 @@
       <c r="Q44" s="4">
         <v>13010207</v>
       </c>
-      <c r="R44" s="4" t="s">
+      <c r="R44" s="4"/>
+      <c r="S44" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="S44" s="4" t="s">
+      <c r="T44" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T44" s="19" t="s">
+      <c r="U44" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>43020504</v>
       </c>
@@ -7358,17 +7611,18 @@
       <c r="Q45" s="4">
         <v>13010209</v>
       </c>
-      <c r="R45" s="4" t="s">
+      <c r="R45" s="4"/>
+      <c r="S45" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="S45" s="4" t="s">
+      <c r="T45" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T45" s="19" t="s">
+      <c r="U45" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>43020505</v>
       </c>
@@ -7410,17 +7664,18 @@
       <c r="Q46" s="4">
         <v>13010206</v>
       </c>
-      <c r="R46" s="27" t="s">
+      <c r="R46" s="4"/>
+      <c r="S46" s="27" t="s">
         <v>410</v>
       </c>
-      <c r="S46" s="4" t="s">
+      <c r="T46" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T46" s="19" t="s">
+      <c r="U46" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>43020506</v>
       </c>
@@ -7460,17 +7715,18 @@
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
       <c r="Q47" s="27"/>
-      <c r="R47" s="27" t="s">
+      <c r="R47" s="27"/>
+      <c r="S47" s="27" t="s">
         <v>409</v>
       </c>
-      <c r="S47" s="4" t="s">
+      <c r="T47" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T47" s="19" t="s">
+      <c r="U47" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>43020601</v>
       </c>
@@ -7510,17 +7766,18 @@
       <c r="O48" s="4"/>
       <c r="P48" s="4"/>
       <c r="Q48" s="4"/>
-      <c r="R48" s="4" t="s">
+      <c r="R48" s="4"/>
+      <c r="S48" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="S48" s="4" t="s">
+      <c r="T48" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T48" s="19" t="s">
+      <c r="U48" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>43020602</v>
       </c>
@@ -7560,17 +7817,18 @@
       <c r="Q49" s="4">
         <v>13010110</v>
       </c>
-      <c r="R49" s="4" t="s">
+      <c r="R49" s="4"/>
+      <c r="S49" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="S49" s="4" t="s">
+      <c r="T49" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T49" s="19" t="s">
+      <c r="U49" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>43020603</v>
       </c>
@@ -7608,17 +7866,18 @@
       <c r="O50" s="4"/>
       <c r="P50" s="4"/>
       <c r="Q50" s="4"/>
-      <c r="R50" s="4" t="s">
+      <c r="R50" s="4"/>
+      <c r="S50" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="S50" s="4" t="s">
+      <c r="T50" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T50" s="19" t="s">
+      <c r="U50" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>43020604</v>
       </c>
@@ -7658,100 +7917,141 @@
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
       <c r="Q51" s="4"/>
-      <c r="R51" s="4" t="s">
+      <c r="R51" s="4"/>
+      <c r="S51" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="S51" s="4" t="s">
+      <c r="T51" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T51" s="19" t="s">
+      <c r="U51" s="19" t="s">
         <v>208</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E23:E25 E27:E43 E4:E19 E45:E51">
-    <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="42" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="43" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="44" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="17" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="18" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="19" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5">
+    <cfRule type="containsBlanks" dxfId="15" priority="8">
+      <formula>LEN(TRIM(R5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R8">
+    <cfRule type="containsBlanks" dxfId="14" priority="7">
+      <formula>LEN(TRIM(R8))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R6">
+    <cfRule type="containsBlanks" dxfId="13" priority="6">
+      <formula>LEN(TRIM(R6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R7">
+    <cfRule type="containsBlanks" dxfId="12" priority="5">
+      <formula>LEN(TRIM(R7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R9">
+    <cfRule type="containsBlanks" dxfId="11" priority="4">
+      <formula>LEN(TRIM(R9))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R11">
+    <cfRule type="containsBlanks" dxfId="10" priority="3">
+      <formula>LEN(TRIM(R11))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R12">
+    <cfRule type="containsBlanks" dxfId="9" priority="2">
+      <formula>LEN(TRIM(R12))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R13">
+    <cfRule type="containsBlanks" dxfId="8" priority="1">
+      <formula>LEN(TRIM(R13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7764,13 +8064,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T50"/>
+  <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="I22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:Q3"/>
+      <selection pane="bottomRight" activeCell="R1" sqref="R1:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7783,12 +8083,12 @@
     <col min="11" max="12" width="10.625" customWidth="1"/>
     <col min="13" max="14" width="6.125" customWidth="1"/>
     <col min="15" max="16" width="27.125" customWidth="1"/>
-    <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="19" max="19" width="10.625" customWidth="1"/>
-    <col min="20" max="20" width="8" customWidth="1"/>
+    <col min="17" max="18" width="13" customWidth="1"/>
+    <col min="20" max="20" width="10.625" customWidth="1"/>
+    <col min="21" max="21" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>151</v>
       </c>
@@ -7840,17 +8140,20 @@
       <c r="Q1" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="11" t="s">
+        <v>436</v>
+      </c>
+      <c r="S1" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>149</v>
       </c>
@@ -7902,17 +8205,20 @@
       <c r="Q2" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>160</v>
       </c>
@@ -7965,16 +8271,19 @@
         <v>432</v>
       </c>
       <c r="R3" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="S3" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43000001</v>
       </c>
@@ -8016,15 +8325,16 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="4"/>
+      <c r="S4" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43000002</v>
       </c>
@@ -8066,15 +8376,16 @@
       <c r="O5" s="4"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="6"/>
+      <c r="S5" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43000003</v>
       </c>
@@ -8116,15 +8427,16 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="4" t="s">
+      <c r="R6" s="4"/>
+      <c r="S6" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="T6" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43000004</v>
       </c>
@@ -8166,15 +8478,16 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="4"/>
+      <c r="S7" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="S7" s="4" t="s">
+      <c r="T7" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43000005</v>
       </c>
@@ -8216,15 +8529,16 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-      <c r="R8" s="4" t="s">
+      <c r="R8" s="4"/>
+      <c r="S8" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="T8" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43000007</v>
       </c>
@@ -8266,15 +8580,16 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="4"/>
+      <c r="S9" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="T9" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43000008</v>
       </c>
@@ -8316,15 +8631,16 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-      <c r="R10" s="4" t="s">
+      <c r="R10" s="4"/>
+      <c r="S10" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="S10" s="4" t="s">
+      <c r="T10" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43000009</v>
       </c>
@@ -8366,15 +8682,16 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="4"/>
+      <c r="S11" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="T11" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43000010</v>
       </c>
@@ -8416,15 +8733,16 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-      <c r="R12" s="4" t="s">
+      <c r="R12" s="4"/>
+      <c r="S12" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="S12" s="4" t="s">
+      <c r="T12" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43000011</v>
       </c>
@@ -8466,15 +8784,16 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="4" t="s">
+      <c r="R13" s="4"/>
+      <c r="S13" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="S13" s="4" t="s">
+      <c r="T13" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43000012</v>
       </c>
@@ -8516,15 +8835,16 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-      <c r="R14" s="4" t="s">
+      <c r="R14" s="4"/>
+      <c r="S14" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="S14" s="4" t="s">
+      <c r="T14" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43000013</v>
       </c>
@@ -8566,15 +8886,16 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
-      <c r="R15" s="4" t="s">
+      <c r="R15" s="4"/>
+      <c r="S15" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="S15" s="4" t="s">
+      <c r="T15" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43000014</v>
       </c>
@@ -8616,15 +8937,16 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-      <c r="R16" s="4" t="s">
+      <c r="R16" s="4"/>
+      <c r="S16" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="S16" s="4" t="s">
+      <c r="T16" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43000015</v>
       </c>
@@ -8666,15 +8988,16 @@
       <c r="O17" s="4"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
-      <c r="R17" s="4" t="s">
+      <c r="R17" s="6"/>
+      <c r="S17" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="S17" s="4" t="s">
+      <c r="T17" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43000016</v>
       </c>
@@ -8716,15 +9039,16 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-      <c r="R18" s="4" t="s">
+      <c r="R18" s="4"/>
+      <c r="S18" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="S18" s="4" t="s">
+      <c r="T18" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43000017</v>
       </c>
@@ -8766,15 +9090,16 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
-      <c r="R19" s="4" t="s">
+      <c r="R19" s="4"/>
+      <c r="S19" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="S19" s="4" t="s">
+      <c r="T19" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43000018</v>
       </c>
@@ -8816,15 +9141,16 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
-      <c r="R20" s="4" t="s">
+      <c r="R20" s="4"/>
+      <c r="S20" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="S20" s="4" t="s">
+      <c r="T20" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43000019</v>
       </c>
@@ -8866,15 +9192,16 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
-      <c r="R21" s="4" t="s">
+      <c r="R21" s="4"/>
+      <c r="S21" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="S21" s="4" t="s">
+      <c r="T21" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T21" s="17"/>
+      <c r="U21" s="17"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43000020</v>
       </c>
@@ -8916,15 +9243,16 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
-      <c r="R22" s="4" t="s">
+      <c r="R22" s="4"/>
+      <c r="S22" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="S22" s="4" t="s">
+      <c r="T22" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43000021</v>
       </c>
@@ -8966,15 +9294,16 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
-      <c r="R23" s="4" t="s">
+      <c r="R23" s="4"/>
+      <c r="S23" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="S23" s="4" t="s">
+      <c r="T23" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T23" s="17"/>
+      <c r="U23" s="17"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43000022</v>
       </c>
@@ -9016,15 +9345,16 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
-      <c r="R24" s="4" t="s">
+      <c r="R24" s="4"/>
+      <c r="S24" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="S24" s="4" t="s">
+      <c r="T24" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43000023</v>
       </c>
@@ -9066,15 +9396,16 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
-      <c r="R25" s="4" t="s">
+      <c r="R25" s="4"/>
+      <c r="S25" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="S25" s="4" t="s">
+      <c r="T25" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43000024</v>
       </c>
@@ -9116,15 +9447,16 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
-      <c r="R26" s="4" t="s">
+      <c r="R26" s="4"/>
+      <c r="S26" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="S26" s="4" t="s">
+      <c r="T26" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T26" s="17"/>
+      <c r="U26" s="17"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43000025</v>
       </c>
@@ -9166,15 +9498,16 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
-      <c r="R27" s="4" t="s">
+      <c r="R27" s="4"/>
+      <c r="S27" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="S27" s="4" t="s">
+      <c r="T27" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T27" s="17"/>
+      <c r="U27" s="17"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43000026</v>
       </c>
@@ -9216,15 +9549,16 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
-      <c r="R28" s="4" t="s">
+      <c r="R28" s="4"/>
+      <c r="S28" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="S28" s="4" t="s">
+      <c r="T28" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43000027</v>
       </c>
@@ -9266,15 +9600,16 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
-      <c r="R29" s="4" t="s">
+      <c r="R29" s="4"/>
+      <c r="S29" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="S29" s="4" t="s">
+      <c r="T29" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T29" s="17"/>
+      <c r="U29" s="17"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43000028</v>
       </c>
@@ -9316,15 +9651,16 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
-      <c r="R30" s="4" t="s">
+      <c r="R30" s="4"/>
+      <c r="S30" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="S30" s="4" t="s">
+      <c r="T30" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T30" s="17"/>
+      <c r="U30" s="17"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43000029</v>
       </c>
@@ -9366,15 +9702,16 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
-      <c r="R31" s="4" t="s">
+      <c r="R31" s="4"/>
+      <c r="S31" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="S31" s="4" t="s">
+      <c r="T31" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T31" s="17"/>
+      <c r="U31" s="17"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43000030</v>
       </c>
@@ -9416,15 +9753,16 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
-      <c r="R32" s="4" t="s">
+      <c r="R32" s="4"/>
+      <c r="S32" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="S32" s="4" t="s">
+      <c r="T32" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43000031</v>
       </c>
@@ -9466,15 +9804,16 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
-      <c r="R33" s="4" t="s">
+      <c r="R33" s="4"/>
+      <c r="S33" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="S33" s="4" t="s">
+      <c r="T33" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43000032</v>
       </c>
@@ -9516,15 +9855,16 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
-      <c r="R34" s="4" t="s">
+      <c r="R34" s="4"/>
+      <c r="S34" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="S34" s="4" t="s">
+      <c r="T34" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43000033</v>
       </c>
@@ -9566,15 +9906,16 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
-      <c r="R35" s="4" t="s">
+      <c r="R35" s="4"/>
+      <c r="S35" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="S35" s="4" t="s">
+      <c r="T35" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T35" s="17"/>
+      <c r="U35" s="17"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43000035</v>
       </c>
@@ -9616,15 +9957,16 @@
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
-      <c r="R36" s="4" t="s">
+      <c r="R36" s="4"/>
+      <c r="S36" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="S36" s="4" t="s">
+      <c r="T36" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43000037</v>
       </c>
@@ -9666,15 +10008,16 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
-      <c r="R37" s="4" t="s">
+      <c r="R37" s="4"/>
+      <c r="S37" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="S37" s="4" t="s">
+      <c r="T37" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43000038</v>
       </c>
@@ -9716,15 +10059,16 @@
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
-      <c r="R38" s="4" t="s">
+      <c r="R38" s="4"/>
+      <c r="S38" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="S38" s="4" t="s">
+      <c r="T38" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T38" s="35"/>
+      <c r="U38" s="35"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A39" s="37">
         <v>43001001</v>
       </c>
@@ -9768,15 +10112,16 @@
       </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
-      <c r="R39" s="4" t="s">
+      <c r="R39" s="4"/>
+      <c r="S39" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="S39" s="6" t="s">
+      <c r="T39" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="T39" s="17"/>
+      <c r="U39" s="17"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A40" s="37">
         <v>43001002</v>
       </c>
@@ -9820,15 +10165,16 @@
       </c>
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
-      <c r="R40" s="4" t="s">
+      <c r="R40" s="4"/>
+      <c r="S40" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="S40" s="4" t="s">
+      <c r="T40" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T40" s="36"/>
+      <c r="U40" s="36"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A41" s="37">
         <v>43001003</v>
       </c>
@@ -9872,15 +10218,16 @@
       </c>
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
-      <c r="R41" s="4" t="s">
+      <c r="R41" s="4"/>
+      <c r="S41" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="S41" s="4" t="s">
+      <c r="T41" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T41" s="27"/>
+      <c r="U41" s="27"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A42" s="37">
         <v>43001004</v>
       </c>
@@ -9924,15 +10271,16 @@
       </c>
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
-      <c r="R42" s="4" t="s">
+      <c r="R42" s="4"/>
+      <c r="S42" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="S42" s="34" t="s">
+      <c r="T42" s="34" t="s">
         <v>424</v>
       </c>
-      <c r="T42" s="17"/>
+      <c r="U42" s="17"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A43" s="37">
         <v>43001005</v>
       </c>
@@ -9976,15 +10324,16 @@
       </c>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
-      <c r="R43" s="4" t="s">
+      <c r="R43" s="4"/>
+      <c r="S43" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="S43" s="4" t="s">
+      <c r="T43" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T43" s="17"/>
+      <c r="U43" s="17"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A44" s="37">
         <v>43001006</v>
       </c>
@@ -10028,15 +10377,16 @@
       </c>
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
-      <c r="R44" s="4" t="s">
+      <c r="R44" s="4"/>
+      <c r="S44" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="S44" s="6" t="s">
+      <c r="T44" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="T44" s="36"/>
+      <c r="U44" s="36"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A45" s="38">
         <v>43002001</v>
       </c>
@@ -10078,15 +10428,16 @@
       <c r="O45" s="27"/>
       <c r="P45" s="27"/>
       <c r="Q45" s="27"/>
-      <c r="R45" s="4" t="s">
+      <c r="R45" s="27"/>
+      <c r="S45" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="S45" s="27" t="s">
+      <c r="T45" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="T45" s="27"/>
+      <c r="U45" s="27"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A46" s="38">
         <v>43002002</v>
       </c>
@@ -10128,15 +10479,16 @@
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
       <c r="Q46" s="27"/>
-      <c r="R46" s="4" t="s">
+      <c r="R46" s="27"/>
+      <c r="S46" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="S46" s="27" t="s">
+      <c r="T46" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="T46" s="27"/>
+      <c r="U46" s="27"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A47" s="38">
         <v>43002003</v>
       </c>
@@ -10178,15 +10530,16 @@
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
       <c r="Q47" s="27"/>
-      <c r="R47" s="4" t="s">
+      <c r="R47" s="27"/>
+      <c r="S47" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="S47" s="27" t="s">
+      <c r="T47" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="T47" s="27"/>
+      <c r="U47" s="27"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A48" s="38">
         <v>43002004</v>
       </c>
@@ -10228,15 +10581,16 @@
       <c r="O48" s="27"/>
       <c r="P48" s="27"/>
       <c r="Q48" s="13"/>
-      <c r="R48" s="31" t="s">
+      <c r="R48" s="13"/>
+      <c r="S48" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="S48" s="27" t="s">
+      <c r="T48" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="T48" s="27"/>
+      <c r="U48" s="27"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A49" s="38">
         <v>43002005</v>
       </c>
@@ -10278,15 +10632,16 @@
       <c r="O49" s="27"/>
       <c r="P49" s="27"/>
       <c r="Q49" s="13"/>
-      <c r="R49" s="31" t="s">
+      <c r="R49" s="13"/>
+      <c r="S49" s="31" t="s">
         <v>343</v>
       </c>
-      <c r="S49" s="27" t="s">
+      <c r="T49" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="T49" s="27"/>
+      <c r="U49" s="27"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A50" s="38">
         <v>43002006</v>
       </c>
@@ -10328,19 +10683,20 @@
       <c r="O50" s="27"/>
       <c r="P50" s="27"/>
       <c r="Q50" s="13"/>
-      <c r="R50" s="31" t="s">
+      <c r="R50" s="13"/>
+      <c r="S50" s="31" t="s">
         <v>344</v>
       </c>
-      <c r="S50" s="27" t="s">
+      <c r="T50" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="T50" s="27"/>
+      <c r="U50" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="S42">
+  <conditionalFormatting sqref="T42">
     <cfRule type="containsBlanks" dxfId="7" priority="9">
-      <formula>LEN(TRIM(S42))=0</formula>
+      <formula>LEN(TRIM(T42))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
@@ -10348,9 +10704,9 @@
       <formula>LEN(TRIM(C47))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R47">
+  <conditionalFormatting sqref="S47">
     <cfRule type="containsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(R47))=0</formula>
+      <formula>LEN(TRIM(S47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C50">
@@ -10358,9 +10714,9 @@
       <formula>LEN(TRIM(C48))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R48:R50">
+  <conditionalFormatting sqref="S48:S50">
     <cfRule type="containsBlanks" dxfId="3" priority="3">
-      <formula>LEN(TRIM(R48))=0</formula>
+      <formula>LEN(TRIM(S48))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
@@ -10383,13 +10739,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q1" sqref="Q1"/>
+      <selection pane="bottomRight" activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10403,12 +10759,12 @@
     <col min="13" max="14" width="6.125" customWidth="1"/>
     <col min="15" max="15" width="28.375" customWidth="1"/>
     <col min="16" max="16" width="19.5" customWidth="1"/>
-    <col min="17" max="17" width="9.875" customWidth="1"/>
-    <col min="19" max="19" width="10.625" customWidth="1"/>
-    <col min="20" max="20" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.875" customWidth="1"/>
+    <col min="20" max="20" width="10.625" customWidth="1"/>
+    <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>151</v>
       </c>
@@ -10460,17 +10816,20 @@
       <c r="Q1" s="25" t="s">
         <v>429</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="25" t="s">
+        <v>435</v>
+      </c>
+      <c r="S1" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="T1" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="U1" s="25" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>149</v>
       </c>
@@ -10522,17 +10881,20 @@
       <c r="Q2" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="S2" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="U2" s="8" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>160</v>
       </c>
@@ -10585,16 +10947,19 @@
         <v>432</v>
       </c>
       <c r="R3" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="S3" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="T3" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="T3" s="18" t="s">
+      <c r="U3" s="18" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43010001</v>
       </c>
@@ -10636,15 +11001,16 @@
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="6"/>
+      <c r="S4" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43010002</v>
       </c>
@@ -10684,15 +11050,16 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="4"/>
+      <c r="S5" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43010003</v>
       </c>
@@ -10732,15 +11099,16 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="4" t="s">
+      <c r="R6" s="4"/>
+      <c r="S6" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="T6" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43010004</v>
       </c>
@@ -10780,15 +11148,16 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="4"/>
+      <c r="S7" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="S7" s="4" t="s">
+      <c r="T7" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43010005</v>
       </c>
@@ -10830,15 +11199,16 @@
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-      <c r="R8" s="6" t="s">
+      <c r="R8" s="4"/>
+      <c r="S8" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="T8" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43010006</v>
       </c>
@@ -10880,15 +11250,16 @@
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="6" t="s">
+      <c r="R9" s="4"/>
+      <c r="S9" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="T9" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43010101</v>
       </c>
@@ -10926,15 +11297,16 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-      <c r="R10" s="4" t="s">
+      <c r="R10" s="4"/>
+      <c r="S10" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="S10" s="4" t="s">
+      <c r="T10" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43010102</v>
       </c>
@@ -10972,15 +11344,16 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="4"/>
+      <c r="S11" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="T11" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43010103</v>
       </c>
@@ -11018,15 +11391,16 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-      <c r="R12" s="4" t="s">
+      <c r="R12" s="4"/>
+      <c r="S12" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="S12" s="4" t="s">
+      <c r="T12" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43010104</v>
       </c>
@@ -11064,15 +11438,16 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="4" t="s">
+      <c r="R13" s="4"/>
+      <c r="S13" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="S13" s="4" t="s">
+      <c r="T13" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43010105</v>
       </c>
@@ -11110,13 +11485,14 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-      <c r="R14" s="4" t="s">
+      <c r="R14" s="4"/>
+      <c r="S14" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="S14" s="4" t="s">
+      <c r="T14" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
a people chess can live in 2 scenes
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="430">
   <si>
     <t>老鼠</t>
   </si>
@@ -1458,75 +1458,8 @@
     <t>51000216;10;2;51000216;10;4</t>
   </si>
   <si>
-    <t>初始场景id</t>
-  </si>
-  <si>
-    <t>初始场景id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BornSceneId</t>
-  </si>
-  <si>
-    <t>BornSceneId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Figue</t>
     <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>綁定事件</t>
-  </si>
-  <si>
-    <t>綁定事件</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BindQuest</t>
-  </si>
-  <si>
-    <t>BindQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npcsainisi</t>
-  </si>
-  <si>
-    <t>npcsaibasi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npcaolai</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npckedi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npcweia</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npcmilanda</t>
-  </si>
-  <si>
-    <t>npcbeilukai</t>
-  </si>
-  <si>
-    <t>npcleiluo</t>
-  </si>
-  <si>
-    <t>npcbaludi</t>
   </si>
 </sst>
 </file>
@@ -2440,92 +2373,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="111">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="97">
     <dxf>
       <fill>
         <patternFill>
@@ -2851,54 +2699,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="宋体"/>
         <scheme val="none"/>
@@ -2955,35 +2755,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -3594,25 +3365,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -4160,35 +3912,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -4780,99 +4503,93 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:U51" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109" tableBorderDxfId="108">
-  <autoFilter ref="A3:U51"/>
-  <sortState ref="A4:U50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:S51" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95" tableBorderDxfId="94">
+  <autoFilter ref="A3:S51"/>
+  <sortState ref="A4:S50">
     <sortCondition ref="A3:A50"/>
   </sortState>
-  <tableColumns count="21">
-    <tableColumn id="1" name="Id" dataDxfId="107"/>
-    <tableColumn id="2" name="Name" dataDxfId="106"/>
-    <tableColumn id="18" name="Ename" dataDxfId="105"/>
-    <tableColumn id="3" name="Type" dataDxfId="104"/>
-    <tableColumn id="21" name="Quality" dataDxfId="103"/>
-    <tableColumn id="6" name="World" dataDxfId="102"/>
-    <tableColumn id="10" name="Job" dataDxfId="101"/>
-    <tableColumn id="11" name="Level" dataDxfId="100"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="99"/>
-    <tableColumn id="13" name="Method" dataDxfId="98"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="97"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="96"/>
-    <tableColumn id="12" name="EpRecoverRate" dataDxfId="95"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="94"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="93"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="92"/>
-    <tableColumn id="7" name="BornSceneId" dataDxfId="91"/>
-    <tableColumn id="8" name="BindQuest" dataDxfId="41"/>
-    <tableColumn id="17" name="Figue" dataDxfId="90"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="89"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="88"/>
+  <tableColumns count="19">
+    <tableColumn id="1" name="Id" dataDxfId="93"/>
+    <tableColumn id="2" name="Name" dataDxfId="92"/>
+    <tableColumn id="18" name="Ename" dataDxfId="91"/>
+    <tableColumn id="3" name="Type" dataDxfId="90"/>
+    <tableColumn id="21" name="Quality" dataDxfId="89"/>
+    <tableColumn id="6" name="World" dataDxfId="88"/>
+    <tableColumn id="10" name="Job" dataDxfId="87"/>
+    <tableColumn id="11" name="Level" dataDxfId="86"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="85"/>
+    <tableColumn id="13" name="Method" dataDxfId="84"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="83"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="82"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="81"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="80"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="79"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="78"/>
+    <tableColumn id="17" name="Figue" dataDxfId="77"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="76"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:U50" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86" tableBorderDxfId="85">
-  <autoFilter ref="A3:U50"/>
-  <sortState ref="A4:U50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:S50" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72">
+  <autoFilter ref="A3:S50"/>
+  <sortState ref="A4:S50">
     <sortCondition ref="A3:A50"/>
   </sortState>
-  <tableColumns count="21">
-    <tableColumn id="1" name="Id" dataDxfId="84"/>
-    <tableColumn id="2" name="Name" dataDxfId="83"/>
-    <tableColumn id="18" name="Ename" dataDxfId="82"/>
-    <tableColumn id="3" name="Type" dataDxfId="81"/>
-    <tableColumn id="7" name="Quality" dataDxfId="80"/>
-    <tableColumn id="6" name="World" dataDxfId="79"/>
-    <tableColumn id="10" name="Job" dataDxfId="78"/>
-    <tableColumn id="11" name="Level" dataDxfId="77"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="76"/>
-    <tableColumn id="13" name="Method" dataDxfId="75"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="74"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="73"/>
-    <tableColumn id="12" name="EpRecoverRate" dataDxfId="72"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="71"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="70"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="69"/>
-    <tableColumn id="8" name="BornSceneId" dataDxfId="68"/>
-    <tableColumn id="21" name="BindQuest" dataDxfId="40"/>
-    <tableColumn id="17" name="Figue" dataDxfId="67"/>
-    <tableColumn id="9" name="BattleMap" dataDxfId="66"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="65"/>
+  <tableColumns count="19">
+    <tableColumn id="1" name="Id" dataDxfId="71"/>
+    <tableColumn id="2" name="Name" dataDxfId="70"/>
+    <tableColumn id="18" name="Ename" dataDxfId="69"/>
+    <tableColumn id="3" name="Type" dataDxfId="68"/>
+    <tableColumn id="7" name="Quality" dataDxfId="67"/>
+    <tableColumn id="6" name="World" dataDxfId="66"/>
+    <tableColumn id="10" name="Job" dataDxfId="65"/>
+    <tableColumn id="11" name="Level" dataDxfId="64"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="63"/>
+    <tableColumn id="13" name="Method" dataDxfId="62"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="61"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="60"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="59"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="58"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="57"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="56"/>
+    <tableColumn id="17" name="Figue" dataDxfId="55"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="54"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:U14" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
-  <autoFilter ref="A3:U14"/>
-  <sortState ref="A4:T83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:S14" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51" tableBorderDxfId="50">
+  <autoFilter ref="A3:S14"/>
+  <sortState ref="A4:R83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="21">
-    <tableColumn id="1" name="Id" dataDxfId="61"/>
-    <tableColumn id="2" name="Name" dataDxfId="60"/>
-    <tableColumn id="18" name="Ename" dataDxfId="59"/>
-    <tableColumn id="3" name="Type" dataDxfId="58"/>
-    <tableColumn id="7" name="Quality" dataDxfId="57"/>
-    <tableColumn id="6" name="World" dataDxfId="56"/>
-    <tableColumn id="10" name="Job" dataDxfId="55"/>
-    <tableColumn id="11" name="Level" dataDxfId="54"/>
-    <tableColumn id="5" name="AutoAddLevel" dataDxfId="53"/>
-    <tableColumn id="13" name="Method" dataDxfId="52"/>
-    <tableColumn id="14" name="Emethod" dataDxfId="51"/>
-    <tableColumn id="20" name="KingTowerId" dataDxfId="50"/>
-    <tableColumn id="12" name="EpRecoverRate" dataDxfId="49"/>
-    <tableColumn id="19" name="CardReduce" dataDxfId="48"/>
-    <tableColumn id="15" name="RightMon" dataDxfId="47"/>
-    <tableColumn id="4" name="PetMon" dataDxfId="46"/>
-    <tableColumn id="8" name="BornSceneId" dataDxfId="45"/>
-    <tableColumn id="21" name="BindQuest" dataDxfId="0"/>
-    <tableColumn id="9" name="Figue" dataDxfId="44"/>
-    <tableColumn id="17" name="BattleMap" dataDxfId="43"/>
-    <tableColumn id="16" name="InRandomQuest" dataDxfId="42"/>
+  <tableColumns count="19">
+    <tableColumn id="1" name="Id" dataDxfId="49"/>
+    <tableColumn id="2" name="Name" dataDxfId="48"/>
+    <tableColumn id="18" name="Ename" dataDxfId="47"/>
+    <tableColumn id="3" name="Type" dataDxfId="46"/>
+    <tableColumn id="7" name="Quality" dataDxfId="45"/>
+    <tableColumn id="6" name="World" dataDxfId="44"/>
+    <tableColumn id="10" name="Job" dataDxfId="43"/>
+    <tableColumn id="11" name="Level" dataDxfId="42"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="41"/>
+    <tableColumn id="13" name="Method" dataDxfId="40"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="39"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="38"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="37"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="36"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="35"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="34"/>
+    <tableColumn id="9" name="Figue" dataDxfId="33"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="32"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5199,13 +4916,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R1" sqref="R1:R3"/>
+      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5217,11 +4934,10 @@
     <col min="10" max="10" width="9.5" customWidth="1"/>
     <col min="11" max="12" width="10.625" customWidth="1"/>
     <col min="13" max="16" width="5.875" customWidth="1"/>
-    <col min="17" max="18" width="9.75" customWidth="1"/>
-    <col min="20" max="20" width="10.625" customWidth="1"/>
+    <col min="18" max="18" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="72" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>151</v>
       </c>
@@ -5270,23 +4986,17 @@
       <c r="P1" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="Q1" s="11" t="s">
-        <v>430</v>
+      <c r="Q1" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>436</v>
-      </c>
-      <c r="S1" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="T1" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>149</v>
       </c>
@@ -5335,23 +5045,17 @@
       <c r="P2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>431</v>
+      <c r="Q2" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="S2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="U2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>160</v>
       </c>
@@ -5401,22 +5105,16 @@
         <v>240</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="T3" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="S3" s="16" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43020101</v>
       </c>
@@ -5453,21 +5151,15 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="4">
-        <v>13010002</v>
+      <c r="Q4" s="4" t="s">
+        <v>345</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="T4" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U4" s="19"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S4" s="19"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43020102</v>
       </c>
@@ -5504,21 +5196,15 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="4">
-        <v>13010003</v>
-      </c>
-      <c r="R5" s="32" t="s">
-        <v>441</v>
-      </c>
-      <c r="S5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U5" s="19"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S5" s="19"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43020103</v>
       </c>
@@ -5557,23 +5243,17 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="4">
-        <v>13010004</v>
-      </c>
-      <c r="R6" s="32" t="s">
-        <v>443</v>
-      </c>
-      <c r="S6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="T6" s="4" t="s">
+      <c r="R6" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U6" s="19" t="s">
+      <c r="S6" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43020104</v>
       </c>
@@ -5612,21 +5292,15 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="4">
-        <v>13010007</v>
-      </c>
-      <c r="R7" s="32" t="s">
-        <v>444</v>
-      </c>
-      <c r="S7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="T7" s="4" t="s">
+      <c r="R7" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U7" s="19"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S7" s="19"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43020105</v>
       </c>
@@ -5665,23 +5339,17 @@
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="4">
-        <v>13010009</v>
-      </c>
-      <c r="R8" s="32" t="s">
-        <v>442</v>
-      </c>
-      <c r="S8" s="4" t="s">
+      <c r="Q8" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="T8" s="4" t="s">
+      <c r="R8" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U8" s="19" t="s">
+      <c r="S8" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43020106</v>
       </c>
@@ -5720,23 +5388,17 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="4">
-        <v>13010008</v>
-      </c>
-      <c r="R9" s="32" t="s">
-        <v>445</v>
-      </c>
-      <c r="S9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="R9" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U9" s="19" t="s">
+      <c r="S9" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43020107</v>
       </c>
@@ -5775,19 +5437,17 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="T10" s="4" t="s">
+      <c r="R10" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U10" s="19" t="s">
+      <c r="S10" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43020108</v>
       </c>
@@ -5826,23 +5486,17 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="4">
-        <v>13010203</v>
-      </c>
-      <c r="R11" s="32" t="s">
-        <v>446</v>
-      </c>
-      <c r="S11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="R11" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U11" s="19" t="s">
+      <c r="S11" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43020109</v>
       </c>
@@ -5881,23 +5535,17 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="4">
-        <v>13010202</v>
-      </c>
-      <c r="R12" s="32" t="s">
-        <v>447</v>
-      </c>
-      <c r="S12" s="4" t="s">
+      <c r="Q12" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="T12" s="4" t="s">
+      <c r="R12" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U12" s="19" t="s">
+      <c r="S12" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43020110</v>
       </c>
@@ -5936,23 +5584,17 @@
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="4">
-        <v>13010203</v>
-      </c>
-      <c r="R13" s="32" t="s">
-        <v>448</v>
-      </c>
-      <c r="S13" s="4" t="s">
+      <c r="Q13" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="T13" s="4" t="s">
+      <c r="R13" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U13" s="19" t="s">
+      <c r="S13" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43020201</v>
       </c>
@@ -5991,21 +5633,17 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="4">
-        <v>13010103</v>
-      </c>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4" t="s">
+      <c r="Q14" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="T14" s="4" t="s">
+      <c r="R14" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U14" s="19" t="s">
+      <c r="S14" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43020202</v>
       </c>
@@ -6044,19 +5682,17 @@
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4" t="s">
+      <c r="Q15" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="T15" s="4" t="s">
+      <c r="R15" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U15" s="19" t="s">
+      <c r="S15" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43020203</v>
       </c>
@@ -6095,19 +5731,17 @@
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4" t="s">
+      <c r="Q16" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="T16" s="4" t="s">
+      <c r="R16" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U16" s="19" t="s">
+      <c r="S16" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43020204</v>
       </c>
@@ -6146,21 +5780,17 @@
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="4">
-        <v>13010107</v>
-      </c>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4" t="s">
+      <c r="Q17" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="T17" s="4" t="s">
+      <c r="R17" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U17" s="19" t="s">
+      <c r="S17" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43020205</v>
       </c>
@@ -6197,21 +5827,17 @@
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
-      <c r="Q18" s="4">
-        <v>13010202</v>
-      </c>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4" t="s">
+      <c r="Q18" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="T18" s="4" t="s">
+      <c r="R18" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U18" s="19" t="s">
+      <c r="S18" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43020206</v>
       </c>
@@ -6250,21 +5876,17 @@
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="4">
-        <v>13010205</v>
-      </c>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4" t="s">
+      <c r="Q19" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="T19" s="4" t="s">
+      <c r="R19" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U19" s="19" t="s">
+      <c r="S19" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43020207</v>
       </c>
@@ -6303,19 +5925,17 @@
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4" t="s">
+      <c r="Q20" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="T20" s="4" t="s">
+      <c r="R20" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U20" s="19" t="s">
+      <c r="S20" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43020301</v>
       </c>
@@ -6354,21 +5974,17 @@
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
-      <c r="Q21" s="4">
-        <v>13010102</v>
-      </c>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4" t="s">
+      <c r="Q21" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="T21" s="4" t="s">
+      <c r="R21" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U21" s="19" t="s">
+      <c r="S21" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43020302</v>
       </c>
@@ -6407,19 +6023,17 @@
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4" t="s">
+      <c r="Q22" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="T22" s="4" t="s">
+      <c r="R22" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U22" s="19" t="s">
+      <c r="S22" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43020303</v>
       </c>
@@ -6456,21 +6070,17 @@
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
-      <c r="Q23" s="4">
-        <v>13010106</v>
-      </c>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4" t="s">
+      <c r="Q23" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="T23" s="4" t="s">
+      <c r="R23" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U23" s="19" t="s">
+      <c r="S23" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43020304</v>
       </c>
@@ -6509,19 +6119,17 @@
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4" t="s">
+      <c r="Q24" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="T24" s="4" t="s">
+      <c r="R24" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U24" s="19" t="s">
+      <c r="S24" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43020305</v>
       </c>
@@ -6560,21 +6168,17 @@
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
-      <c r="Q25" s="4">
-        <v>13010204</v>
-      </c>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4" t="s">
+      <c r="Q25" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="T25" s="4" t="s">
+      <c r="R25" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U25" s="19" t="s">
+      <c r="S25" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43020306</v>
       </c>
@@ -6613,21 +6217,17 @@
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
-      <c r="Q26" s="4">
-        <v>13010204</v>
-      </c>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4" t="s">
+      <c r="Q26" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="T26" s="4" t="s">
+      <c r="R26" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U26" s="19" t="s">
+      <c r="S26" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43020307</v>
       </c>
@@ -6666,21 +6266,17 @@
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
-      <c r="Q27" s="4">
-        <v>13010102</v>
-      </c>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4" t="s">
+      <c r="Q27" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="T27" s="4" t="s">
+      <c r="R27" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U27" s="19" t="s">
+      <c r="S27" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43020308</v>
       </c>
@@ -6719,19 +6315,17 @@
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4" t="s">
+      <c r="Q28" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="T28" s="4" t="s">
+      <c r="R28" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U28" s="19" t="s">
+      <c r="S28" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43020309</v>
       </c>
@@ -6770,21 +6364,17 @@
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
-      <c r="Q29" s="4">
-        <v>13010105</v>
-      </c>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4" t="s">
+      <c r="Q29" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="T29" s="4" t="s">
+      <c r="R29" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U29" s="19" t="s">
+      <c r="S29" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43020310</v>
       </c>
@@ -6823,21 +6413,17 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
-      <c r="Q30" s="4">
-        <v>13010105</v>
-      </c>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4" t="s">
+      <c r="Q30" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="T30" s="4" t="s">
+      <c r="R30" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U30" s="19" t="s">
+      <c r="S30" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43020311</v>
       </c>
@@ -6876,19 +6462,17 @@
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4" t="s">
+      <c r="Q31" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="T31" s="4" t="s">
+      <c r="R31" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U31" s="19" t="s">
+      <c r="S31" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43020312</v>
       </c>
@@ -6927,19 +6511,17 @@
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4" t="s">
+      <c r="Q32" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="T32" s="4" t="s">
+      <c r="R32" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U32" s="19" t="s">
+      <c r="S32" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43020401</v>
       </c>
@@ -6978,21 +6560,17 @@
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
-      <c r="Q33" s="4">
-        <v>13010108</v>
-      </c>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4" t="s">
+      <c r="Q33" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="T33" s="4" t="s">
+      <c r="R33" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U33" s="19" t="s">
+      <c r="S33" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43020402</v>
       </c>
@@ -7031,21 +6609,17 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
-      <c r="Q34" s="4">
-        <v>13010103</v>
-      </c>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4" t="s">
+      <c r="Q34" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="T34" s="4" t="s">
+      <c r="R34" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U34" s="19" t="s">
+      <c r="S34" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43020403</v>
       </c>
@@ -7084,19 +6658,17 @@
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4" t="s">
+      <c r="Q35" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="T35" s="4" t="s">
+      <c r="R35" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U35" s="19" t="s">
+      <c r="S35" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43020404</v>
       </c>
@@ -7135,21 +6707,17 @@
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
-      <c r="Q36" s="4">
-        <v>13010208</v>
-      </c>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4" t="s">
+      <c r="Q36" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="T36" s="4" t="s">
+      <c r="R36" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U36" s="19" t="s">
+      <c r="S36" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43020405</v>
       </c>
@@ -7188,21 +6756,17 @@
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
-      <c r="Q37" s="4">
-        <v>13010108</v>
-      </c>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4" t="s">
+      <c r="Q37" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="T37" s="4" t="s">
+      <c r="R37" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U37" s="19" t="s">
+      <c r="S37" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43020406</v>
       </c>
@@ -7241,21 +6805,17 @@
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
-      <c r="Q38" s="4">
-        <v>13010104</v>
-      </c>
-      <c r="R38" s="4"/>
-      <c r="S38" s="4" t="s">
+      <c r="Q38" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="T38" s="4" t="s">
+      <c r="R38" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U38" s="19" t="s">
+      <c r="S38" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>43020407</v>
       </c>
@@ -7294,21 +6854,17 @@
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
-      <c r="Q39" s="4">
-        <v>13010209</v>
-      </c>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4" t="s">
+      <c r="Q39" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="T39" s="4" t="s">
+      <c r="R39" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U39" s="19" t="s">
+      <c r="S39" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>43020408</v>
       </c>
@@ -7347,21 +6903,17 @@
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
-      <c r="Q40" s="4">
-        <v>13010205</v>
-      </c>
-      <c r="R40" s="4"/>
-      <c r="S40" s="4" t="s">
+      <c r="Q40" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="T40" s="4" t="s">
+      <c r="R40" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U40" s="19" t="s">
+      <c r="S40" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>43020409</v>
       </c>
@@ -7400,19 +6952,17 @@
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
-      <c r="S41" s="4" t="s">
+      <c r="Q41" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="T41" s="4" t="s">
+      <c r="R41" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U41" s="19" t="s">
+      <c r="S41" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>43020501</v>
       </c>
@@ -7451,19 +7001,17 @@
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4"/>
-      <c r="S42" s="4" t="s">
+      <c r="Q42" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="T42" s="4" t="s">
+      <c r="R42" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U42" s="19" t="s">
+      <c r="S42" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>43020502</v>
       </c>
@@ -7502,21 +7050,17 @@
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
-      <c r="Q43" s="4">
-        <v>13010109</v>
-      </c>
-      <c r="R43" s="4"/>
-      <c r="S43" s="4" t="s">
+      <c r="Q43" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="T43" s="4" t="s">
+      <c r="R43" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U43" s="19" t="s">
+      <c r="S43" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43020503</v>
       </c>
@@ -7555,21 +7099,17 @@
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
       <c r="P44" s="4"/>
-      <c r="Q44" s="4">
-        <v>13010207</v>
-      </c>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4" t="s">
+      <c r="Q44" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="T44" s="4" t="s">
+      <c r="R44" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U44" s="19" t="s">
+      <c r="S44" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>43020504</v>
       </c>
@@ -7608,21 +7148,17 @@
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
       <c r="P45" s="4"/>
-      <c r="Q45" s="4">
-        <v>13010209</v>
-      </c>
-      <c r="R45" s="4"/>
-      <c r="S45" s="4" t="s">
+      <c r="Q45" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="T45" s="4" t="s">
+      <c r="R45" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U45" s="19" t="s">
+      <c r="S45" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>43020505</v>
       </c>
@@ -7661,21 +7197,17 @@
       <c r="N46" s="4"/>
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
-      <c r="Q46" s="4">
-        <v>13010206</v>
-      </c>
-      <c r="R46" s="4"/>
-      <c r="S46" s="27" t="s">
+      <c r="Q46" s="27" t="s">
         <v>410</v>
       </c>
-      <c r="T46" s="4" t="s">
+      <c r="R46" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U46" s="19" t="s">
+      <c r="S46" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>43020506</v>
       </c>
@@ -7714,19 +7246,17 @@
       <c r="N47" s="4"/>
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
-      <c r="Q47" s="27"/>
-      <c r="R47" s="27"/>
-      <c r="S47" s="27" t="s">
+      <c r="Q47" s="27" t="s">
         <v>409</v>
       </c>
-      <c r="T47" s="4" t="s">
+      <c r="R47" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U47" s="19" t="s">
+      <c r="S47" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>43020601</v>
       </c>
@@ -7765,19 +7295,17 @@
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
       <c r="P48" s="4"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
-      <c r="S48" s="4" t="s">
+      <c r="Q48" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="T48" s="4" t="s">
+      <c r="R48" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U48" s="19" t="s">
+      <c r="S48" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>43020602</v>
       </c>
@@ -7814,21 +7342,17 @@
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
       <c r="P49" s="4"/>
-      <c r="Q49" s="4">
-        <v>13010110</v>
-      </c>
-      <c r="R49" s="4"/>
-      <c r="S49" s="4" t="s">
+      <c r="Q49" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="T49" s="4" t="s">
+      <c r="R49" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U49" s="19" t="s">
+      <c r="S49" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>43020603</v>
       </c>
@@ -7865,19 +7389,17 @@
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
       <c r="P50" s="4"/>
-      <c r="Q50" s="4"/>
-      <c r="R50" s="4"/>
-      <c r="S50" s="4" t="s">
+      <c r="Q50" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="T50" s="4" t="s">
+      <c r="R50" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U50" s="19" t="s">
+      <c r="S50" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>43020604</v>
       </c>
@@ -7916,142 +7438,100 @@
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
-      <c r="Q51" s="4"/>
-      <c r="R51" s="4"/>
-      <c r="S51" s="4" t="s">
+      <c r="Q51" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="T51" s="4" t="s">
+      <c r="R51" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="U51" s="19" t="s">
+      <c r="S51" s="19" t="s">
         <v>208</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E23:E25 E27:E43 E4:E19 E45:E51">
-    <cfRule type="cellIs" dxfId="39" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="42" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="43" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="44" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="45" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="37" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="38" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="39" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="40" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="31" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="17" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="18" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="23" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
       <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R5">
-    <cfRule type="containsBlanks" dxfId="15" priority="8">
-      <formula>LEN(TRIM(R5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R8">
-    <cfRule type="containsBlanks" dxfId="14" priority="7">
-      <formula>LEN(TRIM(R8))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R6">
-    <cfRule type="containsBlanks" dxfId="13" priority="6">
-      <formula>LEN(TRIM(R6))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R7">
-    <cfRule type="containsBlanks" dxfId="12" priority="5">
-      <formula>LEN(TRIM(R7))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R9">
-    <cfRule type="containsBlanks" dxfId="11" priority="4">
-      <formula>LEN(TRIM(R9))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R11">
-    <cfRule type="containsBlanks" dxfId="10" priority="3">
-      <formula>LEN(TRIM(R11))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R12">
-    <cfRule type="containsBlanks" dxfId="9" priority="2">
-      <formula>LEN(TRIM(R12))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R13">
-    <cfRule type="containsBlanks" dxfId="8" priority="1">
-      <formula>LEN(TRIM(R13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8064,13 +7544,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U50"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="I22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R1" sqref="R1:R3"/>
+      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8083,12 +7563,11 @@
     <col min="11" max="12" width="10.625" customWidth="1"/>
     <col min="13" max="14" width="6.125" customWidth="1"/>
     <col min="15" max="16" width="27.125" customWidth="1"/>
-    <col min="17" max="18" width="13" customWidth="1"/>
-    <col min="20" max="20" width="10.625" customWidth="1"/>
-    <col min="21" max="21" width="8" customWidth="1"/>
+    <col min="18" max="18" width="10.625" customWidth="1"/>
+    <col min="19" max="19" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>151</v>
       </c>
@@ -8137,23 +7616,17 @@
       <c r="P1" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="Q1" s="11" t="s">
-        <v>429</v>
+      <c r="Q1" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>436</v>
-      </c>
-      <c r="S1" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="T1" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>149</v>
       </c>
@@ -8202,23 +7675,17 @@
       <c r="P2" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>231</v>
+      <c r="Q2" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="T2" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>160</v>
       </c>
@@ -8268,22 +7735,16 @@
         <v>185</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>432</v>
+        <v>168</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="T3" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="S3" s="16" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43000001</v>
       </c>
@@ -8324,17 +7785,15 @@
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="U4" s="17"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S4" s="17"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43000002</v>
       </c>
@@ -8375,17 +7834,15 @@
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="U5" s="17"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S5" s="17"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43000003</v>
       </c>
@@ -8426,17 +7883,15 @@
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="T6" s="4" t="s">
+      <c r="R6" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U6" s="17"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S6" s="17"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43000004</v>
       </c>
@@ -8477,17 +7932,15 @@
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="T7" s="4" t="s">
+      <c r="R7" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U7" s="17"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S7" s="17"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43000005</v>
       </c>
@@ -8528,17 +7981,15 @@
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4" t="s">
+      <c r="Q8" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="T8" s="4" t="s">
+      <c r="R8" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U8" s="17"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S8" s="17"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43000007</v>
       </c>
@@ -8579,17 +8030,15 @@
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="R9" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="U9" s="17"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S9" s="17"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43000008</v>
       </c>
@@ -8630,17 +8079,15 @@
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="T10" s="4" t="s">
+      <c r="R10" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U10" s="17"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S10" s="17"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43000009</v>
       </c>
@@ -8681,17 +8128,15 @@
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="R11" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U11" s="17"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S11" s="17"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43000010</v>
       </c>
@@ -8732,17 +8177,15 @@
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4" t="s">
+      <c r="Q12" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="T12" s="4" t="s">
+      <c r="R12" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U12" s="17"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S12" s="17"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43000011</v>
       </c>
@@ -8783,17 +8226,15 @@
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4" t="s">
+      <c r="Q13" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="T13" s="4" t="s">
+      <c r="R13" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U13" s="17"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S13" s="17"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43000012</v>
       </c>
@@ -8834,17 +8275,15 @@
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4" t="s">
+      <c r="Q14" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="T14" s="4" t="s">
+      <c r="R14" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U14" s="17"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S14" s="17"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43000013</v>
       </c>
@@ -8885,17 +8324,15 @@
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4" t="s">
+      <c r="Q15" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="T15" s="4" t="s">
+      <c r="R15" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U15" s="17"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S15" s="17"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43000014</v>
       </c>
@@ -8936,17 +8373,15 @@
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4" t="s">
+      <c r="Q16" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="T16" s="4" t="s">
+      <c r="R16" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="17"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S16" s="17"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43000015</v>
       </c>
@@ -8987,17 +8422,15 @@
       </c>
       <c r="O17" s="4"/>
       <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="4" t="s">
+      <c r="Q17" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="T17" s="4" t="s">
+      <c r="R17" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U17" s="17"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S17" s="17"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43000016</v>
       </c>
@@ -9038,17 +8471,15 @@
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4" t="s">
+      <c r="Q18" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="T18" s="4" t="s">
+      <c r="R18" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U18" s="17"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S18" s="17"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43000017</v>
       </c>
@@ -9089,17 +8520,15 @@
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4" t="s">
+      <c r="Q19" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="T19" s="4" t="s">
+      <c r="R19" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U19" s="17"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S19" s="17"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43000018</v>
       </c>
@@ -9140,17 +8569,15 @@
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4" t="s">
+      <c r="Q20" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="T20" s="4" t="s">
+      <c r="R20" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U20" s="17"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S20" s="17"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43000019</v>
       </c>
@@ -9191,17 +8618,15 @@
       </c>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4" t="s">
+      <c r="Q21" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="T21" s="4" t="s">
+      <c r="R21" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U21" s="17"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S21" s="17"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43000020</v>
       </c>
@@ -9242,17 +8667,15 @@
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4" t="s">
+      <c r="Q22" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="T22" s="4" t="s">
+      <c r="R22" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U22" s="17"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S22" s="17"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43000021</v>
       </c>
@@ -9293,17 +8716,15 @@
       </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4" t="s">
+      <c r="Q23" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="T23" s="4" t="s">
+      <c r="R23" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U23" s="17"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S23" s="17"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43000022</v>
       </c>
@@ -9344,17 +8765,15 @@
       </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4" t="s">
+      <c r="Q24" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="T24" s="4" t="s">
+      <c r="R24" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U24" s="17"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S24" s="17"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43000023</v>
       </c>
@@ -9395,17 +8814,15 @@
       </c>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4" t="s">
+      <c r="Q25" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="T25" s="4" t="s">
+      <c r="R25" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U25" s="17"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S25" s="17"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43000024</v>
       </c>
@@ -9446,17 +8863,15 @@
       </c>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4" t="s">
+      <c r="Q26" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="T26" s="4" t="s">
+      <c r="R26" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U26" s="17"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S26" s="17"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43000025</v>
       </c>
@@ -9497,17 +8912,15 @@
       </c>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4" t="s">
+      <c r="Q27" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="T27" s="4" t="s">
+      <c r="R27" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U27" s="17"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S27" s="17"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43000026</v>
       </c>
@@ -9548,17 +8961,15 @@
       </c>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4" t="s">
+      <c r="Q28" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="T28" s="4" t="s">
+      <c r="R28" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U28" s="17"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S28" s="17"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43000027</v>
       </c>
@@ -9599,17 +9010,15 @@
       </c>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4" t="s">
+      <c r="Q29" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="T29" s="4" t="s">
+      <c r="R29" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U29" s="17"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S29" s="17"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43000028</v>
       </c>
@@ -9650,17 +9059,15 @@
       </c>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4" t="s">
+      <c r="Q30" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="T30" s="4" t="s">
+      <c r="R30" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U30" s="17"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S30" s="17"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43000029</v>
       </c>
@@ -9701,17 +9108,15 @@
       </c>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4" t="s">
+      <c r="Q31" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="T31" s="4" t="s">
+      <c r="R31" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U31" s="17"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S31" s="17"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43000030</v>
       </c>
@@ -9752,17 +9157,15 @@
       </c>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4" t="s">
+      <c r="Q32" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="T32" s="4" t="s">
+      <c r="R32" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U32" s="17"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S32" s="17"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43000031</v>
       </c>
@@ -9803,17 +9206,15 @@
       </c>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4" t="s">
+      <c r="Q33" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="T33" s="4" t="s">
+      <c r="R33" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U33" s="17"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S33" s="17"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43000032</v>
       </c>
@@ -9854,17 +9255,15 @@
       </c>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4" t="s">
+      <c r="Q34" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="T34" s="4" t="s">
+      <c r="R34" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U34" s="17"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S34" s="17"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43000033</v>
       </c>
@@ -9905,17 +9304,15 @@
       </c>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4" t="s">
+      <c r="Q35" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="T35" s="4" t="s">
+      <c r="R35" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U35" s="17"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S35" s="17"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43000035</v>
       </c>
@@ -9956,17 +9353,15 @@
       </c>
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4" t="s">
+      <c r="Q36" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="T36" s="4" t="s">
+      <c r="R36" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U36" s="17"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S36" s="17"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43000037</v>
       </c>
@@ -10007,17 +9402,15 @@
       </c>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4" t="s">
+      <c r="Q37" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="T37" s="4" t="s">
+      <c r="R37" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U37" s="13"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S37" s="13"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43000038</v>
       </c>
@@ -10058,17 +9451,15 @@
       </c>
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
-      <c r="S38" s="4" t="s">
+      <c r="Q38" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="T38" s="4" t="s">
+      <c r="R38" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U38" s="35"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S38" s="35"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A39" s="37">
         <v>43001001</v>
       </c>
@@ -10111,17 +9502,15 @@
         <v>423</v>
       </c>
       <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4" t="s">
+      <c r="Q39" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="T39" s="6" t="s">
+      <c r="R39" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="U39" s="17"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S39" s="17"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A40" s="37">
         <v>43001002</v>
       </c>
@@ -10164,17 +9553,15 @@
         <v>426</v>
       </c>
       <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4"/>
-      <c r="S40" s="4" t="s">
+      <c r="Q40" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="T40" s="4" t="s">
+      <c r="R40" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U40" s="36"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S40" s="36"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A41" s="37">
         <v>43001003</v>
       </c>
@@ -10217,17 +9604,15 @@
         <v>263</v>
       </c>
       <c r="P41" s="4"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
-      <c r="S41" s="4" t="s">
+      <c r="Q41" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="T41" s="4" t="s">
+      <c r="R41" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U41" s="27"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S41" s="27"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A42" s="37">
         <v>43001004</v>
       </c>
@@ -10270,17 +9655,15 @@
         <v>425</v>
       </c>
       <c r="P42" s="4"/>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4"/>
-      <c r="S42" s="4" t="s">
+      <c r="Q42" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="T42" s="34" t="s">
+      <c r="R42" s="34" t="s">
         <v>424</v>
       </c>
-      <c r="U42" s="17"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S42" s="17"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A43" s="37">
         <v>43001005</v>
       </c>
@@ -10323,17 +9706,15 @@
         <v>427</v>
       </c>
       <c r="P43" s="4"/>
-      <c r="Q43" s="4"/>
-      <c r="R43" s="4"/>
-      <c r="S43" s="4" t="s">
+      <c r="Q43" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="T43" s="4" t="s">
+      <c r="R43" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U43" s="17"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S43" s="17"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A44" s="37">
         <v>43001006</v>
       </c>
@@ -10376,17 +9757,15 @@
         <v>428</v>
       </c>
       <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4" t="s">
+      <c r="Q44" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="T44" s="6" t="s">
+      <c r="R44" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="U44" s="36"/>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S44" s="36"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A45" s="38">
         <v>43002001</v>
       </c>
@@ -10427,17 +9806,15 @@
       </c>
       <c r="O45" s="27"/>
       <c r="P45" s="27"/>
-      <c r="Q45" s="27"/>
-      <c r="R45" s="27"/>
-      <c r="S45" s="4" t="s">
+      <c r="Q45" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="T45" s="27" t="s">
+      <c r="R45" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="U45" s="27"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S45" s="27"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A46" s="38">
         <v>43002002</v>
       </c>
@@ -10478,17 +9855,15 @@
       </c>
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
-      <c r="Q46" s="27"/>
-      <c r="R46" s="27"/>
-      <c r="S46" s="4" t="s">
+      <c r="Q46" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="T46" s="27" t="s">
+      <c r="R46" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="U46" s="27"/>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S46" s="27"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A47" s="38">
         <v>43002003</v>
       </c>
@@ -10529,17 +9904,15 @@
       </c>
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
-      <c r="Q47" s="27"/>
-      <c r="R47" s="27"/>
-      <c r="S47" s="4" t="s">
+      <c r="Q47" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="T47" s="27" t="s">
+      <c r="R47" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="U47" s="27"/>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S47" s="27"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A48" s="38">
         <v>43002004</v>
       </c>
@@ -10580,17 +9953,15 @@
       </c>
       <c r="O48" s="27"/>
       <c r="P48" s="27"/>
-      <c r="Q48" s="13"/>
-      <c r="R48" s="13"/>
-      <c r="S48" s="31" t="s">
+      <c r="Q48" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="T48" s="27" t="s">
+      <c r="R48" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="U48" s="27"/>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S48" s="27"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A49" s="38">
         <v>43002005</v>
       </c>
@@ -10631,17 +10002,15 @@
       </c>
       <c r="O49" s="27"/>
       <c r="P49" s="27"/>
-      <c r="Q49" s="13"/>
-      <c r="R49" s="13"/>
-      <c r="S49" s="31" t="s">
+      <c r="Q49" s="31" t="s">
         <v>343</v>
       </c>
-      <c r="T49" s="27" t="s">
+      <c r="R49" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="U49" s="27"/>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S49" s="27"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A50" s="38">
         <v>43002006</v>
       </c>
@@ -10682,50 +10051,48 @@
       </c>
       <c r="O50" s="27"/>
       <c r="P50" s="27"/>
-      <c r="Q50" s="13"/>
-      <c r="R50" s="13"/>
-      <c r="S50" s="31" t="s">
+      <c r="Q50" s="31" t="s">
         <v>344</v>
       </c>
-      <c r="T50" s="27" t="s">
+      <c r="R50" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="U50" s="27"/>
+      <c r="S50" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="T42">
-    <cfRule type="containsBlanks" dxfId="7" priority="9">
-      <formula>LEN(TRIM(T42))=0</formula>
+  <conditionalFormatting sqref="R42">
+    <cfRule type="containsBlanks" dxfId="6" priority="9">
+      <formula>LEN(TRIM(R42))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsBlanks" dxfId="6" priority="8">
+    <cfRule type="containsBlanks" dxfId="5" priority="8">
       <formula>LEN(TRIM(C47))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S47">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(S47))=0</formula>
+  <conditionalFormatting sqref="Q47">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
+      <formula>LEN(TRIM(Q47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C50">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="3" priority="5">
       <formula>LEN(TRIM(C48))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S48:S50">
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
-      <formula>LEN(TRIM(S48))=0</formula>
+  <conditionalFormatting sqref="Q48:Q50">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(Q48))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(K47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:K50">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(K48))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10739,13 +10106,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R1" sqref="R1"/>
+      <selection pane="bottomRight" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10759,12 +10126,11 @@
     <col min="13" max="14" width="6.125" customWidth="1"/>
     <col min="15" max="15" width="28.375" customWidth="1"/>
     <col min="16" max="16" width="19.5" customWidth="1"/>
-    <col min="17" max="18" width="9.875" customWidth="1"/>
-    <col min="20" max="20" width="10.625" customWidth="1"/>
-    <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.625" customWidth="1"/>
+    <col min="19" max="19" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>151</v>
       </c>
@@ -10813,23 +10179,17 @@
       <c r="P1" s="25" t="s">
         <v>238</v>
       </c>
-      <c r="Q1" s="25" t="s">
-        <v>429</v>
+      <c r="Q1" s="26" t="s">
+        <v>159</v>
       </c>
       <c r="R1" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="S1" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="T1" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="S1" s="25" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>149</v>
       </c>
@@ -10878,23 +10238,17 @@
       <c r="P2" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="Q2" s="8" t="s">
-        <v>231</v>
+      <c r="Q2" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="T2" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>160</v>
       </c>
@@ -10944,22 +10298,16 @@
         <v>186</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>432</v>
+        <v>168</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="T3" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="U3" s="18" t="s">
+      <c r="S3" s="18" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43010001</v>
       </c>
@@ -11000,17 +10348,15 @@
         <v>243</v>
       </c>
       <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U4" s="15"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S4" s="15"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43010002</v>
       </c>
@@ -11049,17 +10395,15 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U5" s="14"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S5" s="14"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43010003</v>
       </c>
@@ -11098,17 +10442,15 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="T6" s="4" t="s">
+      <c r="R6" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U6" s="14"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S6" s="14"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43010004</v>
       </c>
@@ -11147,17 +10489,15 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="T7" s="4" t="s">
+      <c r="R7" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U7" s="14"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S7" s="14"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43010005</v>
       </c>
@@ -11198,17 +10538,15 @@
         <v>244</v>
       </c>
       <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="6" t="s">
+      <c r="Q8" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="T8" s="4" t="s">
+      <c r="R8" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U8" s="14"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S8" s="14"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43010006</v>
       </c>
@@ -11249,17 +10587,15 @@
         <v>245</v>
       </c>
       <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="6" t="s">
+      <c r="Q9" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="R9" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U9" s="14"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S9" s="14"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43010101</v>
       </c>
@@ -11296,17 +10632,15 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="T10" s="4" t="s">
+      <c r="R10" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U10" s="14"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S10" s="14"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43010102</v>
       </c>
@@ -11343,17 +10677,15 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="R11" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U11" s="14"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S11" s="14"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43010103</v>
       </c>
@@ -11390,17 +10722,15 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4" t="s">
+      <c r="Q12" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="T12" s="4" t="s">
+      <c r="R12" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U12" s="14"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S12" s="14"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43010104</v>
       </c>
@@ -11437,17 +10767,15 @@
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4" t="s">
+      <c r="Q13" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="T13" s="4" t="s">
+      <c r="R13" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U13" s="14"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="S13" s="14"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43010105</v>
       </c>
@@ -11484,15 +10812,13 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4" t="s">
+      <c r="Q14" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="T14" s="4" t="s">
+      <c r="R14" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U14" s="14"/>
+      <c r="S14" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
new func of quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3D329967-7B7A-4123-A98A-FD60A2968191}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0DD7E68D-78DB-4088-9E3B-834617644058}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="437">
   <si>
     <t>老鼠</t>
   </si>
@@ -1461,9 +1461,6 @@
   </si>
   <si>
     <t>结识：击败</t>
-  </si>
-  <si>
-    <t>结识：击败</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1472,13 +1469,26 @@
   </si>
   <si>
     <t>RivalDefeat</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>赛尼斯</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>结识：任务</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiaqia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RivalQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>RivalDefeat</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>赛尼斯</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2414,7 +2424,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="100">
+  <dxfs count="103">
     <dxf>
       <font>
         <b val="0"/>
@@ -2873,6 +2883,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -3483,6 +3522,25 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -4057,6 +4115,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -4553,93 +4640,96 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2_4" displayName="表2_4" ref="A3:T51" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98" tableBorderDxfId="97">
-  <autoFilter ref="A3:T51" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState ref="A4:T50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2_4" displayName="表2_4" ref="A3:U51" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101" tableBorderDxfId="100">
+  <autoFilter ref="A3:U51" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState ref="A4:U50">
     <sortCondition ref="A3:A50"/>
   </sortState>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="96"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="95"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Ename" dataDxfId="94"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="93"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Quality" dataDxfId="92"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="World" dataDxfId="91"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Job" dataDxfId="90"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Level" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="AutoAddLevel" dataDxfId="88"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Method" dataDxfId="87"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Emethod" dataDxfId="86"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="KingTowerId" dataDxfId="85"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="EpRecoverRate" dataDxfId="84"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="CardReduce" dataDxfId="83"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="RightMon" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="PetMon" dataDxfId="81"/>
-    <tableColumn id="7" xr3:uid="{1D7F579A-8D29-4340-99EB-C9106F5EEBF1}" name="RivalDefeat" dataDxfId="33"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Figue" dataDxfId="80"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BattleMap" dataDxfId="79"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="InRandomQuest" dataDxfId="78"/>
+  <tableColumns count="21">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="98"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Ename" dataDxfId="97"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="96"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Quality" dataDxfId="95"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="World" dataDxfId="94"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Job" dataDxfId="93"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Level" dataDxfId="92"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="AutoAddLevel" dataDxfId="91"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Method" dataDxfId="90"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Emethod" dataDxfId="89"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="KingTowerId" dataDxfId="88"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="EpRecoverRate" dataDxfId="87"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="CardReduce" dataDxfId="86"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="RightMon" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="PetMon" dataDxfId="84"/>
+    <tableColumn id="7" xr3:uid="{1D7F579A-8D29-4340-99EB-C9106F5EEBF1}" name="RivalDefeat" dataDxfId="83"/>
+    <tableColumn id="8" xr3:uid="{C3570C71-FFB0-4A70-A97D-D30B4B61E1E8}" name="RivalQuest" dataDxfId="33"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Figue" dataDxfId="82"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BattleMap" dataDxfId="81"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="InRandomQuest" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表2" displayName="表2" ref="A3:T50" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75">
-  <autoFilter ref="A3:T50" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState ref="A4:T50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表2" displayName="表2" ref="A3:U50" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" tableBorderDxfId="77">
+  <autoFilter ref="A3:U50" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState ref="A4:U50">
     <sortCondition ref="A3:A50"/>
   </sortState>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="73"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Ename" dataDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Quality" dataDxfId="70"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="World" dataDxfId="69"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Job" dataDxfId="68"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Level" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="AutoAddLevel" dataDxfId="66"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Method" dataDxfId="65"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Emethod" dataDxfId="64"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="KingTowerId" dataDxfId="63"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="EpRecoverRate" dataDxfId="62"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="CardReduce" dataDxfId="61"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="RightMon" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PetMon" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{CE1793B8-6380-4459-BED9-CDFF98B47C07}" name="RivalDefeat" dataDxfId="32"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Figue" dataDxfId="58"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BattleMap" dataDxfId="57"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="InRandomQuest" dataDxfId="56"/>
+  <tableColumns count="21">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="75"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Ename" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Quality" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="World" dataDxfId="71"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Job" dataDxfId="70"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Level" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="AutoAddLevel" dataDxfId="68"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Method" dataDxfId="67"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Emethod" dataDxfId="66"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="KingTowerId" dataDxfId="65"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="EpRecoverRate" dataDxfId="64"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="CardReduce" dataDxfId="63"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="RightMon" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PetMon" dataDxfId="61"/>
+    <tableColumn id="8" xr3:uid="{CE1793B8-6380-4459-BED9-CDFF98B47C07}" name="RivalDefeat" dataDxfId="60"/>
+    <tableColumn id="21" xr3:uid="{2DA56599-F82F-42E1-A946-1E928F1DEA73}" name="RivalQuest" dataDxfId="32"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Figue" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BattleMap" dataDxfId="58"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="InRandomQuest" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表2_2" displayName="表2_2" ref="A3:T14" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53">
-  <autoFilter ref="A3:T14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A4:S83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表2_2" displayName="表2_2" ref="A3:U14" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
+  <autoFilter ref="A3:U14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A4:T83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="51"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Ename" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type" dataDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Quality" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="World" dataDxfId="47"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Job" dataDxfId="46"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Level" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="AutoAddLevel" dataDxfId="44"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Method" dataDxfId="43"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Emethod" dataDxfId="42"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="KingTowerId" dataDxfId="41"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="EpRecoverRate" dataDxfId="40"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="CardReduce" dataDxfId="39"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="RightMon" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="PetMon" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{2FC8C9B2-866B-4CC7-9861-C44D809107E9}" name="RivalDefeat" dataDxfId="0"/>
+  <tableColumns count="21">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="52"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Ename" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Quality" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="World" dataDxfId="48"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Job" dataDxfId="47"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Level" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="AutoAddLevel" dataDxfId="45"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Method" dataDxfId="44"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Emethod" dataDxfId="43"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="KingTowerId" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="EpRecoverRate" dataDxfId="41"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="CardReduce" dataDxfId="40"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="RightMon" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="PetMon" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{2FC8C9B2-866B-4CC7-9861-C44D809107E9}" name="RivalDefeat" dataDxfId="37"/>
+    <tableColumn id="21" xr3:uid="{4A49EC52-110E-429E-B5C1-90836365D98D}" name="RivalQuest" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Figue" dataDxfId="36"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="BattleMap" dataDxfId="35"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="InRandomQuest" dataDxfId="34"/>
@@ -4969,13 +5059,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T51"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4987,11 +5077,11 @@
     <col min="10" max="10" width="9.5" customWidth="1"/>
     <col min="11" max="12" width="10.625" customWidth="1"/>
     <col min="13" max="16" width="5.875" customWidth="1"/>
-    <col min="17" max="17" width="8.875" customWidth="1"/>
-    <col min="19" max="19" width="10.625" customWidth="1"/>
+    <col min="17" max="18" width="8.875" customWidth="1"/>
+    <col min="20" max="20" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" ht="72" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>150</v>
       </c>
@@ -5041,19 +5131,22 @@
         <v>238</v>
       </c>
       <c r="Q1" s="39" t="s">
-        <v>430</v>
-      </c>
-      <c r="R1" s="23" t="s">
+        <v>429</v>
+      </c>
+      <c r="R1" s="39" t="s">
+        <v>433</v>
+      </c>
+      <c r="S1" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>148</v>
       </c>
@@ -5103,19 +5196,22 @@
         <v>168</v>
       </c>
       <c r="Q2" s="40" t="s">
-        <v>431</v>
-      </c>
-      <c r="R2" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="R2" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="3" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>159</v>
       </c>
@@ -5165,24 +5261,27 @@
         <v>239</v>
       </c>
       <c r="Q3" s="41" t="s">
-        <v>433</v>
-      </c>
-      <c r="R3" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="R3" s="41" t="s">
+        <v>435</v>
+      </c>
+      <c r="S3" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43020101</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>221</v>
@@ -5217,15 +5316,16 @@
       <c r="Q4" s="4">
         <v>1</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="4"/>
+      <c r="S4" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T4" s="19"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U4" s="19"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43020102</v>
       </c>
@@ -5264,14 +5364,17 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="S5" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T5" s="19"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U5" s="19"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43020103</v>
       </c>
@@ -5311,17 +5414,18 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="4" t="s">
+      <c r="R6" s="4"/>
+      <c r="S6" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="T6" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T6" s="19" t="s">
+      <c r="U6" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43020104</v>
       </c>
@@ -5361,15 +5465,16 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="4"/>
+      <c r="S7" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="S7" s="4" t="s">
+      <c r="T7" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T7" s="19"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U7" s="19"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43020105</v>
       </c>
@@ -5409,17 +5514,18 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-      <c r="R8" s="4" t="s">
+      <c r="R8" s="4"/>
+      <c r="S8" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="T8" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T8" s="19" t="s">
+      <c r="U8" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43020106</v>
       </c>
@@ -5459,17 +5565,18 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="4"/>
+      <c r="S9" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="T9" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T9" s="19" t="s">
+      <c r="U9" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43020107</v>
       </c>
@@ -5509,17 +5616,18 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-      <c r="R10" s="4" t="s">
+      <c r="R10" s="4"/>
+      <c r="S10" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="S10" s="4" t="s">
+      <c r="T10" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T10" s="19" t="s">
+      <c r="U10" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43020108</v>
       </c>
@@ -5559,17 +5667,18 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="4"/>
+      <c r="S11" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="T11" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T11" s="19" t="s">
+      <c r="U11" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43020109</v>
       </c>
@@ -5609,17 +5718,18 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-      <c r="R12" s="4" t="s">
+      <c r="R12" s="4"/>
+      <c r="S12" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="S12" s="4" t="s">
+      <c r="T12" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T12" s="19" t="s">
+      <c r="U12" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43020110</v>
       </c>
@@ -5659,17 +5769,18 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="4" t="s">
+      <c r="R13" s="4"/>
+      <c r="S13" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="S13" s="4" t="s">
+      <c r="T13" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T13" s="19" t="s">
+      <c r="U13" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43020201</v>
       </c>
@@ -5709,17 +5820,18 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-      <c r="R14" s="4" t="s">
+      <c r="R14" s="4"/>
+      <c r="S14" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="S14" s="4" t="s">
+      <c r="T14" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T14" s="19" t="s">
+      <c r="U14" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43020202</v>
       </c>
@@ -5759,17 +5871,18 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
-      <c r="R15" s="4" t="s">
+      <c r="R15" s="4"/>
+      <c r="S15" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="S15" s="4" t="s">
+      <c r="T15" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T15" s="19" t="s">
+      <c r="U15" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43020203</v>
       </c>
@@ -5809,17 +5922,18 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-      <c r="R16" s="4" t="s">
+      <c r="R16" s="4"/>
+      <c r="S16" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="S16" s="4" t="s">
+      <c r="T16" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T16" s="19" t="s">
+      <c r="U16" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43020204</v>
       </c>
@@ -5859,17 +5973,18 @@
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
-      <c r="R17" s="4" t="s">
+      <c r="R17" s="4"/>
+      <c r="S17" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="S17" s="4" t="s">
+      <c r="T17" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T17" s="19" t="s">
+      <c r="U17" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43020205</v>
       </c>
@@ -5907,17 +6022,18 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-      <c r="R18" s="4" t="s">
+      <c r="R18" s="4"/>
+      <c r="S18" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="S18" s="4" t="s">
+      <c r="T18" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T18" s="19" t="s">
+      <c r="U18" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43020206</v>
       </c>
@@ -5957,17 +6073,18 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
-      <c r="R19" s="4" t="s">
+      <c r="R19" s="4"/>
+      <c r="S19" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="S19" s="4" t="s">
+      <c r="T19" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T19" s="19" t="s">
+      <c r="U19" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43020207</v>
       </c>
@@ -6007,17 +6124,18 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
-      <c r="R20" s="4" t="s">
+      <c r="R20" s="4"/>
+      <c r="S20" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="S20" s="4" t="s">
+      <c r="T20" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T20" s="19" t="s">
+      <c r="U20" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43020301</v>
       </c>
@@ -6057,17 +6175,18 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
-      <c r="R21" s="4" t="s">
+      <c r="R21" s="4"/>
+      <c r="S21" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="S21" s="4" t="s">
+      <c r="T21" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T21" s="19" t="s">
+      <c r="U21" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43020302</v>
       </c>
@@ -6107,17 +6226,18 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
-      <c r="R22" s="4" t="s">
+      <c r="R22" s="4"/>
+      <c r="S22" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="S22" s="4" t="s">
+      <c r="T22" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T22" s="19" t="s">
+      <c r="U22" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43020303</v>
       </c>
@@ -6155,17 +6275,18 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
-      <c r="R23" s="4" t="s">
+      <c r="R23" s="4"/>
+      <c r="S23" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="S23" s="4" t="s">
+      <c r="T23" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T23" s="19" t="s">
+      <c r="U23" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43020304</v>
       </c>
@@ -6205,17 +6326,18 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
-      <c r="R24" s="4" t="s">
+      <c r="R24" s="4"/>
+      <c r="S24" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="S24" s="4" t="s">
+      <c r="T24" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T24" s="19" t="s">
+      <c r="U24" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43020305</v>
       </c>
@@ -6255,17 +6377,18 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
-      <c r="R25" s="4" t="s">
+      <c r="R25" s="4"/>
+      <c r="S25" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="S25" s="4" t="s">
+      <c r="T25" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T25" s="19" t="s">
+      <c r="U25" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43020306</v>
       </c>
@@ -6305,17 +6428,18 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
-      <c r="R26" s="4" t="s">
+      <c r="R26" s="4"/>
+      <c r="S26" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="S26" s="4" t="s">
+      <c r="T26" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T26" s="19" t="s">
+      <c r="U26" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43020307</v>
       </c>
@@ -6355,17 +6479,18 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
-      <c r="R27" s="4" t="s">
+      <c r="R27" s="4"/>
+      <c r="S27" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="S27" s="4" t="s">
+      <c r="T27" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T27" s="19" t="s">
+      <c r="U27" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43020308</v>
       </c>
@@ -6405,17 +6530,18 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
-      <c r="R28" s="4" t="s">
+      <c r="R28" s="4"/>
+      <c r="S28" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="S28" s="4" t="s">
+      <c r="T28" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T28" s="19" t="s">
+      <c r="U28" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43020309</v>
       </c>
@@ -6455,17 +6581,18 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
-      <c r="R29" s="4" t="s">
+      <c r="R29" s="4"/>
+      <c r="S29" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="S29" s="4" t="s">
+      <c r="T29" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T29" s="19" t="s">
+      <c r="U29" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43020310</v>
       </c>
@@ -6505,17 +6632,18 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
-      <c r="R30" s="4" t="s">
+      <c r="R30" s="4"/>
+      <c r="S30" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="S30" s="4" t="s">
+      <c r="T30" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T30" s="19" t="s">
+      <c r="U30" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43020311</v>
       </c>
@@ -6555,17 +6683,18 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
-      <c r="R31" s="4" t="s">
+      <c r="R31" s="4"/>
+      <c r="S31" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="S31" s="4" t="s">
+      <c r="T31" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T31" s="19" t="s">
+      <c r="U31" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43020312</v>
       </c>
@@ -6605,17 +6734,18 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
-      <c r="R32" s="4" t="s">
+      <c r="R32" s="4"/>
+      <c r="S32" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="S32" s="4" t="s">
+      <c r="T32" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T32" s="19" t="s">
+      <c r="U32" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43020401</v>
       </c>
@@ -6655,17 +6785,18 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
-      <c r="R33" s="4" t="s">
+      <c r="R33" s="4"/>
+      <c r="S33" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="S33" s="4" t="s">
+      <c r="T33" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T33" s="19" t="s">
+      <c r="U33" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43020402</v>
       </c>
@@ -6705,17 +6836,18 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
-      <c r="R34" s="4" t="s">
+      <c r="R34" s="4"/>
+      <c r="S34" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="S34" s="4" t="s">
+      <c r="T34" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T34" s="19" t="s">
+      <c r="U34" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43020403</v>
       </c>
@@ -6755,17 +6887,18 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
-      <c r="R35" s="4" t="s">
+      <c r="R35" s="4"/>
+      <c r="S35" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="S35" s="4" t="s">
+      <c r="T35" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T35" s="19" t="s">
+      <c r="U35" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43020404</v>
       </c>
@@ -6805,17 +6938,18 @@
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
-      <c r="R36" s="4" t="s">
+      <c r="R36" s="4"/>
+      <c r="S36" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="S36" s="4" t="s">
+      <c r="T36" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T36" s="19" t="s">
+      <c r="U36" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43020405</v>
       </c>
@@ -6855,17 +6989,18 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
-      <c r="R37" s="4" t="s">
+      <c r="R37" s="4"/>
+      <c r="S37" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="S37" s="4" t="s">
+      <c r="T37" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T37" s="19" t="s">
+      <c r="U37" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43020406</v>
       </c>
@@ -6905,17 +7040,18 @@
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
-      <c r="R38" s="4" t="s">
+      <c r="R38" s="4"/>
+      <c r="S38" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="S38" s="4" t="s">
+      <c r="T38" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T38" s="19" t="s">
+      <c r="U38" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>43020407</v>
       </c>
@@ -6955,17 +7091,18 @@
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
-      <c r="R39" s="4" t="s">
+      <c r="R39" s="4"/>
+      <c r="S39" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="S39" s="4" t="s">
+      <c r="T39" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T39" s="19" t="s">
+      <c r="U39" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>43020408</v>
       </c>
@@ -7005,17 +7142,18 @@
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
-      <c r="R40" s="4" t="s">
+      <c r="R40" s="4"/>
+      <c r="S40" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="S40" s="4" t="s">
+      <c r="T40" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T40" s="19" t="s">
+      <c r="U40" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>43020409</v>
       </c>
@@ -7055,17 +7193,18 @@
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
-      <c r="R41" s="4" t="s">
+      <c r="R41" s="4"/>
+      <c r="S41" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="S41" s="4" t="s">
+      <c r="T41" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T41" s="19" t="s">
+      <c r="U41" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>43020501</v>
       </c>
@@ -7105,17 +7244,18 @@
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
-      <c r="R42" s="4" t="s">
+      <c r="R42" s="4"/>
+      <c r="S42" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="S42" s="4" t="s">
+      <c r="T42" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T42" s="19" t="s">
+      <c r="U42" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>43020502</v>
       </c>
@@ -7155,17 +7295,18 @@
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
-      <c r="R43" s="4" t="s">
+      <c r="R43" s="4"/>
+      <c r="S43" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="S43" s="4" t="s">
+      <c r="T43" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T43" s="19" t="s">
+      <c r="U43" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43020503</v>
       </c>
@@ -7205,17 +7346,18 @@
       <c r="O44" s="4"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
-      <c r="R44" s="4" t="s">
+      <c r="R44" s="4"/>
+      <c r="S44" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="S44" s="4" t="s">
+      <c r="T44" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T44" s="19" t="s">
+      <c r="U44" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>43020504</v>
       </c>
@@ -7255,17 +7397,18 @@
       <c r="O45" s="4"/>
       <c r="P45" s="4"/>
       <c r="Q45" s="4"/>
-      <c r="R45" s="4" t="s">
+      <c r="R45" s="4"/>
+      <c r="S45" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="S45" s="4" t="s">
+      <c r="T45" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T45" s="19" t="s">
+      <c r="U45" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>43020505</v>
       </c>
@@ -7305,17 +7448,18 @@
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
       <c r="Q46" s="27"/>
-      <c r="R46" s="27" t="s">
+      <c r="R46" s="27"/>
+      <c r="S46" s="27" t="s">
         <v>409</v>
       </c>
-      <c r="S46" s="4" t="s">
+      <c r="T46" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T46" s="19" t="s">
+      <c r="U46" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>43020506</v>
       </c>
@@ -7355,17 +7499,18 @@
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
       <c r="Q47" s="27"/>
-      <c r="R47" s="27" t="s">
+      <c r="R47" s="27"/>
+      <c r="S47" s="27" t="s">
         <v>408</v>
       </c>
-      <c r="S47" s="4" t="s">
+      <c r="T47" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T47" s="19" t="s">
+      <c r="U47" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>43020601</v>
       </c>
@@ -7405,17 +7550,18 @@
       <c r="O48" s="4"/>
       <c r="P48" s="4"/>
       <c r="Q48" s="4"/>
-      <c r="R48" s="4" t="s">
+      <c r="R48" s="4"/>
+      <c r="S48" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="S48" s="4" t="s">
+      <c r="T48" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T48" s="19" t="s">
+      <c r="U48" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>43020602</v>
       </c>
@@ -7453,17 +7599,18 @@
       <c r="O49" s="4"/>
       <c r="P49" s="4"/>
       <c r="Q49" s="4"/>
-      <c r="R49" s="4" t="s">
+      <c r="R49" s="4"/>
+      <c r="S49" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="S49" s="4" t="s">
+      <c r="T49" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T49" s="19" t="s">
+      <c r="U49" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>43020603</v>
       </c>
@@ -7501,17 +7648,18 @@
       <c r="O50" s="4"/>
       <c r="P50" s="4"/>
       <c r="Q50" s="4"/>
-      <c r="R50" s="4" t="s">
+      <c r="R50" s="4"/>
+      <c r="S50" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="S50" s="4" t="s">
+      <c r="T50" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T50" s="19" t="s">
+      <c r="U50" s="19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>43020604</v>
       </c>
@@ -7551,13 +7699,14 @@
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
       <c r="Q51" s="4"/>
-      <c r="R51" s="4" t="s">
+      <c r="R51" s="4"/>
+      <c r="S51" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="S51" s="4" t="s">
+      <c r="T51" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="T51" s="19" t="s">
+      <c r="U51" s="19" t="s">
         <v>207</v>
       </c>
     </row>
@@ -7657,7 +7806,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T50"/>
+  <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
@@ -7676,12 +7825,12 @@
     <col min="11" max="12" width="10.625" customWidth="1"/>
     <col min="13" max="14" width="6.125" customWidth="1"/>
     <col min="15" max="16" width="27.125" customWidth="1"/>
-    <col min="17" max="17" width="10.875" customWidth="1"/>
-    <col min="19" max="19" width="10.625" customWidth="1"/>
-    <col min="20" max="20" width="8" customWidth="1"/>
+    <col min="17" max="18" width="10.875" customWidth="1"/>
+    <col min="20" max="20" width="10.625" customWidth="1"/>
+    <col min="21" max="21" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>150</v>
       </c>
@@ -7730,20 +7879,23 @@
       <c r="P1" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="Q1" s="11" t="s">
-        <v>430</v>
-      </c>
-      <c r="R1" s="23" t="s">
+      <c r="Q1" s="39" t="s">
+        <v>429</v>
+      </c>
+      <c r="R1" s="39" t="s">
+        <v>433</v>
+      </c>
+      <c r="S1" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>148</v>
       </c>
@@ -7792,20 +7944,23 @@
       <c r="P2" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="R2" s="3" t="s">
+      <c r="Q2" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="R2" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>159</v>
       </c>
@@ -7854,20 +8009,23 @@
       <c r="P3" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="Q3" s="5" t="s">
-        <v>433</v>
-      </c>
-      <c r="R3" s="5" t="s">
+      <c r="Q3" s="41" t="s">
+        <v>436</v>
+      </c>
+      <c r="R3" s="41" t="s">
+        <v>435</v>
+      </c>
+      <c r="S3" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43000001</v>
       </c>
@@ -7909,15 +8067,16 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="4"/>
+      <c r="S4" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="T4" s="17"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U4" s="17"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43000002</v>
       </c>
@@ -7959,15 +8118,16 @@
       <c r="O5" s="4"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="6"/>
+      <c r="S5" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="T5" s="17"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U5" s="17"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43000003</v>
       </c>
@@ -8009,15 +8169,16 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="4" t="s">
+      <c r="R6" s="4"/>
+      <c r="S6" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="T6" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T6" s="17"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U6" s="17"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43000004</v>
       </c>
@@ -8059,15 +8220,16 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="4"/>
+      <c r="S7" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="S7" s="4" t="s">
+      <c r="T7" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T7" s="17"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U7" s="17"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43000005</v>
       </c>
@@ -8109,15 +8271,16 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-      <c r="R8" s="4" t="s">
+      <c r="R8" s="4"/>
+      <c r="S8" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="T8" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T8" s="17"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U8" s="17"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43000007</v>
       </c>
@@ -8159,15 +8322,16 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="4"/>
+      <c r="S9" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="T9" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="T9" s="17"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U9" s="17"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43000008</v>
       </c>
@@ -8209,15 +8373,16 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-      <c r="R10" s="4" t="s">
+      <c r="R10" s="4"/>
+      <c r="S10" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="S10" s="4" t="s">
+      <c r="T10" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T10" s="17"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U10" s="17"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43000009</v>
       </c>
@@ -8259,15 +8424,16 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="4"/>
+      <c r="S11" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="T11" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T11" s="17"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U11" s="17"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43000010</v>
       </c>
@@ -8309,15 +8475,16 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-      <c r="R12" s="4" t="s">
+      <c r="R12" s="4"/>
+      <c r="S12" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="S12" s="4" t="s">
+      <c r="T12" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T12" s="17"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U12" s="17"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43000011</v>
       </c>
@@ -8359,15 +8526,16 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="4" t="s">
+      <c r="R13" s="4"/>
+      <c r="S13" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="S13" s="4" t="s">
+      <c r="T13" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T13" s="17"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U13" s="17"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43000012</v>
       </c>
@@ -8409,15 +8577,16 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-      <c r="R14" s="4" t="s">
+      <c r="R14" s="4"/>
+      <c r="S14" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="S14" s="4" t="s">
+      <c r="T14" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T14" s="17"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U14" s="17"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43000013</v>
       </c>
@@ -8459,15 +8628,16 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
-      <c r="R15" s="4" t="s">
+      <c r="R15" s="4"/>
+      <c r="S15" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="S15" s="4" t="s">
+      <c r="T15" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T15" s="17"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U15" s="17"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43000014</v>
       </c>
@@ -8509,15 +8679,16 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-      <c r="R16" s="4" t="s">
+      <c r="R16" s="4"/>
+      <c r="S16" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="S16" s="4" t="s">
+      <c r="T16" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T16" s="17"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U16" s="17"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43000015</v>
       </c>
@@ -8559,15 +8730,16 @@
       <c r="O17" s="4"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
-      <c r="R17" s="4" t="s">
+      <c r="R17" s="6"/>
+      <c r="S17" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="S17" s="4" t="s">
+      <c r="T17" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T17" s="17"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U17" s="17"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43000016</v>
       </c>
@@ -8609,15 +8781,16 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-      <c r="R18" s="4" t="s">
+      <c r="R18" s="4"/>
+      <c r="S18" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="S18" s="4" t="s">
+      <c r="T18" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T18" s="17"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U18" s="17"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43000017</v>
       </c>
@@ -8659,15 +8832,16 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
-      <c r="R19" s="4" t="s">
+      <c r="R19" s="4"/>
+      <c r="S19" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="S19" s="4" t="s">
+      <c r="T19" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T19" s="17"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U19" s="17"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43000018</v>
       </c>
@@ -8709,15 +8883,16 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
-      <c r="R20" s="4" t="s">
+      <c r="R20" s="4"/>
+      <c r="S20" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="S20" s="4" t="s">
+      <c r="T20" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T20" s="17"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U20" s="17"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43000019</v>
       </c>
@@ -8759,15 +8934,16 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
-      <c r="R21" s="4" t="s">
+      <c r="R21" s="4"/>
+      <c r="S21" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="S21" s="4" t="s">
+      <c r="T21" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T21" s="17"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U21" s="17"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43000020</v>
       </c>
@@ -8809,15 +8985,16 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
-      <c r="R22" s="4" t="s">
+      <c r="R22" s="4"/>
+      <c r="S22" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="S22" s="4" t="s">
+      <c r="T22" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T22" s="17"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U22" s="17"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43000021</v>
       </c>
@@ -8859,15 +9036,16 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
-      <c r="R23" s="4" t="s">
+      <c r="R23" s="4"/>
+      <c r="S23" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="S23" s="4" t="s">
+      <c r="T23" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T23" s="17"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U23" s="17"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43000022</v>
       </c>
@@ -8909,15 +9087,16 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
-      <c r="R24" s="4" t="s">
+      <c r="R24" s="4"/>
+      <c r="S24" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="S24" s="4" t="s">
+      <c r="T24" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T24" s="17"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U24" s="17"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43000023</v>
       </c>
@@ -8959,15 +9138,16 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
-      <c r="R25" s="4" t="s">
+      <c r="R25" s="4"/>
+      <c r="S25" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="S25" s="4" t="s">
+      <c r="T25" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T25" s="17"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U25" s="17"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43000024</v>
       </c>
@@ -9009,15 +9189,16 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
-      <c r="R26" s="4" t="s">
+      <c r="R26" s="4"/>
+      <c r="S26" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="S26" s="4" t="s">
+      <c r="T26" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T26" s="17"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U26" s="17"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43000025</v>
       </c>
@@ -9059,15 +9240,16 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
-      <c r="R27" s="4" t="s">
+      <c r="R27" s="4"/>
+      <c r="S27" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="S27" s="4" t="s">
+      <c r="T27" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T27" s="17"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U27" s="17"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43000026</v>
       </c>
@@ -9109,15 +9291,16 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
-      <c r="R28" s="4" t="s">
+      <c r="R28" s="4"/>
+      <c r="S28" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="S28" s="4" t="s">
+      <c r="T28" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T28" s="17"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U28" s="17"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43000027</v>
       </c>
@@ -9159,15 +9342,16 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
-      <c r="R29" s="4" t="s">
+      <c r="R29" s="4"/>
+      <c r="S29" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="S29" s="4" t="s">
+      <c r="T29" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T29" s="17"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U29" s="17"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43000028</v>
       </c>
@@ -9209,15 +9393,16 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
-      <c r="R30" s="4" t="s">
+      <c r="R30" s="4"/>
+      <c r="S30" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="S30" s="4" t="s">
+      <c r="T30" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T30" s="17"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U30" s="17"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43000029</v>
       </c>
@@ -9259,15 +9444,16 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
-      <c r="R31" s="4" t="s">
+      <c r="R31" s="4"/>
+      <c r="S31" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="S31" s="4" t="s">
+      <c r="T31" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T31" s="17"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U31" s="17"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43000030</v>
       </c>
@@ -9309,15 +9495,16 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
-      <c r="R32" s="4" t="s">
+      <c r="R32" s="4"/>
+      <c r="S32" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="S32" s="4" t="s">
+      <c r="T32" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T32" s="17"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U32" s="17"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43000031</v>
       </c>
@@ -9359,15 +9546,16 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
-      <c r="R33" s="4" t="s">
+      <c r="R33" s="4"/>
+      <c r="S33" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="S33" s="4" t="s">
+      <c r="T33" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T33" s="17"/>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U33" s="17"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43000032</v>
       </c>
@@ -9409,15 +9597,16 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
-      <c r="R34" s="4" t="s">
+      <c r="R34" s="4"/>
+      <c r="S34" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="S34" s="4" t="s">
+      <c r="T34" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T34" s="17"/>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U34" s="17"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43000033</v>
       </c>
@@ -9459,15 +9648,16 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
-      <c r="R35" s="4" t="s">
+      <c r="R35" s="4"/>
+      <c r="S35" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="S35" s="4" t="s">
+      <c r="T35" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T35" s="17"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U35" s="17"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43000035</v>
       </c>
@@ -9509,15 +9699,16 @@
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
-      <c r="R36" s="4" t="s">
+      <c r="R36" s="4"/>
+      <c r="S36" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="S36" s="4" t="s">
+      <c r="T36" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T36" s="17"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U36" s="17"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43000037</v>
       </c>
@@ -9559,15 +9750,16 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
-      <c r="R37" s="4" t="s">
+      <c r="R37" s="4"/>
+      <c r="S37" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="S37" s="4" t="s">
+      <c r="T37" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T37" s="13"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U37" s="13"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43000038</v>
       </c>
@@ -9609,15 +9801,16 @@
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
-      <c r="R38" s="4" t="s">
+      <c r="R38" s="4"/>
+      <c r="S38" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="S38" s="4" t="s">
+      <c r="T38" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T38" s="35"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U38" s="35"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A39" s="37">
         <v>43001001</v>
       </c>
@@ -9661,15 +9854,16 @@
       </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
-      <c r="R39" s="4" t="s">
+      <c r="R39" s="4"/>
+      <c r="S39" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="S39" s="6" t="s">
+      <c r="T39" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="T39" s="17"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U39" s="17"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A40" s="37">
         <v>43001002</v>
       </c>
@@ -9713,15 +9907,16 @@
       </c>
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
-      <c r="R40" s="4" t="s">
+      <c r="R40" s="4"/>
+      <c r="S40" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="S40" s="4" t="s">
+      <c r="T40" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T40" s="36"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U40" s="36"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A41" s="37">
         <v>43001003</v>
       </c>
@@ -9765,15 +9960,16 @@
       </c>
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
-      <c r="R41" s="4" t="s">
+      <c r="R41" s="4"/>
+      <c r="S41" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="S41" s="4" t="s">
+      <c r="T41" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T41" s="27"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U41" s="27"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A42" s="37">
         <v>43001004</v>
       </c>
@@ -9817,15 +10013,16 @@
       </c>
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
-      <c r="R42" s="4" t="s">
+      <c r="R42" s="4"/>
+      <c r="S42" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="S42" s="34" t="s">
+      <c r="T42" s="34" t="s">
         <v>423</v>
       </c>
-      <c r="T42" s="17"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U42" s="17"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A43" s="37">
         <v>43001005</v>
       </c>
@@ -9869,15 +10066,16 @@
       </c>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
-      <c r="R43" s="4" t="s">
+      <c r="R43" s="4"/>
+      <c r="S43" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="S43" s="4" t="s">
+      <c r="T43" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T43" s="17"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U43" s="17"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A44" s="37">
         <v>43001006</v>
       </c>
@@ -9921,15 +10119,16 @@
       </c>
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
-      <c r="R44" s="4" t="s">
+      <c r="R44" s="4"/>
+      <c r="S44" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="S44" s="6" t="s">
+      <c r="T44" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="T44" s="36"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U44" s="36"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A45" s="38">
         <v>43002001</v>
       </c>
@@ -9971,15 +10170,16 @@
       <c r="O45" s="27"/>
       <c r="P45" s="27"/>
       <c r="Q45" s="27"/>
-      <c r="R45" s="4" t="s">
+      <c r="R45" s="27"/>
+      <c r="S45" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="S45" s="27" t="s">
+      <c r="T45" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="T45" s="27"/>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U45" s="27"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A46" s="38">
         <v>43002002</v>
       </c>
@@ -10021,15 +10221,16 @@
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
       <c r="Q46" s="27"/>
-      <c r="R46" s="4" t="s">
+      <c r="R46" s="27"/>
+      <c r="S46" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="S46" s="27" t="s">
+      <c r="T46" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="T46" s="27"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U46" s="27"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A47" s="38">
         <v>43002003</v>
       </c>
@@ -10071,15 +10272,16 @@
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
       <c r="Q47" s="27"/>
-      <c r="R47" s="4" t="s">
+      <c r="R47" s="27"/>
+      <c r="S47" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="S47" s="27" t="s">
+      <c r="T47" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="T47" s="27"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U47" s="27"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A48" s="38">
         <v>43002004</v>
       </c>
@@ -10121,15 +10323,16 @@
       <c r="O48" s="27"/>
       <c r="P48" s="27"/>
       <c r="Q48" s="13"/>
-      <c r="R48" s="31" t="s">
+      <c r="R48" s="13"/>
+      <c r="S48" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="S48" s="27" t="s">
+      <c r="T48" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="T48" s="27"/>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U48" s="27"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A49" s="38">
         <v>43002005</v>
       </c>
@@ -10171,15 +10374,16 @@
       <c r="O49" s="27"/>
       <c r="P49" s="27"/>
       <c r="Q49" s="13"/>
-      <c r="R49" s="31" t="s">
+      <c r="R49" s="13"/>
+      <c r="S49" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="S49" s="27" t="s">
+      <c r="T49" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="T49" s="27"/>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U49" s="27"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A50" s="38">
         <v>43002006</v>
       </c>
@@ -10221,19 +10425,20 @@
       <c r="O50" s="27"/>
       <c r="P50" s="27"/>
       <c r="Q50" s="13"/>
-      <c r="R50" s="31" t="s">
+      <c r="R50" s="13"/>
+      <c r="S50" s="31" t="s">
         <v>343</v>
       </c>
-      <c r="S50" s="27" t="s">
+      <c r="T50" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="T50" s="27"/>
+      <c r="U50" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="S42">
+  <conditionalFormatting sqref="T42">
     <cfRule type="containsBlanks" dxfId="7" priority="9">
-      <formula>LEN(TRIM(S42))=0</formula>
+      <formula>LEN(TRIM(T42))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
@@ -10241,9 +10446,9 @@
       <formula>LEN(TRIM(C47))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R47">
+  <conditionalFormatting sqref="S47">
     <cfRule type="containsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(R47))=0</formula>
+      <formula>LEN(TRIM(S47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C50">
@@ -10251,9 +10456,9 @@
       <formula>LEN(TRIM(C48))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R48:R50">
+  <conditionalFormatting sqref="S48:S50">
     <cfRule type="containsBlanks" dxfId="3" priority="3">
-      <formula>LEN(TRIM(R48))=0</formula>
+      <formula>LEN(TRIM(S48))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
@@ -10276,13 +10481,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q1" sqref="Q1"/>
+      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10296,12 +10501,12 @@
     <col min="13" max="14" width="6.125" customWidth="1"/>
     <col min="15" max="15" width="28.375" customWidth="1"/>
     <col min="16" max="16" width="19.5" customWidth="1"/>
-    <col min="17" max="17" width="9.875" customWidth="1"/>
-    <col min="19" max="19" width="10.625" customWidth="1"/>
-    <col min="20" max="20" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.875" customWidth="1"/>
+    <col min="20" max="20" width="10.625" customWidth="1"/>
+    <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>150</v>
       </c>
@@ -10350,20 +10555,23 @@
       <c r="P1" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="Q1" s="39" t="s">
         <v>429</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="39" t="s">
+        <v>433</v>
+      </c>
+      <c r="S1" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="T1" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="U1" s="25" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>148</v>
       </c>
@@ -10412,20 +10620,23 @@
       <c r="P2" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="Q2" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="R2" s="9" t="s">
+      <c r="Q2" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="R2" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="T2" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="U2" s="8" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>159</v>
       </c>
@@ -10474,20 +10685,23 @@
       <c r="P3" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="Q3" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="R3" s="10" t="s">
+      <c r="Q3" s="41" t="s">
+        <v>436</v>
+      </c>
+      <c r="R3" s="41" t="s">
+        <v>435</v>
+      </c>
+      <c r="S3" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="T3" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="T3" s="18" t="s">
+      <c r="U3" s="18" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43010001</v>
       </c>
@@ -10529,15 +10743,16 @@
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="6"/>
+      <c r="S4" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T4" s="15"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U4" s="15"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43010002</v>
       </c>
@@ -10577,15 +10792,16 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="4"/>
+      <c r="S5" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T5" s="14"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U5" s="14"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43010003</v>
       </c>
@@ -10625,15 +10841,16 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="4" t="s">
+      <c r="R6" s="4"/>
+      <c r="S6" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="T6" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T6" s="14"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U6" s="14"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43010004</v>
       </c>
@@ -10673,15 +10890,16 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="4"/>
+      <c r="S7" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="S7" s="4" t="s">
+      <c r="T7" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T7" s="14"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U7" s="14"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43010005</v>
       </c>
@@ -10723,15 +10941,16 @@
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-      <c r="R8" s="6" t="s">
+      <c r="R8" s="4"/>
+      <c r="S8" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="T8" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T8" s="14"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U8" s="14"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43010006</v>
       </c>
@@ -10773,15 +10992,16 @@
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="6" t="s">
+      <c r="R9" s="4"/>
+      <c r="S9" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="T9" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T9" s="14"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U9" s="14"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43010101</v>
       </c>
@@ -10819,15 +11039,16 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-      <c r="R10" s="4" t="s">
+      <c r="R10" s="4"/>
+      <c r="S10" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="S10" s="4" t="s">
+      <c r="T10" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T10" s="14"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U10" s="14"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43010102</v>
       </c>
@@ -10865,15 +11086,16 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="4"/>
+      <c r="S11" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="T11" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T11" s="14"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U11" s="14"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43010103</v>
       </c>
@@ -10911,15 +11133,16 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-      <c r="R12" s="4" t="s">
+      <c r="R12" s="4"/>
+      <c r="S12" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="S12" s="4" t="s">
+      <c r="T12" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T12" s="14"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U12" s="14"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43010104</v>
       </c>
@@ -10957,15 +11180,16 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="4" t="s">
+      <c r="R13" s="4"/>
+      <c r="S13" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="S13" s="4" t="s">
+      <c r="T13" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T13" s="14"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U13" s="14"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43010105</v>
       </c>
@@ -11003,13 +11227,14 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-      <c r="R14" s="4" t="s">
+      <c r="R14" s="4"/>
+      <c r="S14" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="S14" s="4" t="s">
+      <c r="T14" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
support record type for people rival condition
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/People.xlsx
+++ b/ConfigData/Xlsx/People.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C321C84F-C890-44D1-A6F1-6E1DCF680A69}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="人物" sheetId="4" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="501">
   <si>
     <t>老鼠</t>
   </si>
@@ -1721,13 +1720,48 @@
   </si>
   <si>
     <t>性格卑鄙无耻，为了获胜不择手段。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>威阿伊丁</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>奥莱伊李</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>赛尼斯</t>
+  </si>
+  <si>
+    <t>selectjob</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RivalRecordId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>结识：记录id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>结识：记录值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RivalRecordValue</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2662,190 +2696,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="112">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
+  <dxfs count="118">
     <dxf>
       <font>
         <b val="0"/>
@@ -3248,6 +3099,134 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="宋体"/>
         <scheme val="none"/>
@@ -3304,6 +3283,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -3943,6 +3951,106 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -4456,6 +4564,57 @@
         <name val="宋体"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -4509,6 +4668,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -5049,6 +5237,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -5061,108 +5317,114 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2_4" displayName="表2_4" ref="A3:X51" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110" tableBorderDxfId="109">
-  <autoFilter ref="A3:X51" xr:uid="{96403043-FC8D-48CF-907D-DA53CF3A1E55}"/>
-  <sortState ref="A4:U50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:Z51" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116" tableBorderDxfId="115">
+  <autoFilter ref="A3:Z51"/>
+  <sortState ref="A4:W50">
     <sortCondition ref="A3:A50"/>
   </sortState>
-  <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="107"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Ename" dataDxfId="106"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="105"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Quality" dataDxfId="104"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="World" dataDxfId="103"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Job" dataDxfId="102"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Level" dataDxfId="101"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="AutoAddLevel" dataDxfId="100"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Method" dataDxfId="99"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Emethod" dataDxfId="98"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="KingTowerId" dataDxfId="97"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="EpRecoverRate" dataDxfId="96"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="CardReduce" dataDxfId="95"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="RightMon" dataDxfId="94"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="PetMon" dataDxfId="93"/>
-    <tableColumn id="7" xr3:uid="{1D7F579A-8D29-4340-99EB-C9106F5EEBF1}" name="RivalDefeat" dataDxfId="92"/>
-    <tableColumn id="8" xr3:uid="{C3570C71-FFB0-4A70-A97D-D30B4B61E1E8}" name="RivalQuest" dataDxfId="42"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Figue" dataDxfId="91"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BattleMap" dataDxfId="90"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="InRandomQuest" dataDxfId="89"/>
-    <tableColumn id="22" xr3:uid="{E6063290-5AA4-4DF0-BCE4-7BF2DC622F1A}" name="~History" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{05F9E6AE-9857-4C0F-8366-5FCCCF6052D7}" name="~Like" dataDxfId="7"/>
-    <tableColumn id="24" xr3:uid="{713DDA20-E8BF-4233-80FF-235895476D33}" name="~Hate" dataDxfId="6"/>
+  <tableColumns count="26">
+    <tableColumn id="1" name="Id" dataDxfId="114"/>
+    <tableColumn id="2" name="Name" dataDxfId="113"/>
+    <tableColumn id="18" name="Ename" dataDxfId="112"/>
+    <tableColumn id="3" name="Type" dataDxfId="111"/>
+    <tableColumn id="21" name="Quality" dataDxfId="110"/>
+    <tableColumn id="6" name="World" dataDxfId="109"/>
+    <tableColumn id="10" name="Job" dataDxfId="108"/>
+    <tableColumn id="11" name="Level" dataDxfId="107"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="106"/>
+    <tableColumn id="13" name="Method" dataDxfId="105"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="104"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="103"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="102"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="101"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="100"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="99"/>
+    <tableColumn id="7" name="RivalDefeat" dataDxfId="98"/>
+    <tableColumn id="8" name="RivalQuest" dataDxfId="97"/>
+    <tableColumn id="25" name="RivalRecordId" dataDxfId="36"/>
+    <tableColumn id="26" name="RivalRecordValue" dataDxfId="33"/>
+    <tableColumn id="17" name="Figue" dataDxfId="96"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="95"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="94"/>
+    <tableColumn id="22" name="~History" dataDxfId="93"/>
+    <tableColumn id="23" name="~Like" dataDxfId="92"/>
+    <tableColumn id="24" name="~Hate" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表2" displayName="表2" ref="A3:X50" totalsRowShown="0" headerRowDxfId="88" dataDxfId="87" tableBorderDxfId="86">
-  <autoFilter ref="A3:X50" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState ref="A4:U50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Z50" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89" tableBorderDxfId="88">
+  <autoFilter ref="A3:Z50"/>
+  <sortState ref="A4:W50">
     <sortCondition ref="A3:A50"/>
   </sortState>
-  <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="84"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Ename" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="82"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Quality" dataDxfId="81"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="World" dataDxfId="80"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Job" dataDxfId="79"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Level" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="AutoAddLevel" dataDxfId="77"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Method" dataDxfId="76"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Emethod" dataDxfId="75"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="KingTowerId" dataDxfId="74"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="EpRecoverRate" dataDxfId="73"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="CardReduce" dataDxfId="72"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="RightMon" dataDxfId="71"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PetMon" dataDxfId="70"/>
-    <tableColumn id="8" xr3:uid="{CE1793B8-6380-4459-BED9-CDFF98B47C07}" name="RivalDefeat" dataDxfId="69"/>
-    <tableColumn id="21" xr3:uid="{2DA56599-F82F-42E1-A946-1E928F1DEA73}" name="RivalQuest" dataDxfId="41"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Figue" dataDxfId="68"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BattleMap" dataDxfId="67"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="InRandomQuest" dataDxfId="66"/>
-    <tableColumn id="22" xr3:uid="{ACA9B916-DB05-408B-AFB2-02A543FC7A79}" name="~History" dataDxfId="5"/>
-    <tableColumn id="23" xr3:uid="{B6092D72-AD8A-46AC-AA70-34E4EEC50B2A}" name="~Like" dataDxfId="4"/>
-    <tableColumn id="24" xr3:uid="{BAE9B3F8-4D7E-4850-80C1-73B427DD99A3}" name="~Hate" dataDxfId="3"/>
+  <tableColumns count="26">
+    <tableColumn id="1" name="Id" dataDxfId="87"/>
+    <tableColumn id="2" name="Name" dataDxfId="86"/>
+    <tableColumn id="18" name="Ename" dataDxfId="85"/>
+    <tableColumn id="3" name="Type" dataDxfId="84"/>
+    <tableColumn id="7" name="Quality" dataDxfId="83"/>
+    <tableColumn id="6" name="World" dataDxfId="82"/>
+    <tableColumn id="10" name="Job" dataDxfId="81"/>
+    <tableColumn id="11" name="Level" dataDxfId="80"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="79"/>
+    <tableColumn id="13" name="Method" dataDxfId="78"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="77"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="76"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="75"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="74"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="73"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="72"/>
+    <tableColumn id="8" name="RivalDefeat" dataDxfId="71"/>
+    <tableColumn id="21" name="RivalQuest" dataDxfId="70"/>
+    <tableColumn id="25" name="RivalRecordId" dataDxfId="35"/>
+    <tableColumn id="26" name="RivalRecordValue" dataDxfId="32"/>
+    <tableColumn id="17" name="Figue" dataDxfId="69"/>
+    <tableColumn id="9" name="BattleMap" dataDxfId="68"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="67"/>
+    <tableColumn id="22" name="~History" dataDxfId="66"/>
+    <tableColumn id="23" name="~Like" dataDxfId="65"/>
+    <tableColumn id="24" name="~Hate" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表2_2" displayName="表2_2" ref="A3:X14" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
-  <autoFilter ref="A3:X14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A4:T83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="A3:Z14" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" tableBorderDxfId="61">
+  <autoFilter ref="A3:Z14"/>
+  <sortState ref="A4:V83">
     <sortCondition ref="A3:A83"/>
   </sortState>
-  <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="61"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Ename" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Quality" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="World" dataDxfId="57"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Job" dataDxfId="56"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Level" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="AutoAddLevel" dataDxfId="54"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Method" dataDxfId="53"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Emethod" dataDxfId="52"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="KingTowerId" dataDxfId="51"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="EpRecoverRate" dataDxfId="50"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="CardReduce" dataDxfId="49"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="RightMon" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="PetMon" dataDxfId="47"/>
-    <tableColumn id="8" xr3:uid="{2FC8C9B2-866B-4CC7-9861-C44D809107E9}" name="RivalDefeat" dataDxfId="46"/>
-    <tableColumn id="21" xr3:uid="{4A49EC52-110E-429E-B5C1-90836365D98D}" name="RivalQuest" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Figue" dataDxfId="45"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="BattleMap" dataDxfId="44"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="InRandomQuest" dataDxfId="43"/>
-    <tableColumn id="22" xr3:uid="{7AA4E86A-4E35-45D7-821D-EC4DE41E2747}" name="~History" dataDxfId="2"/>
-    <tableColumn id="23" xr3:uid="{067A5620-C7EF-461B-A6C3-B0EA379EDDB3}" name="~Like" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{CCC91CC0-81E5-4050-B57E-702A772288C0}" name="~Hate" dataDxfId="0"/>
+  <tableColumns count="26">
+    <tableColumn id="1" name="Id" dataDxfId="60"/>
+    <tableColumn id="2" name="Name" dataDxfId="59"/>
+    <tableColumn id="18" name="Ename" dataDxfId="58"/>
+    <tableColumn id="3" name="Type" dataDxfId="57"/>
+    <tableColumn id="7" name="Quality" dataDxfId="56"/>
+    <tableColumn id="6" name="World" dataDxfId="55"/>
+    <tableColumn id="10" name="Job" dataDxfId="54"/>
+    <tableColumn id="11" name="Level" dataDxfId="53"/>
+    <tableColumn id="5" name="AutoAddLevel" dataDxfId="52"/>
+    <tableColumn id="13" name="Method" dataDxfId="51"/>
+    <tableColumn id="14" name="Emethod" dataDxfId="50"/>
+    <tableColumn id="20" name="KingTowerId" dataDxfId="49"/>
+    <tableColumn id="12" name="EpRecoverRate" dataDxfId="48"/>
+    <tableColumn id="19" name="CardReduce" dataDxfId="47"/>
+    <tableColumn id="15" name="RightMon" dataDxfId="46"/>
+    <tableColumn id="4" name="PetMon" dataDxfId="45"/>
+    <tableColumn id="8" name="RivalDefeat" dataDxfId="44"/>
+    <tableColumn id="21" name="RivalQuest" dataDxfId="43"/>
+    <tableColumn id="25" name="RivalRecordId" dataDxfId="34"/>
+    <tableColumn id="26" name="RivalRecordValue" dataDxfId="0"/>
+    <tableColumn id="9" name="Figue" dataDxfId="42"/>
+    <tableColumn id="17" name="BattleMap" dataDxfId="41"/>
+    <tableColumn id="16" name="InRandomQuest" dataDxfId="40"/>
+    <tableColumn id="22" name="~History" dataDxfId="39"/>
+    <tableColumn id="23" name="~Like" dataDxfId="38"/>
+    <tableColumn id="24" name="~Hate" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5176,7 +5438,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -5488,14 +5750,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V13" sqref="V13"/>
+      <selection pane="bottomRight" activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5507,12 +5769,14 @@
     <col min="10" max="10" width="9.5" customWidth="1"/>
     <col min="11" max="12" width="10.625" customWidth="1"/>
     <col min="13" max="16" width="5.875" customWidth="1"/>
-    <col min="17" max="18" width="8.875" customWidth="1"/>
-    <col min="20" max="20" width="10.625" customWidth="1"/>
-    <col min="22" max="22" width="30" customWidth="1"/>
+    <col min="17" max="17" width="5.25" customWidth="1"/>
+    <col min="18" max="18" width="7.25" customWidth="1"/>
+    <col min="19" max="20" width="5.625" customWidth="1"/>
+    <col min="22" max="22" width="10.625" customWidth="1"/>
+    <col min="24" max="24" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>145</v>
       </c>
@@ -5567,26 +5831,32 @@
       <c r="R1" s="39" t="s">
         <v>428</v>
       </c>
-      <c r="S1" s="23" t="s">
+      <c r="S1" s="39" t="s">
+        <v>498</v>
+      </c>
+      <c r="T1" s="39" t="s">
+        <v>499</v>
+      </c>
+      <c r="U1" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="V1" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="W1" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="V1" s="29" t="s">
+      <c r="X1" s="29" t="s">
         <v>432</v>
       </c>
-      <c r="W1" s="29" t="s">
+      <c r="Y1" s="29" t="s">
         <v>436</v>
       </c>
-      <c r="X1" s="29" t="s">
+      <c r="Z1" s="29" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>143</v>
       </c>
@@ -5641,26 +5911,32 @@
       <c r="R2" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="40" t="s">
+        <v>496</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>496</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="V2" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="W2" s="30" t="s">
-        <v>144</v>
       </c>
       <c r="X2" s="30" t="s">
         <v>144</v>
       </c>
+      <c r="Y2" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z2" s="30" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>154</v>
       </c>
@@ -5715,26 +5991,32 @@
       <c r="R3" s="41" t="s">
         <v>430</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="41" t="s">
+        <v>497</v>
+      </c>
+      <c r="T3" s="41" t="s">
+        <v>500</v>
+      </c>
+      <c r="U3" s="5" t="s">
         <v>423</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="V3" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="W3" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="V3" s="18" t="s">
+      <c r="X3" s="18" t="s">
         <v>434</v>
       </c>
-      <c r="W3" s="18" t="s">
+      <c r="Y3" s="18" t="s">
         <v>433</v>
       </c>
-      <c r="X3" s="18" t="s">
+      <c r="Z3" s="18" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43020101</v>
       </c>
@@ -5775,20 +6057,22 @@
         <v>1</v>
       </c>
       <c r="R4" s="4"/>
-      <c r="S4" s="4" t="s">
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U4" s="19"/>
-      <c r="V4" s="43" t="s">
+      <c r="W4" s="19"/>
+      <c r="X4" s="43" t="s">
         <v>438</v>
       </c>
-      <c r="W4" s="42"/>
-      <c r="X4" s="42"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="42"/>
     </row>
-    <row r="5" spans="1:24" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43020102</v>
       </c>
@@ -5829,20 +6113,22 @@
       <c r="R5" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="V5" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U5" s="19"/>
-      <c r="V5" s="43" t="s">
+      <c r="W5" s="19"/>
+      <c r="X5" s="43" t="s">
         <v>439</v>
       </c>
-      <c r="W5" s="42"/>
-      <c r="X5" s="42"/>
+      <c r="Y5" s="42"/>
+      <c r="Z5" s="42"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43020103</v>
       </c>
@@ -5883,27 +6169,35 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="4" t="s">
+      <c r="S6" s="4">
+        <v>19</v>
+      </c>
+      <c r="T6" s="4">
+        <v>10</v>
+      </c>
+      <c r="U6" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="T6" s="4" t="s">
+      <c r="V6" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U6" s="19" t="s">
+      <c r="W6" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V6" s="19" t="s">
+      <c r="X6" s="19" t="s">
         <v>440</v>
       </c>
-      <c r="W6" s="42"/>
-      <c r="X6" s="42"/>
+      <c r="Y6" s="42"/>
+      <c r="Z6" s="42" t="s">
+        <v>494</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43020104</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>59</v>
+        <v>492</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>60</v>
@@ -5939,25 +6233,29 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
-      <c r="S7" s="4" t="s">
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="T7" s="4" t="s">
+      <c r="V7" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19" t="s">
+      <c r="W7" s="19"/>
+      <c r="X7" s="19" t="s">
         <v>441</v>
       </c>
-      <c r="W7" s="42"/>
-      <c r="X7" s="42"/>
+      <c r="Y7" s="42"/>
+      <c r="Z7" s="42" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43020105</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>61</v>
+        <v>493</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>62</v>
@@ -5993,22 +6291,26 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
-      <c r="S8" s="4" t="s">
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="T8" s="4" t="s">
+      <c r="V8" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U8" s="19" t="s">
+      <c r="W8" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V8" s="19" t="s">
+      <c r="X8" s="19" t="s">
         <v>443</v>
       </c>
-      <c r="W8" s="42"/>
-      <c r="X8" s="42"/>
+      <c r="Y8" s="42"/>
+      <c r="Z8" s="42" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43020106</v>
       </c>
@@ -6048,23 +6350,27 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4" t="s">
+      <c r="R9" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="V9" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U9" s="19" t="s">
+      <c r="W9" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V9" s="43" t="s">
+      <c r="X9" s="43" t="s">
         <v>442</v>
       </c>
-      <c r="W9" s="42"/>
-      <c r="X9" s="42"/>
+      <c r="Y9" s="42"/>
+      <c r="Z9" s="42"/>
     </row>
-    <row r="10" spans="1:24" ht="27" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43020107</v>
       </c>
@@ -6105,22 +6411,24 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
-      <c r="S10" s="4" t="s">
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="T10" s="4" t="s">
+      <c r="V10" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U10" s="19" t="s">
+      <c r="W10" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V10" s="43" t="s">
+      <c r="X10" s="43" t="s">
         <v>445</v>
       </c>
-      <c r="W10" s="42"/>
-      <c r="X10" s="42"/>
+      <c r="Y10" s="42"/>
+      <c r="Z10" s="42"/>
     </row>
-    <row r="11" spans="1:24" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:26" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43020108</v>
       </c>
@@ -6161,22 +6469,24 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
-      <c r="S11" s="4" t="s">
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="V11" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U11" s="19" t="s">
+      <c r="W11" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V11" s="43" t="s">
+      <c r="X11" s="43" t="s">
         <v>446</v>
       </c>
-      <c r="W11" s="42"/>
-      <c r="X11" s="42"/>
+      <c r="Y11" s="42"/>
+      <c r="Z11" s="42"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43020109</v>
       </c>
@@ -6217,22 +6527,24 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
-      <c r="S12" s="4" t="s">
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="T12" s="4" t="s">
+      <c r="V12" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U12" s="19" t="s">
+      <c r="W12" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V12" s="19" t="s">
+      <c r="X12" s="19" t="s">
         <v>444</v>
       </c>
-      <c r="W12" s="42"/>
-      <c r="X12" s="42"/>
+      <c r="Y12" s="42"/>
+      <c r="Z12" s="42"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43020110</v>
       </c>
@@ -6273,22 +6585,24 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
-      <c r="S13" s="4" t="s">
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="T13" s="4" t="s">
+      <c r="V13" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U13" s="19" t="s">
+      <c r="W13" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V13" s="19" t="s">
+      <c r="X13" s="19" t="s">
         <v>447</v>
       </c>
-      <c r="W13" s="42"/>
-      <c r="X13" s="42"/>
+      <c r="Y13" s="42"/>
+      <c r="Z13" s="42"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43020201</v>
       </c>
@@ -6329,22 +6643,24 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
-      <c r="S14" s="4" t="s">
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="T14" s="4" t="s">
+      <c r="V14" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U14" s="19" t="s">
+      <c r="W14" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V14" s="19" t="s">
+      <c r="X14" s="19" t="s">
         <v>485</v>
       </c>
-      <c r="W14" s="42"/>
-      <c r="X14" s="42"/>
+      <c r="Y14" s="42"/>
+      <c r="Z14" s="42"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43020202</v>
       </c>
@@ -6385,22 +6701,24 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
-      <c r="S15" s="4" t="s">
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="T15" s="4" t="s">
+      <c r="V15" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U15" s="19" t="s">
+      <c r="W15" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V15" s="19" t="s">
+      <c r="X15" s="19" t="s">
         <v>486</v>
       </c>
-      <c r="W15" s="42"/>
-      <c r="X15" s="42"/>
+      <c r="Y15" s="42"/>
+      <c r="Z15" s="42"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43020203</v>
       </c>
@@ -6441,22 +6759,24 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
-      <c r="S16" s="4" t="s">
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="T16" s="4" t="s">
+      <c r="V16" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U16" s="19" t="s">
+      <c r="W16" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V16" s="19" t="s">
+      <c r="X16" s="19" t="s">
         <v>488</v>
       </c>
-      <c r="W16" s="42"/>
-      <c r="X16" s="42"/>
+      <c r="Y16" s="42"/>
+      <c r="Z16" s="42"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43020204</v>
       </c>
@@ -6497,22 +6817,24 @@
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
-      <c r="S17" s="4" t="s">
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="T17" s="4" t="s">
+      <c r="V17" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U17" s="19" t="s">
+      <c r="W17" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V17" s="19" t="s">
+      <c r="X17" s="19" t="s">
         <v>491</v>
       </c>
-      <c r="W17" s="42"/>
-      <c r="X17" s="42"/>
+      <c r="Y17" s="42"/>
+      <c r="Z17" s="42"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43020205</v>
       </c>
@@ -6551,22 +6873,24 @@
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
-      <c r="S18" s="4" t="s">
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="T18" s="4" t="s">
+      <c r="V18" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U18" s="19" t="s">
+      <c r="W18" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V18" s="19" t="s">
+      <c r="X18" s="19" t="s">
         <v>487</v>
       </c>
-      <c r="W18" s="42"/>
-      <c r="X18" s="42"/>
+      <c r="Y18" s="42"/>
+      <c r="Z18" s="42"/>
     </row>
-    <row r="19" spans="1:24" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:26" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43020206</v>
       </c>
@@ -6607,22 +6931,24 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
-      <c r="S19" s="4" t="s">
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="T19" s="4" t="s">
+      <c r="V19" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U19" s="19" t="s">
+      <c r="W19" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V19" s="43" t="s">
+      <c r="X19" s="43" t="s">
         <v>489</v>
       </c>
-      <c r="W19" s="42"/>
-      <c r="X19" s="42"/>
+      <c r="Y19" s="42"/>
+      <c r="Z19" s="42"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43020207</v>
       </c>
@@ -6663,22 +6989,24 @@
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
-      <c r="S20" s="4" t="s">
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="T20" s="4" t="s">
+      <c r="V20" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U20" s="19" t="s">
+      <c r="W20" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V20" s="19" t="s">
+      <c r="X20" s="19" t="s">
         <v>490</v>
       </c>
-      <c r="W20" s="42"/>
-      <c r="X20" s="42"/>
+      <c r="Y20" s="42"/>
+      <c r="Z20" s="42"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43020301</v>
       </c>
@@ -6719,22 +7047,24 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
-      <c r="S21" s="4" t="s">
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="T21" s="4" t="s">
+      <c r="V21" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U21" s="19" t="s">
+      <c r="W21" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V21" s="19" t="s">
+      <c r="X21" s="19" t="s">
         <v>452</v>
       </c>
-      <c r="W21" s="42"/>
-      <c r="X21" s="42"/>
+      <c r="Y21" s="42"/>
+      <c r="Z21" s="42"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43020302</v>
       </c>
@@ -6775,22 +7105,24 @@
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
-      <c r="S22" s="4" t="s">
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="T22" s="4" t="s">
+      <c r="V22" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U22" s="19" t="s">
+      <c r="W22" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V22" s="19" t="s">
+      <c r="X22" s="19" t="s">
         <v>453</v>
       </c>
-      <c r="W22" s="42"/>
-      <c r="X22" s="42"/>
+      <c r="Y22" s="42"/>
+      <c r="Z22" s="42"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43020303</v>
       </c>
@@ -6829,24 +7161,26 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
-      <c r="S23" s="4" t="s">
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="T23" s="4" t="s">
+      <c r="V23" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U23" s="19" t="s">
+      <c r="W23" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V23" s="19" t="s">
+      <c r="X23" s="19" t="s">
         <v>454</v>
       </c>
-      <c r="W23" s="42" t="s">
+      <c r="Y23" s="42" t="s">
         <v>451</v>
       </c>
-      <c r="X23" s="42"/>
+      <c r="Z23" s="42"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43020304</v>
       </c>
@@ -6887,22 +7221,24 @@
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
-      <c r="S24" s="4" t="s">
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="T24" s="4" t="s">
+      <c r="V24" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U24" s="19" t="s">
+      <c r="W24" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V24" s="19" t="s">
+      <c r="X24" s="19" t="s">
         <v>455</v>
       </c>
-      <c r="W24" s="42"/>
-      <c r="X24" s="42"/>
+      <c r="Y24" s="42"/>
+      <c r="Z24" s="42"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43020305</v>
       </c>
@@ -6943,22 +7279,24 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
-      <c r="S25" s="4" t="s">
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="T25" s="4" t="s">
+      <c r="V25" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U25" s="19" t="s">
+      <c r="W25" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V25" s="19" t="s">
+      <c r="X25" s="19" t="s">
         <v>456</v>
       </c>
-      <c r="W25" s="42"/>
-      <c r="X25" s="42"/>
+      <c r="Y25" s="42"/>
+      <c r="Z25" s="42"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43020306</v>
       </c>
@@ -6999,22 +7337,24 @@
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
-      <c r="S26" s="4" t="s">
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="T26" s="4" t="s">
+      <c r="V26" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U26" s="19" t="s">
+      <c r="W26" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V26" s="19" t="s">
+      <c r="X26" s="19" t="s">
         <v>457</v>
       </c>
-      <c r="W26" s="42"/>
-      <c r="X26" s="42"/>
+      <c r="Y26" s="42"/>
+      <c r="Z26" s="42"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43020307</v>
       </c>
@@ -7055,22 +7395,24 @@
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
-      <c r="S27" s="4" t="s">
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="T27" s="4" t="s">
+      <c r="V27" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U27" s="19" t="s">
+      <c r="W27" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V27" s="19" t="s">
+      <c r="X27" s="19" t="s">
         <v>458</v>
       </c>
-      <c r="W27" s="42"/>
-      <c r="X27" s="42"/>
+      <c r="Y27" s="42"/>
+      <c r="Z27" s="42"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43020308</v>
       </c>
@@ -7111,22 +7453,24 @@
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
-      <c r="S28" s="4" t="s">
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="T28" s="4" t="s">
+      <c r="V28" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U28" s="19" t="s">
+      <c r="W28" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V28" s="19" t="s">
+      <c r="X28" s="19" t="s">
         <v>458</v>
       </c>
-      <c r="W28" s="42"/>
-      <c r="X28" s="42"/>
+      <c r="Y28" s="42"/>
+      <c r="Z28" s="42"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43020309</v>
       </c>
@@ -7167,24 +7511,26 @@
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
-      <c r="S29" s="4" t="s">
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="T29" s="4" t="s">
+      <c r="V29" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U29" s="19" t="s">
+      <c r="W29" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V29" s="19" t="s">
+      <c r="X29" s="19" t="s">
         <v>459</v>
       </c>
-      <c r="W29" s="42" t="s">
+      <c r="Y29" s="42" t="s">
         <v>449</v>
       </c>
-      <c r="X29" s="42"/>
+      <c r="Z29" s="42"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43020310</v>
       </c>
@@ -7225,22 +7571,24 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
-      <c r="S30" s="4" t="s">
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="T30" s="4" t="s">
+      <c r="V30" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U30" s="19" t="s">
+      <c r="W30" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V30" s="19" t="s">
+      <c r="X30" s="19" t="s">
         <v>460</v>
       </c>
-      <c r="W30" s="42"/>
-      <c r="X30" s="42"/>
+      <c r="Y30" s="42"/>
+      <c r="Z30" s="42"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43020311</v>
       </c>
@@ -7281,22 +7629,24 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
-      <c r="S31" s="4" t="s">
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="T31" s="4" t="s">
+      <c r="V31" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U31" s="19" t="s">
+      <c r="W31" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V31" s="19" t="s">
+      <c r="X31" s="19" t="s">
         <v>461</v>
       </c>
-      <c r="W31" s="42"/>
-      <c r="X31" s="42"/>
+      <c r="Y31" s="42"/>
+      <c r="Z31" s="42"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43020312</v>
       </c>
@@ -7337,22 +7687,24 @@
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
-      <c r="S32" s="4" t="s">
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="T32" s="4" t="s">
+      <c r="V32" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U32" s="19" t="s">
+      <c r="W32" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V32" s="19" t="s">
+      <c r="X32" s="19" t="s">
         <v>462</v>
       </c>
-      <c r="W32" s="42"/>
-      <c r="X32" s="42"/>
+      <c r="Y32" s="42"/>
+      <c r="Z32" s="42"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43020401</v>
       </c>
@@ -7393,24 +7745,26 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
-      <c r="S33" s="4" t="s">
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="T33" s="4" t="s">
+      <c r="V33" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U33" s="19" t="s">
+      <c r="W33" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V33" s="19" t="s">
+      <c r="X33" s="19" t="s">
         <v>465</v>
       </c>
-      <c r="W33" s="42" t="s">
+      <c r="Y33" s="42" t="s">
         <v>464</v>
       </c>
-      <c r="X33" s="42"/>
+      <c r="Z33" s="42"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43020402</v>
       </c>
@@ -7451,24 +7805,26 @@
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
-      <c r="S34" s="4" t="s">
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="T34" s="4" t="s">
+      <c r="V34" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U34" s="19" t="s">
+      <c r="W34" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V34" s="19" t="s">
+      <c r="X34" s="19" t="s">
         <v>468</v>
       </c>
-      <c r="W34" s="42" t="s">
+      <c r="Y34" s="42" t="s">
         <v>467</v>
       </c>
-      <c r="X34" s="42"/>
+      <c r="Z34" s="42"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43020403</v>
       </c>
@@ -7509,24 +7865,26 @@
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
-      <c r="S35" s="4" t="s">
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="T35" s="4" t="s">
+      <c r="V35" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U35" s="19" t="s">
+      <c r="W35" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V35" s="19" t="s">
+      <c r="X35" s="19" t="s">
         <v>469</v>
       </c>
-      <c r="W35" s="42" t="s">
+      <c r="Y35" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="X35" s="42"/>
+      <c r="Z35" s="42"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43020404</v>
       </c>
@@ -7567,24 +7925,26 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
-      <c r="S36" s="4" t="s">
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="T36" s="4" t="s">
+      <c r="V36" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U36" s="19" t="s">
+      <c r="W36" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V36" s="19" t="s">
+      <c r="X36" s="19" t="s">
         <v>470</v>
       </c>
-      <c r="W36" s="42" t="s">
+      <c r="Y36" s="42" t="s">
         <v>471</v>
       </c>
-      <c r="X36" s="42"/>
+      <c r="Z36" s="42"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43020405</v>
       </c>
@@ -7625,22 +7985,24 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
-      <c r="S37" s="4" t="s">
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="T37" s="4" t="s">
+      <c r="V37" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U37" s="19" t="s">
+      <c r="W37" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V37" s="19" t="s">
+      <c r="X37" s="19" t="s">
         <v>473</v>
       </c>
-      <c r="W37" s="42"/>
-      <c r="X37" s="42"/>
+      <c r="Y37" s="42"/>
+      <c r="Z37" s="42"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43020406</v>
       </c>
@@ -7681,22 +8043,24 @@
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
-      <c r="S38" s="4" t="s">
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="T38" s="4" t="s">
+      <c r="V38" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U38" s="19" t="s">
+      <c r="W38" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V38" s="19" t="s">
+      <c r="X38" s="19" t="s">
         <v>474</v>
       </c>
-      <c r="W38" s="42"/>
-      <c r="X38" s="42"/>
+      <c r="Y38" s="42"/>
+      <c r="Z38" s="42"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>43020407</v>
       </c>
@@ -7737,22 +8101,24 @@
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
-      <c r="S39" s="4" t="s">
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="T39" s="4" t="s">
+      <c r="V39" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U39" s="19" t="s">
+      <c r="W39" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V39" s="19" t="s">
+      <c r="X39" s="19" t="s">
         <v>475</v>
       </c>
-      <c r="W39" s="42"/>
-      <c r="X39" s="42"/>
+      <c r="Y39" s="42"/>
+      <c r="Z39" s="42"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>43020408</v>
       </c>
@@ -7793,22 +8159,24 @@
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
-      <c r="S40" s="4" t="s">
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="T40" s="4" t="s">
+      <c r="V40" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U40" s="19" t="s">
+      <c r="W40" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V40" s="19" t="s">
+      <c r="X40" s="19" t="s">
         <v>476</v>
       </c>
-      <c r="W40" s="42"/>
-      <c r="X40" s="42"/>
+      <c r="Y40" s="42"/>
+      <c r="Z40" s="42"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>43020409</v>
       </c>
@@ -7849,22 +8217,24 @@
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
-      <c r="S41" s="4" t="s">
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="T41" s="4" t="s">
+      <c r="V41" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U41" s="19" t="s">
+      <c r="W41" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V41" s="19" t="s">
+      <c r="X41" s="19" t="s">
         <v>477</v>
       </c>
-      <c r="W41" s="42"/>
-      <c r="X41" s="42"/>
+      <c r="Y41" s="42"/>
+      <c r="Z41" s="42"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>43020501</v>
       </c>
@@ -7905,22 +8275,24 @@
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
-      <c r="S42" s="4" t="s">
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="T42" s="4" t="s">
+      <c r="V42" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U42" s="19" t="s">
+      <c r="W42" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V42" s="19" t="s">
+      <c r="X42" s="19" t="s">
         <v>479</v>
       </c>
-      <c r="W42" s="42"/>
-      <c r="X42" s="42"/>
+      <c r="Y42" s="42"/>
+      <c r="Z42" s="42"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>43020502</v>
       </c>
@@ -7961,22 +8333,24 @@
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
-      <c r="S43" s="4" t="s">
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="T43" s="4" t="s">
+      <c r="V43" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U43" s="19" t="s">
+      <c r="W43" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V43" s="19" t="s">
+      <c r="X43" s="19" t="s">
         <v>478</v>
       </c>
-      <c r="W43" s="42"/>
-      <c r="X43" s="42"/>
+      <c r="Y43" s="42"/>
+      <c r="Z43" s="42"/>
     </row>
-    <row r="44" spans="1:24" ht="54" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:26" ht="54" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43020503</v>
       </c>
@@ -8017,22 +8391,24 @@
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
-      <c r="S44" s="4" t="s">
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="T44" s="4" t="s">
+      <c r="V44" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U44" s="19" t="s">
+      <c r="W44" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V44" s="43" t="s">
+      <c r="X44" s="43" t="s">
         <v>480</v>
       </c>
-      <c r="W44" s="42"/>
-      <c r="X44" s="42"/>
+      <c r="Y44" s="42"/>
+      <c r="Z44" s="42"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>43020504</v>
       </c>
@@ -8073,22 +8449,24 @@
       <c r="P45" s="4"/>
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
-      <c r="S45" s="4" t="s">
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="T45" s="4" t="s">
+      <c r="V45" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U45" s="19" t="s">
+      <c r="W45" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V45" s="19" t="s">
+      <c r="X45" s="19" t="s">
         <v>481</v>
       </c>
-      <c r="W45" s="42"/>
-      <c r="X45" s="42"/>
+      <c r="Y45" s="42"/>
+      <c r="Z45" s="42"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>43020505</v>
       </c>
@@ -8129,24 +8507,26 @@
       <c r="P46" s="27"/>
       <c r="Q46" s="27"/>
       <c r="R46" s="27"/>
-      <c r="S46" s="27" t="s">
+      <c r="S46" s="27"/>
+      <c r="T46" s="27"/>
+      <c r="U46" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="T46" s="4" t="s">
+      <c r="V46" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U46" s="19" t="s">
+      <c r="W46" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V46" s="19" t="s">
+      <c r="X46" s="19" t="s">
         <v>482</v>
       </c>
-      <c r="W46" s="4" t="s">
+      <c r="Y46" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="X46" s="42"/>
+      <c r="Z46" s="42"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>43020506</v>
       </c>
@@ -8187,24 +8567,26 @@
       <c r="P47" s="27"/>
       <c r="Q47" s="27"/>
       <c r="R47" s="27"/>
-      <c r="S47" s="27" t="s">
+      <c r="S47" s="27"/>
+      <c r="T47" s="27"/>
+      <c r="U47" s="27" t="s">
         <v>403</v>
       </c>
-      <c r="T47" s="4" t="s">
+      <c r="V47" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U47" s="19" t="s">
+      <c r="W47" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V47" s="19" t="s">
+      <c r="X47" s="19" t="s">
         <v>483</v>
       </c>
-      <c r="W47" s="42" t="s">
+      <c r="Y47" s="42" t="s">
         <v>484</v>
       </c>
-      <c r="X47" s="42"/>
+      <c r="Z47" s="42"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>43020601</v>
       </c>
@@ -8245,20 +8627,22 @@
       <c r="P48" s="4"/>
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
-      <c r="S48" s="4" t="s">
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="T48" s="4" t="s">
+      <c r="V48" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U48" s="19" t="s">
+      <c r="W48" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V48" s="19"/>
-      <c r="W48" s="42"/>
-      <c r="X48" s="42"/>
+      <c r="X48" s="19"/>
+      <c r="Y48" s="42"/>
+      <c r="Z48" s="42"/>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>43020602</v>
       </c>
@@ -8297,20 +8681,22 @@
       <c r="P49" s="4"/>
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
-      <c r="S49" s="4" t="s">
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="T49" s="4" t="s">
+      <c r="V49" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U49" s="19" t="s">
+      <c r="W49" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V49" s="19"/>
-      <c r="W49" s="42"/>
-      <c r="X49" s="42"/>
+      <c r="X49" s="19"/>
+      <c r="Y49" s="42"/>
+      <c r="Z49" s="42"/>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>43020603</v>
       </c>
@@ -8349,20 +8735,22 @@
       <c r="P50" s="4"/>
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
-      <c r="S50" s="4" t="s">
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="T50" s="4" t="s">
+      <c r="V50" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U50" s="19" t="s">
+      <c r="W50" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V50" s="19"/>
-      <c r="W50" s="42"/>
-      <c r="X50" s="42"/>
+      <c r="X50" s="19"/>
+      <c r="Y50" s="42"/>
+      <c r="Z50" s="42"/>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>43020604</v>
       </c>
@@ -8403,102 +8791,104 @@
       <c r="P51" s="4"/>
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
-      <c r="S51" s="4" t="s">
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
+      <c r="U51" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="T51" s="4" t="s">
+      <c r="V51" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="U51" s="19" t="s">
+      <c r="W51" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="V51" s="19"/>
-      <c r="W51" s="42"/>
-      <c r="X51" s="42"/>
+      <c r="X51" s="19"/>
+      <c r="Y51" s="42"/>
+      <c r="Z51" s="42"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E23:E25 E27:E43 E4:E19 E45:E51">
-    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="42" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="43" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="44" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="45" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="37" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="38" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="39" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="40" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="32" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="28" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8511,14 +8901,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="G22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V1" sqref="V1:X3"/>
+      <selection pane="bottomRight" activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8531,12 +8921,12 @@
     <col min="11" max="12" width="10.625" customWidth="1"/>
     <col min="13" max="14" width="6.125" customWidth="1"/>
     <col min="15" max="16" width="27.125" customWidth="1"/>
-    <col min="17" max="18" width="10.875" customWidth="1"/>
-    <col min="20" max="20" width="10.625" customWidth="1"/>
-    <col min="21" max="21" width="8" customWidth="1"/>
+    <col min="17" max="20" width="5.375" customWidth="1"/>
+    <col min="22" max="22" width="10.625" customWidth="1"/>
+    <col min="23" max="23" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>145</v>
       </c>
@@ -8591,26 +8981,32 @@
       <c r="R1" s="39" t="s">
         <v>428</v>
       </c>
-      <c r="S1" s="23" t="s">
+      <c r="S1" s="39" t="s">
+        <v>498</v>
+      </c>
+      <c r="T1" s="39" t="s">
+        <v>499</v>
+      </c>
+      <c r="U1" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="V1" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="W1" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="V1" s="29" t="s">
+      <c r="X1" s="29" t="s">
         <v>432</v>
       </c>
-      <c r="W1" s="29" t="s">
+      <c r="Y1" s="29" t="s">
         <v>436</v>
       </c>
-      <c r="X1" s="29" t="s">
+      <c r="Z1" s="29" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>143</v>
       </c>
@@ -8665,26 +9061,32 @@
       <c r="R2" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="40" t="s">
+        <v>496</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>496</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="V2" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="W2" s="30" t="s">
-        <v>144</v>
       </c>
       <c r="X2" s="30" t="s">
         <v>144</v>
       </c>
+      <c r="Y2" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z2" s="30" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>154</v>
       </c>
@@ -8739,26 +9141,32 @@
       <c r="R3" s="41" t="s">
         <v>430</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="41" t="s">
+        <v>497</v>
+      </c>
+      <c r="T3" s="41" t="s">
+        <v>500</v>
+      </c>
+      <c r="U3" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="V3" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="W3" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>434</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
         <v>433</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="Z3" s="16" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43000001</v>
       </c>
@@ -8801,18 +9209,20 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
-      <c r="S4" s="4" t="s">
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="U4" s="17"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
+      <c r="W4" s="17"/>
       <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43000002</v>
       </c>
@@ -8855,18 +9265,20 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
-      <c r="S5" s="4" t="s">
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="V5" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="U5" s="17"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
+      <c r="W5" s="17"/>
       <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43000003</v>
       </c>
@@ -8909,18 +9321,20 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="4" t="s">
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="T6" s="4" t="s">
+      <c r="V6" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U6" s="17"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
+      <c r="W6" s="17"/>
       <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43000004</v>
       </c>
@@ -8963,18 +9377,20 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
-      <c r="S7" s="4" t="s">
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="T7" s="4" t="s">
+      <c r="V7" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U7" s="17"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
+      <c r="W7" s="17"/>
       <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43000005</v>
       </c>
@@ -9017,18 +9433,20 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
-      <c r="S8" s="4" t="s">
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="T8" s="4" t="s">
+      <c r="V8" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U8" s="17"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
+      <c r="W8" s="17"/>
       <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43000007</v>
       </c>
@@ -9071,18 +9489,20 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
-      <c r="S9" s="4" t="s">
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="V9" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="U9" s="17"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
+      <c r="W9" s="17"/>
       <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43000008</v>
       </c>
@@ -9125,18 +9545,20 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
-      <c r="S10" s="4" t="s">
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="T10" s="4" t="s">
+      <c r="V10" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U10" s="17"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
+      <c r="W10" s="17"/>
       <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43000009</v>
       </c>
@@ -9179,18 +9601,20 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
-      <c r="S11" s="4" t="s">
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="V11" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U11" s="17"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
+      <c r="W11" s="17"/>
       <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43000010</v>
       </c>
@@ -9233,18 +9657,20 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
-      <c r="S12" s="4" t="s">
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="T12" s="4" t="s">
+      <c r="V12" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U12" s="17"/>
-      <c r="V12" s="13"/>
-      <c r="W12" s="13"/>
+      <c r="W12" s="17"/>
       <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43000011</v>
       </c>
@@ -9287,18 +9713,20 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
-      <c r="S13" s="4" t="s">
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="T13" s="4" t="s">
+      <c r="V13" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U13" s="17"/>
-      <c r="V13" s="13"/>
-      <c r="W13" s="13"/>
+      <c r="W13" s="17"/>
       <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43000012</v>
       </c>
@@ -9341,18 +9769,20 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
-      <c r="S14" s="4" t="s">
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="T14" s="4" t="s">
+      <c r="V14" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U14" s="17"/>
-      <c r="V14" s="13"/>
-      <c r="W14" s="13"/>
+      <c r="W14" s="17"/>
       <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>43000013</v>
       </c>
@@ -9395,18 +9825,20 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
-      <c r="S15" s="4" t="s">
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="T15" s="4" t="s">
+      <c r="V15" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U15" s="17"/>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13"/>
+      <c r="W15" s="17"/>
       <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>43000014</v>
       </c>
@@ -9449,18 +9881,20 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
-      <c r="S16" s="4" t="s">
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="T16" s="4" t="s">
+      <c r="V16" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U16" s="17"/>
-      <c r="V16" s="13"/>
-      <c r="W16" s="13"/>
+      <c r="W16" s="17"/>
       <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>43000015</v>
       </c>
@@ -9503,18 +9937,20 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
-      <c r="S17" s="4" t="s">
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="T17" s="4" t="s">
+      <c r="V17" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U17" s="17"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
+      <c r="W17" s="17"/>
       <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>43000016</v>
       </c>
@@ -9557,18 +9993,20 @@
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
-      <c r="S18" s="4" t="s">
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="T18" s="4" t="s">
+      <c r="V18" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U18" s="17"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
+      <c r="W18" s="17"/>
       <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="13"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>43000017</v>
       </c>
@@ -9611,18 +10049,20 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
-      <c r="S19" s="4" t="s">
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="T19" s="4" t="s">
+      <c r="V19" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U19" s="17"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
+      <c r="W19" s="17"/>
       <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>43000018</v>
       </c>
@@ -9665,18 +10105,20 @@
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
-      <c r="S20" s="4" t="s">
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="T20" s="4" t="s">
+      <c r="V20" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U20" s="17"/>
-      <c r="V20" s="13"/>
-      <c r="W20" s="13"/>
+      <c r="W20" s="17"/>
       <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="Z20" s="13"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>43000019</v>
       </c>
@@ -9719,18 +10161,20 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
-      <c r="S21" s="4" t="s">
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="T21" s="4" t="s">
+      <c r="V21" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U21" s="17"/>
-      <c r="V21" s="13"/>
-      <c r="W21" s="13"/>
+      <c r="W21" s="17"/>
       <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>43000020</v>
       </c>
@@ -9773,18 +10217,20 @@
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
-      <c r="S22" s="4" t="s">
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="T22" s="4" t="s">
+      <c r="V22" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U22" s="17"/>
-      <c r="V22" s="13"/>
-      <c r="W22" s="13"/>
+      <c r="W22" s="17"/>
       <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>43000021</v>
       </c>
@@ -9827,18 +10273,20 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
-      <c r="S23" s="4" t="s">
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="T23" s="4" t="s">
+      <c r="V23" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U23" s="17"/>
-      <c r="V23" s="13"/>
-      <c r="W23" s="13"/>
+      <c r="W23" s="17"/>
       <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="13"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>43000022</v>
       </c>
@@ -9881,18 +10329,20 @@
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
-      <c r="S24" s="4" t="s">
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="T24" s="4" t="s">
+      <c r="V24" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U24" s="17"/>
-      <c r="V24" s="13"/>
-      <c r="W24" s="13"/>
+      <c r="W24" s="17"/>
       <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
+      <c r="Z24" s="13"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>43000023</v>
       </c>
@@ -9935,18 +10385,20 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
-      <c r="S25" s="4" t="s">
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="T25" s="4" t="s">
+      <c r="V25" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U25" s="17"/>
-      <c r="V25" s="13"/>
-      <c r="W25" s="13"/>
+      <c r="W25" s="17"/>
       <c r="X25" s="13"/>
+      <c r="Y25" s="13"/>
+      <c r="Z25" s="13"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>43000024</v>
       </c>
@@ -9989,18 +10441,20 @@
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
-      <c r="S26" s="4" t="s">
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="T26" s="4" t="s">
+      <c r="V26" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U26" s="17"/>
-      <c r="V26" s="13"/>
-      <c r="W26" s="13"/>
+      <c r="W26" s="17"/>
       <c r="X26" s="13"/>
+      <c r="Y26" s="13"/>
+      <c r="Z26" s="13"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>43000025</v>
       </c>
@@ -10043,18 +10497,20 @@
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
-      <c r="S27" s="4" t="s">
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="T27" s="4" t="s">
+      <c r="V27" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U27" s="17"/>
-      <c r="V27" s="13"/>
-      <c r="W27" s="13"/>
+      <c r="W27" s="17"/>
       <c r="X27" s="13"/>
+      <c r="Y27" s="13"/>
+      <c r="Z27" s="13"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>43000026</v>
       </c>
@@ -10097,18 +10553,20 @@
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
-      <c r="S28" s="4" t="s">
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="T28" s="4" t="s">
+      <c r="V28" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U28" s="17"/>
-      <c r="V28" s="13"/>
-      <c r="W28" s="13"/>
+      <c r="W28" s="17"/>
       <c r="X28" s="13"/>
+      <c r="Y28" s="13"/>
+      <c r="Z28" s="13"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>43000027</v>
       </c>
@@ -10151,18 +10609,20 @@
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
-      <c r="S29" s="4" t="s">
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="T29" s="4" t="s">
+      <c r="V29" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U29" s="17"/>
-      <c r="V29" s="13"/>
-      <c r="W29" s="13"/>
+      <c r="W29" s="17"/>
       <c r="X29" s="13"/>
+      <c r="Y29" s="13"/>
+      <c r="Z29" s="13"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>43000028</v>
       </c>
@@ -10205,18 +10665,20 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
-      <c r="S30" s="4" t="s">
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="T30" s="4" t="s">
+      <c r="V30" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U30" s="17"/>
-      <c r="V30" s="13"/>
-      <c r="W30" s="13"/>
+      <c r="W30" s="17"/>
       <c r="X30" s="13"/>
+      <c r="Y30" s="13"/>
+      <c r="Z30" s="13"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>43000029</v>
       </c>
@@ -10259,18 +10721,20 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
-      <c r="S31" s="4" t="s">
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="T31" s="4" t="s">
+      <c r="V31" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U31" s="17"/>
-      <c r="V31" s="13"/>
-      <c r="W31" s="13"/>
+      <c r="W31" s="17"/>
       <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
+      <c r="Z31" s="13"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>43000030</v>
       </c>
@@ -10313,18 +10777,20 @@
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
-      <c r="S32" s="4" t="s">
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="T32" s="4" t="s">
+      <c r="V32" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U32" s="17"/>
-      <c r="V32" s="13"/>
-      <c r="W32" s="13"/>
+      <c r="W32" s="17"/>
       <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="13"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>43000031</v>
       </c>
@@ -10367,18 +10833,20 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
-      <c r="S33" s="4" t="s">
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="T33" s="4" t="s">
+      <c r="V33" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U33" s="17"/>
-      <c r="V33" s="13"/>
-      <c r="W33" s="13"/>
+      <c r="W33" s="17"/>
       <c r="X33" s="13"/>
+      <c r="Y33" s="13"/>
+      <c r="Z33" s="13"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>43000032</v>
       </c>
@@ -10421,18 +10889,20 @@
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
-      <c r="S34" s="4" t="s">
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="T34" s="4" t="s">
+      <c r="V34" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U34" s="17"/>
-      <c r="V34" s="13"/>
-      <c r="W34" s="13"/>
+      <c r="W34" s="17"/>
       <c r="X34" s="13"/>
+      <c r="Y34" s="13"/>
+      <c r="Z34" s="13"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>43000033</v>
       </c>
@@ -10475,18 +10945,20 @@
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
-      <c r="S35" s="4" t="s">
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="T35" s="4" t="s">
+      <c r="V35" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U35" s="17"/>
-      <c r="V35" s="13"/>
-      <c r="W35" s="13"/>
+      <c r="W35" s="17"/>
       <c r="X35" s="13"/>
+      <c r="Y35" s="13"/>
+      <c r="Z35" s="13"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>43000035</v>
       </c>
@@ -10529,18 +11001,20 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
-      <c r="S36" s="4" t="s">
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="T36" s="4" t="s">
+      <c r="V36" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U36" s="17"/>
-      <c r="V36" s="13"/>
-      <c r="W36" s="13"/>
+      <c r="W36" s="17"/>
       <c r="X36" s="13"/>
+      <c r="Y36" s="13"/>
+      <c r="Z36" s="13"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>43000037</v>
       </c>
@@ -10583,18 +11057,20 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
-      <c r="S37" s="4" t="s">
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="T37" s="4" t="s">
+      <c r="V37" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U37" s="13"/>
-      <c r="V37" s="13"/>
       <c r="W37" s="13"/>
       <c r="X37" s="13"/>
+      <c r="Y37" s="13"/>
+      <c r="Z37" s="13"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>43000038</v>
       </c>
@@ -10637,18 +11113,20 @@
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
-      <c r="S38" s="4" t="s">
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="T38" s="4" t="s">
+      <c r="V38" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U38" s="35"/>
-      <c r="V38" s="13"/>
-      <c r="W38" s="13"/>
+      <c r="W38" s="35"/>
       <c r="X38" s="13"/>
+      <c r="Y38" s="13"/>
+      <c r="Z38" s="13"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A39" s="37">
         <v>43001001</v>
       </c>
@@ -10693,18 +11171,20 @@
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
-      <c r="S39" s="4" t="s">
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="T39" s="6" t="s">
+      <c r="V39" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="U39" s="17"/>
-      <c r="V39" s="13"/>
-      <c r="W39" s="13"/>
+      <c r="W39" s="17"/>
       <c r="X39" s="13"/>
+      <c r="Y39" s="13"/>
+      <c r="Z39" s="13"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A40" s="37">
         <v>43001002</v>
       </c>
@@ -10749,18 +11229,20 @@
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
-      <c r="S40" s="4" t="s">
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="T40" s="4" t="s">
+      <c r="V40" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U40" s="36"/>
-      <c r="V40" s="13"/>
-      <c r="W40" s="13"/>
+      <c r="W40" s="36"/>
       <c r="X40" s="13"/>
+      <c r="Y40" s="13"/>
+      <c r="Z40" s="13"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A41" s="37">
         <v>43001003</v>
       </c>
@@ -10805,18 +11287,20 @@
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
-      <c r="S41" s="4" t="s">
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="T41" s="4" t="s">
+      <c r="V41" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U41" s="27"/>
-      <c r="V41" s="13"/>
-      <c r="W41" s="13"/>
+      <c r="W41" s="27"/>
       <c r="X41" s="13"/>
+      <c r="Y41" s="13"/>
+      <c r="Z41" s="13"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A42" s="37">
         <v>43001004</v>
       </c>
@@ -10861,18 +11345,20 @@
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
-      <c r="S42" s="4" t="s">
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="T42" s="34" t="s">
+      <c r="V42" s="34" t="s">
         <v>418</v>
       </c>
-      <c r="U42" s="17"/>
-      <c r="V42" s="13"/>
-      <c r="W42" s="13"/>
+      <c r="W42" s="17"/>
       <c r="X42" s="13"/>
+      <c r="Y42" s="13"/>
+      <c r="Z42" s="13"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A43" s="37">
         <v>43001005</v>
       </c>
@@ -10917,18 +11403,20 @@
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
-      <c r="S43" s="4" t="s">
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="T43" s="4" t="s">
+      <c r="V43" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U43" s="17"/>
-      <c r="V43" s="13"/>
-      <c r="W43" s="13"/>
+      <c r="W43" s="17"/>
       <c r="X43" s="13"/>
+      <c r="Y43" s="13"/>
+      <c r="Z43" s="13"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A44" s="37">
         <v>43001006</v>
       </c>
@@ -10973,18 +11461,20 @@
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
-      <c r="S44" s="4" t="s">
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="T44" s="6" t="s">
+      <c r="V44" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="U44" s="36"/>
-      <c r="V44" s="13"/>
-      <c r="W44" s="13"/>
+      <c r="W44" s="36"/>
       <c r="X44" s="13"/>
+      <c r="Y44" s="13"/>
+      <c r="Z44" s="13"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A45" s="38">
         <v>43002001</v>
       </c>
@@ -11027,18 +11517,20 @@
       <c r="P45" s="27"/>
       <c r="Q45" s="27"/>
       <c r="R45" s="27"/>
-      <c r="S45" s="4" t="s">
+      <c r="S45" s="27"/>
+      <c r="T45" s="27"/>
+      <c r="U45" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="T45" s="27" t="s">
+      <c r="V45" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="U45" s="27"/>
-      <c r="V45" s="13"/>
-      <c r="W45" s="13"/>
+      <c r="W45" s="27"/>
       <c r="X45" s="13"/>
+      <c r="Y45" s="13"/>
+      <c r="Z45" s="13"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A46" s="38">
         <v>43002002</v>
       </c>
@@ -11081,18 +11573,20 @@
       <c r="P46" s="27"/>
       <c r="Q46" s="27"/>
       <c r="R46" s="27"/>
-      <c r="S46" s="4" t="s">
+      <c r="S46" s="27"/>
+      <c r="T46" s="27"/>
+      <c r="U46" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="T46" s="27" t="s">
+      <c r="V46" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="U46" s="27"/>
-      <c r="V46" s="13"/>
-      <c r="W46" s="13"/>
+      <c r="W46" s="27"/>
       <c r="X46" s="13"/>
+      <c r="Y46" s="13"/>
+      <c r="Z46" s="13"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A47" s="38">
         <v>43002003</v>
       </c>
@@ -11135,18 +11629,20 @@
       <c r="P47" s="27"/>
       <c r="Q47" s="27"/>
       <c r="R47" s="27"/>
-      <c r="S47" s="4" t="s">
+      <c r="S47" s="27"/>
+      <c r="T47" s="27"/>
+      <c r="U47" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="T47" s="27" t="s">
+      <c r="V47" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="U47" s="27"/>
-      <c r="V47" s="13"/>
-      <c r="W47" s="13"/>
+      <c r="W47" s="27"/>
       <c r="X47" s="13"/>
+      <c r="Y47" s="13"/>
+      <c r="Z47" s="13"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A48" s="38">
         <v>43002004</v>
       </c>
@@ -11189,18 +11685,20 @@
       <c r="P48" s="27"/>
       <c r="Q48" s="13"/>
       <c r="R48" s="13"/>
-      <c r="S48" s="31" t="s">
+      <c r="S48" s="13"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="31" t="s">
         <v>336</v>
       </c>
-      <c r="T48" s="27" t="s">
+      <c r="V48" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="U48" s="27"/>
-      <c r="V48" s="13"/>
-      <c r="W48" s="13"/>
+      <c r="W48" s="27"/>
       <c r="X48" s="13"/>
+      <c r="Y48" s="13"/>
+      <c r="Z48" s="13"/>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A49" s="38">
         <v>43002005</v>
       </c>
@@ -11243,18 +11741,20 @@
       <c r="P49" s="27"/>
       <c r="Q49" s="13"/>
       <c r="R49" s="13"/>
-      <c r="S49" s="31" t="s">
+      <c r="S49" s="13"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="T49" s="27" t="s">
+      <c r="V49" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="U49" s="27"/>
-      <c r="V49" s="13"/>
-      <c r="W49" s="13"/>
+      <c r="W49" s="27"/>
       <c r="X49" s="13"/>
+      <c r="Y49" s="13"/>
+      <c r="Z49" s="13"/>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A50" s="38">
         <v>43002006</v>
       </c>
@@ -11297,51 +11797,53 @@
       <c r="P50" s="27"/>
       <c r="Q50" s="13"/>
       <c r="R50" s="13"/>
-      <c r="S50" s="31" t="s">
+      <c r="S50" s="13"/>
+      <c r="T50" s="13"/>
+      <c r="U50" s="31" t="s">
         <v>338</v>
       </c>
-      <c r="T50" s="27" t="s">
+      <c r="V50" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="U50" s="27"/>
-      <c r="V50" s="13"/>
-      <c r="W50" s="13"/>
+      <c r="W50" s="27"/>
       <c r="X50" s="13"/>
+      <c r="Y50" s="13"/>
+      <c r="Z50" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="T42">
-    <cfRule type="containsBlanks" dxfId="16" priority="9">
-      <formula>LEN(TRIM(T42))=0</formula>
+  <conditionalFormatting sqref="V42">
+    <cfRule type="containsBlanks" dxfId="7" priority="9">
+      <formula>LEN(TRIM(V42))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsBlanks" dxfId="15" priority="8">
+    <cfRule type="containsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(C47))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S47">
-    <cfRule type="containsBlanks" dxfId="14" priority="6">
-      <formula>LEN(TRIM(S47))=0</formula>
+  <conditionalFormatting sqref="U47">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(U47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C50">
-    <cfRule type="containsBlanks" dxfId="13" priority="5">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(C48))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S48:S50">
-    <cfRule type="containsBlanks" dxfId="12" priority="3">
-      <formula>LEN(TRIM(S48))=0</formula>
+  <conditionalFormatting sqref="U48:U50">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
+      <formula>LEN(TRIM(U48))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="containsBlanks" dxfId="11" priority="2">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(K47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:K50">
-    <cfRule type="containsBlanks" dxfId="10" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(K48))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11354,14 +11856,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:X14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W8" sqref="W8"/>
+      <selection pane="bottomRight" activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -11375,12 +11877,12 @@
     <col min="13" max="14" width="6.125" customWidth="1"/>
     <col min="15" max="15" width="28.375" customWidth="1"/>
     <col min="16" max="16" width="19.5" customWidth="1"/>
-    <col min="17" max="18" width="9.875" customWidth="1"/>
-    <col min="20" max="20" width="10.625" customWidth="1"/>
-    <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="4.125" customWidth="1"/>
+    <col min="22" max="22" width="10.625" customWidth="1"/>
+    <col min="23" max="23" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>145</v>
       </c>
@@ -11435,26 +11937,32 @@
       <c r="R1" s="39" t="s">
         <v>428</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="S1" s="39" t="s">
+        <v>498</v>
+      </c>
+      <c r="T1" s="39" t="s">
+        <v>499</v>
+      </c>
+      <c r="U1" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="V1" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="W1" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="V1" s="29" t="s">
+      <c r="X1" s="29" t="s">
         <v>432</v>
       </c>
-      <c r="W1" s="29" t="s">
+      <c r="Y1" s="29" t="s">
         <v>436</v>
       </c>
-      <c r="X1" s="29" t="s">
+      <c r="Z1" s="29" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>143</v>
       </c>
@@ -11509,26 +12017,32 @@
       <c r="R2" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="S2" s="40" t="s">
+        <v>496</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>496</v>
+      </c>
+      <c r="U2" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="V2" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="W2" s="8" t="s">
         <v>200</v>
-      </c>
-      <c r="V2" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="W2" s="30" t="s">
-        <v>144</v>
       </c>
       <c r="X2" s="30" t="s">
         <v>144</v>
       </c>
+      <c r="Y2" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z2" s="30" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>154</v>
       </c>
@@ -11583,26 +12097,32 @@
       <c r="R3" s="41" t="s">
         <v>430</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="S3" s="41" t="s">
+        <v>497</v>
+      </c>
+      <c r="T3" s="41" t="s">
+        <v>500</v>
+      </c>
+      <c r="U3" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="V3" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="U3" s="18" t="s">
+      <c r="W3" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="V3" s="18" t="s">
+      <c r="X3" s="18" t="s">
         <v>434</v>
       </c>
-      <c r="W3" s="18" t="s">
+      <c r="Y3" s="18" t="s">
         <v>433</v>
       </c>
-      <c r="X3" s="18" t="s">
+      <c r="Z3" s="18" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>43010001</v>
       </c>
@@ -11645,18 +12165,20 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
-      <c r="S4" s="4" t="s">
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U4" s="15"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="42"/>
+      <c r="W4" s="15"/>
       <c r="X4" s="42"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="42"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>43010002</v>
       </c>
@@ -11697,18 +12219,20 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="4" t="s">
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="V5" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U5" s="14"/>
-      <c r="V5" s="42"/>
-      <c r="W5" s="42"/>
+      <c r="W5" s="14"/>
       <c r="X5" s="42"/>
+      <c r="Y5" s="42"/>
+      <c r="Z5" s="42"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>43010003</v>
       </c>
@@ -11749,18 +12273,20 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="4" t="s">
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="T6" s="4" t="s">
+      <c r="V6" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U6" s="14"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="42"/>
+      <c r="W6" s="14"/>
       <c r="X6" s="42"/>
+      <c r="Y6" s="42"/>
+      <c r="Z6" s="42"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>43010004</v>
       </c>
@@ -11801,18 +12327,20 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
-      <c r="S7" s="4" t="s">
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="T7" s="4" t="s">
+      <c r="V7" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U7" s="14"/>
-      <c r="V7" s="42"/>
-      <c r="W7" s="42"/>
+      <c r="W7" s="14"/>
       <c r="X7" s="42"/>
+      <c r="Y7" s="42"/>
+      <c r="Z7" s="42"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>43010005</v>
       </c>
@@ -11855,18 +12383,20 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
-      <c r="S8" s="6" t="s">
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="T8" s="4" t="s">
+      <c r="V8" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U8" s="14"/>
-      <c r="V8" s="42"/>
-      <c r="W8" s="42"/>
+      <c r="W8" s="14"/>
       <c r="X8" s="42"/>
+      <c r="Y8" s="42"/>
+      <c r="Z8" s="42"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>43010006</v>
       </c>
@@ -11909,18 +12439,20 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
-      <c r="S9" s="6" t="s">
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="V9" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U9" s="14"/>
-      <c r="V9" s="42"/>
-      <c r="W9" s="42"/>
+      <c r="W9" s="14"/>
       <c r="X9" s="42"/>
+      <c r="Y9" s="42"/>
+      <c r="Z9" s="42"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>43010101</v>
       </c>
@@ -11959,18 +12491,20 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
-      <c r="S10" s="4" t="s">
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="T10" s="4" t="s">
+      <c r="V10" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U10" s="14"/>
-      <c r="V10" s="42"/>
-      <c r="W10" s="42"/>
+      <c r="W10" s="14"/>
       <c r="X10" s="42"/>
+      <c r="Y10" s="42"/>
+      <c r="Z10" s="42"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>43010102</v>
       </c>
@@ -12009,18 +12543,20 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
-      <c r="S11" s="4" t="s">
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="V11" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U11" s="14"/>
-      <c r="V11" s="42"/>
-      <c r="W11" s="42"/>
+      <c r="W11" s="14"/>
       <c r="X11" s="42"/>
+      <c r="Y11" s="42"/>
+      <c r="Z11" s="42"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>43010103</v>
       </c>
@@ -12059,18 +12595,20 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
-      <c r="S12" s="4" t="s">
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="T12" s="4" t="s">
+      <c r="V12" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U12" s="14"/>
-      <c r="V12" s="42"/>
-      <c r="W12" s="42"/>
+      <c r="W12" s="14"/>
       <c r="X12" s="42"/>
+      <c r="Y12" s="42"/>
+      <c r="Z12" s="42"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>43010104</v>
       </c>
@@ -12109,18 +12647,20 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
-      <c r="S13" s="4" t="s">
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="T13" s="4" t="s">
+      <c r="V13" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U13" s="14"/>
-      <c r="V13" s="42"/>
-      <c r="W13" s="42"/>
+      <c r="W13" s="14"/>
       <c r="X13" s="42"/>
+      <c r="Y13" s="42"/>
+      <c r="Z13" s="42"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>43010105</v>
       </c>
@@ -12159,16 +12699,18 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
-      <c r="S14" s="4" t="s">
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="T14" s="4" t="s">
+      <c r="V14" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="U14" s="14"/>
-      <c r="V14" s="42"/>
-      <c r="W14" s="42"/>
+      <c r="W14" s="14"/>
       <c r="X14" s="42"/>
+      <c r="Y14" s="42"/>
+      <c r="Z14" s="42"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>